<commit_message>
Chapter 3 into final review, and Chapter 4.1-3 done review 1
</commit_message>
<xml_diff>
--- a/Word/PlanAndDealines.xlsx
+++ b/Word/PlanAndDealines.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ksung\Desktop\GitHub\GTCS-GameEngine2\Word\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C1E16656-E7DD-49D9-9ABE-96237A38E702}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{424735CD-23F1-412C-BCB6-45675E43750D}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="38400" windowHeight="20025" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="189" uniqueCount="129">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="190" uniqueCount="132">
   <si>
     <t>First Pass</t>
   </si>
@@ -445,6 +445,15 @@
   </si>
   <si>
     <t xml:space="preserve">Jeb + Mattew </t>
+  </si>
+  <si>
+    <t>https://www.w3.org/TR/html52/browsers.html#the-window-object</t>
+  </si>
+  <si>
+    <t>Matthew: more, but straightforward changes</t>
+  </si>
+  <si>
+    <t>Jeb: need to explain oscillate</t>
   </si>
 </sst>
 </file>
@@ -1069,7 +1078,7 @@
   <dimension ref="B1:S142"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="220" zoomScaleNormal="220" workbookViewId="0">
-      <selection activeCell="F7" sqref="F7"/>
+      <selection activeCell="J6" sqref="J6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1"/>
@@ -1274,7 +1283,9 @@
       <c r="I5" s="42" t="s">
         <v>6</v>
       </c>
-      <c r="J5" s="43"/>
+      <c r="J5" s="43">
+        <v>44297</v>
+      </c>
       <c r="K5" s="47" t="s">
         <v>16</v>
       </c>
@@ -1372,8 +1383,8 @@
       <c r="B8" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="E8" s="46" t="s">
-        <v>8</v>
+      <c r="E8" s="33" t="s">
+        <v>130</v>
       </c>
       <c r="F8" s="45"/>
       <c r="G8" s="46"/>
@@ -1402,7 +1413,7 @@
         <v>13</v>
       </c>
       <c r="E9" s="46" t="s">
-        <v>6</v>
+        <v>131</v>
       </c>
       <c r="F9" s="45"/>
       <c r="G9" s="46"/>
@@ -1691,7 +1702,9 @@
       <c r="N23" s="41"/>
     </row>
     <row r="24" spans="5:14" ht="15.75" customHeight="1">
-      <c r="E24" s="41"/>
+      <c r="E24" s="41" t="s">
+        <v>129</v>
+      </c>
       <c r="F24" s="41"/>
       <c r="G24" s="41"/>
       <c r="H24" s="41"/>

</xml_diff>

<commit_message>
Final update on Chapter 3
</commit_message>
<xml_diff>
--- a/Word/PlanAndDealines.xlsx
+++ b/Word/PlanAndDealines.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ksung\Desktop\GitHub\GTCS-GameEngine2\Word\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{424735CD-23F1-412C-BCB6-45675E43750D}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C442AB43-33B4-40C1-BF21-82C3780E384D}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="38400" windowHeight="20025" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="190" uniqueCount="132">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="192" uniqueCount="134">
   <si>
     <t>First Pass</t>
   </si>
@@ -454,6 +454,12 @@
   </si>
   <si>
     <t>Jeb: need to explain oscillate</t>
+  </si>
+  <si>
+    <t>SHOULD WE?</t>
+  </si>
+  <si>
+    <t>Integrate loading icon into the last final engine?</t>
   </si>
 </sst>
 </file>
@@ -713,7 +719,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="63">
+  <cellXfs count="65">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
@@ -856,6 +862,12 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1077,8 +1089,8 @@
   </sheetPr>
   <dimension ref="B1:S142"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="220" zoomScaleNormal="220" workbookViewId="0">
-      <selection activeCell="J6" sqref="J6"/>
+    <sheetView tabSelected="1" topLeftCell="A10" zoomScale="220" zoomScaleNormal="220" workbookViewId="0">
+      <selection activeCell="O17" sqref="O17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1"/>
@@ -1606,9 +1618,11 @@
       <c r="K16" s="41"/>
       <c r="L16" s="41"/>
       <c r="M16" s="41"/>
-      <c r="N16" s="41"/>
-    </row>
-    <row r="17" spans="5:14" ht="15.75" customHeight="1">
+      <c r="O16" s="63" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="17" spans="5:15" ht="15.75" customHeight="1">
       <c r="E17" s="56" t="s">
         <v>120</v>
       </c>
@@ -1620,9 +1634,11 @@
       <c r="K17" s="41"/>
       <c r="L17" s="41"/>
       <c r="M17" s="41"/>
-      <c r="N17" s="41"/>
-    </row>
-    <row r="18" spans="5:14" ht="15.75" customHeight="1">
+      <c r="O17" s="56" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="18" spans="5:15" ht="15.75" customHeight="1">
       <c r="E18" s="56" t="s">
         <v>121</v>
       </c>
@@ -1634,9 +1650,10 @@
       <c r="K18" s="41"/>
       <c r="L18" s="41"/>
       <c r="M18" s="41"/>
-      <c r="N18" s="41"/>
-    </row>
-    <row r="19" spans="5:14" ht="15.75" customHeight="1">
+      <c r="N18" s="64"/>
+      <c r="O18" s="29"/>
+    </row>
+    <row r="19" spans="5:15" ht="15.75" customHeight="1">
       <c r="E19" s="56" t="s">
         <v>122</v>
       </c>
@@ -1648,9 +1665,10 @@
       <c r="K19" s="41"/>
       <c r="L19" s="41"/>
       <c r="M19" s="41"/>
-      <c r="N19" s="41"/>
-    </row>
-    <row r="20" spans="5:14" ht="15.75" customHeight="1">
+      <c r="N19" s="64"/>
+      <c r="O19" s="29"/>
+    </row>
+    <row r="20" spans="5:15" ht="15.75" customHeight="1">
       <c r="F20" s="41"/>
       <c r="G20" s="41"/>
       <c r="H20" s="41"/>
@@ -1659,9 +1677,10 @@
       <c r="K20" s="41"/>
       <c r="L20" s="41"/>
       <c r="M20" s="41"/>
-      <c r="N20" s="41"/>
-    </row>
-    <row r="21" spans="5:14" ht="15.75" customHeight="1">
+      <c r="N20" s="64"/>
+      <c r="O20" s="29"/>
+    </row>
+    <row r="21" spans="5:15" ht="15.75" customHeight="1">
       <c r="E21" s="56" t="s">
         <v>117</v>
       </c>
@@ -1673,9 +1692,10 @@
       <c r="K21" s="41"/>
       <c r="L21" s="41"/>
       <c r="M21" s="41"/>
-      <c r="N21" s="41"/>
-    </row>
-    <row r="22" spans="5:14" ht="15.75" customHeight="1">
+      <c r="N21" s="64"/>
+      <c r="O21" s="29"/>
+    </row>
+    <row r="22" spans="5:15" ht="15.75" customHeight="1">
       <c r="E22" s="56" t="s">
         <v>118</v>
       </c>
@@ -1687,9 +1707,10 @@
       <c r="K22" s="41"/>
       <c r="L22" s="41"/>
       <c r="M22" s="41"/>
-      <c r="N22" s="41"/>
-    </row>
-    <row r="23" spans="5:14" ht="15.75" customHeight="1">
+      <c r="N22" s="64"/>
+      <c r="O22" s="29"/>
+    </row>
+    <row r="23" spans="5:15" ht="15.75" customHeight="1">
       <c r="E23" s="41"/>
       <c r="F23" s="41"/>
       <c r="G23" s="41"/>
@@ -1699,9 +1720,10 @@
       <c r="K23" s="41"/>
       <c r="L23" s="41"/>
       <c r="M23" s="41"/>
-      <c r="N23" s="41"/>
-    </row>
-    <row r="24" spans="5:14" ht="15.75" customHeight="1">
+      <c r="N23" s="64"/>
+      <c r="O23" s="29"/>
+    </row>
+    <row r="24" spans="5:15" ht="15.75" customHeight="1">
       <c r="E24" s="41" t="s">
         <v>129</v>
       </c>
@@ -1713,9 +1735,10 @@
       <c r="K24" s="41"/>
       <c r="L24" s="41"/>
       <c r="M24" s="41"/>
-      <c r="N24" s="41"/>
-    </row>
-    <row r="25" spans="5:14" ht="15.75" customHeight="1">
+      <c r="N24" s="64"/>
+      <c r="O24" s="29"/>
+    </row>
+    <row r="25" spans="5:15" ht="15.75" customHeight="1">
       <c r="E25" s="41"/>
       <c r="F25" s="41"/>
       <c r="G25" s="41"/>
@@ -1725,9 +1748,10 @@
       <c r="K25" s="41"/>
       <c r="L25" s="41"/>
       <c r="M25" s="41"/>
-      <c r="N25" s="41"/>
-    </row>
-    <row r="26" spans="5:14" ht="15.75" customHeight="1">
+      <c r="N25" s="64"/>
+      <c r="O25" s="29"/>
+    </row>
+    <row r="26" spans="5:15" ht="15.75" customHeight="1">
       <c r="E26" s="41"/>
       <c r="F26" s="41"/>
       <c r="G26" s="41"/>
@@ -1737,9 +1761,10 @@
       <c r="K26" s="41"/>
       <c r="L26" s="41"/>
       <c r="M26" s="41"/>
-      <c r="N26" s="41"/>
-    </row>
-    <row r="27" spans="5:14" ht="15.75" customHeight="1">
+      <c r="N26" s="64"/>
+      <c r="O26" s="29"/>
+    </row>
+    <row r="27" spans="5:15" ht="15.75" customHeight="1">
       <c r="E27" s="41"/>
       <c r="F27" s="41"/>
       <c r="G27" s="41"/>
@@ -1749,9 +1774,10 @@
       <c r="K27" s="41"/>
       <c r="L27" s="41"/>
       <c r="M27" s="41"/>
-      <c r="N27" s="41"/>
-    </row>
-    <row r="28" spans="5:14" ht="15.75" customHeight="1">
+      <c r="N27" s="64"/>
+      <c r="O27" s="29"/>
+    </row>
+    <row r="28" spans="5:15" ht="15.75" customHeight="1">
       <c r="E28" s="41"/>
       <c r="F28" s="41"/>
       <c r="G28" s="41"/>
@@ -1761,9 +1787,10 @@
       <c r="K28" s="41"/>
       <c r="L28" s="41"/>
       <c r="M28" s="41"/>
-      <c r="N28" s="41"/>
-    </row>
-    <row r="29" spans="5:14" ht="15.75" customHeight="1">
+      <c r="N28" s="64"/>
+      <c r="O28" s="29"/>
+    </row>
+    <row r="29" spans="5:15" ht="15.75" customHeight="1">
       <c r="E29" s="41"/>
       <c r="F29" s="41"/>
       <c r="G29" s="41"/>
@@ -1773,9 +1800,10 @@
       <c r="K29" s="41"/>
       <c r="L29" s="41"/>
       <c r="M29" s="41"/>
-      <c r="N29" s="41"/>
-    </row>
-    <row r="30" spans="5:14" ht="15.75" customHeight="1">
+      <c r="N29" s="64"/>
+      <c r="O29" s="29"/>
+    </row>
+    <row r="30" spans="5:15" ht="15.75" customHeight="1">
       <c r="E30" s="41"/>
       <c r="F30" s="41"/>
       <c r="G30" s="41"/>
@@ -1785,9 +1813,10 @@
       <c r="K30" s="41"/>
       <c r="L30" s="41"/>
       <c r="M30" s="41"/>
-      <c r="N30" s="41"/>
-    </row>
-    <row r="31" spans="5:14" ht="15.75" customHeight="1">
+      <c r="N30" s="64"/>
+      <c r="O30" s="29"/>
+    </row>
+    <row r="31" spans="5:15" ht="15.75" customHeight="1">
       <c r="E31" s="41"/>
       <c r="F31" s="41"/>
       <c r="G31" s="41"/>
@@ -1797,9 +1826,10 @@
       <c r="K31" s="41"/>
       <c r="L31" s="41"/>
       <c r="M31" s="41"/>
-      <c r="N31" s="41"/>
-    </row>
-    <row r="32" spans="5:14" ht="15.75" customHeight="1">
+      <c r="N31" s="64"/>
+      <c r="O31" s="29"/>
+    </row>
+    <row r="32" spans="5:15" ht="15.75" customHeight="1">
       <c r="E32" s="41"/>
       <c r="F32" s="41"/>
       <c r="G32" s="41"/>
@@ -1809,7 +1839,8 @@
       <c r="K32" s="41"/>
       <c r="L32" s="41"/>
       <c r="M32" s="41"/>
-      <c r="N32" s="41"/>
+      <c r="N32" s="64"/>
+      <c r="O32" s="29"/>
     </row>
     <row r="33" spans="5:14" ht="15.75" customHeight="1">
       <c r="E33" s="41"/>

</xml_diff>

<commit_message>
First pass physics working
</commit_message>
<xml_diff>
--- a/Word/PlanAndDealines.xlsx
+++ b/Word/PlanAndDealines.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ksung\Desktop\GitHub\GTCS-GameEngine2\Word\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C442AB43-33B4-40C1-BF21-82C3780E384D}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A07A88E0-802C-4F04-A8AF-CF65BC517C86}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="38400" windowHeight="20025" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="192" uniqueCount="134">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="193" uniqueCount="134">
   <si>
     <t>First Pass</t>
   </si>
@@ -1089,8 +1089,8 @@
   </sheetPr>
   <dimension ref="B1:S142"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" zoomScale="220" zoomScaleNormal="220" workbookViewId="0">
-      <selection activeCell="O17" sqref="O17"/>
+    <sheetView tabSelected="1" topLeftCell="C1" zoomScale="220" zoomScaleNormal="220" workbookViewId="0">
+      <selection activeCell="R7" sqref="R7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1"/>
@@ -1306,20 +1306,22 @@
         <v>8</v>
       </c>
       <c r="N5" s="43"/>
-      <c r="O5" s="28"/>
+      <c r="O5" s="28" t="s">
+        <v>116</v>
+      </c>
       <c r="P5" s="58">
         <v>44298</v>
       </c>
       <c r="Q5" s="57">
         <f>DATE(YEAR(P5),MONTH(P5),DAY(P5)+S5)</f>
-        <v>44305</v>
+        <v>44299</v>
       </c>
       <c r="R5">
-        <v>7</v>
+        <v>1</v>
       </c>
       <c r="S5">
         <f>SUM(R5)</f>
-        <v>7</v>
+        <v>1</v>
       </c>
     </row>
     <row r="6" spans="2:19" ht="26.25" customHeight="1">
@@ -1355,11 +1357,14 @@
       </c>
       <c r="Q6" s="57">
         <f t="shared" ref="Q6:Q14" si="0">DATE(YEAR(P6),MONTH(P6),DAY(P6)+S6)</f>
-        <v>44305</v>
+        <v>44302</v>
+      </c>
+      <c r="R6">
+        <v>3</v>
       </c>
       <c r="S6">
         <f>SUM(R6,S5)</f>
-        <v>7</v>
+        <v>4</v>
       </c>
     </row>
     <row r="7" spans="2:19" ht="26.25" customHeight="1">
@@ -1384,11 +1389,11 @@
       </c>
       <c r="Q7" s="57">
         <f t="shared" si="0"/>
-        <v>44312</v>
+        <v>44309</v>
       </c>
       <c r="S7">
         <f t="shared" ref="S7:S14" si="1">SUM(R7,S6)</f>
-        <v>7</v>
+        <v>4</v>
       </c>
     </row>
     <row r="8" spans="2:19" ht="26.25" customHeight="1">
@@ -1413,11 +1418,11 @@
       </c>
       <c r="Q8" s="57">
         <f t="shared" si="0"/>
-        <v>44319</v>
+        <v>44316</v>
       </c>
       <c r="S8">
         <f t="shared" si="1"/>
-        <v>7</v>
+        <v>4</v>
       </c>
     </row>
     <row r="9" spans="2:19" ht="26.25" customHeight="1">
@@ -1442,11 +1447,11 @@
       </c>
       <c r="Q9" s="57">
         <f t="shared" si="0"/>
-        <v>44319</v>
+        <v>44316</v>
       </c>
       <c r="S9">
         <f t="shared" si="1"/>
-        <v>7</v>
+        <v>4</v>
       </c>
     </row>
     <row r="10" spans="2:19" ht="26.25" customHeight="1">
@@ -1471,11 +1476,11 @@
       </c>
       <c r="Q10" s="57">
         <f t="shared" si="0"/>
-        <v>44326</v>
+        <v>44323</v>
       </c>
       <c r="S10">
         <f t="shared" si="1"/>
-        <v>7</v>
+        <v>4</v>
       </c>
     </row>
     <row r="11" spans="2:19" ht="26.25" customHeight="1">
@@ -1501,11 +1506,11 @@
       </c>
       <c r="Q11" s="57">
         <f t="shared" si="0"/>
-        <v>44347</v>
+        <v>44344</v>
       </c>
       <c r="S11">
         <f t="shared" si="1"/>
-        <v>7</v>
+        <v>4</v>
       </c>
     </row>
     <row r="12" spans="2:19" ht="26.25" customHeight="1">
@@ -1531,11 +1536,11 @@
       </c>
       <c r="Q12" s="57">
         <f t="shared" si="0"/>
-        <v>44361</v>
+        <v>44358</v>
       </c>
       <c r="S12">
         <f t="shared" si="1"/>
-        <v>7</v>
+        <v>4</v>
       </c>
     </row>
     <row r="13" spans="2:19" ht="26.25" customHeight="1">
@@ -1558,11 +1563,11 @@
       </c>
       <c r="Q13" s="57">
         <f t="shared" si="0"/>
-        <v>44368</v>
+        <v>44365</v>
       </c>
       <c r="S13">
         <f t="shared" si="1"/>
-        <v>7</v>
+        <v>4</v>
       </c>
     </row>
     <row r="14" spans="2:19" ht="26.25" customHeight="1" thickBot="1">
@@ -1587,11 +1592,11 @@
       </c>
       <c r="Q14" s="57">
         <f t="shared" si="0"/>
-        <v>44375</v>
+        <v>44372</v>
       </c>
       <c r="S14">
         <f t="shared" si="1"/>
-        <v>7</v>
+        <v>4</v>
       </c>
     </row>
     <row r="15" spans="2:19" ht="15.75" customHeight="1" thickTop="1">

</xml_diff>

<commit_message>
Chapter 4, PassTwoReviewed Done. Moving on to Matthew
</commit_message>
<xml_diff>
--- a/Word/PlanAndDealines.xlsx
+++ b/Word/PlanAndDealines.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ksung\Desktop\GitHub\GTCS-GameEngine2\Word\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A07A88E0-802C-4F04-A8AF-CF65BC517C86}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1A5AA5F2-0C71-4B09-8DAF-BE15B0CBABED}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="38400" windowHeight="20025" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="193" uniqueCount="134">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="195" uniqueCount="136">
   <si>
     <t>First Pass</t>
   </si>
@@ -461,12 +461,18 @@
   <si>
     <t>Integrate loading icon into the last final engine?</t>
   </si>
+  <si>
+    <t>Chapter 4: Add a section before "Resource Map" talking about async load.</t>
+  </si>
+  <si>
+    <t>https://developer.mozilla.org/en-US/docs/Learn/JavaScript/Asynchronous</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="27">
+  <fonts count="28">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -619,6 +625,12 @@
       <name val="Arial"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
   </fonts>
   <fills count="3">
     <fill>
@@ -719,7 +731,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="65">
+  <cellXfs count="66">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
@@ -857,18 +869,19 @@
     <xf numFmtId="0" fontId="24" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
+    <xf numFmtId="0" fontId="27" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1089,8 +1102,8 @@
   </sheetPr>
   <dimension ref="B1:S142"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" zoomScale="220" zoomScaleNormal="220" workbookViewId="0">
-      <selection activeCell="R7" sqref="R7"/>
+    <sheetView tabSelected="1" topLeftCell="C13" zoomScale="220" zoomScaleNormal="220" workbookViewId="0">
+      <selection activeCell="P22" sqref="P22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1"/>
@@ -1113,26 +1126,26 @@
     <row r="1" spans="2:19" ht="12.75">
       <c r="C1" s="1"/>
       <c r="D1" s="1"/>
-      <c r="E1" s="61" t="s">
+      <c r="E1" s="63" t="s">
         <v>0</v>
       </c>
-      <c r="F1" s="62"/>
-      <c r="G1" s="61" t="s">
+      <c r="F1" s="64"/>
+      <c r="G1" s="63" t="s">
         <v>1</v>
       </c>
-      <c r="H1" s="62"/>
-      <c r="I1" s="61" t="s">
+      <c r="H1" s="64"/>
+      <c r="I1" s="63" t="s">
         <v>2</v>
       </c>
-      <c r="J1" s="62"/>
-      <c r="K1" s="61" t="s">
+      <c r="J1" s="64"/>
+      <c r="K1" s="63" t="s">
         <v>1</v>
       </c>
-      <c r="L1" s="62"/>
-      <c r="M1" s="61" t="s">
+      <c r="L1" s="64"/>
+      <c r="M1" s="63" t="s">
         <v>3</v>
       </c>
-      <c r="N1" s="62"/>
+      <c r="N1" s="64"/>
       <c r="O1" s="30" t="s">
         <v>4</v>
       </c>
@@ -1623,11 +1636,11 @@
       <c r="K16" s="41"/>
       <c r="L16" s="41"/>
       <c r="M16" s="41"/>
-      <c r="O16" s="63" t="s">
+      <c r="O16" s="61" t="s">
         <v>132</v>
       </c>
     </row>
-    <row r="17" spans="5:15" ht="15.75" customHeight="1">
+    <row r="17" spans="5:16" ht="15.75" customHeight="1">
       <c r="E17" s="56" t="s">
         <v>120</v>
       </c>
@@ -1643,7 +1656,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="18" spans="5:15" ht="15.75" customHeight="1">
+    <row r="18" spans="5:16" ht="15.75" customHeight="1">
       <c r="E18" s="56" t="s">
         <v>121</v>
       </c>
@@ -1655,10 +1668,12 @@
       <c r="K18" s="41"/>
       <c r="L18" s="41"/>
       <c r="M18" s="41"/>
-      <c r="N18" s="64"/>
-      <c r="O18" s="29"/>
-    </row>
-    <row r="19" spans="5:15" ht="15.75" customHeight="1">
+      <c r="N18" s="62"/>
+      <c r="O18" s="29" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="19" spans="5:16" ht="15.75" customHeight="1">
       <c r="E19" s="56" t="s">
         <v>122</v>
       </c>
@@ -1670,10 +1685,13 @@
       <c r="K19" s="41"/>
       <c r="L19" s="41"/>
       <c r="M19" s="41"/>
-      <c r="N19" s="64"/>
+      <c r="N19" s="62"/>
       <c r="O19" s="29"/>
-    </row>
-    <row r="20" spans="5:15" ht="15.75" customHeight="1">
+      <c r="P19" s="65" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="20" spans="5:16" ht="15.75" customHeight="1">
       <c r="F20" s="41"/>
       <c r="G20" s="41"/>
       <c r="H20" s="41"/>
@@ -1682,10 +1700,10 @@
       <c r="K20" s="41"/>
       <c r="L20" s="41"/>
       <c r="M20" s="41"/>
-      <c r="N20" s="64"/>
+      <c r="N20" s="62"/>
       <c r="O20" s="29"/>
     </row>
-    <row r="21" spans="5:15" ht="15.75" customHeight="1">
+    <row r="21" spans="5:16" ht="15.75" customHeight="1">
       <c r="E21" s="56" t="s">
         <v>117</v>
       </c>
@@ -1697,10 +1715,10 @@
       <c r="K21" s="41"/>
       <c r="L21" s="41"/>
       <c r="M21" s="41"/>
-      <c r="N21" s="64"/>
+      <c r="N21" s="62"/>
       <c r="O21" s="29"/>
     </row>
-    <row r="22" spans="5:15" ht="15.75" customHeight="1">
+    <row r="22" spans="5:16" ht="15.75" customHeight="1">
       <c r="E22" s="56" t="s">
         <v>118</v>
       </c>
@@ -1712,10 +1730,10 @@
       <c r="K22" s="41"/>
       <c r="L22" s="41"/>
       <c r="M22" s="41"/>
-      <c r="N22" s="64"/>
+      <c r="N22" s="62"/>
       <c r="O22" s="29"/>
     </row>
-    <row r="23" spans="5:15" ht="15.75" customHeight="1">
+    <row r="23" spans="5:16" ht="15.75" customHeight="1">
       <c r="E23" s="41"/>
       <c r="F23" s="41"/>
       <c r="G23" s="41"/>
@@ -1725,10 +1743,10 @@
       <c r="K23" s="41"/>
       <c r="L23" s="41"/>
       <c r="M23" s="41"/>
-      <c r="N23" s="64"/>
+      <c r="N23" s="62"/>
       <c r="O23" s="29"/>
     </row>
-    <row r="24" spans="5:15" ht="15.75" customHeight="1">
+    <row r="24" spans="5:16" ht="15.75" customHeight="1">
       <c r="E24" s="41" t="s">
         <v>129</v>
       </c>
@@ -1740,10 +1758,10 @@
       <c r="K24" s="41"/>
       <c r="L24" s="41"/>
       <c r="M24" s="41"/>
-      <c r="N24" s="64"/>
+      <c r="N24" s="62"/>
       <c r="O24" s="29"/>
     </row>
-    <row r="25" spans="5:15" ht="15.75" customHeight="1">
+    <row r="25" spans="5:16" ht="15.75" customHeight="1">
       <c r="E25" s="41"/>
       <c r="F25" s="41"/>
       <c r="G25" s="41"/>
@@ -1753,10 +1771,10 @@
       <c r="K25" s="41"/>
       <c r="L25" s="41"/>
       <c r="M25" s="41"/>
-      <c r="N25" s="64"/>
+      <c r="N25" s="62"/>
       <c r="O25" s="29"/>
     </row>
-    <row r="26" spans="5:15" ht="15.75" customHeight="1">
+    <row r="26" spans="5:16" ht="15.75" customHeight="1">
       <c r="E26" s="41"/>
       <c r="F26" s="41"/>
       <c r="G26" s="41"/>
@@ -1766,10 +1784,10 @@
       <c r="K26" s="41"/>
       <c r="L26" s="41"/>
       <c r="M26" s="41"/>
-      <c r="N26" s="64"/>
+      <c r="N26" s="62"/>
       <c r="O26" s="29"/>
     </row>
-    <row r="27" spans="5:15" ht="15.75" customHeight="1">
+    <row r="27" spans="5:16" ht="15.75" customHeight="1">
       <c r="E27" s="41"/>
       <c r="F27" s="41"/>
       <c r="G27" s="41"/>
@@ -1779,10 +1797,10 @@
       <c r="K27" s="41"/>
       <c r="L27" s="41"/>
       <c r="M27" s="41"/>
-      <c r="N27" s="64"/>
+      <c r="N27" s="62"/>
       <c r="O27" s="29"/>
     </row>
-    <row r="28" spans="5:15" ht="15.75" customHeight="1">
+    <row r="28" spans="5:16" ht="15.75" customHeight="1">
       <c r="E28" s="41"/>
       <c r="F28" s="41"/>
       <c r="G28" s="41"/>
@@ -1792,10 +1810,10 @@
       <c r="K28" s="41"/>
       <c r="L28" s="41"/>
       <c r="M28" s="41"/>
-      <c r="N28" s="64"/>
+      <c r="N28" s="62"/>
       <c r="O28" s="29"/>
     </row>
-    <row r="29" spans="5:15" ht="15.75" customHeight="1">
+    <row r="29" spans="5:16" ht="15.75" customHeight="1">
       <c r="E29" s="41"/>
       <c r="F29" s="41"/>
       <c r="G29" s="41"/>
@@ -1805,10 +1823,10 @@
       <c r="K29" s="41"/>
       <c r="L29" s="41"/>
       <c r="M29" s="41"/>
-      <c r="N29" s="64"/>
+      <c r="N29" s="62"/>
       <c r="O29" s="29"/>
     </row>
-    <row r="30" spans="5:15" ht="15.75" customHeight="1">
+    <row r="30" spans="5:16" ht="15.75" customHeight="1">
       <c r="E30" s="41"/>
       <c r="F30" s="41"/>
       <c r="G30" s="41"/>
@@ -1818,10 +1836,10 @@
       <c r="K30" s="41"/>
       <c r="L30" s="41"/>
       <c r="M30" s="41"/>
-      <c r="N30" s="64"/>
+      <c r="N30" s="62"/>
       <c r="O30" s="29"/>
     </row>
-    <row r="31" spans="5:15" ht="15.75" customHeight="1">
+    <row r="31" spans="5:16" ht="15.75" customHeight="1">
       <c r="E31" s="41"/>
       <c r="F31" s="41"/>
       <c r="G31" s="41"/>
@@ -1831,10 +1849,10 @@
       <c r="K31" s="41"/>
       <c r="L31" s="41"/>
       <c r="M31" s="41"/>
-      <c r="N31" s="64"/>
+      <c r="N31" s="62"/>
       <c r="O31" s="29"/>
     </row>
-    <row r="32" spans="5:15" ht="15.75" customHeight="1">
+    <row r="32" spans="5:16" ht="15.75" customHeight="1">
       <c r="E32" s="41"/>
       <c r="F32" s="41"/>
       <c r="G32" s="41"/>
@@ -1844,7 +1862,7 @@
       <c r="K32" s="41"/>
       <c r="L32" s="41"/>
       <c r="M32" s="41"/>
-      <c r="N32" s="64"/>
+      <c r="N32" s="62"/>
       <c r="O32" s="29"/>
     </row>
     <row r="33" spans="5:14" ht="15.75" customHeight="1">

</xml_diff>

<commit_message>
Examples 9.3 to 9,7 first rough draft
</commit_message>
<xml_diff>
--- a/Word/PlanAndDealines.xlsx
+++ b/Word/PlanAndDealines.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ksung\Desktop\GitHub\GTCS-GameEngine2\Word\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1A5AA5F2-0C71-4B09-8DAF-BE15B0CBABED}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{730486D4-CDA3-4CD2-890A-AF01DFAC5F02}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="38400" windowHeight="20025" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="195" uniqueCount="136">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="193" uniqueCount="133">
   <si>
     <t>First Pass</t>
   </si>
@@ -441,9 +441,6 @@
     <t>Total delays</t>
   </si>
   <si>
-    <t>Matthew (?)</t>
-  </si>
-  <si>
     <t xml:space="preserve">Jeb + Mattew </t>
   </si>
   <si>
@@ -460,12 +457,6 @@
   </si>
   <si>
     <t>Integrate loading icon into the last final engine?</t>
-  </si>
-  <si>
-    <t>Chapter 4: Add a section before "Resource Map" talking about async load.</t>
-  </si>
-  <si>
-    <t>https://developer.mozilla.org/en-US/docs/Learn/JavaScript/Asynchronous</t>
   </si>
 </sst>
 </file>
@@ -731,7 +722,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="66">
+  <cellXfs count="67">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
@@ -882,6 +873,9 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="27" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1102,8 +1096,8 @@
   </sheetPr>
   <dimension ref="B1:S142"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C13" zoomScale="220" zoomScaleNormal="220" workbookViewId="0">
-      <selection activeCell="P22" sqref="P22"/>
+    <sheetView tabSelected="1" topLeftCell="A8" zoomScale="220" zoomScaleNormal="220" workbookViewId="0">
+      <selection activeCell="Q17" sqref="Q17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1"/>
@@ -1314,11 +1308,15 @@
       <c r="K5" s="47" t="s">
         <v>16</v>
       </c>
-      <c r="L5" s="43"/>
+      <c r="L5" s="43">
+        <v>44298</v>
+      </c>
       <c r="M5" s="44" t="s">
         <v>8</v>
       </c>
-      <c r="N5" s="43"/>
+      <c r="N5" s="43">
+        <v>44299</v>
+      </c>
       <c r="O5" s="28" t="s">
         <v>116</v>
       </c>
@@ -1345,21 +1343,25 @@
       <c r="E6" s="42" t="s">
         <v>8</v>
       </c>
-      <c r="F6" s="43">
-        <v>44296</v>
-      </c>
+      <c r="F6" s="43"/>
       <c r="G6" s="44" t="s">
         <v>16</v>
       </c>
-      <c r="H6" s="43"/>
+      <c r="H6" s="43">
+        <v>44300</v>
+      </c>
       <c r="I6" s="42" t="s">
         <v>8</v>
       </c>
-      <c r="J6" s="43"/>
+      <c r="J6" s="43">
+        <v>44300</v>
+      </c>
       <c r="K6" s="47" t="s">
         <v>16</v>
       </c>
-      <c r="L6" s="43"/>
+      <c r="L6" s="43">
+        <v>44301</v>
+      </c>
       <c r="M6" s="44" t="s">
         <v>6</v>
       </c>
@@ -1384,8 +1386,8 @@
       <c r="B7" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="E7" s="46" t="s">
-        <v>127</v>
+      <c r="E7" s="44" t="s">
+        <v>6</v>
       </c>
       <c r="F7" s="45"/>
       <c r="G7" s="46"/>
@@ -1413,8 +1415,8 @@
       <c r="B8" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="E8" s="33" t="s">
-        <v>130</v>
+      <c r="E8" s="66" t="s">
+        <v>129</v>
       </c>
       <c r="F8" s="45"/>
       <c r="G8" s="46"/>
@@ -1443,7 +1445,7 @@
         <v>13</v>
       </c>
       <c r="E9" s="46" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="F9" s="45"/>
       <c r="G9" s="46"/>
@@ -1472,7 +1474,7 @@
         <v>14</v>
       </c>
       <c r="E10" s="46" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="F10" s="45"/>
       <c r="G10" s="46"/>
@@ -1637,7 +1639,7 @@
       <c r="L16" s="41"/>
       <c r="M16" s="41"/>
       <c r="O16" s="61" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
     </row>
     <row r="17" spans="5:16" ht="15.75" customHeight="1">
@@ -1653,7 +1655,7 @@
       <c r="L17" s="41"/>
       <c r="M17" s="41"/>
       <c r="O17" s="56" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
     </row>
     <row r="18" spans="5:16" ht="15.75" customHeight="1">
@@ -1669,9 +1671,7 @@
       <c r="L18" s="41"/>
       <c r="M18" s="41"/>
       <c r="N18" s="62"/>
-      <c r="O18" s="29" t="s">
-        <v>134</v>
-      </c>
+      <c r="O18" s="29"/>
     </row>
     <row r="19" spans="5:16" ht="15.75" customHeight="1">
       <c r="E19" s="56" t="s">
@@ -1687,9 +1687,7 @@
       <c r="M19" s="41"/>
       <c r="N19" s="62"/>
       <c r="O19" s="29"/>
-      <c r="P19" s="65" t="s">
-        <v>135</v>
-      </c>
+      <c r="P19" s="65"/>
     </row>
     <row r="20" spans="5:16" ht="15.75" customHeight="1">
       <c r="F20" s="41"/>
@@ -1748,7 +1746,7 @@
     </row>
     <row r="24" spans="5:16" ht="15.75" customHeight="1">
       <c r="E24" s="41" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="F24" s="41"/>
       <c r="G24" s="41"/>

</xml_diff>

<commit_message>
Chapter 7 first review done
</commit_message>
<xml_diff>
--- a/Word/PlanAndDealines.xlsx
+++ b/Word/PlanAndDealines.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20372"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20373"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ksung\Desktop\GitHub\GTCS-GameEngine2\Word\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{908D8FBB-B9AE-4745-AEB8-F1E2AD89613D}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D004D14F-8907-484C-996B-6EED8D012817}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView minimized="1" xWindow="0" yWindow="0" windowWidth="38400" windowHeight="20025" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="38400" windowHeight="20025" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Chapter Status" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="193" uniqueCount="133">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="200" uniqueCount="130">
   <si>
     <t>First Pass</t>
   </si>
@@ -441,16 +441,7 @@
     <t>Total delays</t>
   </si>
   <si>
-    <t xml:space="preserve">Jeb + Mattew </t>
-  </si>
-  <si>
     <t>https://www.w3.org/TR/html52/browsers.html#the-window-object</t>
-  </si>
-  <si>
-    <t>Matthew: more, but straightforward changes</t>
-  </si>
-  <si>
-    <t>Jeb: need to explain oscillate</t>
   </si>
   <si>
     <t>SHOULD WE?</t>
@@ -1096,8 +1087,8 @@
   </sheetPr>
   <dimension ref="B1:S142"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" zoomScale="220" zoomScaleNormal="220" workbookViewId="0">
-      <selection activeCell="S18" sqref="S18"/>
+    <sheetView tabSelected="1" zoomScale="205" zoomScaleNormal="205" workbookViewId="0">
+      <selection activeCell="L10" sqref="L10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1"/>
@@ -1394,12 +1385,24 @@
         <v>6</v>
       </c>
       <c r="F7" s="45"/>
-      <c r="G7" s="46"/>
-      <c r="H7" s="45"/>
-      <c r="I7" s="46"/>
-      <c r="J7" s="45"/>
-      <c r="K7" s="46"/>
-      <c r="L7" s="45"/>
+      <c r="G7" s="46" t="s">
+        <v>16</v>
+      </c>
+      <c r="H7" s="43">
+        <v>44309</v>
+      </c>
+      <c r="I7" s="46" t="s">
+        <v>6</v>
+      </c>
+      <c r="J7" s="43">
+        <v>44310</v>
+      </c>
+      <c r="K7" s="46" t="s">
+        <v>16</v>
+      </c>
+      <c r="L7" s="43">
+        <v>44312</v>
+      </c>
       <c r="M7" s="46"/>
       <c r="N7" s="45"/>
       <c r="O7" s="29"/>
@@ -1408,11 +1411,14 @@
       </c>
       <c r="Q7" s="57">
         <f t="shared" si="0"/>
-        <v>44309</v>
+        <v>44314</v>
+      </c>
+      <c r="R7">
+        <v>5</v>
       </c>
       <c r="S7">
         <f t="shared" ref="S7:S14" si="1">SUM(R7,S6)</f>
-        <v>4</v>
+        <v>9</v>
       </c>
     </row>
     <row r="8" spans="2:19" ht="26.25" customHeight="1">
@@ -1420,12 +1426,16 @@
         <v>12</v>
       </c>
       <c r="E8" s="64" t="s">
-        <v>129</v>
+        <v>6</v>
       </c>
       <c r="F8" s="45"/>
-      <c r="G8" s="46"/>
+      <c r="G8" s="46" t="s">
+        <v>16</v>
+      </c>
       <c r="H8" s="45"/>
-      <c r="I8" s="46"/>
+      <c r="I8" s="46" t="s">
+        <v>6</v>
+      </c>
       <c r="J8" s="45"/>
       <c r="K8" s="46"/>
       <c r="L8" s="45"/>
@@ -1437,11 +1447,11 @@
       </c>
       <c r="Q8" s="57">
         <f t="shared" si="0"/>
-        <v>44316</v>
+        <v>44321</v>
       </c>
       <c r="S8">
         <f t="shared" si="1"/>
-        <v>4</v>
+        <v>9</v>
       </c>
     </row>
     <row r="9" spans="2:19" ht="26.25" customHeight="1">
@@ -1449,12 +1459,18 @@
         <v>13</v>
       </c>
       <c r="E9" s="46" t="s">
-        <v>130</v>
-      </c>
-      <c r="F9" s="45"/>
-      <c r="G9" s="46"/>
+        <v>8</v>
+      </c>
+      <c r="F9" s="43">
+        <v>44312</v>
+      </c>
+      <c r="G9" s="46" t="s">
+        <v>16</v>
+      </c>
       <c r="H9" s="45"/>
-      <c r="I9" s="46"/>
+      <c r="I9" s="46" t="s">
+        <v>8</v>
+      </c>
       <c r="J9" s="45"/>
       <c r="K9" s="46"/>
       <c r="L9" s="45"/>
@@ -1466,11 +1482,11 @@
       </c>
       <c r="Q9" s="57">
         <f t="shared" si="0"/>
-        <v>44316</v>
+        <v>44321</v>
       </c>
       <c r="S9">
         <f t="shared" si="1"/>
-        <v>4</v>
+        <v>9</v>
       </c>
     </row>
     <row r="10" spans="2:19" ht="26.25" customHeight="1">
@@ -1478,7 +1494,7 @@
         <v>14</v>
       </c>
       <c r="E10" s="46" t="s">
-        <v>127</v>
+        <v>8</v>
       </c>
       <c r="F10" s="45"/>
       <c r="G10" s="46"/>
@@ -1495,11 +1511,11 @@
       </c>
       <c r="Q10" s="57">
         <f t="shared" si="0"/>
-        <v>44323</v>
+        <v>44328</v>
       </c>
       <c r="S10">
         <f t="shared" si="1"/>
-        <v>4</v>
+        <v>9</v>
       </c>
     </row>
     <row r="11" spans="2:19" ht="26.25" customHeight="1">
@@ -1525,11 +1541,11 @@
       </c>
       <c r="Q11" s="57">
         <f t="shared" si="0"/>
-        <v>44344</v>
+        <v>44349</v>
       </c>
       <c r="S11">
         <f t="shared" si="1"/>
-        <v>4</v>
+        <v>9</v>
       </c>
     </row>
     <row r="12" spans="2:19" ht="26.25" customHeight="1">
@@ -1555,11 +1571,11 @@
       </c>
       <c r="Q12" s="57">
         <f t="shared" si="0"/>
-        <v>44358</v>
+        <v>44363</v>
       </c>
       <c r="S12">
         <f t="shared" si="1"/>
-        <v>4</v>
+        <v>9</v>
       </c>
     </row>
     <row r="13" spans="2:19" ht="26.25" customHeight="1">
@@ -1582,11 +1598,11 @@
       </c>
       <c r="Q13" s="57">
         <f t="shared" si="0"/>
-        <v>44365</v>
+        <v>44370</v>
       </c>
       <c r="S13">
         <f t="shared" si="1"/>
-        <v>4</v>
+        <v>9</v>
       </c>
     </row>
     <row r="14" spans="2:19" ht="26.25" customHeight="1" thickBot="1">
@@ -1611,11 +1627,11 @@
       </c>
       <c r="Q14" s="57">
         <f t="shared" si="0"/>
-        <v>44372</v>
+        <v>44377</v>
       </c>
       <c r="S14">
         <f t="shared" si="1"/>
-        <v>4</v>
+        <v>9</v>
       </c>
     </row>
     <row r="15" spans="2:19" ht="15.75" customHeight="1" thickTop="1">
@@ -1643,7 +1659,7 @@
       <c r="L16" s="41"/>
       <c r="M16" s="41"/>
       <c r="O16" s="61" t="s">
-        <v>131</v>
+        <v>128</v>
       </c>
     </row>
     <row r="17" spans="5:16" ht="15.75" customHeight="1">
@@ -1659,7 +1675,7 @@
       <c r="L17" s="41"/>
       <c r="M17" s="41"/>
       <c r="O17" s="56" t="s">
-        <v>132</v>
+        <v>129</v>
       </c>
     </row>
     <row r="18" spans="5:16" ht="15.75" customHeight="1">
@@ -1750,7 +1766,7 @@
     </row>
     <row r="24" spans="5:16" ht="15.75" customHeight="1">
       <c r="E24" s="41" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="F24" s="41"/>
       <c r="G24" s="41"/>

</xml_diff>

<commit_message>
Chap 5 submitted. 7 move to final review.
</commit_message>
<xml_diff>
--- a/Word/PlanAndDealines.xlsx
+++ b/Word/PlanAndDealines.xlsx
@@ -8,25 +8,26 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ksung\Desktop\GitHub\GTCS-GameEngine2\Word\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A5ACED6F-A1E7-4A8B-AD9B-141A36663414}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3B3A58C8-5F66-4079-9C3F-984F8BF44D33}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="38400" windowHeight="20025" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="38400" windowHeight="20025" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Chapter Status" sheetId="1" r:id="rId1"/>
     <sheet name="Summary" sheetId="2" r:id="rId2"/>
-    <sheet name="Chap1 What, who and when" sheetId="3" r:id="rId3"/>
-    <sheet name="Chap 2" sheetId="4" r:id="rId4"/>
-    <sheet name="Chap 3" sheetId="5" r:id="rId5"/>
-    <sheet name="Chap 4" sheetId="6" r:id="rId6"/>
-    <sheet name="Chap x-template" sheetId="7" r:id="rId7"/>
+    <sheet name="Final Changes Must make" sheetId="8" r:id="rId3"/>
+    <sheet name="Chap1 What, who and when" sheetId="3" r:id="rId4"/>
+    <sheet name="Chap 2" sheetId="4" r:id="rId5"/>
+    <sheet name="Chap 3" sheetId="5" r:id="rId6"/>
+    <sheet name="Chap 4" sheetId="6" r:id="rId7"/>
+    <sheet name="Chap x-template" sheetId="7" r:id="rId8"/>
   </sheets>
   <calcPr calcId="191029"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="520" uniqueCount="130">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="211" uniqueCount="140">
   <si>
     <t>First Pass</t>
   </si>
@@ -449,12 +450,42 @@
   <si>
     <t>Integrate loading icon into the last final engine?</t>
   </si>
+  <si>
+    <t>1. Update camera to match API from Chap 7 (with setting and getting WC Center, e.g.)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">… identical to previous code ..   </t>
+  </si>
+  <si>
+    <t>vs</t>
+  </si>
+  <si>
+    <t xml:space="preserve">… identical to previous projcet … </t>
+  </si>
+  <si>
+    <t>.. Implementation to follow …</t>
+  </si>
+  <si>
+    <t>// new fuctinality to be define here in the next subsection</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    … more implementation details in the following steps …(Chap 5)</t>
+  </si>
+  <si>
+    <t>Same:</t>
+  </si>
+  <si>
+    <t>to show:</t>
+  </si>
+  <si>
+    <t>2. consistency needed … (with or without //, which one to use?)  [Need to review Chapters 1, 2, 3, 4, 5]</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="27">
+  <fonts count="29">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -607,6 +638,17 @@
       <name val="Calibri"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="9"/>
+      <color rgb="FF000000"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <color rgb="FF000000"/>
+      <name val="TheSansMonoConNormal"/>
+    </font>
   </fonts>
   <fills count="3">
     <fill>
@@ -707,7 +749,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="68">
+  <cellXfs count="72">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
@@ -846,24 +888,32 @@
     <xf numFmtId="0" fontId="23" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="16" fontId="24" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="14" fontId="24" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="16" fontId="24" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="14" fontId="24" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
+    <xf numFmtId="0" fontId="27" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="28" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1084,7 +1134,7 @@
   </sheetPr>
   <dimension ref="B1:S142"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="205" zoomScaleNormal="205" workbookViewId="0">
+    <sheetView zoomScale="205" zoomScaleNormal="205" workbookViewId="0">
       <selection activeCell="N6" sqref="N6"/>
     </sheetView>
   </sheetViews>
@@ -1108,26 +1158,26 @@
     <row r="1" spans="2:19" ht="12.75">
       <c r="C1" s="1"/>
       <c r="D1" s="1"/>
-      <c r="E1" s="62" t="s">
+      <c r="E1" s="66" t="s">
         <v>0</v>
       </c>
-      <c r="F1" s="63"/>
-      <c r="G1" s="62" t="s">
+      <c r="F1" s="67"/>
+      <c r="G1" s="66" t="s">
         <v>1</v>
       </c>
-      <c r="H1" s="63"/>
-      <c r="I1" s="62" t="s">
+      <c r="H1" s="67"/>
+      <c r="I1" s="66" t="s">
         <v>2</v>
       </c>
-      <c r="J1" s="63"/>
-      <c r="K1" s="62" t="s">
+      <c r="J1" s="67"/>
+      <c r="K1" s="66" t="s">
         <v>1</v>
       </c>
-      <c r="L1" s="63"/>
-      <c r="M1" s="62" t="s">
+      <c r="L1" s="67"/>
+      <c r="M1" s="66" t="s">
         <v>3</v>
       </c>
-      <c r="N1" s="63"/>
+      <c r="N1" s="67"/>
       <c r="O1" s="29" t="s">
         <v>4</v>
       </c>
@@ -1305,10 +1355,10 @@
       <c r="N5" s="50">
         <v>44299</v>
       </c>
-      <c r="O5" s="64" t="s">
+      <c r="O5" s="62" t="s">
         <v>116</v>
       </c>
-      <c r="P5" s="65">
+      <c r="P5" s="63">
         <v>44298</v>
       </c>
       <c r="Q5" s="54">
@@ -1356,10 +1406,10 @@
       <c r="N6" s="50">
         <v>44331</v>
       </c>
-      <c r="O6" s="64">
+      <c r="O6" s="62">
         <v>44302</v>
       </c>
-      <c r="P6" s="65">
+      <c r="P6" s="63">
         <v>44298</v>
       </c>
       <c r="Q6" s="54">
@@ -1381,7 +1431,7 @@
       <c r="E7" s="49" t="s">
         <v>6</v>
       </c>
-      <c r="F7" s="66"/>
+      <c r="F7" s="64"/>
       <c r="G7" s="49" t="s">
         <v>16</v>
       </c>
@@ -1401,9 +1451,9 @@
         <v>44312</v>
       </c>
       <c r="M7" s="49"/>
-      <c r="N7" s="66"/>
-      <c r="O7" s="67"/>
-      <c r="P7" s="65">
+      <c r="N7" s="64"/>
+      <c r="O7" s="65"/>
+      <c r="P7" s="63">
         <v>44305</v>
       </c>
       <c r="Q7" s="54">
@@ -3610,6 +3660,63 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D8AC00B6-697C-45E4-9E65-51AD1E2696C6}">
+  <dimension ref="A3:L6"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A4" sqref="A4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="12.75"/>
+  <sheetData>
+    <row r="3" spans="1:12">
+      <c r="A3" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12">
+      <c r="A4" s="70" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12">
+      <c r="B5" s="71" t="s">
+        <v>137</v>
+      </c>
+      <c r="C5" t="s">
+        <v>131</v>
+      </c>
+      <c r="F5" t="s">
+        <v>132</v>
+      </c>
+      <c r="G5" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12">
+      <c r="B6" s="71" t="s">
+        <v>138</v>
+      </c>
+      <c r="C6" t="s">
+        <v>134</v>
+      </c>
+      <c r="F6" t="s">
+        <v>132</v>
+      </c>
+      <c r="G6" s="68" t="s">
+        <v>135</v>
+      </c>
+      <c r="L6" s="69" t="s">
+        <v>136</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
@@ -3822,7 +3929,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
@@ -3881,7 +3988,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
@@ -3938,7 +4045,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
@@ -3985,7 +4092,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>

</xml_diff>

<commit_message>
Chap 7 First submission
</commit_message>
<xml_diff>
--- a/Word/PlanAndDealines.xlsx
+++ b/Word/PlanAndDealines.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ksung\Desktop\GitHub\GTCS-GameEngine2\Word\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{466FB926-3F1E-4B49-A9E5-34D4EED66201}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E96647B1-9F22-4396-B9A2-D88CFC0A4EB0}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="38400" windowHeight="20025" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="223" uniqueCount="152">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="225" uniqueCount="154">
   <si>
     <t>First Pass</t>
   </si>
@@ -515,6 +515,12 @@
   </si>
   <si>
     <t>5. Chapter 1: debugging from VS Code extension: Debugger for Chrome</t>
+  </si>
+  <si>
+    <t>Chaper 2.</t>
+  </si>
+  <si>
+    <t>The first encounter of # must explain with a note, "For readability, variables will be referred to without the # symbol"</t>
   </si>
 </sst>
 </file>
@@ -3717,7 +3723,7 @@
   <dimension ref="A3:R18"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="190" zoomScaleNormal="190" workbookViewId="0">
-      <selection activeCell="A12" sqref="A12"/>
+      <selection activeCell="B13" sqref="B13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
@@ -3798,6 +3804,14 @@
     <row r="12" spans="1:18">
       <c r="A12" s="66" t="s">
         <v>151</v>
+      </c>
+    </row>
+    <row r="13" spans="1:18">
+      <c r="A13" s="67" t="s">
+        <v>152</v>
+      </c>
+      <c r="B13" s="66" t="s">
+        <v>153</v>
       </c>
     </row>
     <row r="16" spans="1:18">

</xml_diff>

<commit_message>
Slow by steady progress of final game
</commit_message>
<xml_diff>
--- a/Word/PlanAndDealines.xlsx
+++ b/Word/PlanAndDealines.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ksung\Desktop\GitHub\GTCS-GameEngine2\Word\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9BDFABF6-2F49-4E5A-9BBE-F4F25298A511}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FA85F73D-5FC5-4C9C-B955-A58DE8A62836}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="33645" windowHeight="15855" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="247" uniqueCount="158">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="249" uniqueCount="160">
   <si>
     <t>First Pass</t>
   </si>
@@ -580,6 +580,23 @@
         <family val="2"/>
       </rPr>
       <t>Need to review Chapters 1, 2, 3, 4, 5]</t>
+    </r>
+  </si>
+  <si>
+    <t>Chapter 4: resource_map: now has reference count!</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">texture.js: </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>unload must check if can actually delete</t>
     </r>
   </si>
 </sst>
@@ -3391,10 +3408,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D8AC00B6-697C-45E4-9E65-51AD1E2696C6}">
-  <dimension ref="A3:R32"/>
+  <dimension ref="A3:R33"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="190" zoomScaleNormal="190" workbookViewId="0">
-      <selection activeCell="A23" sqref="A23:D33"/>
+      <selection activeCell="B20" sqref="B20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
@@ -3510,63 +3527,63 @@
     </row>
     <row r="18" spans="1:3">
       <c r="A18" s="67" t="s">
+        <v>158</v>
+      </c>
+      <c r="B18" s="66"/>
+    </row>
+    <row r="19" spans="1:3">
+      <c r="A19" s="67" t="s">
         <v>148</v>
       </c>
-      <c r="B18" t="s">
+      <c r="B19" t="s">
         <v>149</v>
       </c>
-    </row>
-    <row r="19" spans="1:3">
-      <c r="A19" s="66"/>
     </row>
     <row r="20" spans="1:3">
       <c r="A20" s="66"/>
+      <c r="B20" s="67" t="s">
+        <v>159</v>
+      </c>
     </row>
     <row r="21" spans="1:3">
       <c r="A21" s="66"/>
     </row>
-    <row r="23" spans="1:3">
-      <c r="A23" s="3" t="s">
+    <row r="22" spans="1:3">
+      <c r="A22" s="66"/>
+    </row>
+    <row r="24" spans="1:3">
+      <c r="A24" s="3" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="24" spans="1:3">
-      <c r="A24" s="11" t="s">
+    <row r="25" spans="1:3">
+      <c r="A25" s="11" t="s">
         <v>56</v>
       </c>
-      <c r="B24" s="12"/>
-      <c r="C24" s="12"/>
-    </row>
-    <row r="25" spans="1:3">
-      <c r="A25" s="13" t="s">
+      <c r="B25" s="12"/>
+      <c r="C25" s="12"/>
+    </row>
+    <row r="26" spans="1:3">
+      <c r="A26" s="13" t="s">
         <v>57</v>
       </c>
-      <c r="B25" s="12"/>
-      <c r="C25" s="11" t="s">
+      <c r="B26" s="12"/>
+      <c r="C26" s="11" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="26" spans="1:3" ht="15.75">
-      <c r="A26" s="13" t="s">
+    <row r="27" spans="1:3" ht="15.75">
+      <c r="A27" s="13" t="s">
         <v>59</v>
       </c>
-      <c r="B26" s="12"/>
-      <c r="C26" s="14" t="s">
+      <c r="B27" s="12"/>
+      <c r="C27" s="14" t="s">
         <v>60</v>
-      </c>
-    </row>
-    <row r="27" spans="1:3">
-      <c r="A27" s="13" t="s">
-        <v>61</v>
-      </c>
-      <c r="B27" s="12"/>
-      <c r="C27" s="11" t="s">
-        <v>62</v>
       </c>
     </row>
     <row r="28" spans="1:3">
       <c r="A28" s="13" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="B28" s="12"/>
       <c r="C28" s="11" t="s">
@@ -3575,37 +3592,46 @@
     </row>
     <row r="29" spans="1:3">
       <c r="A29" s="13" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B29" s="12"/>
       <c r="C29" s="11" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
     </row>
     <row r="30" spans="1:3">
       <c r="A30" s="13" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="B30" s="12"/>
       <c r="C30" s="11" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
     </row>
     <row r="31" spans="1:3">
       <c r="A31" s="13" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="B31" s="12"/>
       <c r="C31" s="11" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
     </row>
     <row r="32" spans="1:3">
       <c r="A32" s="13" t="s">
-        <v>41</v>
+        <v>68</v>
       </c>
       <c r="B32" s="12"/>
       <c r="C32" s="11" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3">
+      <c r="A33" s="13" t="s">
+        <v>41</v>
+      </c>
+      <c r="B33" s="12"/>
+      <c r="C33" s="11" t="s">
         <v>70</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Bug fixes from implementing Chapter 12
</commit_message>
<xml_diff>
--- a/Word/PlanAndDealines.xlsx
+++ b/Word/PlanAndDealines.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ksung\Desktop\GitHub\GTCS-GameEngine2\Word\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{96772D4E-CA23-439C-98BE-42F90044708F}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2506F457-6342-4B4C-992A-66D2086D7530}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="33645" windowHeight="15855" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="251" uniqueCount="162">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="253" uniqueCount="164">
   <si>
     <t>First Pass</t>
   </si>
@@ -613,7 +613,90 @@
         <rFont val="Arial"/>
         <family val="2"/>
       </rPr>
-      <t>change into one sentence "Remember to update the engine access file, index.js, to export the newly defined THIS AND THAT.</t>
+      <t>change into one sentence "Lastly, remember to update the engine access file, index.js, to forward the newly defined functionality to the client.</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>"</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">Organize the Source Code: </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">compare this section to </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>Chapter 6: Organize the source code</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> and refine. </t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Remove: </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">the note on top of Page 6 (on </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>aClass.prototype.method</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>)</t>
     </r>
   </si>
 </sst>
@@ -3428,7 +3511,7 @@
   <dimension ref="A3:R34"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="190" zoomScaleNormal="190" workbookViewId="0">
-      <selection activeCell="B21" sqref="B21"/>
+      <selection activeCell="B23" sqref="B23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
@@ -3572,9 +3655,15 @@
     </row>
     <row r="22" spans="1:3">
       <c r="A22" s="66"/>
+      <c r="B22" s="66" t="s">
+        <v>162</v>
+      </c>
     </row>
     <row r="23" spans="1:3">
       <c r="A23" s="66"/>
+      <c r="B23" s="67" t="s">
+        <v>163</v>
+      </c>
     </row>
     <row r="25" spans="1:3">
       <c r="A25" s="3" t="s">

</xml_diff>

<commit_message>
Chap-11 Review 1 done
</commit_message>
<xml_diff>
--- a/Word/PlanAndDealines.xlsx
+++ b/Word/PlanAndDealines.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ksung\Desktop\GitHub\GTCS-GameEngine2\Word\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C3D1994F-8F99-4594-905E-D84608D3D872}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6FECA9A4-C36C-4ADE-BB3A-F11DD0A85E71}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="33645" windowHeight="15855" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="257" uniqueCount="166">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="259" uniqueCount="168">
   <si>
     <t>First Pass</t>
   </si>
@@ -705,12 +705,18 @@
   <si>
     <t>Support collision: returning T/F and the colliding object  … this can be a programming exercise?</t>
   </si>
+  <si>
+    <t>New class: update index.js … here is the language</t>
+  </si>
+  <si>
+    <t>Lastly, remember to update the engine access file, index.js, to forward the newly defined functionality to the client.</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="32">
+  <fonts count="33">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -899,6 +905,11 @@
       <name val="Arial"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="9"/>
+      <color rgb="FF000000"/>
+      <name val="Utopia"/>
+    </font>
   </fonts>
   <fills count="3">
     <fill>
@@ -999,7 +1010,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="71">
+  <cellXfs count="72">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
@@ -1154,6 +1165,9 @@
     </xf>
     <xf numFmtId="16" fontId="31" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="32" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -3520,10 +3534,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D8AC00B6-697C-45E4-9E65-51AD1E2696C6}">
-  <dimension ref="A3:R34"/>
+  <dimension ref="A3:R36"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="190" zoomScaleNormal="190" workbookViewId="0">
-      <selection activeCell="L27" sqref="L27"/>
+      <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
@@ -3592,178 +3606,190 @@
       </c>
     </row>
     <row r="9" spans="1:18">
-      <c r="A9" t="s">
-        <v>137</v>
-      </c>
+      <c r="A9" s="56" t="s">
+        <v>166</v>
+      </c>
+      <c r="C9" s="57"/>
     </row>
     <row r="10" spans="1:18">
-      <c r="A10" s="56" t="s">
-        <v>146</v>
-      </c>
+      <c r="B10" s="71" t="s">
+        <v>167</v>
+      </c>
+      <c r="C10" s="57"/>
     </row>
     <row r="11" spans="1:18">
       <c r="A11" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="12" spans="1:18">
+      <c r="A12" s="56" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="13" spans="1:18">
+      <c r="A13" t="s">
         <v>138</v>
       </c>
     </row>
-    <row r="14" spans="1:18">
-      <c r="A14" s="56" t="s">
+    <row r="16" spans="1:18">
+      <c r="A16" s="56" t="s">
         <v>153</v>
       </c>
-      <c r="B14" s="56" t="s">
+      <c r="B16" s="56" t="s">
         <v>154</v>
-      </c>
-    </row>
-    <row r="15" spans="1:18">
-      <c r="A15" s="57" t="s">
-        <v>147</v>
-      </c>
-      <c r="B15" s="56" t="s">
-        <v>155</v>
-      </c>
-    </row>
-    <row r="16" spans="1:18">
-      <c r="A16" s="57"/>
-      <c r="B16" s="56"/>
-      <c r="C16" s="56" t="s">
-        <v>150</v>
       </c>
     </row>
     <row r="17" spans="1:12">
       <c r="A17" s="57" t="s">
-        <v>151</v>
+        <v>147</v>
       </c>
       <c r="B17" s="56" t="s">
-        <v>152</v>
+        <v>155</v>
       </c>
     </row>
     <row r="18" spans="1:12">
-      <c r="A18" s="57" t="s">
-        <v>158</v>
-      </c>
+      <c r="A18" s="57"/>
       <c r="B18" s="56"/>
+      <c r="C18" s="56" t="s">
+        <v>150</v>
+      </c>
     </row>
     <row r="19" spans="1:12">
       <c r="A19" s="57" t="s">
-        <v>148</v>
-      </c>
-      <c r="B19" t="s">
-        <v>149</v>
+        <v>151</v>
+      </c>
+      <c r="B19" s="56" t="s">
+        <v>152</v>
       </c>
     </row>
     <row r="20" spans="1:12">
-      <c r="A20" s="56"/>
-      <c r="B20" s="57" t="s">
-        <v>159</v>
-      </c>
+      <c r="A20" s="57" t="s">
+        <v>158</v>
+      </c>
+      <c r="B20" s="56"/>
     </row>
     <row r="21" spans="1:12">
       <c r="A21" s="57" t="s">
-        <v>160</v>
-      </c>
-      <c r="B21" s="57" t="s">
-        <v>161</v>
+        <v>148</v>
+      </c>
+      <c r="B21" t="s">
+        <v>149</v>
       </c>
     </row>
     <row r="22" spans="1:12">
       <c r="A22" s="56"/>
-      <c r="B22" s="56" t="s">
+      <c r="B22" s="57" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="23" spans="1:12">
+      <c r="A23" s="57" t="s">
+        <v>160</v>
+      </c>
+      <c r="B23" s="57" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="24" spans="1:12">
+      <c r="A24" s="56"/>
+      <c r="B24" s="56" t="s">
         <v>162</v>
       </c>
     </row>
-    <row r="23" spans="1:12">
-      <c r="A23" s="56"/>
-      <c r="B23" s="57" t="s">
+    <row r="25" spans="1:12">
+      <c r="A25" s="56"/>
+      <c r="B25" s="57" t="s">
         <v>163</v>
       </c>
     </row>
-    <row r="25" spans="1:12">
-      <c r="A25" s="2" t="s">
+    <row r="27" spans="1:12">
+      <c r="A27" s="2" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="26" spans="1:12">
-      <c r="A26" s="10" t="s">
+    <row r="28" spans="1:12">
+      <c r="A28" s="10" t="s">
         <v>56</v>
       </c>
-      <c r="B26" s="11"/>
-      <c r="C26" s="11"/>
-      <c r="K26" s="56" t="s">
+      <c r="B28" s="11"/>
+      <c r="C28" s="11"/>
+      <c r="K28" s="56" t="s">
         <v>164</v>
-      </c>
-    </row>
-    <row r="27" spans="1:12">
-      <c r="A27" s="12" t="s">
-        <v>57</v>
-      </c>
-      <c r="B27" s="11"/>
-      <c r="C27" s="10" t="s">
-        <v>58</v>
-      </c>
-      <c r="L27" s="56" t="s">
-        <v>165</v>
-      </c>
-    </row>
-    <row r="28" spans="1:12" ht="15.75">
-      <c r="A28" s="12" t="s">
-        <v>59</v>
-      </c>
-      <c r="B28" s="11"/>
-      <c r="C28" s="13" t="s">
-        <v>60</v>
       </c>
     </row>
     <row r="29" spans="1:12">
       <c r="A29" s="12" t="s">
-        <v>61</v>
+        <v>57</v>
       </c>
       <c r="B29" s="11"/>
       <c r="C29" s="10" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="30" spans="1:12">
+        <v>58</v>
+      </c>
+      <c r="L29" s="56" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="30" spans="1:12" ht="15.75">
       <c r="A30" s="12" t="s">
-        <v>63</v>
+        <v>59</v>
       </c>
       <c r="B30" s="11"/>
-      <c r="C30" s="10" t="s">
-        <v>62</v>
+      <c r="C30" s="13" t="s">
+        <v>60</v>
       </c>
     </row>
     <row r="31" spans="1:12">
       <c r="A31" s="12" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="B31" s="11"/>
       <c r="C31" s="10" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
     </row>
     <row r="32" spans="1:12">
       <c r="A32" s="12" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="B32" s="11"/>
       <c r="C32" s="10" t="s">
-        <v>67</v>
+        <v>62</v>
       </c>
     </row>
     <row r="33" spans="1:3">
       <c r="A33" s="12" t="s">
-        <v>68</v>
+        <v>64</v>
       </c>
       <c r="B33" s="11"/>
       <c r="C33" s="10" t="s">
-        <v>69</v>
+        <v>65</v>
       </c>
     </row>
     <row r="34" spans="1:3">
       <c r="A34" s="12" t="s">
-        <v>41</v>
+        <v>66</v>
       </c>
       <c r="B34" s="11"/>
       <c r="C34" s="10" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="35" spans="1:3">
+      <c r="A35" s="12" t="s">
+        <v>68</v>
+      </c>
+      <c r="B35" s="11"/>
+      <c r="C35" s="10" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="36" spans="1:3">
+      <c r="A36" s="12" t="s">
+        <v>41</v>
+      </c>
+      <c r="B36" s="11"/>
+      <c r="C36" s="10" t="s">
         <v>70</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Figure update and Chap8 update
</commit_message>
<xml_diff>
--- a/Word/PlanAndDealines.xlsx
+++ b/Word/PlanAndDealines.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ksung\Desktop\GitHub\GTCS-GameEngine2\Word\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6FECA9A4-C36C-4ADE-BB3A-F11DD0A85E71}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{895B2B1D-BF84-4FB7-BF74-17D60E03B222}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="33645" windowHeight="15855" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="33645" windowHeight="15855" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Chapter Status" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="259" uniqueCount="168">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="264" uniqueCount="168">
   <si>
     <t>First Pass</t>
   </si>
@@ -716,7 +716,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="33">
+  <fonts count="34">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -910,6 +910,13 @@
       <color rgb="FF000000"/>
       <name val="Utopia"/>
     </font>
+    <font>
+      <b/>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
   </fonts>
   <fills count="3">
     <fill>
@@ -1010,7 +1017,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="72">
+  <cellXfs count="74">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
@@ -1092,6 +1099,9 @@
     <xf numFmtId="16" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -1168,6 +1178,9 @@
     </xf>
     <xf numFmtId="0" fontId="32" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="33" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1389,8 +1402,8 @@
   </sheetPr>
   <dimension ref="B1:S142"/>
   <sheetViews>
-    <sheetView zoomScale="205" zoomScaleNormal="205" workbookViewId="0">
-      <selection activeCell="B9" sqref="B9:O9"/>
+    <sheetView tabSelected="1" zoomScale="205" zoomScaleNormal="205" workbookViewId="0">
+      <selection activeCell="E11" sqref="E11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1"/>
@@ -1413,26 +1426,26 @@
     <row r="1" spans="2:19" ht="12.75">
       <c r="C1" s="1"/>
       <c r="D1" s="1"/>
-      <c r="E1" s="62" t="s">
+      <c r="E1" s="63" t="s">
         <v>0</v>
       </c>
-      <c r="F1" s="63"/>
-      <c r="G1" s="62" t="s">
+      <c r="F1" s="64"/>
+      <c r="G1" s="63" t="s">
         <v>1</v>
       </c>
-      <c r="H1" s="63"/>
-      <c r="I1" s="62" t="s">
+      <c r="H1" s="64"/>
+      <c r="I1" s="63" t="s">
         <v>2</v>
       </c>
-      <c r="J1" s="63"/>
-      <c r="K1" s="62" t="s">
+      <c r="J1" s="64"/>
+      <c r="K1" s="63" t="s">
         <v>1</v>
       </c>
-      <c r="L1" s="63"/>
-      <c r="M1" s="62" t="s">
+      <c r="L1" s="64"/>
+      <c r="M1" s="63" t="s">
         <v>3</v>
       </c>
-      <c r="N1" s="63"/>
+      <c r="N1" s="64"/>
       <c r="O1" s="28" t="s">
         <v>4</v>
       </c>
@@ -1488,43 +1501,43 @@
       </c>
     </row>
     <row r="3" spans="2:19" ht="26.25" customHeight="1" thickTop="1">
-      <c r="B3" s="64" t="s">
+      <c r="B3" s="65" t="s">
         <v>5</v>
       </c>
-      <c r="C3" s="65"/>
-      <c r="D3" s="65"/>
-      <c r="E3" s="66" t="s">
+      <c r="C3" s="66"/>
+      <c r="D3" s="66"/>
+      <c r="E3" s="67" t="s">
         <v>6</v>
       </c>
-      <c r="F3" s="67">
+      <c r="F3" s="68">
         <v>44289</v>
       </c>
-      <c r="G3" s="66" t="s">
+      <c r="G3" s="67" t="s">
         <v>16</v>
       </c>
-      <c r="H3" s="67">
+      <c r="H3" s="68">
         <v>44289</v>
       </c>
-      <c r="I3" s="66" t="s">
+      <c r="I3" s="67" t="s">
         <v>6</v>
       </c>
-      <c r="J3" s="67">
+      <c r="J3" s="68">
         <v>44290</v>
       </c>
-      <c r="K3" s="66" t="s">
+      <c r="K3" s="67" t="s">
         <v>16</v>
       </c>
-      <c r="L3" s="67">
+      <c r="L3" s="68">
         <v>44291</v>
       </c>
-      <c r="M3" s="66" t="s">
+      <c r="M3" s="67" t="s">
         <v>8</v>
       </c>
-      <c r="N3" s="68"/>
-      <c r="O3" s="69" t="s">
+      <c r="N3" s="69"/>
+      <c r="O3" s="70" t="s">
         <v>116</v>
       </c>
-      <c r="P3" s="49">
+      <c r="P3" s="50">
         <v>44291</v>
       </c>
       <c r="Q3" t="s">
@@ -1532,45 +1545,45 @@
       </c>
     </row>
     <row r="4" spans="2:19" ht="26.25" customHeight="1">
-      <c r="B4" s="64" t="s">
+      <c r="B4" s="65" t="s">
         <v>7</v>
       </c>
-      <c r="C4" s="65"/>
-      <c r="D4" s="65"/>
-      <c r="E4" s="66" t="s">
+      <c r="C4" s="66"/>
+      <c r="D4" s="66"/>
+      <c r="E4" s="67" t="s">
         <v>8</v>
       </c>
-      <c r="F4" s="67">
+      <c r="F4" s="68">
         <v>44284</v>
       </c>
-      <c r="G4" s="66" t="s">
+      <c r="G4" s="67" t="s">
         <v>16</v>
       </c>
-      <c r="H4" s="67">
+      <c r="H4" s="68">
         <v>44286</v>
       </c>
-      <c r="I4" s="66" t="s">
+      <c r="I4" s="67" t="s">
         <v>8</v>
       </c>
-      <c r="J4" s="67">
+      <c r="J4" s="68">
         <v>44290</v>
       </c>
-      <c r="K4" s="66" t="s">
+      <c r="K4" s="67" t="s">
         <v>16</v>
       </c>
-      <c r="L4" s="67">
+      <c r="L4" s="68">
         <v>44290</v>
       </c>
-      <c r="M4" s="66" t="s">
+      <c r="M4" s="67" t="s">
         <v>6</v>
       </c>
-      <c r="N4" s="67">
+      <c r="N4" s="68">
         <v>44290</v>
       </c>
-      <c r="O4" s="69" t="s">
+      <c r="O4" s="70" t="s">
         <v>116</v>
       </c>
-      <c r="P4" s="49">
+      <c r="P4" s="50">
         <v>44291</v>
       </c>
       <c r="Q4" t="s">
@@ -1578,48 +1591,48 @@
       </c>
     </row>
     <row r="5" spans="2:19" ht="26.25" customHeight="1">
-      <c r="B5" s="64" t="s">
+      <c r="B5" s="65" t="s">
         <v>9</v>
       </c>
-      <c r="C5" s="65"/>
-      <c r="D5" s="65"/>
-      <c r="E5" s="66" t="s">
+      <c r="C5" s="66"/>
+      <c r="D5" s="66"/>
+      <c r="E5" s="67" t="s">
         <v>6</v>
       </c>
-      <c r="F5" s="67">
+      <c r="F5" s="68">
         <v>44296</v>
       </c>
-      <c r="G5" s="66" t="s">
+      <c r="G5" s="67" t="s">
         <v>16</v>
       </c>
-      <c r="H5" s="67">
+      <c r="H5" s="68">
         <v>44296</v>
       </c>
-      <c r="I5" s="66" t="s">
+      <c r="I5" s="67" t="s">
         <v>6</v>
       </c>
-      <c r="J5" s="67">
+      <c r="J5" s="68">
         <v>44297</v>
       </c>
-      <c r="K5" s="66" t="s">
+      <c r="K5" s="67" t="s">
         <v>16</v>
       </c>
-      <c r="L5" s="67">
+      <c r="L5" s="68">
         <v>44298</v>
       </c>
-      <c r="M5" s="66" t="s">
+      <c r="M5" s="67" t="s">
         <v>8</v>
       </c>
-      <c r="N5" s="67">
+      <c r="N5" s="68">
         <v>44299</v>
       </c>
-      <c r="O5" s="70" t="s">
+      <c r="O5" s="71" t="s">
         <v>116</v>
       </c>
-      <c r="P5" s="55">
+      <c r="P5" s="56">
         <v>44298</v>
       </c>
-      <c r="Q5" s="48">
+      <c r="Q5" s="49">
         <f>DATE(YEAR(P5),MONTH(P5),DAY(P5)+S5)</f>
         <v>44299</v>
       </c>
@@ -1632,46 +1645,46 @@
       </c>
     </row>
     <row r="6" spans="2:19" ht="26.25" customHeight="1">
-      <c r="B6" s="64" t="s">
+      <c r="B6" s="65" t="s">
         <v>10</v>
       </c>
-      <c r="C6" s="65"/>
-      <c r="D6" s="65"/>
-      <c r="E6" s="66" t="s">
+      <c r="C6" s="66"/>
+      <c r="D6" s="66"/>
+      <c r="E6" s="67" t="s">
         <v>8</v>
       </c>
-      <c r="F6" s="67"/>
-      <c r="G6" s="66" t="s">
+      <c r="F6" s="68"/>
+      <c r="G6" s="67" t="s">
         <v>16</v>
       </c>
-      <c r="H6" s="67">
+      <c r="H6" s="68">
         <v>44300</v>
       </c>
-      <c r="I6" s="66" t="s">
+      <c r="I6" s="67" t="s">
         <v>8</v>
       </c>
-      <c r="J6" s="67">
+      <c r="J6" s="68">
         <v>44300</v>
       </c>
-      <c r="K6" s="66" t="s">
+      <c r="K6" s="67" t="s">
         <v>16</v>
       </c>
-      <c r="L6" s="67">
+      <c r="L6" s="68">
         <v>44301</v>
       </c>
-      <c r="M6" s="66" t="s">
+      <c r="M6" s="67" t="s">
         <v>6</v>
       </c>
-      <c r="N6" s="67">
+      <c r="N6" s="68">
         <v>44331</v>
       </c>
-      <c r="O6" s="70">
+      <c r="O6" s="71">
         <v>44302</v>
       </c>
-      <c r="P6" s="55">
+      <c r="P6" s="56">
         <v>44298</v>
       </c>
-      <c r="Q6" s="48">
+      <c r="Q6" s="49">
         <f t="shared" ref="Q6:Q14" si="0">DATE(YEAR(P6),MONTH(P6),DAY(P6)+S6)</f>
         <v>44302</v>
       </c>
@@ -1684,40 +1697,40 @@
       </c>
     </row>
     <row r="7" spans="2:19" ht="26.25" customHeight="1">
-      <c r="B7" s="64" t="s">
+      <c r="B7" s="65" t="s">
         <v>11</v>
       </c>
-      <c r="C7" s="65"/>
-      <c r="D7" s="65"/>
-      <c r="E7" s="66" t="s">
+      <c r="C7" s="66"/>
+      <c r="D7" s="66"/>
+      <c r="E7" s="67" t="s">
         <v>6</v>
       </c>
-      <c r="F7" s="68"/>
-      <c r="G7" s="66" t="s">
+      <c r="F7" s="69"/>
+      <c r="G7" s="67" t="s">
         <v>16</v>
       </c>
-      <c r="H7" s="67">
+      <c r="H7" s="68">
         <v>44309</v>
       </c>
-      <c r="I7" s="66" t="s">
+      <c r="I7" s="67" t="s">
         <v>6</v>
       </c>
-      <c r="J7" s="67">
+      <c r="J7" s="68">
         <v>44310</v>
       </c>
-      <c r="K7" s="66" t="s">
+      <c r="K7" s="67" t="s">
         <v>16</v>
       </c>
-      <c r="L7" s="67">
+      <c r="L7" s="68">
         <v>44312</v>
       </c>
-      <c r="M7" s="66"/>
-      <c r="N7" s="68"/>
-      <c r="O7" s="69"/>
-      <c r="P7" s="55">
+      <c r="M7" s="67"/>
+      <c r="N7" s="69"/>
+      <c r="O7" s="70"/>
+      <c r="P7" s="56">
         <v>44305</v>
       </c>
-      <c r="Q7" s="48">
+      <c r="Q7" s="49">
         <f t="shared" si="0"/>
         <v>44316</v>
       </c>
@@ -1733,99 +1746,112 @@
       <c r="B8" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="E8" s="54" t="s">
+      <c r="E8" s="55" t="s">
         <v>6</v>
       </c>
-      <c r="F8" s="41"/>
-      <c r="G8" s="42" t="s">
+      <c r="F8" s="42"/>
+      <c r="G8" s="43" t="s">
         <v>16</v>
       </c>
-      <c r="H8" s="41"/>
-      <c r="I8" s="42" t="s">
+      <c r="H8" s="42"/>
+      <c r="I8" s="43" t="s">
         <v>6</v>
       </c>
-      <c r="J8" s="41"/>
-      <c r="K8" s="42"/>
-      <c r="L8" s="41"/>
-      <c r="M8" s="42"/>
-      <c r="N8" s="41"/>
+      <c r="J8" s="42"/>
+      <c r="K8" s="41" t="s">
+        <v>16</v>
+      </c>
+      <c r="L8" s="40">
+        <v>44332</v>
+      </c>
+      <c r="M8" s="41" t="s">
+        <v>8</v>
+      </c>
+      <c r="N8" s="42"/>
       <c r="O8" s="27"/>
-      <c r="P8" s="49">
+      <c r="P8" s="50">
         <v>44312</v>
       </c>
-      <c r="Q8" s="48">
+      <c r="Q8" s="49">
         <f t="shared" si="0"/>
-        <v>44323</v>
+        <v>44334</v>
+      </c>
+      <c r="R8">
+        <v>11</v>
       </c>
       <c r="S8">
         <f t="shared" si="1"/>
-        <v>11</v>
+        <v>22</v>
       </c>
     </row>
     <row r="9" spans="2:19" ht="26.25" customHeight="1">
-      <c r="B9" s="64" t="s">
+      <c r="B9" s="65" t="s">
         <v>13</v>
       </c>
-      <c r="C9" s="65"/>
-      <c r="D9" s="65"/>
-      <c r="E9" s="66" t="s">
+      <c r="C9" s="66"/>
+      <c r="D9" s="66"/>
+      <c r="E9" s="67" t="s">
         <v>8</v>
       </c>
-      <c r="F9" s="67">
+      <c r="F9" s="68">
         <v>44312</v>
       </c>
-      <c r="G9" s="66" t="s">
+      <c r="G9" s="67" t="s">
         <v>16</v>
       </c>
-      <c r="H9" s="68"/>
-      <c r="I9" s="66" t="s">
+      <c r="H9" s="69"/>
+      <c r="I9" s="67" t="s">
         <v>8</v>
       </c>
-      <c r="J9" s="68"/>
-      <c r="K9" s="66"/>
-      <c r="L9" s="68"/>
-      <c r="M9" s="66"/>
-      <c r="N9" s="68"/>
-      <c r="O9" s="69"/>
-      <c r="P9" s="49">
+      <c r="J9" s="69"/>
+      <c r="K9" s="67"/>
+      <c r="L9" s="69"/>
+      <c r="M9" s="67"/>
+      <c r="N9" s="69"/>
+      <c r="O9" s="70"/>
+      <c r="P9" s="50">
         <v>44312</v>
       </c>
-      <c r="Q9" s="48">
+      <c r="Q9" s="49">
         <f t="shared" si="0"/>
-        <v>44323</v>
+        <v>44334</v>
       </c>
       <c r="S9">
         <f t="shared" si="1"/>
-        <v>11</v>
+        <v>22</v>
       </c>
     </row>
     <row r="10" spans="2:19" ht="26.25" customHeight="1">
       <c r="B10" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="E10" s="42" t="s">
+      <c r="E10" s="43" t="s">
         <v>8</v>
       </c>
-      <c r="F10" s="41"/>
-      <c r="G10" s="42"/>
-      <c r="H10" s="41"/>
-      <c r="I10" s="42"/>
-      <c r="J10" s="41"/>
-      <c r="K10" s="42"/>
-      <c r="L10" s="41"/>
-      <c r="M10" s="42"/>
-      <c r="N10" s="41"/>
+      <c r="F10" s="40">
+        <v>44333</v>
+      </c>
+      <c r="G10" s="41" t="s">
+        <v>16</v>
+      </c>
+      <c r="H10" s="42"/>
+      <c r="I10" s="43"/>
+      <c r="J10" s="42"/>
+      <c r="K10" s="43"/>
+      <c r="L10" s="42"/>
+      <c r="M10" s="43"/>
+      <c r="N10" s="42"/>
       <c r="O10" s="27"/>
-      <c r="P10" s="49">
+      <c r="P10" s="50">
         <v>44319</v>
       </c>
-      <c r="Q10" s="48">
+      <c r="Q10" s="49">
         <f t="shared" si="0"/>
-        <v>44330</v>
+        <v>44341</v>
       </c>
       <c r="S10">
         <f t="shared" si="1"/>
-        <v>11</v>
+        <v>22</v>
       </c>
     </row>
     <row r="11" spans="2:19" ht="26.25" customHeight="1">
@@ -1833,29 +1859,29 @@
         <v>15</v>
       </c>
       <c r="D11" s="2"/>
-      <c r="E11" s="43" t="s">
+      <c r="E11" s="73" t="s">
         <v>16</v>
       </c>
-      <c r="F11" s="41"/>
-      <c r="G11" s="42"/>
-      <c r="H11" s="41"/>
-      <c r="I11" s="42"/>
-      <c r="J11" s="41"/>
-      <c r="K11" s="42"/>
-      <c r="L11" s="41"/>
-      <c r="M11" s="42"/>
-      <c r="N11" s="41"/>
+      <c r="F11" s="42"/>
+      <c r="G11" s="43"/>
+      <c r="H11" s="42"/>
+      <c r="I11" s="43"/>
+      <c r="J11" s="42"/>
+      <c r="K11" s="43"/>
+      <c r="L11" s="42"/>
+      <c r="M11" s="43"/>
+      <c r="N11" s="42"/>
       <c r="O11" s="27"/>
-      <c r="P11" s="49">
+      <c r="P11" s="50">
         <v>44340</v>
       </c>
-      <c r="Q11" s="48">
+      <c r="Q11" s="49">
         <f t="shared" si="0"/>
-        <v>44351</v>
+        <v>44362</v>
       </c>
       <c r="S11">
         <f t="shared" si="1"/>
-        <v>11</v>
+        <v>22</v>
       </c>
     </row>
     <row r="12" spans="2:19" ht="26.25" customHeight="1">
@@ -1863,60 +1889,66 @@
         <v>17</v>
       </c>
       <c r="D12" s="2"/>
-      <c r="E12" s="43" t="s">
+      <c r="E12" s="44" t="s">
         <v>8</v>
       </c>
-      <c r="F12" s="41"/>
-      <c r="G12" s="42"/>
-      <c r="H12" s="41"/>
-      <c r="I12" s="42"/>
-      <c r="J12" s="41"/>
-      <c r="K12" s="42"/>
-      <c r="L12" s="41"/>
-      <c r="M12" s="42"/>
-      <c r="N12" s="41"/>
+      <c r="F12" s="42"/>
+      <c r="G12" s="43"/>
+      <c r="H12" s="42"/>
+      <c r="I12" s="43"/>
+      <c r="J12" s="42"/>
+      <c r="K12" s="43"/>
+      <c r="L12" s="42"/>
+      <c r="M12" s="43"/>
+      <c r="N12" s="42"/>
       <c r="O12" s="27"/>
-      <c r="P12" s="49">
+      <c r="P12" s="50">
         <v>44354</v>
       </c>
-      <c r="Q12" s="48">
+      <c r="Q12" s="49">
         <f t="shared" si="0"/>
-        <v>44365</v>
+        <v>44376</v>
       </c>
       <c r="S12">
         <f t="shared" si="1"/>
-        <v>11</v>
+        <v>22</v>
       </c>
     </row>
     <row r="13" spans="2:19" ht="26.25" customHeight="1">
       <c r="B13" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="E13" s="42" t="s">
+      <c r="E13" s="43" t="s">
         <v>6</v>
       </c>
       <c r="F13" s="40">
         <v>44332</v>
       </c>
-      <c r="G13" s="42"/>
-      <c r="H13" s="41"/>
-      <c r="I13" s="42"/>
-      <c r="J13" s="41"/>
-      <c r="K13" s="42"/>
-      <c r="L13" s="41"/>
-      <c r="M13" s="42"/>
-      <c r="N13" s="41"/>
+      <c r="G13" s="41" t="s">
+        <v>16</v>
+      </c>
+      <c r="H13" s="40">
+        <v>44333</v>
+      </c>
+      <c r="I13" s="41" t="s">
+        <v>6</v>
+      </c>
+      <c r="J13" s="42"/>
+      <c r="K13" s="43"/>
+      <c r="L13" s="42"/>
+      <c r="M13" s="43"/>
+      <c r="N13" s="42"/>
       <c r="O13" s="27"/>
-      <c r="P13" s="49">
+      <c r="P13" s="50">
         <v>44361</v>
       </c>
-      <c r="Q13" s="48">
+      <c r="Q13" s="49">
         <f t="shared" si="0"/>
-        <v>44372</v>
+        <v>44383</v>
       </c>
       <c r="S13">
         <f t="shared" si="1"/>
-        <v>11</v>
+        <v>22</v>
       </c>
     </row>
     <row r="14" spans="2:19" ht="26.25" customHeight="1" thickBot="1">
@@ -1925,29 +1957,29 @@
       </c>
       <c r="C14" s="37"/>
       <c r="D14" s="37"/>
-      <c r="E14" s="44" t="s">
+      <c r="E14" s="45" t="s">
         <v>8</v>
       </c>
-      <c r="F14" s="45"/>
-      <c r="G14" s="44"/>
-      <c r="H14" s="45"/>
-      <c r="I14" s="44"/>
-      <c r="J14" s="45"/>
-      <c r="K14" s="44"/>
-      <c r="L14" s="45"/>
-      <c r="M14" s="44"/>
-      <c r="N14" s="45"/>
-      <c r="O14" s="46"/>
-      <c r="P14" s="50">
+      <c r="F14" s="46"/>
+      <c r="G14" s="45"/>
+      <c r="H14" s="46"/>
+      <c r="I14" s="45"/>
+      <c r="J14" s="46"/>
+      <c r="K14" s="45"/>
+      <c r="L14" s="46"/>
+      <c r="M14" s="45"/>
+      <c r="N14" s="46"/>
+      <c r="O14" s="47"/>
+      <c r="P14" s="51">
         <v>44368</v>
       </c>
-      <c r="Q14" s="48">
+      <c r="Q14" s="49">
         <f t="shared" si="0"/>
-        <v>44379</v>
+        <v>44390</v>
       </c>
       <c r="S14">
         <f t="shared" si="1"/>
-        <v>11</v>
+        <v>22</v>
       </c>
     </row>
     <row r="15" spans="2:19" ht="15.75" customHeight="1" thickTop="1">
@@ -1963,7 +1995,7 @@
       <c r="N15" s="38"/>
     </row>
     <row r="16" spans="2:19" ht="15.75" customHeight="1">
-      <c r="E16" s="47" t="s">
+      <c r="E16" s="48" t="s">
         <v>119</v>
       </c>
       <c r="F16" s="39"/>
@@ -1974,12 +2006,12 @@
       <c r="K16" s="39"/>
       <c r="L16" s="39"/>
       <c r="M16" s="39"/>
-      <c r="O16" s="51" t="s">
+      <c r="O16" s="52" t="s">
         <v>128</v>
       </c>
     </row>
     <row r="17" spans="5:16" ht="15.75" customHeight="1">
-      <c r="E17" s="47" t="s">
+      <c r="E17" s="48" t="s">
         <v>120</v>
       </c>
       <c r="F17" s="39"/>
@@ -1990,12 +2022,12 @@
       <c r="K17" s="39"/>
       <c r="L17" s="39"/>
       <c r="M17" s="39"/>
-      <c r="O17" s="47" t="s">
+      <c r="O17" s="48" t="s">
         <v>129</v>
       </c>
     </row>
     <row r="18" spans="5:16" ht="15.75" customHeight="1">
-      <c r="E18" s="47" t="s">
+      <c r="E18" s="48" t="s">
         <v>121</v>
       </c>
       <c r="F18" s="39"/>
@@ -2006,11 +2038,11 @@
       <c r="K18" s="39"/>
       <c r="L18" s="39"/>
       <c r="M18" s="39"/>
-      <c r="N18" s="52"/>
+      <c r="N18" s="53"/>
       <c r="O18" s="27"/>
     </row>
     <row r="19" spans="5:16" ht="15.75" customHeight="1">
-      <c r="E19" s="47" t="s">
+      <c r="E19" s="48" t="s">
         <v>122</v>
       </c>
       <c r="F19" s="39"/>
@@ -2021,9 +2053,9 @@
       <c r="K19" s="39"/>
       <c r="L19" s="39"/>
       <c r="M19" s="39"/>
-      <c r="N19" s="52"/>
+      <c r="N19" s="53"/>
       <c r="O19" s="27"/>
-      <c r="P19" s="53"/>
+      <c r="P19" s="54"/>
     </row>
     <row r="20" spans="5:16" ht="15.75" customHeight="1">
       <c r="F20" s="39"/>
@@ -2034,11 +2066,11 @@
       <c r="K20" s="39"/>
       <c r="L20" s="39"/>
       <c r="M20" s="39"/>
-      <c r="N20" s="52"/>
+      <c r="N20" s="53"/>
       <c r="O20" s="27"/>
     </row>
     <row r="21" spans="5:16" ht="15.75" customHeight="1">
-      <c r="E21" s="47" t="s">
+      <c r="E21" s="48" t="s">
         <v>117</v>
       </c>
       <c r="F21" s="39"/>
@@ -2049,11 +2081,11 @@
       <c r="K21" s="39"/>
       <c r="L21" s="39"/>
       <c r="M21" s="39"/>
-      <c r="N21" s="52"/>
+      <c r="N21" s="53"/>
       <c r="O21" s="27"/>
     </row>
     <row r="22" spans="5:16" ht="15.75" customHeight="1">
-      <c r="E22" s="47" t="s">
+      <c r="E22" s="48" t="s">
         <v>118</v>
       </c>
       <c r="F22" s="39"/>
@@ -2064,7 +2096,7 @@
       <c r="K22" s="39"/>
       <c r="L22" s="39"/>
       <c r="M22" s="39"/>
-      <c r="N22" s="52"/>
+      <c r="N22" s="53"/>
       <c r="O22" s="27"/>
     </row>
     <row r="23" spans="5:16" ht="15.75" customHeight="1">
@@ -2077,7 +2109,7 @@
       <c r="K23" s="39"/>
       <c r="L23" s="39"/>
       <c r="M23" s="39"/>
-      <c r="N23" s="52"/>
+      <c r="N23" s="53"/>
       <c r="O23" s="27"/>
     </row>
     <row r="24" spans="5:16" ht="15.75" customHeight="1">
@@ -2092,7 +2124,7 @@
       <c r="K24" s="39"/>
       <c r="L24" s="39"/>
       <c r="M24" s="39"/>
-      <c r="N24" s="52"/>
+      <c r="N24" s="53"/>
       <c r="O24" s="27"/>
     </row>
     <row r="25" spans="5:16" ht="15.75" customHeight="1">
@@ -2105,7 +2137,7 @@
       <c r="K25" s="39"/>
       <c r="L25" s="39"/>
       <c r="M25" s="39"/>
-      <c r="N25" s="52"/>
+      <c r="N25" s="53"/>
       <c r="O25" s="27"/>
     </row>
     <row r="26" spans="5:16" ht="15.75" customHeight="1">
@@ -2118,7 +2150,7 @@
       <c r="K26" s="39"/>
       <c r="L26" s="39"/>
       <c r="M26" s="39"/>
-      <c r="N26" s="52"/>
+      <c r="N26" s="53"/>
       <c r="O26" s="27"/>
     </row>
     <row r="27" spans="5:16" ht="15.75" customHeight="1">
@@ -2131,7 +2163,7 @@
       <c r="K27" s="39"/>
       <c r="L27" s="39"/>
       <c r="M27" s="39"/>
-      <c r="N27" s="52"/>
+      <c r="N27" s="53"/>
       <c r="O27" s="27"/>
     </row>
     <row r="28" spans="5:16" ht="15.75" customHeight="1">
@@ -2144,7 +2176,7 @@
       <c r="K28" s="39"/>
       <c r="L28" s="39"/>
       <c r="M28" s="39"/>
-      <c r="N28" s="52"/>
+      <c r="N28" s="53"/>
       <c r="O28" s="27"/>
     </row>
     <row r="29" spans="5:16" ht="15.75" customHeight="1">
@@ -2157,7 +2189,7 @@
       <c r="K29" s="39"/>
       <c r="L29" s="39"/>
       <c r="M29" s="39"/>
-      <c r="N29" s="52"/>
+      <c r="N29" s="53"/>
       <c r="O29" s="27"/>
     </row>
     <row r="30" spans="5:16" ht="15.75" customHeight="1">
@@ -2170,7 +2202,7 @@
       <c r="K30" s="39"/>
       <c r="L30" s="39"/>
       <c r="M30" s="39"/>
-      <c r="N30" s="52"/>
+      <c r="N30" s="53"/>
       <c r="O30" s="27"/>
     </row>
     <row r="31" spans="5:16" ht="15.75" customHeight="1">
@@ -2183,7 +2215,7 @@
       <c r="K31" s="39"/>
       <c r="L31" s="39"/>
       <c r="M31" s="39"/>
-      <c r="N31" s="52"/>
+      <c r="N31" s="53"/>
       <c r="O31" s="27"/>
     </row>
     <row r="32" spans="5:16" ht="15.75" customHeight="1">
@@ -2196,7 +2228,7 @@
       <c r="K32" s="39"/>
       <c r="L32" s="39"/>
       <c r="M32" s="39"/>
-      <c r="N32" s="52"/>
+      <c r="N32" s="53"/>
       <c r="O32" s="27"/>
     </row>
     <row r="33" spans="5:14" ht="15.75" customHeight="1">
@@ -3536,50 +3568,50 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D8AC00B6-697C-45E4-9E65-51AD1E2696C6}">
   <dimension ref="A3:R36"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="190" zoomScaleNormal="190" workbookViewId="0">
+    <sheetView zoomScale="190" zoomScaleNormal="190" workbookViewId="0">
       <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
   <sheetData>
     <row r="3" spans="1:18">
-      <c r="A3" s="57" t="s">
+      <c r="A3" s="58" t="s">
         <v>156</v>
       </c>
     </row>
     <row r="4" spans="1:18">
-      <c r="A4" s="56" t="s">
+      <c r="A4" s="57" t="s">
         <v>157</v>
       </c>
     </row>
     <row r="5" spans="1:18">
-      <c r="B5" s="57" t="s">
+      <c r="B5" s="58" t="s">
         <v>135</v>
       </c>
-      <c r="C5" s="57" t="s">
+      <c r="C5" s="58" t="s">
         <v>130</v>
       </c>
       <c r="F5" t="s">
         <v>131</v>
       </c>
-      <c r="G5" s="59" t="s">
+      <c r="G5" s="60" t="s">
         <v>132</v>
       </c>
     </row>
     <row r="6" spans="1:18">
-      <c r="B6" s="57" t="s">
+      <c r="B6" s="58" t="s">
         <v>136</v>
       </c>
-      <c r="C6" s="57" t="s">
+      <c r="C6" s="58" t="s">
         <v>145</v>
       </c>
       <c r="F6" t="s">
         <v>131</v>
       </c>
-      <c r="G6" s="60" t="s">
+      <c r="G6" s="61" t="s">
         <v>133</v>
       </c>
-      <c r="L6" s="61" t="s">
+      <c r="L6" s="62" t="s">
         <v>134</v>
       </c>
       <c r="R6" t="s">
@@ -3587,35 +3619,35 @@
       </c>
     </row>
     <row r="7" spans="1:18">
-      <c r="B7" s="57" t="s">
+      <c r="B7" s="58" t="s">
         <v>140</v>
       </c>
-      <c r="C7" s="57" t="s">
+      <c r="C7" s="58" t="s">
         <v>141</v>
       </c>
-      <c r="G7" s="58" t="s">
+      <c r="G7" s="59" t="s">
         <v>143</v>
       </c>
-      <c r="L7" s="58" t="s">
+      <c r="L7" s="59" t="s">
         <v>144</v>
       </c>
     </row>
     <row r="8" spans="1:18">
-      <c r="C8" s="57" t="s">
+      <c r="C8" s="58" t="s">
         <v>142</v>
       </c>
     </row>
     <row r="9" spans="1:18">
-      <c r="A9" s="56" t="s">
+      <c r="A9" s="57" t="s">
         <v>166</v>
       </c>
-      <c r="C9" s="57"/>
+      <c r="C9" s="58"/>
     </row>
     <row r="10" spans="1:18">
-      <c r="B10" s="71" t="s">
+      <c r="B10" s="72" t="s">
         <v>167</v>
       </c>
-      <c r="C10" s="57"/>
+      <c r="C10" s="58"/>
     </row>
     <row r="11" spans="1:18">
       <c r="A11" t="s">
@@ -3623,7 +3655,7 @@
       </c>
     </row>
     <row r="12" spans="1:18">
-      <c r="A12" s="56" t="s">
+      <c r="A12" s="57" t="s">
         <v>146</v>
       </c>
     </row>
@@ -3633,44 +3665,44 @@
       </c>
     </row>
     <row r="16" spans="1:18">
-      <c r="A16" s="56" t="s">
+      <c r="A16" s="57" t="s">
         <v>153</v>
       </c>
-      <c r="B16" s="56" t="s">
+      <c r="B16" s="57" t="s">
         <v>154</v>
       </c>
     </row>
     <row r="17" spans="1:12">
-      <c r="A17" s="57" t="s">
+      <c r="A17" s="58" t="s">
         <v>147</v>
       </c>
-      <c r="B17" s="56" t="s">
+      <c r="B17" s="57" t="s">
         <v>155</v>
       </c>
     </row>
     <row r="18" spans="1:12">
-      <c r="A18" s="57"/>
-      <c r="B18" s="56"/>
-      <c r="C18" s="56" t="s">
+      <c r="A18" s="58"/>
+      <c r="B18" s="57"/>
+      <c r="C18" s="57" t="s">
         <v>150</v>
       </c>
     </row>
     <row r="19" spans="1:12">
-      <c r="A19" s="57" t="s">
+      <c r="A19" s="58" t="s">
         <v>151</v>
       </c>
-      <c r="B19" s="56" t="s">
+      <c r="B19" s="57" t="s">
         <v>152</v>
       </c>
     </row>
     <row r="20" spans="1:12">
-      <c r="A20" s="57" t="s">
+      <c r="A20" s="58" t="s">
         <v>158</v>
       </c>
-      <c r="B20" s="56"/>
+      <c r="B20" s="57"/>
     </row>
     <row r="21" spans="1:12">
-      <c r="A21" s="57" t="s">
+      <c r="A21" s="58" t="s">
         <v>148</v>
       </c>
       <c r="B21" t="s">
@@ -3678,28 +3710,28 @@
       </c>
     </row>
     <row r="22" spans="1:12">
-      <c r="A22" s="56"/>
-      <c r="B22" s="57" t="s">
+      <c r="A22" s="57"/>
+      <c r="B22" s="58" t="s">
         <v>159</v>
       </c>
     </row>
     <row r="23" spans="1:12">
-      <c r="A23" s="57" t="s">
+      <c r="A23" s="58" t="s">
         <v>160</v>
       </c>
-      <c r="B23" s="57" t="s">
+      <c r="B23" s="58" t="s">
         <v>161</v>
       </c>
     </row>
     <row r="24" spans="1:12">
-      <c r="A24" s="56"/>
-      <c r="B24" s="56" t="s">
+      <c r="A24" s="57"/>
+      <c r="B24" s="57" t="s">
         <v>162</v>
       </c>
     </row>
     <row r="25" spans="1:12">
-      <c r="A25" s="56"/>
-      <c r="B25" s="57" t="s">
+      <c r="A25" s="57"/>
+      <c r="B25" s="58" t="s">
         <v>163</v>
       </c>
     </row>
@@ -3714,7 +3746,7 @@
       </c>
       <c r="B28" s="11"/>
       <c r="C28" s="11"/>
-      <c r="K28" s="56" t="s">
+      <c r="K28" s="57" t="s">
         <v>164</v>
       </c>
     </row>
@@ -3726,7 +3758,7 @@
       <c r="C29" s="10" t="s">
         <v>58</v>
       </c>
-      <c r="L29" s="56" t="s">
+      <c r="L29" s="57" t="s">
         <v>165</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Two ligh related fixes
1. class name "light_set" to "LightSet" change

2. light/iullum_fs.glsl ... name change "atten" to "strength"
</commit_message>
<xml_diff>
--- a/Word/PlanAndDealines.xlsx
+++ b/Word/PlanAndDealines.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20373"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20374"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ksung\Desktop\GitHub\GTCS-GameEngine2\Word\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{895B2B1D-BF84-4FB7-BF74-17D60E03B222}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2E1A9503-5FBB-46FD-A32B-87F801CDEBC4}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="33645" windowHeight="15855" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="33645" windowHeight="15855" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Chapter Status" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="264" uniqueCount="168">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="263" uniqueCount="166">
   <si>
     <t>First Pass</t>
   </si>
@@ -389,12 +389,6 @@
   </si>
   <si>
     <t>Done</t>
-  </si>
-  <si>
-    <t>Chapter 5 to 8: who on what?</t>
-  </si>
-  <si>
-    <t>Chapter 3: first example index.js explaination, put a comment, leave it to me.</t>
   </si>
   <si>
     <t>Numlist: code and text followed do not get indentation</t>
@@ -601,30 +595,6 @@
   </si>
   <si>
     <t>Chapter 7</t>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">Index.js: </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FF000000"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t>change into one sentence "Lastly, remember to update the engine access file, index.js, to forward the newly defined functionality to the client.</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="10"/>
-        <color rgb="FF000000"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t>"</t>
-    </r>
   </si>
   <si>
     <r>
@@ -710,6 +680,30 @@
   </si>
   <si>
     <t>Lastly, remember to update the engine access file, index.js, to forward the newly defined functionality to the client.</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Index.js: </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>change into one sentence "Lastly, remember to update the engine access file, index.js, to forward the newly defined functionality to the client.</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>"  (introduced in Chapter 6.1)</t>
+    </r>
   </si>
 </sst>
 </file>
@@ -1017,7 +1011,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="74">
+  <cellXfs count="75">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
@@ -1153,12 +1147,6 @@
     <xf numFmtId="0" fontId="28" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="30" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="31" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="31" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -1180,6 +1168,15 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="33" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
   </cellXfs>
@@ -1402,8 +1399,8 @@
   </sheetPr>
   <dimension ref="B1:S142"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="205" zoomScaleNormal="205" workbookViewId="0">
-      <selection activeCell="E11" sqref="E11"/>
+    <sheetView zoomScale="205" zoomScaleNormal="205" workbookViewId="0">
+      <selection activeCell="E21" sqref="E21:E22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1"/>
@@ -1426,26 +1423,26 @@
     <row r="1" spans="2:19" ht="12.75">
       <c r="C1" s="1"/>
       <c r="D1" s="1"/>
-      <c r="E1" s="63" t="s">
+      <c r="E1" s="72" t="s">
         <v>0</v>
       </c>
-      <c r="F1" s="64"/>
-      <c r="G1" s="63" t="s">
+      <c r="F1" s="73"/>
+      <c r="G1" s="72" t="s">
         <v>1</v>
       </c>
-      <c r="H1" s="64"/>
-      <c r="I1" s="63" t="s">
+      <c r="H1" s="73"/>
+      <c r="I1" s="72" t="s">
         <v>2</v>
       </c>
-      <c r="J1" s="64"/>
-      <c r="K1" s="63" t="s">
+      <c r="J1" s="73"/>
+      <c r="K1" s="72" t="s">
         <v>1</v>
       </c>
-      <c r="L1" s="64"/>
-      <c r="M1" s="63" t="s">
+      <c r="L1" s="73"/>
+      <c r="M1" s="72" t="s">
         <v>3</v>
       </c>
-      <c r="N1" s="64"/>
+      <c r="N1" s="73"/>
       <c r="O1" s="28" t="s">
         <v>4</v>
       </c>
@@ -1453,7 +1450,7 @@
         <v>114</v>
       </c>
       <c r="Q1" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
     </row>
     <row r="2" spans="2:19" ht="13.5" thickBot="1">
@@ -1494,139 +1491,139 @@
       </c>
       <c r="P2" s="35"/>
       <c r="R2" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="S2" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
     </row>
     <row r="3" spans="2:19" ht="26.25" customHeight="1" thickTop="1">
-      <c r="B3" s="65" t="s">
+      <c r="B3" s="63" t="s">
         <v>5</v>
       </c>
-      <c r="C3" s="66"/>
-      <c r="D3" s="66"/>
-      <c r="E3" s="67" t="s">
+      <c r="C3" s="64"/>
+      <c r="D3" s="64"/>
+      <c r="E3" s="65" t="s">
         <v>6</v>
       </c>
-      <c r="F3" s="68">
+      <c r="F3" s="66">
         <v>44289</v>
       </c>
-      <c r="G3" s="67" t="s">
+      <c r="G3" s="65" t="s">
         <v>16</v>
       </c>
-      <c r="H3" s="68">
+      <c r="H3" s="66">
         <v>44289</v>
       </c>
-      <c r="I3" s="67" t="s">
+      <c r="I3" s="65" t="s">
         <v>6</v>
       </c>
-      <c r="J3" s="68">
+      <c r="J3" s="66">
         <v>44290</v>
       </c>
-      <c r="K3" s="67" t="s">
+      <c r="K3" s="65" t="s">
         <v>16</v>
       </c>
-      <c r="L3" s="68">
+      <c r="L3" s="66">
         <v>44291</v>
       </c>
-      <c r="M3" s="67" t="s">
+      <c r="M3" s="65" t="s">
         <v>8</v>
       </c>
-      <c r="N3" s="69"/>
-      <c r="O3" s="70" t="s">
+      <c r="N3" s="67"/>
+      <c r="O3" s="68" t="s">
         <v>116</v>
       </c>
       <c r="P3" s="50">
         <v>44291</v>
       </c>
       <c r="Q3" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
     </row>
     <row r="4" spans="2:19" ht="26.25" customHeight="1">
-      <c r="B4" s="65" t="s">
+      <c r="B4" s="63" t="s">
         <v>7</v>
       </c>
-      <c r="C4" s="66"/>
-      <c r="D4" s="66"/>
-      <c r="E4" s="67" t="s">
+      <c r="C4" s="64"/>
+      <c r="D4" s="64"/>
+      <c r="E4" s="65" t="s">
         <v>8</v>
       </c>
-      <c r="F4" s="68">
+      <c r="F4" s="66">
         <v>44284</v>
       </c>
-      <c r="G4" s="67" t="s">
+      <c r="G4" s="65" t="s">
         <v>16</v>
       </c>
-      <c r="H4" s="68">
+      <c r="H4" s="66">
         <v>44286</v>
       </c>
-      <c r="I4" s="67" t="s">
+      <c r="I4" s="65" t="s">
         <v>8</v>
       </c>
-      <c r="J4" s="68">
+      <c r="J4" s="66">
         <v>44290</v>
       </c>
-      <c r="K4" s="67" t="s">
+      <c r="K4" s="65" t="s">
         <v>16</v>
       </c>
-      <c r="L4" s="68">
+      <c r="L4" s="66">
         <v>44290</v>
       </c>
-      <c r="M4" s="67" t="s">
+      <c r="M4" s="65" t="s">
         <v>6</v>
       </c>
-      <c r="N4" s="68">
+      <c r="N4" s="66">
         <v>44290</v>
       </c>
-      <c r="O4" s="70" t="s">
+      <c r="O4" s="68" t="s">
         <v>116</v>
       </c>
       <c r="P4" s="50">
         <v>44291</v>
       </c>
       <c r="Q4" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
     </row>
     <row r="5" spans="2:19" ht="26.25" customHeight="1">
-      <c r="B5" s="65" t="s">
+      <c r="B5" s="63" t="s">
         <v>9</v>
       </c>
-      <c r="C5" s="66"/>
-      <c r="D5" s="66"/>
-      <c r="E5" s="67" t="s">
+      <c r="C5" s="64"/>
+      <c r="D5" s="64"/>
+      <c r="E5" s="65" t="s">
         <v>6</v>
       </c>
-      <c r="F5" s="68">
+      <c r="F5" s="66">
         <v>44296</v>
       </c>
-      <c r="G5" s="67" t="s">
+      <c r="G5" s="65" t="s">
         <v>16</v>
       </c>
-      <c r="H5" s="68">
+      <c r="H5" s="66">
         <v>44296</v>
       </c>
-      <c r="I5" s="67" t="s">
+      <c r="I5" s="65" t="s">
         <v>6</v>
       </c>
-      <c r="J5" s="68">
+      <c r="J5" s="66">
         <v>44297</v>
       </c>
-      <c r="K5" s="67" t="s">
+      <c r="K5" s="65" t="s">
         <v>16</v>
       </c>
-      <c r="L5" s="68">
+      <c r="L5" s="66">
         <v>44298</v>
       </c>
-      <c r="M5" s="67" t="s">
+      <c r="M5" s="65" t="s">
         <v>8</v>
       </c>
-      <c r="N5" s="68">
+      <c r="N5" s="66">
         <v>44299</v>
       </c>
-      <c r="O5" s="71" t="s">
+      <c r="O5" s="69" t="s">
         <v>116</v>
       </c>
       <c r="P5" s="56">
@@ -1645,40 +1642,40 @@
       </c>
     </row>
     <row r="6" spans="2:19" ht="26.25" customHeight="1">
-      <c r="B6" s="65" t="s">
+      <c r="B6" s="63" t="s">
         <v>10</v>
       </c>
-      <c r="C6" s="66"/>
-      <c r="D6" s="66"/>
-      <c r="E6" s="67" t="s">
+      <c r="C6" s="64"/>
+      <c r="D6" s="64"/>
+      <c r="E6" s="65" t="s">
         <v>8</v>
       </c>
-      <c r="F6" s="68"/>
-      <c r="G6" s="67" t="s">
+      <c r="F6" s="66"/>
+      <c r="G6" s="65" t="s">
         <v>16</v>
       </c>
-      <c r="H6" s="68">
+      <c r="H6" s="66">
         <v>44300</v>
       </c>
-      <c r="I6" s="67" t="s">
+      <c r="I6" s="65" t="s">
         <v>8</v>
       </c>
-      <c r="J6" s="68">
+      <c r="J6" s="66">
         <v>44300</v>
       </c>
-      <c r="K6" s="67" t="s">
+      <c r="K6" s="65" t="s">
         <v>16</v>
       </c>
-      <c r="L6" s="68">
+      <c r="L6" s="66">
         <v>44301</v>
       </c>
-      <c r="M6" s="67" t="s">
+      <c r="M6" s="65" t="s">
         <v>6</v>
       </c>
-      <c r="N6" s="68">
+      <c r="N6" s="66">
         <v>44331</v>
       </c>
-      <c r="O6" s="71">
+      <c r="O6" s="69">
         <v>44302</v>
       </c>
       <c r="P6" s="56">
@@ -1697,36 +1694,36 @@
       </c>
     </row>
     <row r="7" spans="2:19" ht="26.25" customHeight="1">
-      <c r="B7" s="65" t="s">
+      <c r="B7" s="63" t="s">
         <v>11</v>
       </c>
-      <c r="C7" s="66"/>
-      <c r="D7" s="66"/>
-      <c r="E7" s="67" t="s">
+      <c r="C7" s="64"/>
+      <c r="D7" s="64"/>
+      <c r="E7" s="65" t="s">
         <v>6</v>
       </c>
-      <c r="F7" s="69"/>
-      <c r="G7" s="67" t="s">
+      <c r="F7" s="67"/>
+      <c r="G7" s="65" t="s">
         <v>16</v>
       </c>
-      <c r="H7" s="68">
+      <c r="H7" s="66">
         <v>44309</v>
       </c>
-      <c r="I7" s="67" t="s">
+      <c r="I7" s="65" t="s">
         <v>6</v>
       </c>
-      <c r="J7" s="68">
+      <c r="J7" s="66">
         <v>44310</v>
       </c>
-      <c r="K7" s="67" t="s">
+      <c r="K7" s="65" t="s">
         <v>16</v>
       </c>
-      <c r="L7" s="68">
+      <c r="L7" s="66">
         <v>44312</v>
       </c>
-      <c r="M7" s="67"/>
-      <c r="N7" s="69"/>
-      <c r="O7" s="70"/>
+      <c r="M7" s="65"/>
+      <c r="N7" s="67"/>
+      <c r="O7" s="68"/>
       <c r="P7" s="56">
         <v>44305</v>
       </c>
@@ -1764,7 +1761,7 @@
       <c r="L8" s="40">
         <v>44332</v>
       </c>
-      <c r="M8" s="41" t="s">
+      <c r="M8" s="74" t="s">
         <v>8</v>
       </c>
       <c r="N8" s="42"/>
@@ -1785,40 +1782,45 @@
       </c>
     </row>
     <row r="9" spans="2:19" ht="26.25" customHeight="1">
-      <c r="B9" s="65" t="s">
+      <c r="B9" s="63" t="s">
         <v>13</v>
       </c>
-      <c r="C9" s="66"/>
-      <c r="D9" s="66"/>
-      <c r="E9" s="67" t="s">
+      <c r="C9" s="64"/>
+      <c r="D9" s="64"/>
+      <c r="E9" s="65" t="s">
         <v>8</v>
       </c>
-      <c r="F9" s="68">
+      <c r="F9" s="66">
         <v>44312</v>
       </c>
-      <c r="G9" s="67" t="s">
+      <c r="G9" s="65" t="s">
         <v>16</v>
       </c>
-      <c r="H9" s="69"/>
-      <c r="I9" s="67" t="s">
+      <c r="H9" s="67"/>
+      <c r="I9" s="65" t="s">
         <v>8</v>
       </c>
-      <c r="J9" s="69"/>
-      <c r="K9" s="67"/>
-      <c r="L9" s="69"/>
-      <c r="M9" s="67"/>
-      <c r="N9" s="69"/>
-      <c r="O9" s="70"/>
+      <c r="J9" s="67"/>
+      <c r="K9" s="65"/>
+      <c r="L9" s="67"/>
+      <c r="M9" s="65"/>
+      <c r="N9" s="67"/>
+      <c r="O9" s="69">
+        <v>44319</v>
+      </c>
       <c r="P9" s="50">
         <v>44312</v>
       </c>
       <c r="Q9" s="49">
         <f t="shared" si="0"/>
-        <v>44334</v>
+        <v>44319</v>
+      </c>
+      <c r="R9">
+        <v>-15</v>
       </c>
       <c r="S9">
         <f t="shared" si="1"/>
-        <v>22</v>
+        <v>7</v>
       </c>
     </row>
     <row r="10" spans="2:19" ht="26.25" customHeight="1">
@@ -1831,7 +1833,7 @@
       <c r="F10" s="40">
         <v>44333</v>
       </c>
-      <c r="G10" s="41" t="s">
+      <c r="G10" s="74" t="s">
         <v>16</v>
       </c>
       <c r="H10" s="42"/>
@@ -1847,11 +1849,11 @@
       </c>
       <c r="Q10" s="49">
         <f t="shared" si="0"/>
-        <v>44341</v>
+        <v>44326</v>
       </c>
       <c r="S10">
         <f t="shared" si="1"/>
-        <v>22</v>
+        <v>7</v>
       </c>
     </row>
     <row r="11" spans="2:19" ht="26.25" customHeight="1">
@@ -1859,7 +1861,7 @@
         <v>15</v>
       </c>
       <c r="D11" s="2"/>
-      <c r="E11" s="73" t="s">
+      <c r="E11" s="71" t="s">
         <v>16</v>
       </c>
       <c r="F11" s="42"/>
@@ -1877,11 +1879,11 @@
       </c>
       <c r="Q11" s="49">
         <f t="shared" si="0"/>
-        <v>44362</v>
+        <v>44347</v>
       </c>
       <c r="S11">
         <f t="shared" si="1"/>
-        <v>22</v>
+        <v>7</v>
       </c>
     </row>
     <row r="12" spans="2:19" ht="26.25" customHeight="1">
@@ -1907,11 +1909,11 @@
       </c>
       <c r="Q12" s="49">
         <f t="shared" si="0"/>
-        <v>44376</v>
+        <v>44361</v>
       </c>
       <c r="S12">
         <f t="shared" si="1"/>
-        <v>22</v>
+        <v>7</v>
       </c>
     </row>
     <row r="13" spans="2:19" ht="26.25" customHeight="1">
@@ -1933,8 +1935,12 @@
       <c r="I13" s="41" t="s">
         <v>6</v>
       </c>
-      <c r="J13" s="42"/>
-      <c r="K13" s="43"/>
+      <c r="J13" s="40">
+        <v>44337</v>
+      </c>
+      <c r="K13" s="74" t="s">
+        <v>16</v>
+      </c>
       <c r="L13" s="42"/>
       <c r="M13" s="43"/>
       <c r="N13" s="42"/>
@@ -1944,11 +1950,11 @@
       </c>
       <c r="Q13" s="49">
         <f t="shared" si="0"/>
-        <v>44383</v>
+        <v>44368</v>
       </c>
       <c r="S13">
         <f t="shared" si="1"/>
-        <v>22</v>
+        <v>7</v>
       </c>
     </row>
     <row r="14" spans="2:19" ht="26.25" customHeight="1" thickBot="1">
@@ -1975,11 +1981,11 @@
       </c>
       <c r="Q14" s="49">
         <f t="shared" si="0"/>
-        <v>44390</v>
+        <v>44375</v>
       </c>
       <c r="S14">
         <f t="shared" si="1"/>
-        <v>22</v>
+        <v>7</v>
       </c>
     </row>
     <row r="15" spans="2:19" ht="15.75" customHeight="1" thickTop="1">
@@ -1996,7 +2002,7 @@
     </row>
     <row r="16" spans="2:19" ht="15.75" customHeight="1">
       <c r="E16" s="48" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="F16" s="39"/>
       <c r="G16" s="39"/>
@@ -2007,12 +2013,12 @@
       <c r="L16" s="39"/>
       <c r="M16" s="39"/>
       <c r="O16" s="52" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
     </row>
     <row r="17" spans="5:16" ht="15.75" customHeight="1">
       <c r="E17" s="48" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="F17" s="39"/>
       <c r="G17" s="39"/>
@@ -2023,12 +2029,12 @@
       <c r="L17" s="39"/>
       <c r="M17" s="39"/>
       <c r="O17" s="48" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
     </row>
     <row r="18" spans="5:16" ht="15.75" customHeight="1">
       <c r="E18" s="48" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="F18" s="39"/>
       <c r="G18" s="39"/>
@@ -2043,7 +2049,7 @@
     </row>
     <row r="19" spans="5:16" ht="15.75" customHeight="1">
       <c r="E19" s="48" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="F19" s="39"/>
       <c r="G19" s="39"/>
@@ -2070,9 +2076,7 @@
       <c r="O20" s="27"/>
     </row>
     <row r="21" spans="5:16" ht="15.75" customHeight="1">
-      <c r="E21" s="48" t="s">
-        <v>117</v>
-      </c>
+      <c r="E21" s="48"/>
       <c r="F21" s="39"/>
       <c r="G21" s="39"/>
       <c r="H21" s="39"/>
@@ -2085,9 +2089,7 @@
       <c r="O21" s="27"/>
     </row>
     <row r="22" spans="5:16" ht="15.75" customHeight="1">
-      <c r="E22" s="48" t="s">
-        <v>118</v>
-      </c>
+      <c r="E22" s="48"/>
       <c r="F22" s="39"/>
       <c r="G22" s="39"/>
       <c r="H22" s="39"/>
@@ -2114,7 +2116,7 @@
     </row>
     <row r="24" spans="5:16" ht="15.75" customHeight="1">
       <c r="E24" s="39" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="F24" s="39"/>
       <c r="G24" s="39"/>
@@ -3568,171 +3570,171 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D8AC00B6-697C-45E4-9E65-51AD1E2696C6}">
   <dimension ref="A3:R36"/>
   <sheetViews>
-    <sheetView zoomScale="190" zoomScaleNormal="190" workbookViewId="0">
-      <selection activeCell="B10" sqref="B10"/>
+    <sheetView tabSelected="1" zoomScale="190" zoomScaleNormal="190" workbookViewId="0">
+      <selection activeCell="B23" sqref="B23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
   <sheetData>
     <row r="3" spans="1:18">
       <c r="A3" s="58" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
     </row>
     <row r="4" spans="1:18">
       <c r="A4" s="57" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
     </row>
     <row r="5" spans="1:18">
       <c r="B5" s="58" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="C5" s="58" t="s">
+        <v>128</v>
+      </c>
+      <c r="F5" t="s">
+        <v>129</v>
+      </c>
+      <c r="G5" s="60" t="s">
         <v>130</v>
-      </c>
-      <c r="F5" t="s">
-        <v>131</v>
-      </c>
-      <c r="G5" s="60" t="s">
-        <v>132</v>
       </c>
     </row>
     <row r="6" spans="1:18">
       <c r="B6" s="58" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="C6" s="58" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="F6" t="s">
+        <v>129</v>
+      </c>
+      <c r="G6" s="61" t="s">
         <v>131</v>
       </c>
-      <c r="G6" s="61" t="s">
-        <v>133</v>
-      </c>
       <c r="L6" s="62" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="R6" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
     </row>
     <row r="7" spans="1:18">
       <c r="B7" s="58" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="C7" s="58" t="s">
+        <v>139</v>
+      </c>
+      <c r="G7" s="59" t="s">
         <v>141</v>
       </c>
-      <c r="G7" s="59" t="s">
-        <v>143</v>
-      </c>
       <c r="L7" s="59" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
     </row>
     <row r="8" spans="1:18">
       <c r="C8" s="58" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
     </row>
     <row r="9" spans="1:18">
       <c r="A9" s="57" t="s">
-        <v>166</v>
+        <v>163</v>
       </c>
       <c r="C9" s="58"/>
     </row>
     <row r="10" spans="1:18">
-      <c r="B10" s="72" t="s">
-        <v>167</v>
+      <c r="B10" s="70" t="s">
+        <v>164</v>
       </c>
       <c r="C10" s="58"/>
     </row>
     <row r="11" spans="1:18">
       <c r="A11" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
     </row>
     <row r="12" spans="1:18">
       <c r="A12" s="57" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
     </row>
     <row r="13" spans="1:18">
       <c r="A13" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
     </row>
     <row r="16" spans="1:18">
       <c r="A16" s="57" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="B16" s="57" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
     </row>
     <row r="17" spans="1:12">
       <c r="A17" s="58" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="B17" s="57" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
     </row>
     <row r="18" spans="1:12">
       <c r="A18" s="58"/>
       <c r="B18" s="57"/>
       <c r="C18" s="57" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
     </row>
     <row r="19" spans="1:12">
       <c r="A19" s="58" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="B19" s="57" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
     </row>
     <row r="20" spans="1:12">
       <c r="A20" s="58" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="B20" s="57"/>
     </row>
     <row r="21" spans="1:12">
       <c r="A21" s="58" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="B21" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
     </row>
     <row r="22" spans="1:12">
       <c r="A22" s="57"/>
       <c r="B22" s="58" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
     </row>
     <row r="23" spans="1:12">
       <c r="A23" s="58" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="B23" s="58" t="s">
-        <v>161</v>
+        <v>165</v>
       </c>
     </row>
     <row r="24" spans="1:12">
       <c r="A24" s="57"/>
       <c r="B24" s="57" t="s">
-        <v>162</v>
+        <v>159</v>
       </c>
     </row>
     <row r="25" spans="1:12">
       <c r="A25" s="57"/>
       <c r="B25" s="58" t="s">
-        <v>163</v>
+        <v>160</v>
       </c>
     </row>
     <row r="27" spans="1:12">
@@ -3747,7 +3749,7 @@
       <c r="B28" s="11"/>
       <c r="C28" s="11"/>
       <c r="K28" s="57" t="s">
-        <v>164</v>
+        <v>161</v>
       </c>
     </row>
     <row r="29" spans="1:12">
@@ -3759,7 +3761,7 @@
         <v>58</v>
       </c>
       <c r="L29" s="57" t="s">
-        <v>165</v>
+        <v>162</v>
       </c>
     </row>
     <row r="30" spans="1:12" ht="15.75">

</xml_diff>

<commit_message>
Chap 8 update, almost done.
</commit_message>
<xml_diff>
--- a/Word/PlanAndDealines.xlsx
+++ b/Word/PlanAndDealines.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ksung\Desktop\GitHub\GTCS-GameEngine2\Word\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A16F6C12-1A71-4315-AAFA-7EF49DC5D737}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2F71A5DF-A16F-4E44-BC71-042455F85B6A}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="33645" windowHeight="15855" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="33645" windowHeight="15855" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Chapter Status" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="433" uniqueCount="166">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="266" uniqueCount="169">
   <si>
     <t>First Pass</t>
   </si>
@@ -705,12 +705,70 @@
       <t>"  (introduced in Chapter 6.1)</t>
     </r>
   </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Need to: </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">Add in for CameraState (7.2) NOT exporting to the user … </t>
+    </r>
+  </si>
+  <si>
+    <t>Example 3.1, when introduce the core folder, explain ALL modules within this folder are internal to the engine, NOT exported through index.js</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Note that as the sophistication of the engine increases, so does the complexity of the supporting code. In this case, you have designed a internal utility class, </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="9"/>
+        <rFont val="TheSansMonoConNormal"/>
+      </rPr>
+      <t xml:space="preserve">CameraState, </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="9"/>
+        <color rgb="FF000000"/>
+        <rFont val="Utopia"/>
+      </rPr>
+      <t xml:space="preserve">for storing Camera internal state to support interpolation. This is an internal engine operation. There is no reason for the game programmer to access this class and thus the engine access file, </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <i/>
+        <sz val="9"/>
+        <color rgb="FF000000"/>
+        <rFont val="Utopia"/>
+      </rPr>
+      <t>index.js</t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="9"/>
+        <color rgb="FF000000"/>
+        <rFont val="Utopia"/>
+      </rPr>
+      <t>, should not be modified to forward the definition of this class.</t>
+    </r>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="34">
+  <fonts count="37">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -911,6 +969,24 @@
       <name val="Arial"/>
       <family val="2"/>
     </font>
+    <font>
+      <i/>
+      <sz val="9"/>
+      <color rgb="FF000000"/>
+      <name val="Utopia"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="9"/>
+      <name val="TheSansMonoConNormal"/>
+    </font>
+    <font>
+      <b/>
+      <i/>
+      <sz val="9"/>
+      <color rgb="FF000000"/>
+      <name val="Utopia"/>
+    </font>
   </fonts>
   <fills count="3">
     <fill>
@@ -1011,7 +1087,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="76">
+  <cellXfs count="77">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
@@ -1158,12 +1234,6 @@
     <xf numFmtId="0" fontId="33" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="20" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -1181,6 +1251,15 @@
     </xf>
     <xf numFmtId="0" fontId="20" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="34" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1402,7 +1481,7 @@
   </sheetPr>
   <dimension ref="B1:S142"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="205" zoomScaleNormal="205" workbookViewId="0">
+    <sheetView topLeftCell="B1" zoomScale="205" zoomScaleNormal="205" workbookViewId="0">
       <selection activeCell="E14" sqref="E14"/>
     </sheetView>
   </sheetViews>
@@ -1426,26 +1505,26 @@
     <row r="1" spans="2:19" ht="12.75">
       <c r="C1" s="1"/>
       <c r="D1" s="1"/>
-      <c r="E1" s="68" t="s">
+      <c r="E1" s="74" t="s">
         <v>0</v>
       </c>
-      <c r="F1" s="69"/>
-      <c r="G1" s="68" t="s">
+      <c r="F1" s="75"/>
+      <c r="G1" s="74" t="s">
         <v>1</v>
       </c>
-      <c r="H1" s="69"/>
-      <c r="I1" s="68" t="s">
+      <c r="H1" s="75"/>
+      <c r="I1" s="74" t="s">
         <v>2</v>
       </c>
-      <c r="J1" s="69"/>
-      <c r="K1" s="68" t="s">
+      <c r="J1" s="75"/>
+      <c r="K1" s="74" t="s">
         <v>1</v>
       </c>
-      <c r="L1" s="69"/>
-      <c r="M1" s="68" t="s">
+      <c r="L1" s="75"/>
+      <c r="M1" s="74" t="s">
         <v>3</v>
       </c>
-      <c r="N1" s="69"/>
+      <c r="N1" s="75"/>
       <c r="O1" s="28" t="s">
         <v>4</v>
       </c>
@@ -1534,7 +1613,7 @@
         <v>8</v>
       </c>
       <c r="N3" s="65"/>
-      <c r="O3" s="72" t="s">
+      <c r="O3" s="70" t="s">
         <v>116</v>
       </c>
       <c r="P3" s="49">
@@ -1580,7 +1659,7 @@
       <c r="N4" s="64">
         <v>44290</v>
       </c>
-      <c r="O4" s="72" t="s">
+      <c r="O4" s="70" t="s">
         <v>116</v>
       </c>
       <c r="P4" s="49">
@@ -1626,7 +1705,7 @@
       <c r="N5" s="64">
         <v>44299</v>
       </c>
-      <c r="O5" s="71">
+      <c r="O5" s="69">
         <v>44299</v>
       </c>
       <c r="P5" s="54">
@@ -1678,7 +1757,7 @@
       <c r="N6" s="64">
         <v>44331</v>
       </c>
-      <c r="O6" s="71">
+      <c r="O6" s="69">
         <v>44302</v>
       </c>
       <c r="P6" s="54">
@@ -1726,7 +1805,7 @@
       </c>
       <c r="M7" s="63"/>
       <c r="N7" s="65"/>
-      <c r="O7" s="71">
+      <c r="O7" s="69">
         <v>44316</v>
       </c>
       <c r="P7" s="54">
@@ -1750,7 +1829,7 @@
       </c>
       <c r="C8" s="62"/>
       <c r="D8" s="62"/>
-      <c r="E8" s="73" t="s">
+      <c r="E8" s="71" t="s">
         <v>6</v>
       </c>
       <c r="F8" s="65"/>
@@ -1768,13 +1847,13 @@
       <c r="L8" s="64">
         <v>44332</v>
       </c>
-      <c r="M8" s="74" t="s">
+      <c r="M8" s="72" t="s">
         <v>8</v>
       </c>
       <c r="N8" s="64">
         <v>44339</v>
       </c>
-      <c r="O8" s="71">
+      <c r="O8" s="69">
         <v>44339</v>
       </c>
       <c r="P8" s="49">
@@ -1816,7 +1895,7 @@
       <c r="L9" s="65"/>
       <c r="M9" s="63"/>
       <c r="N9" s="65"/>
-      <c r="O9" s="71">
+      <c r="O9" s="69">
         <v>44319</v>
       </c>
       <c r="P9" s="49">
@@ -1844,7 +1923,7 @@
       <c r="F10" s="40">
         <v>44333</v>
       </c>
-      <c r="G10" s="70" t="s">
+      <c r="G10" s="68" t="s">
         <v>16</v>
       </c>
       <c r="H10" s="42"/>
@@ -1955,7 +2034,7 @@
       <c r="L13" s="40">
         <v>44339</v>
       </c>
-      <c r="M13" s="70" t="s">
+      <c r="M13" s="68" t="s">
         <v>8</v>
       </c>
       <c r="N13" s="42"/>
@@ -1978,7 +2057,7 @@
       </c>
       <c r="C14" s="37"/>
       <c r="D14" s="37"/>
-      <c r="E14" s="75" t="s">
+      <c r="E14" s="73" t="s">
         <v>8</v>
       </c>
       <c r="F14" s="45"/>
@@ -3583,10 +3662,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D8AC00B6-697C-45E4-9E65-51AD1E2696C6}">
-  <dimension ref="A3:R36"/>
+  <dimension ref="A3:R39"/>
   <sheetViews>
-    <sheetView zoomScale="190" zoomScaleNormal="190" workbookViewId="0">
-      <selection activeCell="I24" sqref="I24"/>
+    <sheetView tabSelected="1" zoomScale="190" zoomScaleNormal="190" workbookViewId="0">
+      <selection activeCell="C28" sqref="C28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
@@ -3713,132 +3792,148 @@
       </c>
     </row>
     <row r="20" spans="1:12">
-      <c r="A20" s="56" t="s">
-        <v>156</v>
-      </c>
-      <c r="B20" s="55"/>
+      <c r="A20" s="56"/>
+      <c r="B20" s="55" t="s">
+        <v>167</v>
+      </c>
     </row>
     <row r="21" spans="1:12">
       <c r="A21" s="56" t="s">
+        <v>156</v>
+      </c>
+      <c r="B21" s="55"/>
+    </row>
+    <row r="22" spans="1:12">
+      <c r="A22" s="56" t="s">
         <v>146</v>
       </c>
-      <c r="B21" t="s">
+      <c r="B22" t="s">
         <v>147</v>
       </c>
     </row>
-    <row r="22" spans="1:12">
-      <c r="A22" s="55"/>
-      <c r="B22" s="56" t="s">
+    <row r="23" spans="1:12">
+      <c r="A23" s="55"/>
+      <c r="B23" s="56" t="s">
         <v>157</v>
       </c>
     </row>
-    <row r="23" spans="1:12">
-      <c r="A23" s="56" t="s">
+    <row r="24" spans="1:12">
+      <c r="A24" s="56" t="s">
         <v>158</v>
       </c>
-      <c r="B23" s="56" t="s">
+      <c r="B24" s="56" t="s">
         <v>165</v>
-      </c>
-    </row>
-    <row r="24" spans="1:12">
-      <c r="A24" s="55"/>
-      <c r="B24" s="55" t="s">
-        <v>159</v>
       </c>
     </row>
     <row r="25" spans="1:12">
       <c r="A25" s="55"/>
-      <c r="B25" s="56" t="s">
+      <c r="B25" s="55" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="26" spans="1:12">
+      <c r="A26" s="55"/>
+      <c r="B26" s="56" t="s">
         <v>160</v>
       </c>
     </row>
     <row r="27" spans="1:12">
-      <c r="A27" s="2" t="s">
+      <c r="B27" s="56" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="28" spans="1:12">
+      <c r="C28" s="76" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="30" spans="1:12">
+      <c r="A30" s="2" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="28" spans="1:12">
-      <c r="A28" s="10" t="s">
+    <row r="31" spans="1:12">
+      <c r="A31" s="10" t="s">
         <v>56</v>
       </c>
-      <c r="B28" s="11"/>
-      <c r="C28" s="11"/>
-      <c r="K28" s="55" t="s">
+      <c r="B31" s="11"/>
+      <c r="C31" s="11"/>
+      <c r="K31" s="55" t="s">
         <v>161</v>
-      </c>
-    </row>
-    <row r="29" spans="1:12">
-      <c r="A29" s="12" t="s">
-        <v>57</v>
-      </c>
-      <c r="B29" s="11"/>
-      <c r="C29" s="10" t="s">
-        <v>58</v>
-      </c>
-      <c r="L29" s="55" t="s">
-        <v>162</v>
-      </c>
-    </row>
-    <row r="30" spans="1:12" ht="15.75">
-      <c r="A30" s="12" t="s">
-        <v>59</v>
-      </c>
-      <c r="B30" s="11"/>
-      <c r="C30" s="13" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="31" spans="1:12">
-      <c r="A31" s="12" t="s">
-        <v>61</v>
-      </c>
-      <c r="B31" s="11"/>
-      <c r="C31" s="10" t="s">
-        <v>62</v>
       </c>
     </row>
     <row r="32" spans="1:12">
       <c r="A32" s="12" t="s">
-        <v>63</v>
+        <v>57</v>
       </c>
       <c r="B32" s="11"/>
       <c r="C32" s="10" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="33" spans="1:3">
+        <v>58</v>
+      </c>
+      <c r="L32" s="55" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3" ht="15.75">
       <c r="A33" s="12" t="s">
-        <v>64</v>
+        <v>59</v>
       </c>
       <c r="B33" s="11"/>
-      <c r="C33" s="10" t="s">
-        <v>65</v>
+      <c r="C33" s="13" t="s">
+        <v>60</v>
       </c>
     </row>
     <row r="34" spans="1:3">
       <c r="A34" s="12" t="s">
-        <v>66</v>
+        <v>61</v>
       </c>
       <c r="B34" s="11"/>
       <c r="C34" s="10" t="s">
-        <v>67</v>
+        <v>62</v>
       </c>
     </row>
     <row r="35" spans="1:3">
       <c r="A35" s="12" t="s">
-        <v>68</v>
+        <v>63</v>
       </c>
       <c r="B35" s="11"/>
       <c r="C35" s="10" t="s">
-        <v>69</v>
+        <v>62</v>
       </c>
     </row>
     <row r="36" spans="1:3">
       <c r="A36" s="12" t="s">
-        <v>41</v>
+        <v>64</v>
       </c>
       <c r="B36" s="11"/>
       <c r="C36" s="10" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="37" spans="1:3">
+      <c r="A37" s="12" t="s">
+        <v>66</v>
+      </c>
+      <c r="B37" s="11"/>
+      <c r="C37" s="10" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="38" spans="1:3">
+      <c r="A38" s="12" t="s">
+        <v>68</v>
+      </c>
+      <c r="B38" s="11"/>
+      <c r="C38" s="10" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="39" spans="1:3">
+      <c r="A39" s="12" t="s">
+        <v>41</v>
+      </c>
+      <c r="B39" s="11"/>
+      <c r="C39" s="10" t="s">
         <v>70</v>
       </c>
     </row>

</xml_diff>

<commit_message>
9.5 and 6 are completed
</commit_message>
<xml_diff>
--- a/Word/PlanAndDealines.xlsx
+++ b/Word/PlanAndDealines.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ksung\Desktop\GitHub\GTCS-GameEngine2\Word\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0110088F-B7CC-4D6E-8631-7DF39D00B5D6}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8F8A8472-9F3E-4157-B014-4C3D8F768802}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="33645" windowHeight="15855" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1117,7 +1117,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="81">
+  <cellXfs count="82">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
@@ -1299,6 +1299,9 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="22" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
   </cellXfs>
@@ -1521,8 +1524,8 @@
   </sheetPr>
   <dimension ref="B1:S145"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B12" zoomScale="205" zoomScaleNormal="205" workbookViewId="0">
-      <selection activeCell="J17" sqref="J17"/>
+    <sheetView tabSelected="1" topLeftCell="B6" zoomScale="205" zoomScaleNormal="205" workbookViewId="0">
+      <selection activeCell="I17" sqref="I17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1"/>
@@ -2200,7 +2203,7 @@
       <c r="H17" s="80" t="s">
         <v>176</v>
       </c>
-      <c r="I17" s="74" t="s">
+      <c r="I17" s="81" t="s">
         <v>8</v>
       </c>
       <c r="J17" s="45"/>

</xml_diff>

<commit_message>
Chap 9 first pass done
</commit_message>
<xml_diff>
--- a/Word/PlanAndDealines.xlsx
+++ b/Word/PlanAndDealines.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ksung\Desktop\GitHub\GTCS-GameEngine2\Word\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{38D49E83-86AE-415F-B96D-CCDA4F22D949}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DBBCC124-A3E6-4B59-8B45-F4349EF5180A}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="33645" windowHeight="15855" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="33645" windowHeight="15855" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Chapter Status" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="288" uniqueCount="181">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="290" uniqueCount="181">
   <si>
     <t>First Pass</t>
   </si>
@@ -804,7 +804,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="38">
+  <fonts count="37">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -999,13 +999,6 @@
       <name val="Utopia"/>
     </font>
     <font>
-      <b/>
-      <sz val="10"/>
-      <color theme="1"/>
-      <name val="Arial"/>
-      <family val="2"/>
-    </font>
-    <font>
       <i/>
       <sz val="9"/>
       <color rgb="FF000000"/>
@@ -1129,7 +1122,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="85">
+  <cellXfs count="84">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
@@ -1273,9 +1266,6 @@
     <xf numFmtId="0" fontId="32" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="33" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf numFmtId="0" fontId="20" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -1291,7 +1281,7 @@
     <xf numFmtId="0" fontId="30" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="34" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="33" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="22" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -1300,7 +1290,7 @@
     <xf numFmtId="16" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="37" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="36" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
@@ -1310,20 +1300,20 @@
     <xf numFmtId="0" fontId="20" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="26" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="26" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1545,8 +1535,8 @@
   </sheetPr>
   <dimension ref="B1:S145"/>
   <sheetViews>
-    <sheetView topLeftCell="B3" zoomScale="205" zoomScaleNormal="205" workbookViewId="0">
-      <selection activeCell="I17" sqref="I17"/>
+    <sheetView tabSelected="1" topLeftCell="B3" zoomScale="205" zoomScaleNormal="205" workbookViewId="0">
+      <selection activeCell="G12" sqref="G12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1"/>
@@ -1569,26 +1559,26 @@
     <row r="1" spans="2:19" ht="12.75">
       <c r="C1" s="1"/>
       <c r="D1" s="1"/>
-      <c r="E1" s="80" t="s">
+      <c r="E1" s="82" t="s">
         <v>0</v>
       </c>
-      <c r="F1" s="81"/>
-      <c r="G1" s="80" t="s">
+      <c r="F1" s="83"/>
+      <c r="G1" s="82" t="s">
         <v>1</v>
       </c>
-      <c r="H1" s="81"/>
-      <c r="I1" s="80" t="s">
+      <c r="H1" s="83"/>
+      <c r="I1" s="82" t="s">
         <v>2</v>
       </c>
-      <c r="J1" s="81"/>
-      <c r="K1" s="80" t="s">
+      <c r="J1" s="83"/>
+      <c r="K1" s="82" t="s">
         <v>1</v>
       </c>
-      <c r="L1" s="81"/>
-      <c r="M1" s="80" t="s">
+      <c r="L1" s="83"/>
+      <c r="M1" s="82" t="s">
         <v>3</v>
       </c>
-      <c r="N1" s="81"/>
+      <c r="N1" s="83"/>
       <c r="O1" s="28" t="s">
         <v>4</v>
       </c>
@@ -1677,7 +1667,7 @@
         <v>8</v>
       </c>
       <c r="N3" s="65"/>
-      <c r="O3" s="70" t="s">
+      <c r="O3" s="69" t="s">
         <v>115</v>
       </c>
       <c r="P3" s="49">
@@ -1723,7 +1713,7 @@
       <c r="N4" s="64">
         <v>44290</v>
       </c>
-      <c r="O4" s="70" t="s">
+      <c r="O4" s="69" t="s">
         <v>115</v>
       </c>
       <c r="P4" s="49">
@@ -1769,7 +1759,7 @@
       <c r="N5" s="64">
         <v>44299</v>
       </c>
-      <c r="O5" s="69">
+      <c r="O5" s="68">
         <v>44299</v>
       </c>
       <c r="P5" s="54">
@@ -1821,7 +1811,7 @@
       <c r="N6" s="64">
         <v>44331</v>
       </c>
-      <c r="O6" s="69">
+      <c r="O6" s="68">
         <v>44302</v>
       </c>
       <c r="P6" s="54">
@@ -1869,7 +1859,7 @@
       </c>
       <c r="M7" s="63"/>
       <c r="N7" s="65"/>
-      <c r="O7" s="69">
+      <c r="O7" s="68">
         <v>44316</v>
       </c>
       <c r="P7" s="54">
@@ -1893,7 +1883,7 @@
       </c>
       <c r="C8" s="62"/>
       <c r="D8" s="62"/>
-      <c r="E8" s="71" t="s">
+      <c r="E8" s="70" t="s">
         <v>6</v>
       </c>
       <c r="F8" s="65"/>
@@ -1911,13 +1901,13 @@
       <c r="L8" s="64">
         <v>44332</v>
       </c>
-      <c r="M8" s="72" t="s">
+      <c r="M8" s="71" t="s">
         <v>8</v>
       </c>
       <c r="N8" s="64">
         <v>44339</v>
       </c>
-      <c r="O8" s="69">
+      <c r="O8" s="68">
         <v>44339</v>
       </c>
       <c r="P8" s="49">
@@ -1959,7 +1949,7 @@
       <c r="L9" s="65"/>
       <c r="M9" s="63"/>
       <c r="N9" s="65"/>
-      <c r="O9" s="69">
+      <c r="O9" s="68">
         <v>44319</v>
       </c>
       <c r="P9" s="49">
@@ -1999,13 +1989,13 @@
       <c r="J10" s="40">
         <v>44369</v>
       </c>
-      <c r="K10" s="68" t="s">
+      <c r="K10" s="67" t="s">
         <v>6</v>
       </c>
-      <c r="L10" s="84" t="s">
+      <c r="L10" s="81" t="s">
         <v>178</v>
       </c>
-      <c r="M10" s="83" t="s">
+      <c r="M10" s="80" t="s">
         <v>177</v>
       </c>
       <c r="N10" s="42"/>
@@ -2023,11 +2013,11 @@
       </c>
     </row>
     <row r="11" spans="2:19" ht="26.25" customHeight="1">
-      <c r="B11" s="77" t="s">
+      <c r="B11" s="76" t="s">
         <v>171</v>
       </c>
       <c r="D11" s="2"/>
-      <c r="E11" s="76" t="s">
+      <c r="E11" s="75" t="s">
         <v>15</v>
       </c>
       <c r="F11" s="40">
@@ -2039,7 +2029,7 @@
       <c r="H11" s="40">
         <v>44369</v>
       </c>
-      <c r="I11" s="68" t="s">
+      <c r="I11" s="67" t="s">
         <v>172</v>
       </c>
       <c r="J11" s="42"/>
@@ -2061,23 +2051,23 @@
       </c>
     </row>
     <row r="12" spans="2:19" ht="26.25" customHeight="1">
-      <c r="B12" s="77" t="s">
+      <c r="B12" s="76" t="s">
         <v>173</v>
       </c>
       <c r="D12" s="2"/>
-      <c r="E12" s="76" t="s">
+      <c r="E12" s="75" t="s">
         <v>15</v>
       </c>
       <c r="F12" s="40">
         <v>44362</v>
       </c>
-      <c r="G12" s="68" t="s">
+      <c r="G12" s="41" t="s">
         <v>8</v>
       </c>
       <c r="H12" s="40">
         <v>44375</v>
       </c>
-      <c r="I12" s="41" t="s">
+      <c r="I12" s="67" t="s">
         <v>179</v>
       </c>
       <c r="J12" s="42"/>
@@ -2090,15 +2080,19 @@
       <c r="Q12" s="48"/>
     </row>
     <row r="13" spans="2:19" ht="26.25" customHeight="1">
-      <c r="B13" s="77" t="s">
+      <c r="B13" s="76" t="s">
         <v>174</v>
       </c>
       <c r="D13" s="2"/>
-      <c r="E13" s="76" t="s">
+      <c r="E13" s="75" t="s">
         <v>15</v>
       </c>
-      <c r="F13" s="42"/>
-      <c r="G13" s="43"/>
+      <c r="F13" s="40">
+        <v>44376</v>
+      </c>
+      <c r="G13" s="67" t="s">
+        <v>8</v>
+      </c>
       <c r="H13" s="42"/>
       <c r="I13" s="43"/>
       <c r="J13" s="42"/>
@@ -2111,15 +2105,19 @@
       <c r="Q13" s="48"/>
     </row>
     <row r="14" spans="2:19" ht="26.25" customHeight="1">
-      <c r="B14" s="77" t="s">
+      <c r="B14" s="76" t="s">
         <v>175</v>
       </c>
       <c r="D14" s="2"/>
-      <c r="E14" s="67" t="s">
+      <c r="E14" s="75" t="s">
         <v>15</v>
       </c>
-      <c r="F14" s="42"/>
-      <c r="G14" s="43"/>
+      <c r="F14" s="40">
+        <v>44376</v>
+      </c>
+      <c r="G14" s="67" t="s">
+        <v>8</v>
+      </c>
       <c r="H14" s="42"/>
       <c r="I14" s="43"/>
       <c r="J14" s="42"/>
@@ -2136,13 +2134,13 @@
         <v>16</v>
       </c>
       <c r="D15" s="2"/>
-      <c r="E15" s="76" t="s">
+      <c r="E15" s="75" t="s">
         <v>8</v>
       </c>
       <c r="F15" s="40">
         <v>44354</v>
       </c>
-      <c r="G15" s="68" t="s">
+      <c r="G15" s="67" t="s">
         <v>15</v>
       </c>
       <c r="H15" s="42"/>
@@ -2193,7 +2191,7 @@
       <c r="L16" s="40">
         <v>44339</v>
       </c>
-      <c r="M16" s="68" t="s">
+      <c r="M16" s="67" t="s">
         <v>8</v>
       </c>
       <c r="N16" s="40">
@@ -2220,23 +2218,23 @@
       </c>
       <c r="C17" s="37"/>
       <c r="D17" s="37"/>
-      <c r="E17" s="74" t="s">
+      <c r="E17" s="73" t="s">
         <v>169</v>
       </c>
-      <c r="F17" s="75">
+      <c r="F17" s="74">
         <v>44346</v>
       </c>
-      <c r="G17" s="74" t="s">
+      <c r="G17" s="73" t="s">
         <v>6</v>
       </c>
-      <c r="H17" s="78" t="s">
+      <c r="H17" s="77" t="s">
         <v>176</v>
       </c>
-      <c r="I17" s="79" t="s">
+      <c r="I17" s="78" t="s">
         <v>8</v>
       </c>
       <c r="J17" s="45"/>
-      <c r="K17" s="82" t="s">
+      <c r="K17" s="79" t="s">
         <v>15</v>
       </c>
       <c r="L17" s="45"/>
@@ -3837,7 +3835,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D8AC00B6-697C-45E4-9E65-51AD1E2696C6}">
   <dimension ref="A3:R41"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="190" zoomScaleNormal="190" workbookViewId="0">
+    <sheetView zoomScale="190" zoomScaleNormal="190" workbookViewId="0">
       <selection activeCell="B23" sqref="B23"/>
     </sheetView>
   </sheetViews>
@@ -4029,7 +4027,7 @@
       </c>
     </row>
     <row r="30" spans="1:3">
-      <c r="C30" s="73" t="s">
+      <c r="C30" s="72" t="s">
         <v>167</v>
       </c>
     </row>

</xml_diff>

<commit_message>
9.1 chapter overview is done
</commit_message>
<xml_diff>
--- a/Word/PlanAndDealines.xlsx
+++ b/Word/PlanAndDealines.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ksung\Desktop\GitHub\GTCS-GameEngine2\Word\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DBBCC124-A3E6-4B59-8B45-F4349EF5180A}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AB586F7D-C9CF-4DB0-A7B1-FE191103D6E7}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="33645" windowHeight="15855" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="290" uniqueCount="181">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="290" uniqueCount="180">
   <si>
     <t>First Pass</t>
   </si>
@@ -771,9 +771,6 @@
   </si>
   <si>
     <t>Chpater 9-1</t>
-  </si>
-  <si>
-    <t>Kelvin needs to update the intro before passing on</t>
   </si>
   <si>
     <t>Chpater 9-2-4</t>
@@ -1535,8 +1532,8 @@
   </sheetPr>
   <dimension ref="B1:S145"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B3" zoomScale="205" zoomScaleNormal="205" workbookViewId="0">
-      <selection activeCell="G12" sqref="G12"/>
+    <sheetView tabSelected="1" topLeftCell="B4" zoomScale="205" zoomScaleNormal="205" workbookViewId="0">
+      <selection activeCell="I12" sqref="I12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1"/>
@@ -1993,10 +1990,10 @@
         <v>6</v>
       </c>
       <c r="L10" s="81" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="M10" s="80" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="N10" s="42"/>
       <c r="O10" s="27"/>
@@ -2030,7 +2027,7 @@
         <v>44369</v>
       </c>
       <c r="I11" s="67" t="s">
-        <v>172</v>
+        <v>15</v>
       </c>
       <c r="J11" s="42"/>
       <c r="K11" s="43"/>
@@ -2052,7 +2049,7 @@
     </row>
     <row r="12" spans="2:19" ht="26.25" customHeight="1">
       <c r="B12" s="76" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="D12" s="2"/>
       <c r="E12" s="75" t="s">
@@ -2068,7 +2065,7 @@
         <v>44375</v>
       </c>
       <c r="I12" s="67" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="J12" s="42"/>
       <c r="K12" s="43"/>
@@ -2081,7 +2078,7 @@
     </row>
     <row r="13" spans="2:19" ht="26.25" customHeight="1">
       <c r="B13" s="76" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="D13" s="2"/>
       <c r="E13" s="75" t="s">
@@ -2106,7 +2103,7 @@
     </row>
     <row r="14" spans="2:19" ht="26.25" customHeight="1">
       <c r="B14" s="76" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="D14" s="2"/>
       <c r="E14" s="75" t="s">
@@ -2228,7 +2225,7 @@
         <v>6</v>
       </c>
       <c r="H17" s="77" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="I17" s="78" t="s">
         <v>8</v>
@@ -3984,7 +3981,7 @@
     <row r="23" spans="1:3">
       <c r="A23" s="56"/>
       <c r="B23" s="55" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
     </row>
     <row r="24" spans="1:3">

</xml_diff>

<commit_message>
9.1 to 4 almost ready
</commit_message>
<xml_diff>
--- a/Word/PlanAndDealines.xlsx
+++ b/Word/PlanAndDealines.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ksung\Desktop\GitHub\GTCS-GameEngine2\Word\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2FD7AA7F-BD88-44A4-8729-1E021E2FD787}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9AB26F55-3124-4868-B813-0D7D359D705C}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="33645" windowHeight="15855" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="33645" windowHeight="15855" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Chapter Status" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="293" uniqueCount="177">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="295" uniqueCount="179">
   <si>
     <t>First Pass</t>
   </si>
@@ -807,6 +807,12 @@
   </si>
   <si>
     <t>Done date</t>
+  </si>
+  <si>
+    <t>Chapter 8</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> on Page 89 [computeShadowGeometry()], the "Region 1"  should this be changed to match the "Step 1", "Step 2" … as collideCircCirc (on page 26 of Chatper 9), cover in separate steps</t>
   </si>
 </sst>
 </file>
@@ -1332,12 +1338,6 @@
     <xf numFmtId="0" fontId="26" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="37" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="38" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="38" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -1345,6 +1345,12 @@
     </xf>
     <xf numFmtId="16" fontId="38" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1566,8 +1572,8 @@
   </sheetPr>
   <dimension ref="B1:S145"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="205" zoomScaleNormal="205" workbookViewId="0">
-      <selection activeCell="M16" sqref="M16"/>
+    <sheetView topLeftCell="A4" zoomScale="205" zoomScaleNormal="205" workbookViewId="0">
+      <selection activeCell="L13" sqref="L13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1"/>
@@ -1580,7 +1586,7 @@
     <col min="9" max="9" width="7.42578125" style="31" customWidth="1"/>
     <col min="10" max="10" width="7.42578125" style="30" customWidth="1"/>
     <col min="11" max="11" width="7.42578125" style="31" customWidth="1"/>
-    <col min="12" max="12" width="7.42578125" style="30" customWidth="1"/>
+    <col min="12" max="12" width="8.42578125" style="30" customWidth="1"/>
     <col min="13" max="13" width="7.42578125" style="31" customWidth="1"/>
     <col min="14" max="14" width="7.42578125" style="30" customWidth="1"/>
     <col min="15" max="15" width="16.42578125" style="29" customWidth="1"/>
@@ -1590,26 +1596,26 @@
     <row r="1" spans="2:19" ht="12.75">
       <c r="C1" s="1"/>
       <c r="D1" s="1"/>
-      <c r="E1" s="83" t="s">
+      <c r="E1" s="87" t="s">
         <v>0</v>
       </c>
-      <c r="F1" s="84"/>
-      <c r="G1" s="83" t="s">
+      <c r="F1" s="88"/>
+      <c r="G1" s="87" t="s">
         <v>1</v>
       </c>
-      <c r="H1" s="84"/>
-      <c r="I1" s="83" t="s">
+      <c r="H1" s="88"/>
+      <c r="I1" s="87" t="s">
         <v>2</v>
       </c>
-      <c r="J1" s="84"/>
-      <c r="K1" s="83" t="s">
+      <c r="J1" s="88"/>
+      <c r="K1" s="87" t="s">
         <v>1</v>
       </c>
-      <c r="L1" s="84"/>
-      <c r="M1" s="83" t="s">
+      <c r="L1" s="88"/>
+      <c r="M1" s="87" t="s">
         <v>3</v>
       </c>
-      <c r="N1" s="84"/>
+      <c r="N1" s="88"/>
       <c r="O1" s="28" t="s">
         <v>4</v>
       </c>
@@ -1979,36 +1985,36 @@
       </c>
     </row>
     <row r="10" spans="2:19" ht="26.25" customHeight="1">
-      <c r="B10" s="85" t="s">
+      <c r="B10" s="83" t="s">
         <v>14</v>
       </c>
-      <c r="C10" s="86"/>
-      <c r="D10" s="86"/>
-      <c r="E10" s="87" t="s">
+      <c r="C10" s="84"/>
+      <c r="D10" s="84"/>
+      <c r="E10" s="85" t="s">
         <v>8</v>
       </c>
-      <c r="F10" s="88">
+      <c r="F10" s="86">
         <v>44333</v>
       </c>
-      <c r="G10" s="87" t="s">
+      <c r="G10" s="85" t="s">
         <v>15</v>
       </c>
-      <c r="H10" s="88">
+      <c r="H10" s="86">
         <v>44346</v>
       </c>
-      <c r="I10" s="87" t="s">
+      <c r="I10" s="85" t="s">
         <v>8</v>
       </c>
-      <c r="J10" s="88">
+      <c r="J10" s="86">
         <v>44369</v>
       </c>
-      <c r="K10" s="87" t="s">
+      <c r="K10" s="85" t="s">
         <v>6</v>
       </c>
-      <c r="L10" s="88">
+      <c r="L10" s="86">
         <v>44380</v>
       </c>
-      <c r="M10" s="87" t="s">
+      <c r="M10" s="85" t="s">
         <v>15</v>
       </c>
       <c r="N10" s="42"/>
@@ -2052,7 +2058,9 @@
       <c r="K11" s="66" t="s">
         <v>6</v>
       </c>
-      <c r="L11" s="42"/>
+      <c r="L11" s="40">
+        <v>44386</v>
+      </c>
       <c r="M11" s="43"/>
       <c r="N11" s="42"/>
       <c r="O11" s="27"/>
@@ -2093,7 +2101,9 @@
       <c r="K12" s="66" t="s">
         <v>6</v>
       </c>
-      <c r="L12" s="42"/>
+      <c r="L12" s="40">
+        <v>44386</v>
+      </c>
       <c r="M12" s="43"/>
       <c r="N12" s="42"/>
       <c r="O12" s="27"/>
@@ -2173,39 +2183,39 @@
       </c>
     </row>
     <row r="15" spans="2:19" ht="26.25" customHeight="1">
-      <c r="B15" s="85" t="s">
+      <c r="B15" s="83" t="s">
         <v>17</v>
       </c>
-      <c r="C15" s="86"/>
-      <c r="D15" s="86"/>
-      <c r="E15" s="87" t="s">
+      <c r="C15" s="84"/>
+      <c r="D15" s="84"/>
+      <c r="E15" s="85" t="s">
         <v>6</v>
       </c>
-      <c r="F15" s="88">
+      <c r="F15" s="86">
         <v>44332</v>
       </c>
-      <c r="G15" s="87" t="s">
+      <c r="G15" s="85" t="s">
         <v>15</v>
       </c>
-      <c r="H15" s="88">
+      <c r="H15" s="86">
         <v>44333</v>
       </c>
-      <c r="I15" s="87" t="s">
+      <c r="I15" s="85" t="s">
         <v>6</v>
       </c>
-      <c r="J15" s="88">
+      <c r="J15" s="86">
         <v>44337</v>
       </c>
-      <c r="K15" s="87" t="s">
+      <c r="K15" s="85" t="s">
         <v>15</v>
       </c>
-      <c r="L15" s="88">
+      <c r="L15" s="86">
         <v>44339</v>
       </c>
-      <c r="M15" s="87" t="s">
+      <c r="M15" s="85" t="s">
         <v>8</v>
       </c>
-      <c r="N15" s="88">
+      <c r="N15" s="86">
         <v>44354</v>
       </c>
       <c r="O15" s="78">
@@ -3872,10 +3882,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D8AC00B6-697C-45E4-9E65-51AD1E2696C6}">
-  <dimension ref="A3:R41"/>
+  <dimension ref="A3:R43"/>
   <sheetViews>
-    <sheetView zoomScale="190" zoomScaleNormal="190" workbookViewId="0">
-      <selection activeCell="B23" sqref="B23"/>
+    <sheetView tabSelected="1" zoomScale="190" zoomScaleNormal="190" workbookViewId="0">
+      <selection activeCell="B31" sqref="B31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
@@ -4070,93 +4080,101 @@
         <v>167</v>
       </c>
     </row>
-    <row r="32" spans="1:3">
-      <c r="A32" s="2" t="s">
+    <row r="31" spans="1:3">
+      <c r="A31" s="55" t="s">
+        <v>177</v>
+      </c>
+      <c r="B31" s="54" t="s">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="34" spans="1:12">
+      <c r="A34" s="2" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="33" spans="1:12">
-      <c r="A33" s="10" t="s">
+    <row r="35" spans="1:12">
+      <c r="A35" s="10" t="s">
         <v>55</v>
       </c>
-      <c r="B33" s="11"/>
-      <c r="C33" s="11"/>
-      <c r="K33" s="54" t="s">
+      <c r="B35" s="11"/>
+      <c r="C35" s="11"/>
+      <c r="K35" s="54" t="s">
         <v>160</v>
-      </c>
-    </row>
-    <row r="34" spans="1:12">
-      <c r="A34" s="12" t="s">
-        <v>56</v>
-      </c>
-      <c r="B34" s="11"/>
-      <c r="C34" s="10" t="s">
-        <v>57</v>
-      </c>
-      <c r="L34" s="54" t="s">
-        <v>161</v>
-      </c>
-    </row>
-    <row r="35" spans="1:12" ht="15.75">
-      <c r="A35" s="12" t="s">
-        <v>58</v>
-      </c>
-      <c r="B35" s="11"/>
-      <c r="C35" s="13" t="s">
-        <v>59</v>
       </c>
     </row>
     <row r="36" spans="1:12">
       <c r="A36" s="12" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
       <c r="B36" s="11"/>
       <c r="C36" s="10" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="37" spans="1:12">
+        <v>57</v>
+      </c>
+      <c r="L36" s="54" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="37" spans="1:12" ht="15.75">
       <c r="A37" s="12" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
       <c r="B37" s="11"/>
-      <c r="C37" s="10" t="s">
-        <v>61</v>
+      <c r="C37" s="13" t="s">
+        <v>59</v>
       </c>
     </row>
     <row r="38" spans="1:12">
       <c r="A38" s="12" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="B38" s="11"/>
       <c r="C38" s="10" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
     </row>
     <row r="39" spans="1:12">
       <c r="A39" s="12" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="B39" s="11"/>
       <c r="C39" s="10" t="s">
-        <v>66</v>
+        <v>61</v>
       </c>
     </row>
     <row r="40" spans="1:12">
       <c r="A40" s="12" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
       <c r="B40" s="11"/>
       <c r="C40" s="10" t="s">
-        <v>68</v>
+        <v>64</v>
       </c>
     </row>
     <row r="41" spans="1:12">
       <c r="A41" s="12" t="s">
-        <v>40</v>
+        <v>65</v>
       </c>
       <c r="B41" s="11"/>
       <c r="C41" s="10" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="42" spans="1:12">
+      <c r="A42" s="12" t="s">
+        <v>67</v>
+      </c>
+      <c r="B42" s="11"/>
+      <c r="C42" s="10" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="43" spans="1:12">
+      <c r="A43" s="12" t="s">
+        <v>40</v>
+      </c>
+      <c r="B43" s="11"/>
+      <c r="C43" s="10" t="s">
         <v>69</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Chap 10, final review
</commit_message>
<xml_diff>
--- a/Word/PlanAndDealines.xlsx
+++ b/Word/PlanAndDealines.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ksung\Desktop\GitHub\GTCS-GameEngine2\Word\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9AB26F55-3124-4868-B813-0D7D359D705C}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1BC76E3E-660F-4415-8B97-D2E1865850C2}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="33645" windowHeight="15855" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="33645" windowHeight="15855" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Chapter Status" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="295" uniqueCount="179">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="406" uniqueCount="179">
   <si>
     <t>First Pass</t>
   </si>
@@ -819,7 +819,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="39">
+  <fonts count="41">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -1050,6 +1050,19 @@
       <name val="Arial"/>
       <family val="2"/>
     </font>
+    <font>
+      <b/>
+      <sz val="10"/>
+      <color theme="0" tint="-0.249977111117893"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color theme="0" tint="-0.249977111117893"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
   </fonts>
   <fills count="3">
     <fill>
@@ -1150,7 +1163,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="89">
+  <cellXfs count="92">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
@@ -1221,8 +1234,6 @@
     <xf numFmtId="0" fontId="20" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1239,12 +1250,6 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -1309,20 +1314,7 @@
     <xf numFmtId="0" fontId="33" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="16" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf numFmtId="0" fontId="36" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="16" fontId="20" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
@@ -1351,6 +1343,34 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="39" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="40" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="40" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="16" fontId="40" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="39" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="40" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="39" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="40" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="40" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="16" fontId="40" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="40" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="39" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1572,8 +1592,8 @@
   </sheetPr>
   <dimension ref="B1:S145"/>
   <sheetViews>
-    <sheetView topLeftCell="A4" zoomScale="205" zoomScaleNormal="205" workbookViewId="0">
-      <selection activeCell="L13" sqref="L13"/>
+    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="205" zoomScaleNormal="205" workbookViewId="0">
+      <selection activeCell="M10" sqref="M10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1"/>
@@ -1596,26 +1616,26 @@
     <row r="1" spans="2:19" ht="12.75">
       <c r="C1" s="1"/>
       <c r="D1" s="1"/>
-      <c r="E1" s="87" t="s">
+      <c r="E1" s="78" t="s">
         <v>0</v>
       </c>
-      <c r="F1" s="88"/>
-      <c r="G1" s="87" t="s">
+      <c r="F1" s="79"/>
+      <c r="G1" s="78" t="s">
         <v>1</v>
       </c>
-      <c r="H1" s="88"/>
-      <c r="I1" s="87" t="s">
+      <c r="H1" s="79"/>
+      <c r="I1" s="78" t="s">
         <v>2</v>
       </c>
-      <c r="J1" s="88"/>
-      <c r="K1" s="87" t="s">
+      <c r="J1" s="79"/>
+      <c r="K1" s="78" t="s">
         <v>1</v>
       </c>
-      <c r="L1" s="88"/>
-      <c r="M1" s="87" t="s">
+      <c r="L1" s="79"/>
+      <c r="M1" s="78" t="s">
         <v>3</v>
       </c>
-      <c r="N1" s="88"/>
+      <c r="N1" s="79"/>
       <c r="O1" s="28" t="s">
         <v>4</v>
       </c>
@@ -1671,43 +1691,43 @@
       </c>
     </row>
     <row r="3" spans="2:19" ht="26.25" customHeight="1" thickTop="1">
-      <c r="B3" s="60" t="s">
+      <c r="B3" s="56" t="s">
         <v>5</v>
       </c>
-      <c r="C3" s="61"/>
-      <c r="D3" s="61"/>
-      <c r="E3" s="62" t="s">
+      <c r="C3" s="57"/>
+      <c r="D3" s="57"/>
+      <c r="E3" s="58" t="s">
         <v>6</v>
       </c>
-      <c r="F3" s="63">
+      <c r="F3" s="59">
         <v>44289</v>
       </c>
-      <c r="G3" s="62" t="s">
+      <c r="G3" s="58" t="s">
         <v>15</v>
       </c>
-      <c r="H3" s="63">
+      <c r="H3" s="59">
         <v>44289</v>
       </c>
-      <c r="I3" s="62" t="s">
+      <c r="I3" s="58" t="s">
         <v>6</v>
       </c>
-      <c r="J3" s="63">
+      <c r="J3" s="59">
         <v>44290</v>
       </c>
-      <c r="K3" s="62" t="s">
+      <c r="K3" s="58" t="s">
         <v>15</v>
       </c>
-      <c r="L3" s="63">
+      <c r="L3" s="59">
         <v>44291</v>
       </c>
-      <c r="M3" s="62" t="s">
+      <c r="M3" s="58" t="s">
         <v>8</v>
       </c>
-      <c r="N3" s="64"/>
-      <c r="O3" s="68" t="s">
+      <c r="N3" s="60"/>
+      <c r="O3" s="64" t="s">
         <v>115</v>
       </c>
-      <c r="P3" s="48">
+      <c r="P3" s="44">
         <v>44291</v>
       </c>
       <c r="Q3" t="s">
@@ -1715,45 +1735,45 @@
       </c>
     </row>
     <row r="4" spans="2:19" ht="26.25" customHeight="1">
-      <c r="B4" s="60" t="s">
+      <c r="B4" s="56" t="s">
         <v>7</v>
       </c>
-      <c r="C4" s="61"/>
-      <c r="D4" s="61"/>
-      <c r="E4" s="62" t="s">
+      <c r="C4" s="57"/>
+      <c r="D4" s="57"/>
+      <c r="E4" s="58" t="s">
         <v>8</v>
       </c>
-      <c r="F4" s="63">
+      <c r="F4" s="59">
         <v>44284</v>
       </c>
-      <c r="G4" s="62" t="s">
+      <c r="G4" s="58" t="s">
         <v>15</v>
       </c>
-      <c r="H4" s="63">
+      <c r="H4" s="59">
         <v>44286</v>
       </c>
-      <c r="I4" s="62" t="s">
+      <c r="I4" s="58" t="s">
         <v>8</v>
       </c>
-      <c r="J4" s="63">
+      <c r="J4" s="59">
         <v>44290</v>
       </c>
-      <c r="K4" s="62" t="s">
+      <c r="K4" s="58" t="s">
         <v>15</v>
       </c>
-      <c r="L4" s="63">
+      <c r="L4" s="59">
         <v>44290</v>
       </c>
-      <c r="M4" s="62" t="s">
+      <c r="M4" s="58" t="s">
         <v>6</v>
       </c>
-      <c r="N4" s="63">
+      <c r="N4" s="59">
         <v>44290</v>
       </c>
-      <c r="O4" s="68" t="s">
+      <c r="O4" s="64" t="s">
         <v>115</v>
       </c>
-      <c r="P4" s="48">
+      <c r="P4" s="44">
         <v>44291</v>
       </c>
       <c r="Q4" t="s">
@@ -1761,48 +1781,48 @@
       </c>
     </row>
     <row r="5" spans="2:19" ht="26.25" customHeight="1">
-      <c r="B5" s="60" t="s">
+      <c r="B5" s="56" t="s">
         <v>9</v>
       </c>
-      <c r="C5" s="61"/>
-      <c r="D5" s="61"/>
-      <c r="E5" s="62" t="s">
+      <c r="C5" s="57"/>
+      <c r="D5" s="57"/>
+      <c r="E5" s="58" t="s">
         <v>6</v>
       </c>
-      <c r="F5" s="63">
+      <c r="F5" s="59">
         <v>44296</v>
       </c>
-      <c r="G5" s="62" t="s">
+      <c r="G5" s="58" t="s">
         <v>15</v>
       </c>
-      <c r="H5" s="63">
+      <c r="H5" s="59">
         <v>44296</v>
       </c>
-      <c r="I5" s="62" t="s">
+      <c r="I5" s="58" t="s">
         <v>6</v>
       </c>
-      <c r="J5" s="63">
+      <c r="J5" s="59">
         <v>44297</v>
       </c>
-      <c r="K5" s="62" t="s">
+      <c r="K5" s="58" t="s">
         <v>15</v>
       </c>
-      <c r="L5" s="63">
+      <c r="L5" s="59">
         <v>44298</v>
       </c>
-      <c r="M5" s="62" t="s">
+      <c r="M5" s="58" t="s">
         <v>8</v>
       </c>
-      <c r="N5" s="63">
+      <c r="N5" s="59">
         <v>44299</v>
       </c>
-      <c r="O5" s="67">
+      <c r="O5" s="63">
         <v>44299</v>
       </c>
-      <c r="P5" s="53">
+      <c r="P5" s="49">
         <v>44298</v>
       </c>
-      <c r="Q5" s="47">
+      <c r="Q5" s="43">
         <v>44299</v>
       </c>
       <c r="R5">
@@ -1811,46 +1831,46 @@
       </c>
     </row>
     <row r="6" spans="2:19" ht="26.25" customHeight="1">
-      <c r="B6" s="60" t="s">
+      <c r="B6" s="56" t="s">
         <v>10</v>
       </c>
-      <c r="C6" s="61"/>
-      <c r="D6" s="61"/>
-      <c r="E6" s="62" t="s">
+      <c r="C6" s="57"/>
+      <c r="D6" s="57"/>
+      <c r="E6" s="58" t="s">
         <v>8</v>
       </c>
-      <c r="F6" s="63"/>
-      <c r="G6" s="62" t="s">
+      <c r="F6" s="59"/>
+      <c r="G6" s="58" t="s">
         <v>15</v>
       </c>
-      <c r="H6" s="63">
+      <c r="H6" s="59">
         <v>44300</v>
       </c>
-      <c r="I6" s="62" t="s">
+      <c r="I6" s="58" t="s">
         <v>8</v>
       </c>
-      <c r="J6" s="63">
+      <c r="J6" s="59">
         <v>44300</v>
       </c>
-      <c r="K6" s="62" t="s">
+      <c r="K6" s="58" t="s">
         <v>15</v>
       </c>
-      <c r="L6" s="63">
+      <c r="L6" s="59">
         <v>44301</v>
       </c>
-      <c r="M6" s="62" t="s">
+      <c r="M6" s="58" t="s">
         <v>6</v>
       </c>
-      <c r="N6" s="63">
+      <c r="N6" s="59">
         <v>44331</v>
       </c>
-      <c r="O6" s="67">
+      <c r="O6" s="63">
         <v>44302</v>
       </c>
-      <c r="P6" s="53">
+      <c r="P6" s="49">
         <v>44298</v>
       </c>
-      <c r="Q6" s="47">
+      <c r="Q6" s="43">
         <v>44302</v>
       </c>
       <c r="R6">
@@ -1859,42 +1879,42 @@
       </c>
     </row>
     <row r="7" spans="2:19" ht="26.25" customHeight="1">
-      <c r="B7" s="60" t="s">
+      <c r="B7" s="56" t="s">
         <v>11</v>
       </c>
-      <c r="C7" s="61"/>
-      <c r="D7" s="61"/>
-      <c r="E7" s="62" t="s">
+      <c r="C7" s="57"/>
+      <c r="D7" s="57"/>
+      <c r="E7" s="58" t="s">
         <v>6</v>
       </c>
-      <c r="F7" s="64"/>
-      <c r="G7" s="62" t="s">
+      <c r="F7" s="60"/>
+      <c r="G7" s="58" t="s">
         <v>15</v>
       </c>
-      <c r="H7" s="63">
+      <c r="H7" s="59">
         <v>44309</v>
       </c>
-      <c r="I7" s="62" t="s">
+      <c r="I7" s="58" t="s">
         <v>6</v>
       </c>
-      <c r="J7" s="63">
+      <c r="J7" s="59">
         <v>44310</v>
       </c>
-      <c r="K7" s="62" t="s">
+      <c r="K7" s="58" t="s">
         <v>15</v>
       </c>
-      <c r="L7" s="63">
+      <c r="L7" s="59">
         <v>44312</v>
       </c>
-      <c r="M7" s="62"/>
-      <c r="N7" s="64"/>
-      <c r="O7" s="67">
+      <c r="M7" s="58"/>
+      <c r="N7" s="60"/>
+      <c r="O7" s="63">
         <v>44316</v>
       </c>
-      <c r="P7" s="53">
+      <c r="P7" s="49">
         <v>44305</v>
       </c>
-      <c r="Q7" s="47">
+      <c r="Q7" s="43">
         <v>44316</v>
       </c>
       <c r="R7">
@@ -1903,42 +1923,42 @@
       </c>
     </row>
     <row r="8" spans="2:19" ht="26.25" customHeight="1">
-      <c r="B8" s="60" t="s">
+      <c r="B8" s="56" t="s">
         <v>12</v>
       </c>
-      <c r="C8" s="61"/>
-      <c r="D8" s="61"/>
-      <c r="E8" s="69" t="s">
+      <c r="C8" s="57"/>
+      <c r="D8" s="57"/>
+      <c r="E8" s="65" t="s">
         <v>6</v>
       </c>
-      <c r="F8" s="64"/>
-      <c r="G8" s="62" t="s">
+      <c r="F8" s="60"/>
+      <c r="G8" s="58" t="s">
         <v>15</v>
       </c>
-      <c r="H8" s="64"/>
-      <c r="I8" s="62" t="s">
+      <c r="H8" s="60"/>
+      <c r="I8" s="58" t="s">
         <v>6</v>
       </c>
-      <c r="J8" s="64"/>
-      <c r="K8" s="62" t="s">
+      <c r="J8" s="60"/>
+      <c r="K8" s="58" t="s">
         <v>15</v>
       </c>
-      <c r="L8" s="63">
+      <c r="L8" s="59">
         <v>44332</v>
       </c>
-      <c r="M8" s="70" t="s">
+      <c r="M8" s="66" t="s">
         <v>8</v>
       </c>
-      <c r="N8" s="63">
+      <c r="N8" s="59">
         <v>44339</v>
       </c>
-      <c r="O8" s="67">
+      <c r="O8" s="63">
         <v>44339</v>
       </c>
-      <c r="P8" s="48">
+      <c r="P8" s="44">
         <v>44312</v>
       </c>
-      <c r="Q8" s="47">
+      <c r="Q8" s="43">
         <v>44337</v>
       </c>
       <c r="R8">
@@ -1947,36 +1967,36 @@
       </c>
     </row>
     <row r="9" spans="2:19" ht="26.25" customHeight="1">
-      <c r="B9" s="60" t="s">
+      <c r="B9" s="56" t="s">
         <v>13</v>
       </c>
-      <c r="C9" s="61"/>
-      <c r="D9" s="61"/>
-      <c r="E9" s="62" t="s">
+      <c r="C9" s="57"/>
+      <c r="D9" s="57"/>
+      <c r="E9" s="58" t="s">
         <v>8</v>
       </c>
-      <c r="F9" s="63">
+      <c r="F9" s="59">
         <v>44312</v>
       </c>
-      <c r="G9" s="62" t="s">
+      <c r="G9" s="58" t="s">
         <v>15</v>
       </c>
-      <c r="H9" s="64"/>
-      <c r="I9" s="62" t="s">
+      <c r="H9" s="60"/>
+      <c r="I9" s="58" t="s">
         <v>8</v>
       </c>
-      <c r="J9" s="64"/>
-      <c r="K9" s="62"/>
-      <c r="L9" s="64"/>
-      <c r="M9" s="62"/>
-      <c r="N9" s="64"/>
-      <c r="O9" s="67">
+      <c r="J9" s="60"/>
+      <c r="K9" s="58"/>
+      <c r="L9" s="60"/>
+      <c r="M9" s="58"/>
+      <c r="N9" s="60"/>
+      <c r="O9" s="63">
         <v>44319</v>
       </c>
-      <c r="P9" s="48">
+      <c r="P9" s="44">
         <v>44312</v>
       </c>
-      <c r="Q9" s="47">
+      <c r="Q9" s="43">
         <v>44319</v>
       </c>
       <c r="R9">
@@ -1985,46 +2005,46 @@
       </c>
     </row>
     <row r="10" spans="2:19" ht="26.25" customHeight="1">
-      <c r="B10" s="83" t="s">
+      <c r="B10" s="74" t="s">
         <v>14</v>
       </c>
-      <c r="C10" s="84"/>
-      <c r="D10" s="84"/>
-      <c r="E10" s="85" t="s">
+      <c r="C10" s="75"/>
+      <c r="D10" s="75"/>
+      <c r="E10" s="76" t="s">
         <v>8</v>
       </c>
-      <c r="F10" s="86">
+      <c r="F10" s="77">
         <v>44333</v>
       </c>
-      <c r="G10" s="85" t="s">
+      <c r="G10" s="76" t="s">
         <v>15</v>
       </c>
-      <c r="H10" s="86">
+      <c r="H10" s="77">
         <v>44346</v>
       </c>
-      <c r="I10" s="85" t="s">
+      <c r="I10" s="76" t="s">
         <v>8</v>
       </c>
-      <c r="J10" s="86">
+      <c r="J10" s="77">
         <v>44369</v>
       </c>
-      <c r="K10" s="85" t="s">
+      <c r="K10" s="76" t="s">
         <v>6</v>
       </c>
-      <c r="L10" s="86">
+      <c r="L10" s="77">
         <v>44380</v>
       </c>
-      <c r="M10" s="85" t="s">
+      <c r="M10" s="76" t="s">
         <v>15</v>
       </c>
-      <c r="N10" s="42"/>
-      <c r="O10" s="78">
+      <c r="N10" s="40"/>
+      <c r="O10" s="69">
         <v>44382</v>
       </c>
-      <c r="P10" s="48">
+      <c r="P10" s="44">
         <v>44319</v>
       </c>
-      <c r="Q10" s="47">
+      <c r="Q10" s="43">
         <v>44382</v>
       </c>
       <c r="R10">
@@ -2033,148 +2053,159 @@
       </c>
     </row>
     <row r="11" spans="2:19" ht="26.25" customHeight="1">
-      <c r="B11" s="75" t="s">
+      <c r="B11" s="80" t="s">
         <v>170</v>
       </c>
-      <c r="D11" s="2"/>
-      <c r="E11" s="74" t="s">
+      <c r="C11" s="81"/>
+      <c r="D11" s="81"/>
+      <c r="E11" s="82" t="s">
         <v>15</v>
       </c>
-      <c r="F11" s="40">
+      <c r="F11" s="83">
         <v>44362</v>
       </c>
-      <c r="G11" s="41" t="s">
+      <c r="G11" s="82" t="s">
         <v>8</v>
       </c>
-      <c r="H11" s="40">
+      <c r="H11" s="83">
         <v>44369</v>
       </c>
-      <c r="I11" s="41" t="s">
+      <c r="I11" s="82" t="s">
         <v>15</v>
       </c>
-      <c r="J11" s="40">
+      <c r="J11" s="83">
         <v>44378</v>
       </c>
-      <c r="K11" s="66" t="s">
+      <c r="K11" s="84" t="s">
         <v>6</v>
       </c>
-      <c r="L11" s="40">
+      <c r="L11" s="83">
         <v>44386</v>
       </c>
-      <c r="M11" s="43"/>
-      <c r="N11" s="42"/>
-      <c r="O11" s="27"/>
-      <c r="P11" s="48">
+      <c r="M11" s="82"/>
+      <c r="N11" s="85"/>
+      <c r="O11" s="69">
+        <v>44389</v>
+      </c>
+      <c r="P11" s="44">
         <v>44340</v>
       </c>
-      <c r="Q11" s="47">
-        <v>44396</v>
+      <c r="Q11" s="43">
+        <v>44389</v>
       </c>
       <c r="R11">
         <f t="shared" si="0"/>
-        <v>56</v>
+        <v>49</v>
       </c>
     </row>
     <row r="12" spans="2:19" ht="26.25" customHeight="1">
-      <c r="B12" s="75" t="s">
+      <c r="B12" s="80" t="s">
         <v>174</v>
       </c>
-      <c r="D12" s="2"/>
-      <c r="E12" s="74" t="s">
+      <c r="C12" s="81"/>
+      <c r="D12" s="81"/>
+      <c r="E12" s="82" t="s">
         <v>15</v>
       </c>
-      <c r="F12" s="40">
+      <c r="F12" s="83">
         <v>44362</v>
       </c>
-      <c r="G12" s="41" t="s">
+      <c r="G12" s="82" t="s">
         <v>8</v>
       </c>
-      <c r="H12" s="40">
+      <c r="H12" s="83">
         <v>44375</v>
       </c>
-      <c r="I12" s="41" t="s">
+      <c r="I12" s="82" t="s">
         <v>172</v>
       </c>
-      <c r="J12" s="40">
+      <c r="J12" s="83">
         <v>44378</v>
       </c>
-      <c r="K12" s="66" t="s">
+      <c r="K12" s="84" t="s">
         <v>6</v>
       </c>
-      <c r="L12" s="40">
+      <c r="L12" s="83">
         <v>44386</v>
       </c>
-      <c r="M12" s="43"/>
-      <c r="N12" s="42"/>
-      <c r="O12" s="27"/>
-      <c r="P12" s="48"/>
-      <c r="Q12" s="47"/>
+      <c r="M12" s="82"/>
+      <c r="N12" s="85"/>
+      <c r="O12" s="69">
+        <v>44389</v>
+      </c>
+      <c r="P12" s="44"/>
+      <c r="Q12" s="43"/>
     </row>
     <row r="13" spans="2:19" ht="26.25" customHeight="1">
-      <c r="B13" s="75" t="s">
+      <c r="B13" s="80" t="s">
         <v>173</v>
       </c>
-      <c r="D13" s="2"/>
-      <c r="E13" s="74" t="s">
+      <c r="C13" s="81"/>
+      <c r="D13" s="81"/>
+      <c r="E13" s="82" t="s">
         <v>15</v>
       </c>
-      <c r="F13" s="40">
+      <c r="F13" s="83">
         <v>44376</v>
       </c>
-      <c r="G13" s="66" t="s">
+      <c r="G13" s="84" t="s">
         <v>8</v>
       </c>
-      <c r="H13" s="40">
+      <c r="H13" s="83">
         <v>44382</v>
       </c>
-      <c r="I13" s="41" t="s">
+      <c r="I13" s="82" t="s">
         <v>15</v>
       </c>
-      <c r="J13" s="40">
+      <c r="J13" s="83">
         <v>44383</v>
       </c>
-      <c r="K13" s="66" t="s">
+      <c r="K13" s="84" t="s">
         <v>6</v>
       </c>
-      <c r="L13" s="42"/>
-      <c r="M13" s="43"/>
-      <c r="N13" s="42"/>
-      <c r="O13" s="27"/>
-      <c r="P13" s="48"/>
-      <c r="Q13" s="47"/>
+      <c r="L13" s="83">
+        <v>44387</v>
+      </c>
+      <c r="M13" s="82"/>
+      <c r="N13" s="85"/>
+      <c r="O13" s="69">
+        <v>44389</v>
+      </c>
+      <c r="P13" s="44"/>
+      <c r="Q13" s="43"/>
     </row>
     <row r="14" spans="2:19" ht="26.25" customHeight="1">
       <c r="B14" s="1" t="s">
         <v>16</v>
       </c>
       <c r="D14" s="2"/>
-      <c r="E14" s="74" t="s">
+      <c r="E14" s="68" t="s">
         <v>8</v>
       </c>
-      <c r="F14" s="40">
+      <c r="F14" s="38">
         <v>44354</v>
       </c>
-      <c r="G14" s="41" t="s">
+      <c r="G14" s="39" t="s">
         <v>15</v>
       </c>
-      <c r="H14" s="40">
+      <c r="H14" s="38">
         <v>44381</v>
       </c>
-      <c r="I14" s="66" t="s">
+      <c r="I14" s="62" t="s">
         <v>8</v>
       </c>
-      <c r="J14" s="42"/>
-      <c r="K14" s="82" t="s">
+      <c r="J14" s="40"/>
+      <c r="K14" s="73" t="s">
         <v>6</v>
       </c>
-      <c r="L14" s="42"/>
-      <c r="M14" s="43"/>
-      <c r="N14" s="42"/>
+      <c r="L14" s="40"/>
+      <c r="M14" s="41"/>
+      <c r="N14" s="40"/>
       <c r="O14" s="27"/>
-      <c r="P14" s="48">
+      <c r="P14" s="44">
         <v>44354</v>
       </c>
-      <c r="Q14" s="47">
+      <c r="Q14" s="43">
         <v>44396</v>
       </c>
       <c r="R14">
@@ -2183,48 +2214,48 @@
       </c>
     </row>
     <row r="15" spans="2:19" ht="26.25" customHeight="1">
-      <c r="B15" s="83" t="s">
+      <c r="B15" s="74" t="s">
         <v>17</v>
       </c>
-      <c r="C15" s="84"/>
-      <c r="D15" s="84"/>
-      <c r="E15" s="85" t="s">
+      <c r="C15" s="75"/>
+      <c r="D15" s="75"/>
+      <c r="E15" s="76" t="s">
         <v>6</v>
       </c>
-      <c r="F15" s="86">
+      <c r="F15" s="77">
         <v>44332</v>
       </c>
-      <c r="G15" s="85" t="s">
+      <c r="G15" s="76" t="s">
         <v>15</v>
       </c>
-      <c r="H15" s="86">
+      <c r="H15" s="77">
         <v>44333</v>
       </c>
-      <c r="I15" s="85" t="s">
+      <c r="I15" s="76" t="s">
         <v>6</v>
       </c>
-      <c r="J15" s="86">
+      <c r="J15" s="77">
         <v>44337</v>
       </c>
-      <c r="K15" s="85" t="s">
+      <c r="K15" s="76" t="s">
         <v>15</v>
       </c>
-      <c r="L15" s="86">
+      <c r="L15" s="77">
         <v>44339</v>
       </c>
-      <c r="M15" s="85" t="s">
+      <c r="M15" s="76" t="s">
         <v>8</v>
       </c>
-      <c r="N15" s="86">
+      <c r="N15" s="77">
         <v>44354</v>
       </c>
-      <c r="O15" s="78">
+      <c r="O15" s="69">
         <v>44381</v>
       </c>
-      <c r="P15" s="48">
+      <c r="P15" s="44">
         <v>44361</v>
       </c>
-      <c r="Q15" s="47">
+      <c r="Q15" s="43">
         <v>44381</v>
       </c>
       <c r="R15">
@@ -2233,44 +2264,46 @@
       </c>
     </row>
     <row r="16" spans="2:19" ht="26.25" customHeight="1" thickBot="1">
-      <c r="B16" s="36" t="s">
+      <c r="B16" s="86" t="s">
         <v>18</v>
       </c>
-      <c r="C16" s="37"/>
-      <c r="D16" s="37"/>
-      <c r="E16" s="72" t="s">
+      <c r="C16" s="87"/>
+      <c r="D16" s="87"/>
+      <c r="E16" s="88" t="s">
         <v>168</v>
       </c>
-      <c r="F16" s="73">
+      <c r="F16" s="89">
         <v>44346</v>
       </c>
-      <c r="G16" s="72" t="s">
+      <c r="G16" s="88" t="s">
         <v>6</v>
       </c>
-      <c r="H16" s="76" t="s">
+      <c r="H16" s="90" t="s">
         <v>171</v>
       </c>
-      <c r="I16" s="72" t="s">
+      <c r="I16" s="88" t="s">
         <v>8</v>
       </c>
-      <c r="J16" s="73">
+      <c r="J16" s="89">
         <v>44382</v>
       </c>
-      <c r="K16" s="72" t="s">
+      <c r="K16" s="88" t="s">
         <v>15</v>
       </c>
-      <c r="L16" s="73">
+      <c r="L16" s="89">
         <v>44383</v>
       </c>
-      <c r="M16" s="77" t="s">
+      <c r="M16" s="91" t="s">
         <v>168</v>
       </c>
-      <c r="N16" s="44"/>
-      <c r="O16" s="45"/>
-      <c r="P16" s="49">
+      <c r="N16" s="90"/>
+      <c r="O16" s="69">
+        <v>44389</v>
+      </c>
+      <c r="P16" s="45">
         <v>44368</v>
       </c>
-      <c r="Q16" s="47">
+      <c r="Q16" s="43">
         <v>44383</v>
       </c>
       <c r="R16">
@@ -2279,1593 +2312,1593 @@
       </c>
     </row>
     <row r="17" spans="5:18" ht="15.75" customHeight="1" thickTop="1">
-      <c r="E17" s="38"/>
-      <c r="F17" s="38"/>
-      <c r="G17" s="38"/>
-      <c r="H17" s="38"/>
-      <c r="I17" s="38"/>
-      <c r="J17" s="38"/>
-      <c r="K17" s="38"/>
-      <c r="L17" s="38"/>
-      <c r="M17" s="38"/>
-      <c r="N17" s="79" t="s">
+      <c r="E17" s="36"/>
+      <c r="F17" s="36"/>
+      <c r="G17" s="36"/>
+      <c r="H17" s="36"/>
+      <c r="I17" s="36"/>
+      <c r="J17" s="36"/>
+      <c r="K17" s="36"/>
+      <c r="L17" s="36"/>
+      <c r="M17" s="36"/>
+      <c r="N17" s="70" t="s">
         <v>176</v>
       </c>
-      <c r="P17" s="80">
+      <c r="P17" s="71">
         <v>44375</v>
       </c>
-      <c r="Q17" s="81">
+      <c r="Q17" s="72">
         <v>44396</v>
       </c>
-      <c r="R17" s="55">
+      <c r="R17" s="51">
         <f>Q17-P17</f>
         <v>21</v>
       </c>
     </row>
     <row r="18" spans="5:18" ht="15.75" customHeight="1">
-      <c r="E18" s="39"/>
-      <c r="F18" s="39"/>
-      <c r="G18" s="39"/>
-      <c r="H18" s="39"/>
-      <c r="I18" s="39"/>
-      <c r="J18" s="39"/>
-      <c r="K18" s="39"/>
-      <c r="L18" s="39"/>
-      <c r="M18" s="39"/>
-      <c r="N18" s="39"/>
+      <c r="E18" s="37"/>
+      <c r="F18" s="37"/>
+      <c r="G18" s="37"/>
+      <c r="H18" s="37"/>
+      <c r="I18" s="37"/>
+      <c r="J18" s="37"/>
+      <c r="K18" s="37"/>
+      <c r="L18" s="37"/>
+      <c r="M18" s="37"/>
+      <c r="N18" s="37"/>
     </row>
     <row r="19" spans="5:18" ht="15.75" customHeight="1">
-      <c r="E19" s="46" t="s">
+      <c r="E19" s="42" t="s">
         <v>116</v>
       </c>
-      <c r="F19" s="39"/>
-      <c r="G19" s="39"/>
-      <c r="H19" s="39"/>
-      <c r="I19" s="39"/>
-      <c r="J19" s="39"/>
-      <c r="K19" s="39"/>
-      <c r="L19" s="39"/>
-      <c r="M19" s="39"/>
-      <c r="O19" s="50" t="s">
+      <c r="F19" s="37"/>
+      <c r="G19" s="37"/>
+      <c r="H19" s="37"/>
+      <c r="I19" s="37"/>
+      <c r="J19" s="37"/>
+      <c r="K19" s="37"/>
+      <c r="L19" s="37"/>
+      <c r="M19" s="37"/>
+      <c r="O19" s="46" t="s">
         <v>125</v>
       </c>
     </row>
     <row r="20" spans="5:18" ht="15.75" customHeight="1">
-      <c r="E20" s="46" t="s">
+      <c r="E20" s="42" t="s">
         <v>117</v>
       </c>
-      <c r="F20" s="39"/>
-      <c r="G20" s="39"/>
-      <c r="H20" s="39"/>
-      <c r="I20" s="39"/>
-      <c r="J20" s="39"/>
-      <c r="K20" s="39"/>
-      <c r="L20" s="39"/>
-      <c r="M20" s="39"/>
-      <c r="O20" s="46" t="s">
+      <c r="F20" s="37"/>
+      <c r="G20" s="37"/>
+      <c r="H20" s="37"/>
+      <c r="I20" s="37"/>
+      <c r="J20" s="37"/>
+      <c r="K20" s="37"/>
+      <c r="L20" s="37"/>
+      <c r="M20" s="37"/>
+      <c r="O20" s="42" t="s">
         <v>126</v>
       </c>
     </row>
     <row r="21" spans="5:18" ht="15.75" customHeight="1">
-      <c r="E21" s="46" t="s">
+      <c r="E21" s="42" t="s">
         <v>118</v>
       </c>
-      <c r="F21" s="39"/>
-      <c r="G21" s="39"/>
-      <c r="H21" s="39"/>
-      <c r="I21" s="39"/>
-      <c r="J21" s="39"/>
-      <c r="K21" s="39"/>
-      <c r="L21" s="39"/>
-      <c r="M21" s="39"/>
-      <c r="N21" s="51"/>
+      <c r="F21" s="37"/>
+      <c r="G21" s="37"/>
+      <c r="H21" s="37"/>
+      <c r="I21" s="37"/>
+      <c r="J21" s="37"/>
+      <c r="K21" s="37"/>
+      <c r="L21" s="37"/>
+      <c r="M21" s="37"/>
+      <c r="N21" s="47"/>
       <c r="O21" s="27"/>
     </row>
     <row r="22" spans="5:18" ht="15.75" customHeight="1">
-      <c r="E22" s="46" t="s">
+      <c r="E22" s="42" t="s">
         <v>119</v>
       </c>
-      <c r="F22" s="39"/>
-      <c r="G22" s="39"/>
-      <c r="H22" s="39"/>
-      <c r="I22" s="39"/>
-      <c r="J22" s="39"/>
-      <c r="K22" s="39"/>
-      <c r="L22" s="39"/>
-      <c r="M22" s="39"/>
-      <c r="N22" s="51"/>
+      <c r="F22" s="37"/>
+      <c r="G22" s="37"/>
+      <c r="H22" s="37"/>
+      <c r="I22" s="37"/>
+      <c r="J22" s="37"/>
+      <c r="K22" s="37"/>
+      <c r="L22" s="37"/>
+      <c r="M22" s="37"/>
+      <c r="N22" s="47"/>
       <c r="O22" s="27"/>
-      <c r="P22" s="52"/>
+      <c r="P22" s="48"/>
     </row>
     <row r="23" spans="5:18" ht="15.75" customHeight="1">
-      <c r="F23" s="39"/>
-      <c r="G23" s="39"/>
-      <c r="H23" s="39"/>
-      <c r="I23" s="39"/>
-      <c r="J23" s="39"/>
-      <c r="K23" s="39"/>
-      <c r="L23" s="39"/>
-      <c r="M23" s="39"/>
-      <c r="N23" s="51"/>
+      <c r="F23" s="37"/>
+      <c r="G23" s="37"/>
+      <c r="H23" s="37"/>
+      <c r="I23" s="37"/>
+      <c r="J23" s="37"/>
+      <c r="K23" s="37"/>
+      <c r="L23" s="37"/>
+      <c r="M23" s="37"/>
+      <c r="N23" s="47"/>
       <c r="O23" s="27"/>
     </row>
     <row r="24" spans="5:18" ht="15.75" customHeight="1">
-      <c r="E24" s="46"/>
-      <c r="F24" s="39"/>
-      <c r="G24" s="39"/>
-      <c r="H24" s="39"/>
-      <c r="I24" s="39"/>
-      <c r="J24" s="39"/>
-      <c r="K24" s="39"/>
-      <c r="L24" s="39"/>
-      <c r="M24" s="39"/>
-      <c r="N24" s="51"/>
+      <c r="E24" s="42"/>
+      <c r="F24" s="37"/>
+      <c r="G24" s="37"/>
+      <c r="H24" s="37"/>
+      <c r="I24" s="37"/>
+      <c r="J24" s="37"/>
+      <c r="K24" s="37"/>
+      <c r="L24" s="37"/>
+      <c r="M24" s="37"/>
+      <c r="N24" s="47"/>
       <c r="O24" s="27"/>
     </row>
     <row r="25" spans="5:18" ht="15.75" customHeight="1">
-      <c r="E25" s="46"/>
-      <c r="F25" s="39"/>
-      <c r="G25" s="39"/>
-      <c r="H25" s="39"/>
-      <c r="I25" s="39"/>
-      <c r="J25" s="39"/>
-      <c r="K25" s="39"/>
-      <c r="L25" s="39"/>
-      <c r="M25" s="39"/>
-      <c r="N25" s="51"/>
+      <c r="E25" s="42"/>
+      <c r="F25" s="37"/>
+      <c r="G25" s="37"/>
+      <c r="H25" s="37"/>
+      <c r="I25" s="37"/>
+      <c r="J25" s="37"/>
+      <c r="K25" s="37"/>
+      <c r="L25" s="37"/>
+      <c r="M25" s="37"/>
+      <c r="N25" s="47"/>
       <c r="O25" s="27"/>
     </row>
     <row r="26" spans="5:18" ht="15.75" customHeight="1">
-      <c r="E26" s="39"/>
-      <c r="F26" s="39"/>
-      <c r="G26" s="39"/>
-      <c r="H26" s="39"/>
-      <c r="I26" s="39"/>
-      <c r="J26" s="39"/>
-      <c r="K26" s="39"/>
-      <c r="L26" s="39"/>
-      <c r="M26" s="39"/>
-      <c r="N26" s="51"/>
+      <c r="E26" s="37"/>
+      <c r="F26" s="37"/>
+      <c r="G26" s="37"/>
+      <c r="H26" s="37"/>
+      <c r="I26" s="37"/>
+      <c r="J26" s="37"/>
+      <c r="K26" s="37"/>
+      <c r="L26" s="37"/>
+      <c r="M26" s="37"/>
+      <c r="N26" s="47"/>
       <c r="O26" s="27"/>
     </row>
     <row r="27" spans="5:18" ht="15.75" customHeight="1">
-      <c r="E27" s="39" t="s">
+      <c r="E27" s="37" t="s">
         <v>124</v>
       </c>
-      <c r="F27" s="39"/>
-      <c r="G27" s="39"/>
-      <c r="H27" s="39"/>
-      <c r="I27" s="39"/>
-      <c r="J27" s="39"/>
-      <c r="K27" s="39"/>
-      <c r="L27" s="39"/>
-      <c r="M27" s="39"/>
-      <c r="N27" s="51"/>
+      <c r="F27" s="37"/>
+      <c r="G27" s="37"/>
+      <c r="H27" s="37"/>
+      <c r="I27" s="37"/>
+      <c r="J27" s="37"/>
+      <c r="K27" s="37"/>
+      <c r="L27" s="37"/>
+      <c r="M27" s="37"/>
+      <c r="N27" s="47"/>
       <c r="O27" s="27"/>
     </row>
     <row r="28" spans="5:18" ht="15.75" customHeight="1">
-      <c r="E28" s="39"/>
-      <c r="F28" s="39"/>
-      <c r="G28" s="39"/>
-      <c r="H28" s="39"/>
-      <c r="I28" s="39"/>
-      <c r="J28" s="39"/>
-      <c r="K28" s="39"/>
-      <c r="L28" s="39"/>
-      <c r="M28" s="39"/>
-      <c r="N28" s="51"/>
+      <c r="E28" s="37"/>
+      <c r="F28" s="37"/>
+      <c r="G28" s="37"/>
+      <c r="H28" s="37"/>
+      <c r="I28" s="37"/>
+      <c r="J28" s="37"/>
+      <c r="K28" s="37"/>
+      <c r="L28" s="37"/>
+      <c r="M28" s="37"/>
+      <c r="N28" s="47"/>
       <c r="O28" s="27"/>
     </row>
     <row r="29" spans="5:18" ht="15.75" customHeight="1">
-      <c r="E29" s="39"/>
-      <c r="F29" s="39"/>
-      <c r="G29" s="39"/>
-      <c r="H29" s="39"/>
-      <c r="I29" s="39"/>
-      <c r="J29" s="39"/>
-      <c r="K29" s="39"/>
-      <c r="L29" s="39"/>
-      <c r="M29" s="39"/>
-      <c r="N29" s="51"/>
+      <c r="E29" s="37"/>
+      <c r="F29" s="37"/>
+      <c r="G29" s="37"/>
+      <c r="H29" s="37"/>
+      <c r="I29" s="37"/>
+      <c r="J29" s="37"/>
+      <c r="K29" s="37"/>
+      <c r="L29" s="37"/>
+      <c r="M29" s="37"/>
+      <c r="N29" s="47"/>
       <c r="O29" s="27"/>
     </row>
     <row r="30" spans="5:18" ht="15.75" customHeight="1">
-      <c r="E30" s="39"/>
-      <c r="F30" s="39"/>
-      <c r="G30" s="39"/>
-      <c r="H30" s="39"/>
-      <c r="I30" s="39"/>
-      <c r="J30" s="39"/>
-      <c r="K30" s="39"/>
-      <c r="L30" s="39"/>
-      <c r="M30" s="39"/>
-      <c r="N30" s="51"/>
+      <c r="E30" s="37"/>
+      <c r="F30" s="37"/>
+      <c r="G30" s="37"/>
+      <c r="H30" s="37"/>
+      <c r="I30" s="37"/>
+      <c r="J30" s="37"/>
+      <c r="K30" s="37"/>
+      <c r="L30" s="37"/>
+      <c r="M30" s="37"/>
+      <c r="N30" s="47"/>
       <c r="O30" s="27"/>
     </row>
     <row r="31" spans="5:18" ht="15.75" customHeight="1">
-      <c r="E31" s="39"/>
-      <c r="F31" s="39"/>
-      <c r="G31" s="39"/>
-      <c r="H31" s="39"/>
-      <c r="I31" s="39"/>
-      <c r="J31" s="39"/>
-      <c r="K31" s="39"/>
-      <c r="L31" s="39"/>
-      <c r="M31" s="39"/>
-      <c r="N31" s="51"/>
+      <c r="E31" s="37"/>
+      <c r="F31" s="37"/>
+      <c r="G31" s="37"/>
+      <c r="H31" s="37"/>
+      <c r="I31" s="37"/>
+      <c r="J31" s="37"/>
+      <c r="K31" s="37"/>
+      <c r="L31" s="37"/>
+      <c r="M31" s="37"/>
+      <c r="N31" s="47"/>
       <c r="O31" s="27"/>
     </row>
     <row r="32" spans="5:18" ht="15.75" customHeight="1">
-      <c r="E32" s="39"/>
-      <c r="F32" s="39"/>
-      <c r="G32" s="39"/>
-      <c r="H32" s="39"/>
-      <c r="I32" s="39"/>
-      <c r="J32" s="39"/>
-      <c r="K32" s="39"/>
-      <c r="L32" s="39"/>
-      <c r="M32" s="39"/>
-      <c r="N32" s="51"/>
+      <c r="E32" s="37"/>
+      <c r="F32" s="37"/>
+      <c r="G32" s="37"/>
+      <c r="H32" s="37"/>
+      <c r="I32" s="37"/>
+      <c r="J32" s="37"/>
+      <c r="K32" s="37"/>
+      <c r="L32" s="37"/>
+      <c r="M32" s="37"/>
+      <c r="N32" s="47"/>
       <c r="O32" s="27"/>
     </row>
     <row r="33" spans="5:15" ht="15.75" customHeight="1">
-      <c r="E33" s="39"/>
-      <c r="F33" s="39"/>
-      <c r="G33" s="39"/>
-      <c r="H33" s="39"/>
-      <c r="I33" s="39"/>
-      <c r="J33" s="39"/>
-      <c r="K33" s="39"/>
-      <c r="L33" s="39"/>
-      <c r="M33" s="39"/>
-      <c r="N33" s="51"/>
+      <c r="E33" s="37"/>
+      <c r="F33" s="37"/>
+      <c r="G33" s="37"/>
+      <c r="H33" s="37"/>
+      <c r="I33" s="37"/>
+      <c r="J33" s="37"/>
+      <c r="K33" s="37"/>
+      <c r="L33" s="37"/>
+      <c r="M33" s="37"/>
+      <c r="N33" s="47"/>
       <c r="O33" s="27"/>
     </row>
     <row r="34" spans="5:15" ht="15.75" customHeight="1">
-      <c r="E34" s="39"/>
-      <c r="F34" s="39"/>
-      <c r="G34" s="39"/>
-      <c r="H34" s="39"/>
-      <c r="I34" s="39"/>
-      <c r="J34" s="39"/>
-      <c r="K34" s="39"/>
-      <c r="L34" s="39"/>
-      <c r="M34" s="39"/>
-      <c r="N34" s="51"/>
+      <c r="E34" s="37"/>
+      <c r="F34" s="37"/>
+      <c r="G34" s="37"/>
+      <c r="H34" s="37"/>
+      <c r="I34" s="37"/>
+      <c r="J34" s="37"/>
+      <c r="K34" s="37"/>
+      <c r="L34" s="37"/>
+      <c r="M34" s="37"/>
+      <c r="N34" s="47"/>
       <c r="O34" s="27"/>
     </row>
     <row r="35" spans="5:15" ht="15.75" customHeight="1">
-      <c r="E35" s="39"/>
-      <c r="F35" s="39"/>
-      <c r="G35" s="39"/>
-      <c r="H35" s="39"/>
-      <c r="I35" s="39"/>
-      <c r="J35" s="39"/>
-      <c r="K35" s="39"/>
-      <c r="L35" s="39"/>
-      <c r="M35" s="39"/>
-      <c r="N35" s="51"/>
+      <c r="E35" s="37"/>
+      <c r="F35" s="37"/>
+      <c r="G35" s="37"/>
+      <c r="H35" s="37"/>
+      <c r="I35" s="37"/>
+      <c r="J35" s="37"/>
+      <c r="K35" s="37"/>
+      <c r="L35" s="37"/>
+      <c r="M35" s="37"/>
+      <c r="N35" s="47"/>
       <c r="O35" s="27"/>
     </row>
     <row r="36" spans="5:15" ht="15.75" customHeight="1">
-      <c r="E36" s="39"/>
-      <c r="F36" s="39"/>
-      <c r="G36" s="39"/>
-      <c r="H36" s="39"/>
-      <c r="I36" s="39"/>
-      <c r="J36" s="39"/>
-      <c r="K36" s="39"/>
-      <c r="L36" s="39"/>
-      <c r="M36" s="39"/>
-      <c r="N36" s="39"/>
+      <c r="E36" s="37"/>
+      <c r="F36" s="37"/>
+      <c r="G36" s="37"/>
+      <c r="H36" s="37"/>
+      <c r="I36" s="37"/>
+      <c r="J36" s="37"/>
+      <c r="K36" s="37"/>
+      <c r="L36" s="37"/>
+      <c r="M36" s="37"/>
+      <c r="N36" s="37"/>
     </row>
     <row r="37" spans="5:15" ht="15.75" customHeight="1">
-      <c r="E37" s="39"/>
-      <c r="F37" s="39"/>
-      <c r="G37" s="39"/>
-      <c r="H37" s="39"/>
-      <c r="I37" s="39"/>
-      <c r="J37" s="39"/>
-      <c r="K37" s="39"/>
-      <c r="L37" s="39"/>
-      <c r="M37" s="39"/>
-      <c r="N37" s="39"/>
+      <c r="E37" s="37"/>
+      <c r="F37" s="37"/>
+      <c r="G37" s="37"/>
+      <c r="H37" s="37"/>
+      <c r="I37" s="37"/>
+      <c r="J37" s="37"/>
+      <c r="K37" s="37"/>
+      <c r="L37" s="37"/>
+      <c r="M37" s="37"/>
+      <c r="N37" s="37"/>
     </row>
     <row r="38" spans="5:15" ht="15.75" customHeight="1">
-      <c r="E38" s="39"/>
-      <c r="F38" s="39"/>
-      <c r="G38" s="39"/>
-      <c r="H38" s="39"/>
-      <c r="I38" s="39"/>
-      <c r="J38" s="39"/>
-      <c r="K38" s="39"/>
-      <c r="L38" s="39"/>
-      <c r="M38" s="39"/>
-      <c r="N38" s="39"/>
+      <c r="E38" s="37"/>
+      <c r="F38" s="37"/>
+      <c r="G38" s="37"/>
+      <c r="H38" s="37"/>
+      <c r="I38" s="37"/>
+      <c r="J38" s="37"/>
+      <c r="K38" s="37"/>
+      <c r="L38" s="37"/>
+      <c r="M38" s="37"/>
+      <c r="N38" s="37"/>
     </row>
     <row r="39" spans="5:15" ht="15.75" customHeight="1">
-      <c r="E39" s="39"/>
-      <c r="F39" s="39"/>
-      <c r="G39" s="39"/>
-      <c r="H39" s="39"/>
-      <c r="I39" s="39"/>
-      <c r="J39" s="39"/>
-      <c r="K39" s="39"/>
-      <c r="L39" s="39"/>
-      <c r="M39" s="39"/>
-      <c r="N39" s="39"/>
+      <c r="E39" s="37"/>
+      <c r="F39" s="37"/>
+      <c r="G39" s="37"/>
+      <c r="H39" s="37"/>
+      <c r="I39" s="37"/>
+      <c r="J39" s="37"/>
+      <c r="K39" s="37"/>
+      <c r="L39" s="37"/>
+      <c r="M39" s="37"/>
+      <c r="N39" s="37"/>
     </row>
     <row r="40" spans="5:15" ht="15.75" customHeight="1">
-      <c r="E40" s="39"/>
-      <c r="F40" s="39"/>
-      <c r="G40" s="39"/>
-      <c r="H40" s="39"/>
-      <c r="I40" s="39"/>
-      <c r="J40" s="39"/>
-      <c r="K40" s="39"/>
-      <c r="L40" s="39"/>
-      <c r="M40" s="39"/>
-      <c r="N40" s="39"/>
+      <c r="E40" s="37"/>
+      <c r="F40" s="37"/>
+      <c r="G40" s="37"/>
+      <c r="H40" s="37"/>
+      <c r="I40" s="37"/>
+      <c r="J40" s="37"/>
+      <c r="K40" s="37"/>
+      <c r="L40" s="37"/>
+      <c r="M40" s="37"/>
+      <c r="N40" s="37"/>
     </row>
     <row r="41" spans="5:15" ht="15.75" customHeight="1">
-      <c r="E41" s="39"/>
-      <c r="F41" s="39"/>
-      <c r="G41" s="39"/>
-      <c r="H41" s="39"/>
-      <c r="I41" s="39"/>
-      <c r="J41" s="39"/>
-      <c r="K41" s="39"/>
-      <c r="L41" s="39"/>
-      <c r="M41" s="39"/>
-      <c r="N41" s="39"/>
+      <c r="E41" s="37"/>
+      <c r="F41" s="37"/>
+      <c r="G41" s="37"/>
+      <c r="H41" s="37"/>
+      <c r="I41" s="37"/>
+      <c r="J41" s="37"/>
+      <c r="K41" s="37"/>
+      <c r="L41" s="37"/>
+      <c r="M41" s="37"/>
+      <c r="N41" s="37"/>
     </row>
     <row r="42" spans="5:15" ht="15.75" customHeight="1">
-      <c r="E42" s="39"/>
-      <c r="F42" s="39"/>
-      <c r="G42" s="39"/>
-      <c r="H42" s="39"/>
-      <c r="I42" s="39"/>
-      <c r="J42" s="39"/>
-      <c r="K42" s="39"/>
-      <c r="L42" s="39"/>
-      <c r="M42" s="39"/>
-      <c r="N42" s="39"/>
+      <c r="E42" s="37"/>
+      <c r="F42" s="37"/>
+      <c r="G42" s="37"/>
+      <c r="H42" s="37"/>
+      <c r="I42" s="37"/>
+      <c r="J42" s="37"/>
+      <c r="K42" s="37"/>
+      <c r="L42" s="37"/>
+      <c r="M42" s="37"/>
+      <c r="N42" s="37"/>
     </row>
     <row r="43" spans="5:15" ht="15.75" customHeight="1">
-      <c r="E43" s="39"/>
-      <c r="F43" s="39"/>
-      <c r="G43" s="39"/>
-      <c r="H43" s="39"/>
-      <c r="I43" s="39"/>
-      <c r="J43" s="39"/>
-      <c r="K43" s="39"/>
-      <c r="L43" s="39"/>
-      <c r="M43" s="39"/>
-      <c r="N43" s="39"/>
+      <c r="E43" s="37"/>
+      <c r="F43" s="37"/>
+      <c r="G43" s="37"/>
+      <c r="H43" s="37"/>
+      <c r="I43" s="37"/>
+      <c r="J43" s="37"/>
+      <c r="K43" s="37"/>
+      <c r="L43" s="37"/>
+      <c r="M43" s="37"/>
+      <c r="N43" s="37"/>
     </row>
     <row r="44" spans="5:15" ht="15.75" customHeight="1">
-      <c r="E44" s="39"/>
-      <c r="F44" s="39"/>
-      <c r="G44" s="39"/>
-      <c r="H44" s="39"/>
-      <c r="I44" s="39"/>
-      <c r="J44" s="39"/>
-      <c r="K44" s="39"/>
-      <c r="L44" s="39"/>
-      <c r="M44" s="39"/>
-      <c r="N44" s="39"/>
+      <c r="E44" s="37"/>
+      <c r="F44" s="37"/>
+      <c r="G44" s="37"/>
+      <c r="H44" s="37"/>
+      <c r="I44" s="37"/>
+      <c r="J44" s="37"/>
+      <c r="K44" s="37"/>
+      <c r="L44" s="37"/>
+      <c r="M44" s="37"/>
+      <c r="N44" s="37"/>
     </row>
     <row r="45" spans="5:15" ht="15.75" customHeight="1">
-      <c r="E45" s="39"/>
-      <c r="F45" s="39"/>
-      <c r="G45" s="39"/>
-      <c r="H45" s="39"/>
-      <c r="I45" s="39"/>
-      <c r="J45" s="39"/>
-      <c r="K45" s="39"/>
-      <c r="L45" s="39"/>
-      <c r="M45" s="39"/>
-      <c r="N45" s="39"/>
+      <c r="E45" s="37"/>
+      <c r="F45" s="37"/>
+      <c r="G45" s="37"/>
+      <c r="H45" s="37"/>
+      <c r="I45" s="37"/>
+      <c r="J45" s="37"/>
+      <c r="K45" s="37"/>
+      <c r="L45" s="37"/>
+      <c r="M45" s="37"/>
+      <c r="N45" s="37"/>
     </row>
     <row r="46" spans="5:15" ht="15.75" customHeight="1">
-      <c r="E46" s="39"/>
-      <c r="F46" s="39"/>
-      <c r="G46" s="39"/>
-      <c r="H46" s="39"/>
-      <c r="I46" s="39"/>
-      <c r="J46" s="39"/>
-      <c r="K46" s="39"/>
-      <c r="L46" s="39"/>
-      <c r="M46" s="39"/>
-      <c r="N46" s="39"/>
+      <c r="E46" s="37"/>
+      <c r="F46" s="37"/>
+      <c r="G46" s="37"/>
+      <c r="H46" s="37"/>
+      <c r="I46" s="37"/>
+      <c r="J46" s="37"/>
+      <c r="K46" s="37"/>
+      <c r="L46" s="37"/>
+      <c r="M46" s="37"/>
+      <c r="N46" s="37"/>
     </row>
     <row r="47" spans="5:15" ht="15.75" customHeight="1">
-      <c r="E47" s="39"/>
-      <c r="F47" s="39"/>
-      <c r="G47" s="39"/>
-      <c r="H47" s="39"/>
-      <c r="I47" s="39"/>
-      <c r="J47" s="39"/>
-      <c r="K47" s="39"/>
-      <c r="L47" s="39"/>
-      <c r="M47" s="39"/>
-      <c r="N47" s="39"/>
+      <c r="E47" s="37"/>
+      <c r="F47" s="37"/>
+      <c r="G47" s="37"/>
+      <c r="H47" s="37"/>
+      <c r="I47" s="37"/>
+      <c r="J47" s="37"/>
+      <c r="K47" s="37"/>
+      <c r="L47" s="37"/>
+      <c r="M47" s="37"/>
+      <c r="N47" s="37"/>
     </row>
     <row r="48" spans="5:15" ht="15.75" customHeight="1">
-      <c r="E48" s="39"/>
-      <c r="F48" s="39"/>
-      <c r="G48" s="39"/>
-      <c r="H48" s="39"/>
-      <c r="I48" s="39"/>
-      <c r="J48" s="39"/>
-      <c r="K48" s="39"/>
-      <c r="L48" s="39"/>
-      <c r="M48" s="39"/>
-      <c r="N48" s="39"/>
+      <c r="E48" s="37"/>
+      <c r="F48" s="37"/>
+      <c r="G48" s="37"/>
+      <c r="H48" s="37"/>
+      <c r="I48" s="37"/>
+      <c r="J48" s="37"/>
+      <c r="K48" s="37"/>
+      <c r="L48" s="37"/>
+      <c r="M48" s="37"/>
+      <c r="N48" s="37"/>
     </row>
     <row r="49" spans="5:14" ht="15.75" customHeight="1">
-      <c r="E49" s="39"/>
-      <c r="F49" s="39"/>
-      <c r="G49" s="39"/>
-      <c r="H49" s="39"/>
-      <c r="I49" s="39"/>
-      <c r="J49" s="39"/>
-      <c r="K49" s="39"/>
-      <c r="L49" s="39"/>
-      <c r="M49" s="39"/>
-      <c r="N49" s="39"/>
+      <c r="E49" s="37"/>
+      <c r="F49" s="37"/>
+      <c r="G49" s="37"/>
+      <c r="H49" s="37"/>
+      <c r="I49" s="37"/>
+      <c r="J49" s="37"/>
+      <c r="K49" s="37"/>
+      <c r="L49" s="37"/>
+      <c r="M49" s="37"/>
+      <c r="N49" s="37"/>
     </row>
     <row r="50" spans="5:14" ht="15.75" customHeight="1">
-      <c r="E50" s="39"/>
-      <c r="F50" s="39"/>
-      <c r="G50" s="39"/>
-      <c r="H50" s="39"/>
-      <c r="I50" s="39"/>
-      <c r="J50" s="39"/>
-      <c r="K50" s="39"/>
-      <c r="L50" s="39"/>
-      <c r="M50" s="39"/>
-      <c r="N50" s="39"/>
+      <c r="E50" s="37"/>
+      <c r="F50" s="37"/>
+      <c r="G50" s="37"/>
+      <c r="H50" s="37"/>
+      <c r="I50" s="37"/>
+      <c r="J50" s="37"/>
+      <c r="K50" s="37"/>
+      <c r="L50" s="37"/>
+      <c r="M50" s="37"/>
+      <c r="N50" s="37"/>
     </row>
     <row r="51" spans="5:14" ht="15.75" customHeight="1">
-      <c r="E51" s="39"/>
-      <c r="F51" s="39"/>
-      <c r="G51" s="39"/>
-      <c r="H51" s="39"/>
-      <c r="I51" s="39"/>
-      <c r="J51" s="39"/>
-      <c r="K51" s="39"/>
-      <c r="L51" s="39"/>
-      <c r="M51" s="39"/>
-      <c r="N51" s="39"/>
+      <c r="E51" s="37"/>
+      <c r="F51" s="37"/>
+      <c r="G51" s="37"/>
+      <c r="H51" s="37"/>
+      <c r="I51" s="37"/>
+      <c r="J51" s="37"/>
+      <c r="K51" s="37"/>
+      <c r="L51" s="37"/>
+      <c r="M51" s="37"/>
+      <c r="N51" s="37"/>
     </row>
     <row r="52" spans="5:14" ht="15.75" customHeight="1">
-      <c r="E52" s="39"/>
-      <c r="F52" s="39"/>
-      <c r="G52" s="39"/>
-      <c r="H52" s="39"/>
-      <c r="I52" s="39"/>
-      <c r="J52" s="39"/>
-      <c r="K52" s="39"/>
-      <c r="L52" s="39"/>
-      <c r="M52" s="39"/>
-      <c r="N52" s="39"/>
+      <c r="E52" s="37"/>
+      <c r="F52" s="37"/>
+      <c r="G52" s="37"/>
+      <c r="H52" s="37"/>
+      <c r="I52" s="37"/>
+      <c r="J52" s="37"/>
+      <c r="K52" s="37"/>
+      <c r="L52" s="37"/>
+      <c r="M52" s="37"/>
+      <c r="N52" s="37"/>
     </row>
     <row r="53" spans="5:14" ht="15.75" customHeight="1">
-      <c r="E53" s="39"/>
-      <c r="F53" s="39"/>
-      <c r="G53" s="39"/>
-      <c r="H53" s="39"/>
-      <c r="I53" s="39"/>
-      <c r="J53" s="39"/>
-      <c r="K53" s="39"/>
-      <c r="L53" s="39"/>
-      <c r="M53" s="39"/>
-      <c r="N53" s="39"/>
+      <c r="E53" s="37"/>
+      <c r="F53" s="37"/>
+      <c r="G53" s="37"/>
+      <c r="H53" s="37"/>
+      <c r="I53" s="37"/>
+      <c r="J53" s="37"/>
+      <c r="K53" s="37"/>
+      <c r="L53" s="37"/>
+      <c r="M53" s="37"/>
+      <c r="N53" s="37"/>
     </row>
     <row r="54" spans="5:14" ht="15.75" customHeight="1">
-      <c r="E54" s="39"/>
-      <c r="F54" s="39"/>
-      <c r="G54" s="39"/>
-      <c r="H54" s="39"/>
-      <c r="I54" s="39"/>
-      <c r="J54" s="39"/>
-      <c r="K54" s="39"/>
-      <c r="L54" s="39"/>
-      <c r="M54" s="39"/>
-      <c r="N54" s="39"/>
+      <c r="E54" s="37"/>
+      <c r="F54" s="37"/>
+      <c r="G54" s="37"/>
+      <c r="H54" s="37"/>
+      <c r="I54" s="37"/>
+      <c r="J54" s="37"/>
+      <c r="K54" s="37"/>
+      <c r="L54" s="37"/>
+      <c r="M54" s="37"/>
+      <c r="N54" s="37"/>
     </row>
     <row r="55" spans="5:14" ht="15.75" customHeight="1">
-      <c r="E55" s="39"/>
-      <c r="F55" s="39"/>
-      <c r="G55" s="39"/>
-      <c r="H55" s="39"/>
-      <c r="I55" s="39"/>
-      <c r="J55" s="39"/>
-      <c r="K55" s="39"/>
-      <c r="L55" s="39"/>
-      <c r="M55" s="39"/>
-      <c r="N55" s="39"/>
+      <c r="E55" s="37"/>
+      <c r="F55" s="37"/>
+      <c r="G55" s="37"/>
+      <c r="H55" s="37"/>
+      <c r="I55" s="37"/>
+      <c r="J55" s="37"/>
+      <c r="K55" s="37"/>
+      <c r="L55" s="37"/>
+      <c r="M55" s="37"/>
+      <c r="N55" s="37"/>
     </row>
     <row r="56" spans="5:14" ht="15.75" customHeight="1">
-      <c r="E56" s="39"/>
-      <c r="F56" s="39"/>
-      <c r="G56" s="39"/>
-      <c r="H56" s="39"/>
-      <c r="I56" s="39"/>
-      <c r="J56" s="39"/>
-      <c r="K56" s="39"/>
-      <c r="L56" s="39"/>
-      <c r="M56" s="39"/>
-      <c r="N56" s="39"/>
+      <c r="E56" s="37"/>
+      <c r="F56" s="37"/>
+      <c r="G56" s="37"/>
+      <c r="H56" s="37"/>
+      <c r="I56" s="37"/>
+      <c r="J56" s="37"/>
+      <c r="K56" s="37"/>
+      <c r="L56" s="37"/>
+      <c r="M56" s="37"/>
+      <c r="N56" s="37"/>
     </row>
     <row r="57" spans="5:14" ht="15.75" customHeight="1">
-      <c r="E57" s="39"/>
-      <c r="F57" s="39"/>
-      <c r="G57" s="39"/>
-      <c r="H57" s="39"/>
-      <c r="I57" s="39"/>
-      <c r="J57" s="39"/>
-      <c r="K57" s="39"/>
-      <c r="L57" s="39"/>
-      <c r="M57" s="39"/>
-      <c r="N57" s="39"/>
+      <c r="E57" s="37"/>
+      <c r="F57" s="37"/>
+      <c r="G57" s="37"/>
+      <c r="H57" s="37"/>
+      <c r="I57" s="37"/>
+      <c r="J57" s="37"/>
+      <c r="K57" s="37"/>
+      <c r="L57" s="37"/>
+      <c r="M57" s="37"/>
+      <c r="N57" s="37"/>
     </row>
     <row r="58" spans="5:14" ht="15.75" customHeight="1">
-      <c r="E58" s="39"/>
-      <c r="F58" s="39"/>
-      <c r="G58" s="39"/>
-      <c r="H58" s="39"/>
-      <c r="I58" s="39"/>
-      <c r="J58" s="39"/>
-      <c r="K58" s="39"/>
-      <c r="L58" s="39"/>
-      <c r="M58" s="39"/>
-      <c r="N58" s="39"/>
+      <c r="E58" s="37"/>
+      <c r="F58" s="37"/>
+      <c r="G58" s="37"/>
+      <c r="H58" s="37"/>
+      <c r="I58" s="37"/>
+      <c r="J58" s="37"/>
+      <c r="K58" s="37"/>
+      <c r="L58" s="37"/>
+      <c r="M58" s="37"/>
+      <c r="N58" s="37"/>
     </row>
     <row r="59" spans="5:14" ht="15.75" customHeight="1">
-      <c r="E59" s="39"/>
-      <c r="F59" s="39"/>
-      <c r="G59" s="39"/>
-      <c r="H59" s="39"/>
-      <c r="I59" s="39"/>
-      <c r="J59" s="39"/>
-      <c r="K59" s="39"/>
-      <c r="L59" s="39"/>
-      <c r="M59" s="39"/>
-      <c r="N59" s="39"/>
+      <c r="E59" s="37"/>
+      <c r="F59" s="37"/>
+      <c r="G59" s="37"/>
+      <c r="H59" s="37"/>
+      <c r="I59" s="37"/>
+      <c r="J59" s="37"/>
+      <c r="K59" s="37"/>
+      <c r="L59" s="37"/>
+      <c r="M59" s="37"/>
+      <c r="N59" s="37"/>
     </row>
     <row r="60" spans="5:14" ht="15.75" customHeight="1">
-      <c r="E60" s="39"/>
-      <c r="F60" s="39"/>
-      <c r="G60" s="39"/>
-      <c r="H60" s="39"/>
-      <c r="I60" s="39"/>
-      <c r="J60" s="39"/>
-      <c r="K60" s="39"/>
-      <c r="L60" s="39"/>
-      <c r="M60" s="39"/>
-      <c r="N60" s="39"/>
+      <c r="E60" s="37"/>
+      <c r="F60" s="37"/>
+      <c r="G60" s="37"/>
+      <c r="H60" s="37"/>
+      <c r="I60" s="37"/>
+      <c r="J60" s="37"/>
+      <c r="K60" s="37"/>
+      <c r="L60" s="37"/>
+      <c r="M60" s="37"/>
+      <c r="N60" s="37"/>
     </row>
     <row r="61" spans="5:14" ht="15.75" customHeight="1">
-      <c r="E61" s="39"/>
-      <c r="F61" s="39"/>
-      <c r="G61" s="39"/>
-      <c r="H61" s="39"/>
-      <c r="I61" s="39"/>
-      <c r="J61" s="39"/>
-      <c r="K61" s="39"/>
-      <c r="L61" s="39"/>
-      <c r="M61" s="39"/>
-      <c r="N61" s="39"/>
+      <c r="E61" s="37"/>
+      <c r="F61" s="37"/>
+      <c r="G61" s="37"/>
+      <c r="H61" s="37"/>
+      <c r="I61" s="37"/>
+      <c r="J61" s="37"/>
+      <c r="K61" s="37"/>
+      <c r="L61" s="37"/>
+      <c r="M61" s="37"/>
+      <c r="N61" s="37"/>
     </row>
     <row r="62" spans="5:14" ht="15.75" customHeight="1">
-      <c r="E62" s="39"/>
-      <c r="F62" s="39"/>
-      <c r="G62" s="39"/>
-      <c r="H62" s="39"/>
-      <c r="I62" s="39"/>
-      <c r="J62" s="39"/>
-      <c r="K62" s="39"/>
-      <c r="L62" s="39"/>
-      <c r="M62" s="39"/>
-      <c r="N62" s="39"/>
+      <c r="E62" s="37"/>
+      <c r="F62" s="37"/>
+      <c r="G62" s="37"/>
+      <c r="H62" s="37"/>
+      <c r="I62" s="37"/>
+      <c r="J62" s="37"/>
+      <c r="K62" s="37"/>
+      <c r="L62" s="37"/>
+      <c r="M62" s="37"/>
+      <c r="N62" s="37"/>
     </row>
     <row r="63" spans="5:14" ht="15.75" customHeight="1">
-      <c r="E63" s="39"/>
-      <c r="F63" s="39"/>
-      <c r="G63" s="39"/>
-      <c r="H63" s="39"/>
-      <c r="I63" s="39"/>
-      <c r="J63" s="39"/>
-      <c r="K63" s="39"/>
-      <c r="L63" s="39"/>
-      <c r="M63" s="39"/>
-      <c r="N63" s="39"/>
+      <c r="E63" s="37"/>
+      <c r="F63" s="37"/>
+      <c r="G63" s="37"/>
+      <c r="H63" s="37"/>
+      <c r="I63" s="37"/>
+      <c r="J63" s="37"/>
+      <c r="K63" s="37"/>
+      <c r="L63" s="37"/>
+      <c r="M63" s="37"/>
+      <c r="N63" s="37"/>
     </row>
     <row r="64" spans="5:14" ht="15.75" customHeight="1">
-      <c r="E64" s="39"/>
-      <c r="F64" s="39"/>
-      <c r="G64" s="39"/>
-      <c r="H64" s="39"/>
-      <c r="I64" s="39"/>
-      <c r="J64" s="39"/>
-      <c r="K64" s="39"/>
-      <c r="L64" s="39"/>
-      <c r="M64" s="39"/>
-      <c r="N64" s="39"/>
+      <c r="E64" s="37"/>
+      <c r="F64" s="37"/>
+      <c r="G64" s="37"/>
+      <c r="H64" s="37"/>
+      <c r="I64" s="37"/>
+      <c r="J64" s="37"/>
+      <c r="K64" s="37"/>
+      <c r="L64" s="37"/>
+      <c r="M64" s="37"/>
+      <c r="N64" s="37"/>
     </row>
     <row r="65" spans="5:14" ht="15.75" customHeight="1">
-      <c r="E65" s="39"/>
-      <c r="F65" s="39"/>
-      <c r="G65" s="39"/>
-      <c r="H65" s="39"/>
-      <c r="I65" s="39"/>
-      <c r="J65" s="39"/>
-      <c r="K65" s="39"/>
-      <c r="L65" s="39"/>
-      <c r="M65" s="39"/>
-      <c r="N65" s="39"/>
+      <c r="E65" s="37"/>
+      <c r="F65" s="37"/>
+      <c r="G65" s="37"/>
+      <c r="H65" s="37"/>
+      <c r="I65" s="37"/>
+      <c r="J65" s="37"/>
+      <c r="K65" s="37"/>
+      <c r="L65" s="37"/>
+      <c r="M65" s="37"/>
+      <c r="N65" s="37"/>
     </row>
     <row r="66" spans="5:14" ht="15.75" customHeight="1">
-      <c r="E66" s="39"/>
-      <c r="F66" s="39"/>
-      <c r="G66" s="39"/>
-      <c r="H66" s="39"/>
-      <c r="I66" s="39"/>
-      <c r="J66" s="39"/>
-      <c r="K66" s="39"/>
-      <c r="L66" s="39"/>
-      <c r="M66" s="39"/>
-      <c r="N66" s="39"/>
+      <c r="E66" s="37"/>
+      <c r="F66" s="37"/>
+      <c r="G66" s="37"/>
+      <c r="H66" s="37"/>
+      <c r="I66" s="37"/>
+      <c r="J66" s="37"/>
+      <c r="K66" s="37"/>
+      <c r="L66" s="37"/>
+      <c r="M66" s="37"/>
+      <c r="N66" s="37"/>
     </row>
     <row r="67" spans="5:14" ht="15.75" customHeight="1">
-      <c r="E67" s="39"/>
-      <c r="F67" s="39"/>
-      <c r="G67" s="39"/>
-      <c r="H67" s="39"/>
-      <c r="I67" s="39"/>
-      <c r="J67" s="39"/>
-      <c r="K67" s="39"/>
-      <c r="L67" s="39"/>
-      <c r="M67" s="39"/>
-      <c r="N67" s="39"/>
+      <c r="E67" s="37"/>
+      <c r="F67" s="37"/>
+      <c r="G67" s="37"/>
+      <c r="H67" s="37"/>
+      <c r="I67" s="37"/>
+      <c r="J67" s="37"/>
+      <c r="K67" s="37"/>
+      <c r="L67" s="37"/>
+      <c r="M67" s="37"/>
+      <c r="N67" s="37"/>
     </row>
     <row r="68" spans="5:14" ht="15.75" customHeight="1">
-      <c r="E68" s="39"/>
-      <c r="F68" s="39"/>
-      <c r="G68" s="39"/>
-      <c r="H68" s="39"/>
-      <c r="I68" s="39"/>
-      <c r="J68" s="39"/>
-      <c r="K68" s="39"/>
-      <c r="L68" s="39"/>
-      <c r="M68" s="39"/>
-      <c r="N68" s="39"/>
+      <c r="E68" s="37"/>
+      <c r="F68" s="37"/>
+      <c r="G68" s="37"/>
+      <c r="H68" s="37"/>
+      <c r="I68" s="37"/>
+      <c r="J68" s="37"/>
+      <c r="K68" s="37"/>
+      <c r="L68" s="37"/>
+      <c r="M68" s="37"/>
+      <c r="N68" s="37"/>
     </row>
     <row r="69" spans="5:14" ht="15.75" customHeight="1">
-      <c r="E69" s="39"/>
-      <c r="F69" s="39"/>
-      <c r="G69" s="39"/>
-      <c r="H69" s="39"/>
-      <c r="I69" s="39"/>
-      <c r="J69" s="39"/>
-      <c r="K69" s="39"/>
-      <c r="L69" s="39"/>
-      <c r="M69" s="39"/>
-      <c r="N69" s="39"/>
+      <c r="E69" s="37"/>
+      <c r="F69" s="37"/>
+      <c r="G69" s="37"/>
+      <c r="H69" s="37"/>
+      <c r="I69" s="37"/>
+      <c r="J69" s="37"/>
+      <c r="K69" s="37"/>
+      <c r="L69" s="37"/>
+      <c r="M69" s="37"/>
+      <c r="N69" s="37"/>
     </row>
     <row r="70" spans="5:14" ht="15.75" customHeight="1">
-      <c r="E70" s="39"/>
-      <c r="F70" s="39"/>
-      <c r="G70" s="39"/>
-      <c r="H70" s="39"/>
-      <c r="I70" s="39"/>
-      <c r="J70" s="39"/>
-      <c r="K70" s="39"/>
-      <c r="L70" s="39"/>
-      <c r="M70" s="39"/>
-      <c r="N70" s="39"/>
+      <c r="E70" s="37"/>
+      <c r="F70" s="37"/>
+      <c r="G70" s="37"/>
+      <c r="H70" s="37"/>
+      <c r="I70" s="37"/>
+      <c r="J70" s="37"/>
+      <c r="K70" s="37"/>
+      <c r="L70" s="37"/>
+      <c r="M70" s="37"/>
+      <c r="N70" s="37"/>
     </row>
     <row r="71" spans="5:14" ht="15.75" customHeight="1">
-      <c r="E71" s="39"/>
-      <c r="F71" s="39"/>
-      <c r="G71" s="39"/>
-      <c r="H71" s="39"/>
-      <c r="I71" s="39"/>
-      <c r="J71" s="39"/>
-      <c r="K71" s="39"/>
-      <c r="L71" s="39"/>
-      <c r="M71" s="39"/>
-      <c r="N71" s="39"/>
+      <c r="E71" s="37"/>
+      <c r="F71" s="37"/>
+      <c r="G71" s="37"/>
+      <c r="H71" s="37"/>
+      <c r="I71" s="37"/>
+      <c r="J71" s="37"/>
+      <c r="K71" s="37"/>
+      <c r="L71" s="37"/>
+      <c r="M71" s="37"/>
+      <c r="N71" s="37"/>
     </row>
     <row r="72" spans="5:14" ht="15.75" customHeight="1">
-      <c r="E72" s="39"/>
-      <c r="F72" s="39"/>
-      <c r="G72" s="39"/>
-      <c r="H72" s="39"/>
-      <c r="I72" s="39"/>
-      <c r="J72" s="39"/>
-      <c r="K72" s="39"/>
-      <c r="L72" s="39"/>
-      <c r="M72" s="39"/>
-      <c r="N72" s="39"/>
+      <c r="E72" s="37"/>
+      <c r="F72" s="37"/>
+      <c r="G72" s="37"/>
+      <c r="H72" s="37"/>
+      <c r="I72" s="37"/>
+      <c r="J72" s="37"/>
+      <c r="K72" s="37"/>
+      <c r="L72" s="37"/>
+      <c r="M72" s="37"/>
+      <c r="N72" s="37"/>
     </row>
     <row r="73" spans="5:14" ht="15.75" customHeight="1">
-      <c r="E73" s="39"/>
-      <c r="F73" s="39"/>
-      <c r="G73" s="39"/>
-      <c r="H73" s="39"/>
-      <c r="I73" s="39"/>
-      <c r="J73" s="39"/>
-      <c r="K73" s="39"/>
-      <c r="L73" s="39"/>
-      <c r="M73" s="39"/>
-      <c r="N73" s="39"/>
+      <c r="E73" s="37"/>
+      <c r="F73" s="37"/>
+      <c r="G73" s="37"/>
+      <c r="H73" s="37"/>
+      <c r="I73" s="37"/>
+      <c r="J73" s="37"/>
+      <c r="K73" s="37"/>
+      <c r="L73" s="37"/>
+      <c r="M73" s="37"/>
+      <c r="N73" s="37"/>
     </row>
     <row r="74" spans="5:14" ht="15.75" customHeight="1">
-      <c r="E74" s="39"/>
-      <c r="F74" s="39"/>
-      <c r="G74" s="39"/>
-      <c r="H74" s="39"/>
-      <c r="I74" s="39"/>
-      <c r="J74" s="39"/>
-      <c r="K74" s="39"/>
-      <c r="L74" s="39"/>
-      <c r="M74" s="39"/>
-      <c r="N74" s="39"/>
+      <c r="E74" s="37"/>
+      <c r="F74" s="37"/>
+      <c r="G74" s="37"/>
+      <c r="H74" s="37"/>
+      <c r="I74" s="37"/>
+      <c r="J74" s="37"/>
+      <c r="K74" s="37"/>
+      <c r="L74" s="37"/>
+      <c r="M74" s="37"/>
+      <c r="N74" s="37"/>
     </row>
     <row r="75" spans="5:14" ht="15.75" customHeight="1">
-      <c r="E75" s="39"/>
-      <c r="F75" s="39"/>
-      <c r="G75" s="39"/>
-      <c r="H75" s="39"/>
-      <c r="I75" s="39"/>
-      <c r="J75" s="39"/>
-      <c r="K75" s="39"/>
-      <c r="L75" s="39"/>
-      <c r="M75" s="39"/>
-      <c r="N75" s="39"/>
+      <c r="E75" s="37"/>
+      <c r="F75" s="37"/>
+      <c r="G75" s="37"/>
+      <c r="H75" s="37"/>
+      <c r="I75" s="37"/>
+      <c r="J75" s="37"/>
+      <c r="K75" s="37"/>
+      <c r="L75" s="37"/>
+      <c r="M75" s="37"/>
+      <c r="N75" s="37"/>
     </row>
     <row r="76" spans="5:14" ht="15.75" customHeight="1">
-      <c r="E76" s="39"/>
-      <c r="F76" s="39"/>
-      <c r="G76" s="39"/>
-      <c r="H76" s="39"/>
-      <c r="I76" s="39"/>
-      <c r="J76" s="39"/>
-      <c r="K76" s="39"/>
-      <c r="L76" s="39"/>
-      <c r="M76" s="39"/>
-      <c r="N76" s="39"/>
+      <c r="E76" s="37"/>
+      <c r="F76" s="37"/>
+      <c r="G76" s="37"/>
+      <c r="H76" s="37"/>
+      <c r="I76" s="37"/>
+      <c r="J76" s="37"/>
+      <c r="K76" s="37"/>
+      <c r="L76" s="37"/>
+      <c r="M76" s="37"/>
+      <c r="N76" s="37"/>
     </row>
     <row r="77" spans="5:14" ht="15.75" customHeight="1">
-      <c r="E77" s="39"/>
-      <c r="F77" s="39"/>
-      <c r="G77" s="39"/>
-      <c r="H77" s="39"/>
-      <c r="I77" s="39"/>
-      <c r="J77" s="39"/>
-      <c r="K77" s="39"/>
-      <c r="L77" s="39"/>
-      <c r="M77" s="39"/>
-      <c r="N77" s="39"/>
+      <c r="E77" s="37"/>
+      <c r="F77" s="37"/>
+      <c r="G77" s="37"/>
+      <c r="H77" s="37"/>
+      <c r="I77" s="37"/>
+      <c r="J77" s="37"/>
+      <c r="K77" s="37"/>
+      <c r="L77" s="37"/>
+      <c r="M77" s="37"/>
+      <c r="N77" s="37"/>
     </row>
     <row r="78" spans="5:14" ht="15.75" customHeight="1">
-      <c r="E78" s="39"/>
-      <c r="F78" s="39"/>
-      <c r="G78" s="39"/>
-      <c r="H78" s="39"/>
-      <c r="I78" s="39"/>
-      <c r="J78" s="39"/>
-      <c r="K78" s="39"/>
-      <c r="L78" s="39"/>
-      <c r="M78" s="39"/>
-      <c r="N78" s="39"/>
+      <c r="E78" s="37"/>
+      <c r="F78" s="37"/>
+      <c r="G78" s="37"/>
+      <c r="H78" s="37"/>
+      <c r="I78" s="37"/>
+      <c r="J78" s="37"/>
+      <c r="K78" s="37"/>
+      <c r="L78" s="37"/>
+      <c r="M78" s="37"/>
+      <c r="N78" s="37"/>
     </row>
     <row r="79" spans="5:14" ht="15.75" customHeight="1">
-      <c r="E79" s="39"/>
-      <c r="F79" s="39"/>
-      <c r="G79" s="39"/>
-      <c r="H79" s="39"/>
-      <c r="I79" s="39"/>
-      <c r="J79" s="39"/>
-      <c r="K79" s="39"/>
-      <c r="L79" s="39"/>
-      <c r="M79" s="39"/>
-      <c r="N79" s="39"/>
+      <c r="E79" s="37"/>
+      <c r="F79" s="37"/>
+      <c r="G79" s="37"/>
+      <c r="H79" s="37"/>
+      <c r="I79" s="37"/>
+      <c r="J79" s="37"/>
+      <c r="K79" s="37"/>
+      <c r="L79" s="37"/>
+      <c r="M79" s="37"/>
+      <c r="N79" s="37"/>
     </row>
     <row r="80" spans="5:14" ht="15.75" customHeight="1">
-      <c r="E80" s="39"/>
-      <c r="F80" s="39"/>
-      <c r="G80" s="39"/>
-      <c r="H80" s="39"/>
-      <c r="I80" s="39"/>
-      <c r="J80" s="39"/>
-      <c r="K80" s="39"/>
-      <c r="L80" s="39"/>
-      <c r="M80" s="39"/>
-      <c r="N80" s="39"/>
+      <c r="E80" s="37"/>
+      <c r="F80" s="37"/>
+      <c r="G80" s="37"/>
+      <c r="H80" s="37"/>
+      <c r="I80" s="37"/>
+      <c r="J80" s="37"/>
+      <c r="K80" s="37"/>
+      <c r="L80" s="37"/>
+      <c r="M80" s="37"/>
+      <c r="N80" s="37"/>
     </row>
     <row r="81" spans="5:14" ht="15.75" customHeight="1">
-      <c r="E81" s="39"/>
-      <c r="F81" s="39"/>
-      <c r="G81" s="39"/>
-      <c r="H81" s="39"/>
-      <c r="I81" s="39"/>
-      <c r="J81" s="39"/>
-      <c r="K81" s="39"/>
-      <c r="L81" s="39"/>
-      <c r="M81" s="39"/>
-      <c r="N81" s="39"/>
+      <c r="E81" s="37"/>
+      <c r="F81" s="37"/>
+      <c r="G81" s="37"/>
+      <c r="H81" s="37"/>
+      <c r="I81" s="37"/>
+      <c r="J81" s="37"/>
+      <c r="K81" s="37"/>
+      <c r="L81" s="37"/>
+      <c r="M81" s="37"/>
+      <c r="N81" s="37"/>
     </row>
     <row r="82" spans="5:14" ht="15.75" customHeight="1">
-      <c r="E82" s="39"/>
-      <c r="F82" s="39"/>
-      <c r="G82" s="39"/>
-      <c r="H82" s="39"/>
-      <c r="I82" s="39"/>
-      <c r="J82" s="39"/>
-      <c r="K82" s="39"/>
-      <c r="L82" s="39"/>
-      <c r="M82" s="39"/>
-      <c r="N82" s="39"/>
+      <c r="E82" s="37"/>
+      <c r="F82" s="37"/>
+      <c r="G82" s="37"/>
+      <c r="H82" s="37"/>
+      <c r="I82" s="37"/>
+      <c r="J82" s="37"/>
+      <c r="K82" s="37"/>
+      <c r="L82" s="37"/>
+      <c r="M82" s="37"/>
+      <c r="N82" s="37"/>
     </row>
     <row r="83" spans="5:14" ht="15.75" customHeight="1">
-      <c r="E83" s="39"/>
-      <c r="F83" s="39"/>
-      <c r="G83" s="39"/>
-      <c r="H83" s="39"/>
-      <c r="I83" s="39"/>
-      <c r="J83" s="39"/>
-      <c r="K83" s="39"/>
-      <c r="L83" s="39"/>
-      <c r="M83" s="39"/>
-      <c r="N83" s="39"/>
+      <c r="E83" s="37"/>
+      <c r="F83" s="37"/>
+      <c r="G83" s="37"/>
+      <c r="H83" s="37"/>
+      <c r="I83" s="37"/>
+      <c r="J83" s="37"/>
+      <c r="K83" s="37"/>
+      <c r="L83" s="37"/>
+      <c r="M83" s="37"/>
+      <c r="N83" s="37"/>
     </row>
     <row r="84" spans="5:14" ht="15.75" customHeight="1">
-      <c r="E84" s="39"/>
-      <c r="F84" s="39"/>
-      <c r="G84" s="39"/>
-      <c r="H84" s="39"/>
-      <c r="I84" s="39"/>
-      <c r="J84" s="39"/>
-      <c r="K84" s="39"/>
-      <c r="L84" s="39"/>
-      <c r="M84" s="39"/>
-      <c r="N84" s="39"/>
+      <c r="E84" s="37"/>
+      <c r="F84" s="37"/>
+      <c r="G84" s="37"/>
+      <c r="H84" s="37"/>
+      <c r="I84" s="37"/>
+      <c r="J84" s="37"/>
+      <c r="K84" s="37"/>
+      <c r="L84" s="37"/>
+      <c r="M84" s="37"/>
+      <c r="N84" s="37"/>
     </row>
     <row r="85" spans="5:14" ht="15.75" customHeight="1">
-      <c r="E85" s="39"/>
-      <c r="F85" s="39"/>
-      <c r="G85" s="39"/>
-      <c r="H85" s="39"/>
-      <c r="I85" s="39"/>
-      <c r="J85" s="39"/>
-      <c r="K85" s="39"/>
-      <c r="L85" s="39"/>
-      <c r="M85" s="39"/>
-      <c r="N85" s="39"/>
+      <c r="E85" s="37"/>
+      <c r="F85" s="37"/>
+      <c r="G85" s="37"/>
+      <c r="H85" s="37"/>
+      <c r="I85" s="37"/>
+      <c r="J85" s="37"/>
+      <c r="K85" s="37"/>
+      <c r="L85" s="37"/>
+      <c r="M85" s="37"/>
+      <c r="N85" s="37"/>
     </row>
     <row r="86" spans="5:14" ht="15.75" customHeight="1">
-      <c r="E86" s="39"/>
-      <c r="F86" s="39"/>
-      <c r="G86" s="39"/>
-      <c r="H86" s="39"/>
-      <c r="I86" s="39"/>
-      <c r="J86" s="39"/>
-      <c r="K86" s="39"/>
-      <c r="L86" s="39"/>
-      <c r="M86" s="39"/>
-      <c r="N86" s="39"/>
+      <c r="E86" s="37"/>
+      <c r="F86" s="37"/>
+      <c r="G86" s="37"/>
+      <c r="H86" s="37"/>
+      <c r="I86" s="37"/>
+      <c r="J86" s="37"/>
+      <c r="K86" s="37"/>
+      <c r="L86" s="37"/>
+      <c r="M86" s="37"/>
+      <c r="N86" s="37"/>
     </row>
     <row r="87" spans="5:14" ht="15.75" customHeight="1">
-      <c r="E87" s="39"/>
-      <c r="F87" s="39"/>
-      <c r="G87" s="39"/>
-      <c r="H87" s="39"/>
-      <c r="I87" s="39"/>
-      <c r="J87" s="39"/>
-      <c r="K87" s="39"/>
-      <c r="L87" s="39"/>
-      <c r="M87" s="39"/>
-      <c r="N87" s="39"/>
+      <c r="E87" s="37"/>
+      <c r="F87" s="37"/>
+      <c r="G87" s="37"/>
+      <c r="H87" s="37"/>
+      <c r="I87" s="37"/>
+      <c r="J87" s="37"/>
+      <c r="K87" s="37"/>
+      <c r="L87" s="37"/>
+      <c r="M87" s="37"/>
+      <c r="N87" s="37"/>
     </row>
     <row r="88" spans="5:14" ht="15.75" customHeight="1">
-      <c r="E88" s="39"/>
-      <c r="F88" s="39"/>
-      <c r="G88" s="39"/>
-      <c r="H88" s="39"/>
-      <c r="I88" s="39"/>
-      <c r="J88" s="39"/>
-      <c r="K88" s="39"/>
-      <c r="L88" s="39"/>
-      <c r="M88" s="39"/>
-      <c r="N88" s="39"/>
+      <c r="E88" s="37"/>
+      <c r="F88" s="37"/>
+      <c r="G88" s="37"/>
+      <c r="H88" s="37"/>
+      <c r="I88" s="37"/>
+      <c r="J88" s="37"/>
+      <c r="K88" s="37"/>
+      <c r="L88" s="37"/>
+      <c r="M88" s="37"/>
+      <c r="N88" s="37"/>
     </row>
     <row r="89" spans="5:14" ht="15.75" customHeight="1">
-      <c r="E89" s="39"/>
-      <c r="F89" s="39"/>
-      <c r="G89" s="39"/>
-      <c r="H89" s="39"/>
-      <c r="I89" s="39"/>
-      <c r="J89" s="39"/>
-      <c r="K89" s="39"/>
-      <c r="L89" s="39"/>
-      <c r="M89" s="39"/>
-      <c r="N89" s="39"/>
+      <c r="E89" s="37"/>
+      <c r="F89" s="37"/>
+      <c r="G89" s="37"/>
+      <c r="H89" s="37"/>
+      <c r="I89" s="37"/>
+      <c r="J89" s="37"/>
+      <c r="K89" s="37"/>
+      <c r="L89" s="37"/>
+      <c r="M89" s="37"/>
+      <c r="N89" s="37"/>
     </row>
     <row r="90" spans="5:14" ht="15.75" customHeight="1">
-      <c r="E90" s="39"/>
-      <c r="F90" s="39"/>
-      <c r="G90" s="39"/>
-      <c r="H90" s="39"/>
-      <c r="I90" s="39"/>
-      <c r="J90" s="39"/>
-      <c r="K90" s="39"/>
-      <c r="L90" s="39"/>
-      <c r="M90" s="39"/>
-      <c r="N90" s="39"/>
+      <c r="E90" s="37"/>
+      <c r="F90" s="37"/>
+      <c r="G90" s="37"/>
+      <c r="H90" s="37"/>
+      <c r="I90" s="37"/>
+      <c r="J90" s="37"/>
+      <c r="K90" s="37"/>
+      <c r="L90" s="37"/>
+      <c r="M90" s="37"/>
+      <c r="N90" s="37"/>
     </row>
     <row r="91" spans="5:14" ht="15.75" customHeight="1">
-      <c r="E91" s="39"/>
-      <c r="F91" s="39"/>
-      <c r="G91" s="39"/>
-      <c r="H91" s="39"/>
-      <c r="I91" s="39"/>
-      <c r="J91" s="39"/>
-      <c r="K91" s="39"/>
-      <c r="L91" s="39"/>
-      <c r="M91" s="39"/>
-      <c r="N91" s="39"/>
+      <c r="E91" s="37"/>
+      <c r="F91" s="37"/>
+      <c r="G91" s="37"/>
+      <c r="H91" s="37"/>
+      <c r="I91" s="37"/>
+      <c r="J91" s="37"/>
+      <c r="K91" s="37"/>
+      <c r="L91" s="37"/>
+      <c r="M91" s="37"/>
+      <c r="N91" s="37"/>
     </row>
     <row r="92" spans="5:14" ht="15.75" customHeight="1">
-      <c r="E92" s="39"/>
-      <c r="F92" s="39"/>
-      <c r="G92" s="39"/>
-      <c r="H92" s="39"/>
-      <c r="I92" s="39"/>
-      <c r="J92" s="39"/>
-      <c r="K92" s="39"/>
-      <c r="L92" s="39"/>
-      <c r="M92" s="39"/>
-      <c r="N92" s="39"/>
+      <c r="E92" s="37"/>
+      <c r="F92" s="37"/>
+      <c r="G92" s="37"/>
+      <c r="H92" s="37"/>
+      <c r="I92" s="37"/>
+      <c r="J92" s="37"/>
+      <c r="K92" s="37"/>
+      <c r="L92" s="37"/>
+      <c r="M92" s="37"/>
+      <c r="N92" s="37"/>
     </row>
     <row r="93" spans="5:14" ht="15.75" customHeight="1">
-      <c r="E93" s="39"/>
-      <c r="F93" s="39"/>
-      <c r="G93" s="39"/>
-      <c r="H93" s="39"/>
-      <c r="I93" s="39"/>
-      <c r="J93" s="39"/>
-      <c r="K93" s="39"/>
-      <c r="L93" s="39"/>
-      <c r="M93" s="39"/>
-      <c r="N93" s="39"/>
+      <c r="E93" s="37"/>
+      <c r="F93" s="37"/>
+      <c r="G93" s="37"/>
+      <c r="H93" s="37"/>
+      <c r="I93" s="37"/>
+      <c r="J93" s="37"/>
+      <c r="K93" s="37"/>
+      <c r="L93" s="37"/>
+      <c r="M93" s="37"/>
+      <c r="N93" s="37"/>
     </row>
     <row r="94" spans="5:14" ht="15.75" customHeight="1">
-      <c r="E94" s="39"/>
-      <c r="F94" s="39"/>
-      <c r="G94" s="39"/>
-      <c r="H94" s="39"/>
-      <c r="I94" s="39"/>
-      <c r="J94" s="39"/>
-      <c r="K94" s="39"/>
-      <c r="L94" s="39"/>
-      <c r="M94" s="39"/>
-      <c r="N94" s="39"/>
+      <c r="E94" s="37"/>
+      <c r="F94" s="37"/>
+      <c r="G94" s="37"/>
+      <c r="H94" s="37"/>
+      <c r="I94" s="37"/>
+      <c r="J94" s="37"/>
+      <c r="K94" s="37"/>
+      <c r="L94" s="37"/>
+      <c r="M94" s="37"/>
+      <c r="N94" s="37"/>
     </row>
     <row r="95" spans="5:14" ht="15.75" customHeight="1">
-      <c r="E95" s="39"/>
-      <c r="F95" s="39"/>
-      <c r="G95" s="39"/>
-      <c r="H95" s="39"/>
-      <c r="I95" s="39"/>
-      <c r="J95" s="39"/>
-      <c r="K95" s="39"/>
-      <c r="L95" s="39"/>
-      <c r="M95" s="39"/>
-      <c r="N95" s="39"/>
+      <c r="E95" s="37"/>
+      <c r="F95" s="37"/>
+      <c r="G95" s="37"/>
+      <c r="H95" s="37"/>
+      <c r="I95" s="37"/>
+      <c r="J95" s="37"/>
+      <c r="K95" s="37"/>
+      <c r="L95" s="37"/>
+      <c r="M95" s="37"/>
+      <c r="N95" s="37"/>
     </row>
     <row r="96" spans="5:14" ht="15.75" customHeight="1">
-      <c r="E96" s="39"/>
-      <c r="F96" s="39"/>
-      <c r="G96" s="39"/>
-      <c r="H96" s="39"/>
-      <c r="I96" s="39"/>
-      <c r="J96" s="39"/>
-      <c r="K96" s="39"/>
-      <c r="L96" s="39"/>
-      <c r="M96" s="39"/>
-      <c r="N96" s="39"/>
+      <c r="E96" s="37"/>
+      <c r="F96" s="37"/>
+      <c r="G96" s="37"/>
+      <c r="H96" s="37"/>
+      <c r="I96" s="37"/>
+      <c r="J96" s="37"/>
+      <c r="K96" s="37"/>
+      <c r="L96" s="37"/>
+      <c r="M96" s="37"/>
+      <c r="N96" s="37"/>
     </row>
     <row r="97" spans="5:14" ht="15.75" customHeight="1">
-      <c r="E97" s="39"/>
-      <c r="F97" s="39"/>
-      <c r="G97" s="39"/>
-      <c r="H97" s="39"/>
-      <c r="I97" s="39"/>
-      <c r="J97" s="39"/>
-      <c r="K97" s="39"/>
-      <c r="L97" s="39"/>
-      <c r="M97" s="39"/>
-      <c r="N97" s="39"/>
+      <c r="E97" s="37"/>
+      <c r="F97" s="37"/>
+      <c r="G97" s="37"/>
+      <c r="H97" s="37"/>
+      <c r="I97" s="37"/>
+      <c r="J97" s="37"/>
+      <c r="K97" s="37"/>
+      <c r="L97" s="37"/>
+      <c r="M97" s="37"/>
+      <c r="N97" s="37"/>
     </row>
     <row r="98" spans="5:14" ht="15.75" customHeight="1">
-      <c r="E98" s="39"/>
-      <c r="F98" s="39"/>
-      <c r="G98" s="39"/>
-      <c r="H98" s="39"/>
-      <c r="I98" s="39"/>
-      <c r="J98" s="39"/>
-      <c r="K98" s="39"/>
-      <c r="L98" s="39"/>
-      <c r="M98" s="39"/>
-      <c r="N98" s="39"/>
+      <c r="E98" s="37"/>
+      <c r="F98" s="37"/>
+      <c r="G98" s="37"/>
+      <c r="H98" s="37"/>
+      <c r="I98" s="37"/>
+      <c r="J98" s="37"/>
+      <c r="K98" s="37"/>
+      <c r="L98" s="37"/>
+      <c r="M98" s="37"/>
+      <c r="N98" s="37"/>
     </row>
     <row r="99" spans="5:14" ht="15.75" customHeight="1">
-      <c r="E99" s="39"/>
-      <c r="F99" s="39"/>
-      <c r="G99" s="39"/>
-      <c r="H99" s="39"/>
-      <c r="I99" s="39"/>
-      <c r="J99" s="39"/>
-      <c r="K99" s="39"/>
-      <c r="L99" s="39"/>
-      <c r="M99" s="39"/>
-      <c r="N99" s="39"/>
+      <c r="E99" s="37"/>
+      <c r="F99" s="37"/>
+      <c r="G99" s="37"/>
+      <c r="H99" s="37"/>
+      <c r="I99" s="37"/>
+      <c r="J99" s="37"/>
+      <c r="K99" s="37"/>
+      <c r="L99" s="37"/>
+      <c r="M99" s="37"/>
+      <c r="N99" s="37"/>
     </row>
     <row r="100" spans="5:14" ht="15.75" customHeight="1">
-      <c r="E100" s="39"/>
-      <c r="F100" s="39"/>
-      <c r="G100" s="39"/>
-      <c r="H100" s="39"/>
-      <c r="I100" s="39"/>
-      <c r="J100" s="39"/>
-      <c r="K100" s="39"/>
-      <c r="L100" s="39"/>
-      <c r="M100" s="39"/>
-      <c r="N100" s="39"/>
+      <c r="E100" s="37"/>
+      <c r="F100" s="37"/>
+      <c r="G100" s="37"/>
+      <c r="H100" s="37"/>
+      <c r="I100" s="37"/>
+      <c r="J100" s="37"/>
+      <c r="K100" s="37"/>
+      <c r="L100" s="37"/>
+      <c r="M100" s="37"/>
+      <c r="N100" s="37"/>
     </row>
     <row r="101" spans="5:14" ht="15.75" customHeight="1">
-      <c r="E101" s="39"/>
-      <c r="F101" s="39"/>
-      <c r="G101" s="39"/>
-      <c r="H101" s="39"/>
-      <c r="I101" s="39"/>
-      <c r="J101" s="39"/>
-      <c r="K101" s="39"/>
-      <c r="L101" s="39"/>
-      <c r="M101" s="39"/>
-      <c r="N101" s="39"/>
+      <c r="E101" s="37"/>
+      <c r="F101" s="37"/>
+      <c r="G101" s="37"/>
+      <c r="H101" s="37"/>
+      <c r="I101" s="37"/>
+      <c r="J101" s="37"/>
+      <c r="K101" s="37"/>
+      <c r="L101" s="37"/>
+      <c r="M101" s="37"/>
+      <c r="N101" s="37"/>
     </row>
     <row r="102" spans="5:14" ht="15.75" customHeight="1">
-      <c r="E102" s="39"/>
-      <c r="F102" s="39"/>
-      <c r="G102" s="39"/>
-      <c r="H102" s="39"/>
-      <c r="I102" s="39"/>
-      <c r="J102" s="39"/>
-      <c r="K102" s="39"/>
-      <c r="L102" s="39"/>
-      <c r="M102" s="39"/>
-      <c r="N102" s="39"/>
+      <c r="E102" s="37"/>
+      <c r="F102" s="37"/>
+      <c r="G102" s="37"/>
+      <c r="H102" s="37"/>
+      <c r="I102" s="37"/>
+      <c r="J102" s="37"/>
+      <c r="K102" s="37"/>
+      <c r="L102" s="37"/>
+      <c r="M102" s="37"/>
+      <c r="N102" s="37"/>
     </row>
     <row r="103" spans="5:14" ht="15.75" customHeight="1">
-      <c r="E103" s="39"/>
-      <c r="F103" s="39"/>
-      <c r="G103" s="39"/>
-      <c r="H103" s="39"/>
-      <c r="I103" s="39"/>
-      <c r="J103" s="39"/>
-      <c r="K103" s="39"/>
-      <c r="L103" s="39"/>
-      <c r="M103" s="39"/>
-      <c r="N103" s="39"/>
+      <c r="E103" s="37"/>
+      <c r="F103" s="37"/>
+      <c r="G103" s="37"/>
+      <c r="H103" s="37"/>
+      <c r="I103" s="37"/>
+      <c r="J103" s="37"/>
+      <c r="K103" s="37"/>
+      <c r="L103" s="37"/>
+      <c r="M103" s="37"/>
+      <c r="N103" s="37"/>
     </row>
     <row r="104" spans="5:14" ht="15.75" customHeight="1">
-      <c r="E104" s="39"/>
-      <c r="F104" s="39"/>
-      <c r="G104" s="39"/>
-      <c r="H104" s="39"/>
-      <c r="I104" s="39"/>
-      <c r="J104" s="39"/>
-      <c r="K104" s="39"/>
-      <c r="L104" s="39"/>
-      <c r="M104" s="39"/>
-      <c r="N104" s="39"/>
+      <c r="E104" s="37"/>
+      <c r="F104" s="37"/>
+      <c r="G104" s="37"/>
+      <c r="H104" s="37"/>
+      <c r="I104" s="37"/>
+      <c r="J104" s="37"/>
+      <c r="K104" s="37"/>
+      <c r="L104" s="37"/>
+      <c r="M104" s="37"/>
+      <c r="N104" s="37"/>
     </row>
     <row r="105" spans="5:14" ht="15.75" customHeight="1">
-      <c r="E105" s="39"/>
-      <c r="F105" s="39"/>
-      <c r="G105" s="39"/>
-      <c r="H105" s="39"/>
-      <c r="I105" s="39"/>
-      <c r="J105" s="39"/>
-      <c r="K105" s="39"/>
-      <c r="L105" s="39"/>
-      <c r="M105" s="39"/>
-      <c r="N105" s="39"/>
+      <c r="E105" s="37"/>
+      <c r="F105" s="37"/>
+      <c r="G105" s="37"/>
+      <c r="H105" s="37"/>
+      <c r="I105" s="37"/>
+      <c r="J105" s="37"/>
+      <c r="K105" s="37"/>
+      <c r="L105" s="37"/>
+      <c r="M105" s="37"/>
+      <c r="N105" s="37"/>
     </row>
     <row r="106" spans="5:14" ht="15.75" customHeight="1">
-      <c r="E106" s="39"/>
-      <c r="F106" s="39"/>
-      <c r="G106" s="39"/>
-      <c r="H106" s="39"/>
-      <c r="I106" s="39"/>
-      <c r="J106" s="39"/>
-      <c r="K106" s="39"/>
-      <c r="L106" s="39"/>
-      <c r="M106" s="39"/>
-      <c r="N106" s="39"/>
+      <c r="E106" s="37"/>
+      <c r="F106" s="37"/>
+      <c r="G106" s="37"/>
+      <c r="H106" s="37"/>
+      <c r="I106" s="37"/>
+      <c r="J106" s="37"/>
+      <c r="K106" s="37"/>
+      <c r="L106" s="37"/>
+      <c r="M106" s="37"/>
+      <c r="N106" s="37"/>
     </row>
     <row r="107" spans="5:14" ht="15.75" customHeight="1">
-      <c r="E107" s="39"/>
-      <c r="F107" s="39"/>
-      <c r="G107" s="39"/>
-      <c r="H107" s="39"/>
-      <c r="I107" s="39"/>
-      <c r="J107" s="39"/>
-      <c r="K107" s="39"/>
-      <c r="L107" s="39"/>
-      <c r="M107" s="39"/>
-      <c r="N107" s="39"/>
+      <c r="E107" s="37"/>
+      <c r="F107" s="37"/>
+      <c r="G107" s="37"/>
+      <c r="H107" s="37"/>
+      <c r="I107" s="37"/>
+      <c r="J107" s="37"/>
+      <c r="K107" s="37"/>
+      <c r="L107" s="37"/>
+      <c r="M107" s="37"/>
+      <c r="N107" s="37"/>
     </row>
     <row r="108" spans="5:14" ht="15.75" customHeight="1">
-      <c r="E108" s="39"/>
-      <c r="F108" s="39"/>
-      <c r="G108" s="39"/>
-      <c r="H108" s="39"/>
-      <c r="I108" s="39"/>
-      <c r="J108" s="39"/>
-      <c r="K108" s="39"/>
-      <c r="L108" s="39"/>
-      <c r="M108" s="39"/>
-      <c r="N108" s="39"/>
+      <c r="E108" s="37"/>
+      <c r="F108" s="37"/>
+      <c r="G108" s="37"/>
+      <c r="H108" s="37"/>
+      <c r="I108" s="37"/>
+      <c r="J108" s="37"/>
+      <c r="K108" s="37"/>
+      <c r="L108" s="37"/>
+      <c r="M108" s="37"/>
+      <c r="N108" s="37"/>
     </row>
     <row r="109" spans="5:14" ht="15.75" customHeight="1">
-      <c r="E109" s="39"/>
-      <c r="F109" s="39"/>
-      <c r="G109" s="39"/>
-      <c r="H109" s="39"/>
-      <c r="I109" s="39"/>
-      <c r="J109" s="39"/>
-      <c r="K109" s="39"/>
-      <c r="L109" s="39"/>
-      <c r="M109" s="39"/>
-      <c r="N109" s="39"/>
+      <c r="E109" s="37"/>
+      <c r="F109" s="37"/>
+      <c r="G109" s="37"/>
+      <c r="H109" s="37"/>
+      <c r="I109" s="37"/>
+      <c r="J109" s="37"/>
+      <c r="K109" s="37"/>
+      <c r="L109" s="37"/>
+      <c r="M109" s="37"/>
+      <c r="N109" s="37"/>
     </row>
     <row r="110" spans="5:14" ht="15.75" customHeight="1">
-      <c r="E110" s="39"/>
-      <c r="F110" s="39"/>
-      <c r="G110" s="39"/>
-      <c r="H110" s="39"/>
-      <c r="I110" s="39"/>
-      <c r="J110" s="39"/>
-      <c r="K110" s="39"/>
-      <c r="L110" s="39"/>
-      <c r="M110" s="39"/>
-      <c r="N110" s="39"/>
+      <c r="E110" s="37"/>
+      <c r="F110" s="37"/>
+      <c r="G110" s="37"/>
+      <c r="H110" s="37"/>
+      <c r="I110" s="37"/>
+      <c r="J110" s="37"/>
+      <c r="K110" s="37"/>
+      <c r="L110" s="37"/>
+      <c r="M110" s="37"/>
+      <c r="N110" s="37"/>
     </row>
     <row r="111" spans="5:14" ht="15.75" customHeight="1">
-      <c r="E111" s="39"/>
-      <c r="F111" s="39"/>
-      <c r="G111" s="39"/>
-      <c r="H111" s="39"/>
-      <c r="I111" s="39"/>
-      <c r="J111" s="39"/>
-      <c r="K111" s="39"/>
-      <c r="L111" s="39"/>
-      <c r="M111" s="39"/>
-      <c r="N111" s="39"/>
+      <c r="E111" s="37"/>
+      <c r="F111" s="37"/>
+      <c r="G111" s="37"/>
+      <c r="H111" s="37"/>
+      <c r="I111" s="37"/>
+      <c r="J111" s="37"/>
+      <c r="K111" s="37"/>
+      <c r="L111" s="37"/>
+      <c r="M111" s="37"/>
+      <c r="N111" s="37"/>
     </row>
     <row r="112" spans="5:14" ht="15.75" customHeight="1">
-      <c r="E112" s="39"/>
-      <c r="F112" s="39"/>
-      <c r="G112" s="39"/>
-      <c r="H112" s="39"/>
-      <c r="I112" s="39"/>
-      <c r="J112" s="39"/>
-      <c r="K112" s="39"/>
-      <c r="L112" s="39"/>
-      <c r="M112" s="39"/>
-      <c r="N112" s="39"/>
+      <c r="E112" s="37"/>
+      <c r="F112" s="37"/>
+      <c r="G112" s="37"/>
+      <c r="H112" s="37"/>
+      <c r="I112" s="37"/>
+      <c r="J112" s="37"/>
+      <c r="K112" s="37"/>
+      <c r="L112" s="37"/>
+      <c r="M112" s="37"/>
+      <c r="N112" s="37"/>
     </row>
     <row r="113" spans="5:14" ht="15.75" customHeight="1">
-      <c r="E113" s="39"/>
-      <c r="F113" s="39"/>
-      <c r="G113" s="39"/>
-      <c r="H113" s="39"/>
-      <c r="I113" s="39"/>
-      <c r="J113" s="39"/>
-      <c r="K113" s="39"/>
-      <c r="L113" s="39"/>
-      <c r="M113" s="39"/>
-      <c r="N113" s="39"/>
+      <c r="E113" s="37"/>
+      <c r="F113" s="37"/>
+      <c r="G113" s="37"/>
+      <c r="H113" s="37"/>
+      <c r="I113" s="37"/>
+      <c r="J113" s="37"/>
+      <c r="K113" s="37"/>
+      <c r="L113" s="37"/>
+      <c r="M113" s="37"/>
+      <c r="N113" s="37"/>
     </row>
     <row r="114" spans="5:14" ht="15.75" customHeight="1">
-      <c r="E114" s="39"/>
-      <c r="F114" s="39"/>
-      <c r="G114" s="39"/>
-      <c r="H114" s="39"/>
-      <c r="I114" s="39"/>
-      <c r="J114" s="39"/>
-      <c r="K114" s="39"/>
-      <c r="L114" s="39"/>
-      <c r="M114" s="39"/>
-      <c r="N114" s="39"/>
+      <c r="E114" s="37"/>
+      <c r="F114" s="37"/>
+      <c r="G114" s="37"/>
+      <c r="H114" s="37"/>
+      <c r="I114" s="37"/>
+      <c r="J114" s="37"/>
+      <c r="K114" s="37"/>
+      <c r="L114" s="37"/>
+      <c r="M114" s="37"/>
+      <c r="N114" s="37"/>
     </row>
     <row r="115" spans="5:14" ht="15.75" customHeight="1">
-      <c r="E115" s="39"/>
-      <c r="F115" s="39"/>
-      <c r="G115" s="39"/>
-      <c r="H115" s="39"/>
-      <c r="I115" s="39"/>
-      <c r="J115" s="39"/>
-      <c r="K115" s="39"/>
-      <c r="L115" s="39"/>
-      <c r="M115" s="39"/>
-      <c r="N115" s="39"/>
+      <c r="E115" s="37"/>
+      <c r="F115" s="37"/>
+      <c r="G115" s="37"/>
+      <c r="H115" s="37"/>
+      <c r="I115" s="37"/>
+      <c r="J115" s="37"/>
+      <c r="K115" s="37"/>
+      <c r="L115" s="37"/>
+      <c r="M115" s="37"/>
+      <c r="N115" s="37"/>
     </row>
     <row r="116" spans="5:14" ht="15.75" customHeight="1">
-      <c r="E116" s="39"/>
-      <c r="F116" s="39"/>
-      <c r="G116" s="39"/>
-      <c r="H116" s="39"/>
-      <c r="I116" s="39"/>
-      <c r="J116" s="39"/>
-      <c r="K116" s="39"/>
-      <c r="L116" s="39"/>
-      <c r="M116" s="39"/>
-      <c r="N116" s="39"/>
+      <c r="E116" s="37"/>
+      <c r="F116" s="37"/>
+      <c r="G116" s="37"/>
+      <c r="H116" s="37"/>
+      <c r="I116" s="37"/>
+      <c r="J116" s="37"/>
+      <c r="K116" s="37"/>
+      <c r="L116" s="37"/>
+      <c r="M116" s="37"/>
+      <c r="N116" s="37"/>
     </row>
     <row r="117" spans="5:14" ht="15.75" customHeight="1">
-      <c r="E117" s="39"/>
-      <c r="F117" s="39"/>
-      <c r="G117" s="39"/>
-      <c r="H117" s="39"/>
-      <c r="I117" s="39"/>
-      <c r="J117" s="39"/>
-      <c r="K117" s="39"/>
-      <c r="L117" s="39"/>
-      <c r="M117" s="39"/>
-      <c r="N117" s="39"/>
+      <c r="E117" s="37"/>
+      <c r="F117" s="37"/>
+      <c r="G117" s="37"/>
+      <c r="H117" s="37"/>
+      <c r="I117" s="37"/>
+      <c r="J117" s="37"/>
+      <c r="K117" s="37"/>
+      <c r="L117" s="37"/>
+      <c r="M117" s="37"/>
+      <c r="N117" s="37"/>
     </row>
     <row r="118" spans="5:14" ht="15.75" customHeight="1">
-      <c r="E118" s="39"/>
-      <c r="F118" s="39"/>
-      <c r="G118" s="39"/>
-      <c r="H118" s="39"/>
-      <c r="I118" s="39"/>
-      <c r="J118" s="39"/>
-      <c r="K118" s="39"/>
-      <c r="L118" s="39"/>
-      <c r="M118" s="39"/>
-      <c r="N118" s="39"/>
+      <c r="E118" s="37"/>
+      <c r="F118" s="37"/>
+      <c r="G118" s="37"/>
+      <c r="H118" s="37"/>
+      <c r="I118" s="37"/>
+      <c r="J118" s="37"/>
+      <c r="K118" s="37"/>
+      <c r="L118" s="37"/>
+      <c r="M118" s="37"/>
+      <c r="N118" s="37"/>
     </row>
     <row r="119" spans="5:14" ht="15.75" customHeight="1">
-      <c r="E119" s="39"/>
-      <c r="F119" s="39"/>
-      <c r="G119" s="39"/>
-      <c r="H119" s="39"/>
-      <c r="I119" s="39"/>
-      <c r="J119" s="39"/>
-      <c r="K119" s="39"/>
-      <c r="L119" s="39"/>
-      <c r="M119" s="39"/>
-      <c r="N119" s="39"/>
+      <c r="E119" s="37"/>
+      <c r="F119" s="37"/>
+      <c r="G119" s="37"/>
+      <c r="H119" s="37"/>
+      <c r="I119" s="37"/>
+      <c r="J119" s="37"/>
+      <c r="K119" s="37"/>
+      <c r="L119" s="37"/>
+      <c r="M119" s="37"/>
+      <c r="N119" s="37"/>
     </row>
     <row r="120" spans="5:14" ht="15.75" customHeight="1">
-      <c r="E120" s="39"/>
-      <c r="F120" s="39"/>
-      <c r="G120" s="39"/>
-      <c r="H120" s="39"/>
-      <c r="I120" s="39"/>
-      <c r="J120" s="39"/>
-      <c r="K120" s="39"/>
-      <c r="L120" s="39"/>
-      <c r="M120" s="39"/>
-      <c r="N120" s="39"/>
+      <c r="E120" s="37"/>
+      <c r="F120" s="37"/>
+      <c r="G120" s="37"/>
+      <c r="H120" s="37"/>
+      <c r="I120" s="37"/>
+      <c r="J120" s="37"/>
+      <c r="K120" s="37"/>
+      <c r="L120" s="37"/>
+      <c r="M120" s="37"/>
+      <c r="N120" s="37"/>
     </row>
     <row r="121" spans="5:14" ht="15.75" customHeight="1">
-      <c r="E121" s="39"/>
-      <c r="F121" s="39"/>
-      <c r="G121" s="39"/>
-      <c r="H121" s="39"/>
-      <c r="I121" s="39"/>
-      <c r="J121" s="39"/>
-      <c r="K121" s="39"/>
-      <c r="L121" s="39"/>
-      <c r="M121" s="39"/>
-      <c r="N121" s="39"/>
+      <c r="E121" s="37"/>
+      <c r="F121" s="37"/>
+      <c r="G121" s="37"/>
+      <c r="H121" s="37"/>
+      <c r="I121" s="37"/>
+      <c r="J121" s="37"/>
+      <c r="K121" s="37"/>
+      <c r="L121" s="37"/>
+      <c r="M121" s="37"/>
+      <c r="N121" s="37"/>
     </row>
     <row r="122" spans="5:14" ht="15.75" customHeight="1">
-      <c r="E122" s="39"/>
-      <c r="F122" s="39"/>
-      <c r="G122" s="39"/>
-      <c r="H122" s="39"/>
-      <c r="I122" s="39"/>
-      <c r="J122" s="39"/>
-      <c r="K122" s="39"/>
-      <c r="L122" s="39"/>
-      <c r="M122" s="39"/>
-      <c r="N122" s="39"/>
+      <c r="E122" s="37"/>
+      <c r="F122" s="37"/>
+      <c r="G122" s="37"/>
+      <c r="H122" s="37"/>
+      <c r="I122" s="37"/>
+      <c r="J122" s="37"/>
+      <c r="K122" s="37"/>
+      <c r="L122" s="37"/>
+      <c r="M122" s="37"/>
+      <c r="N122" s="37"/>
     </row>
     <row r="123" spans="5:14" ht="15.75" customHeight="1">
-      <c r="E123" s="39"/>
-      <c r="F123" s="39"/>
-      <c r="G123" s="39"/>
-      <c r="H123" s="39"/>
-      <c r="I123" s="39"/>
-      <c r="J123" s="39"/>
-      <c r="K123" s="39"/>
-      <c r="L123" s="39"/>
-      <c r="M123" s="39"/>
-      <c r="N123" s="39"/>
+      <c r="E123" s="37"/>
+      <c r="F123" s="37"/>
+      <c r="G123" s="37"/>
+      <c r="H123" s="37"/>
+      <c r="I123" s="37"/>
+      <c r="J123" s="37"/>
+      <c r="K123" s="37"/>
+      <c r="L123" s="37"/>
+      <c r="M123" s="37"/>
+      <c r="N123" s="37"/>
     </row>
     <row r="124" spans="5:14" ht="15.75" customHeight="1">
-      <c r="E124" s="39"/>
-      <c r="F124" s="39"/>
-      <c r="G124" s="39"/>
-      <c r="H124" s="39"/>
-      <c r="I124" s="39"/>
-      <c r="J124" s="39"/>
-      <c r="K124" s="39"/>
-      <c r="L124" s="39"/>
-      <c r="M124" s="39"/>
-      <c r="N124" s="39"/>
+      <c r="E124" s="37"/>
+      <c r="F124" s="37"/>
+      <c r="G124" s="37"/>
+      <c r="H124" s="37"/>
+      <c r="I124" s="37"/>
+      <c r="J124" s="37"/>
+      <c r="K124" s="37"/>
+      <c r="L124" s="37"/>
+      <c r="M124" s="37"/>
+      <c r="N124" s="37"/>
     </row>
     <row r="125" spans="5:14" ht="15.75" customHeight="1">
-      <c r="E125" s="39"/>
-      <c r="F125" s="39"/>
-      <c r="G125" s="39"/>
-      <c r="H125" s="39"/>
-      <c r="I125" s="39"/>
-      <c r="J125" s="39"/>
-      <c r="K125" s="39"/>
-      <c r="L125" s="39"/>
-      <c r="M125" s="39"/>
-      <c r="N125" s="39"/>
+      <c r="E125" s="37"/>
+      <c r="F125" s="37"/>
+      <c r="G125" s="37"/>
+      <c r="H125" s="37"/>
+      <c r="I125" s="37"/>
+      <c r="J125" s="37"/>
+      <c r="K125" s="37"/>
+      <c r="L125" s="37"/>
+      <c r="M125" s="37"/>
+      <c r="N125" s="37"/>
     </row>
     <row r="126" spans="5:14" ht="15.75" customHeight="1">
-      <c r="E126" s="39"/>
-      <c r="F126" s="39"/>
-      <c r="G126" s="39"/>
-      <c r="H126" s="39"/>
-      <c r="I126" s="39"/>
-      <c r="J126" s="39"/>
-      <c r="K126" s="39"/>
-      <c r="L126" s="39"/>
-      <c r="M126" s="39"/>
-      <c r="N126" s="39"/>
+      <c r="E126" s="37"/>
+      <c r="F126" s="37"/>
+      <c r="G126" s="37"/>
+      <c r="H126" s="37"/>
+      <c r="I126" s="37"/>
+      <c r="J126" s="37"/>
+      <c r="K126" s="37"/>
+      <c r="L126" s="37"/>
+      <c r="M126" s="37"/>
+      <c r="N126" s="37"/>
     </row>
     <row r="127" spans="5:14" ht="15.75" customHeight="1">
-      <c r="E127" s="39"/>
-      <c r="F127" s="39"/>
-      <c r="G127" s="39"/>
-      <c r="H127" s="39"/>
-      <c r="I127" s="39"/>
-      <c r="J127" s="39"/>
-      <c r="K127" s="39"/>
-      <c r="L127" s="39"/>
-      <c r="M127" s="39"/>
-      <c r="N127" s="39"/>
+      <c r="E127" s="37"/>
+      <c r="F127" s="37"/>
+      <c r="G127" s="37"/>
+      <c r="H127" s="37"/>
+      <c r="I127" s="37"/>
+      <c r="J127" s="37"/>
+      <c r="K127" s="37"/>
+      <c r="L127" s="37"/>
+      <c r="M127" s="37"/>
+      <c r="N127" s="37"/>
     </row>
     <row r="128" spans="5:14" ht="15.75" customHeight="1">
-      <c r="E128" s="39"/>
-      <c r="F128" s="39"/>
-      <c r="G128" s="39"/>
-      <c r="H128" s="39"/>
-      <c r="I128" s="39"/>
-      <c r="J128" s="39"/>
-      <c r="K128" s="39"/>
-      <c r="L128" s="39"/>
-      <c r="M128" s="39"/>
-      <c r="N128" s="39"/>
+      <c r="E128" s="37"/>
+      <c r="F128" s="37"/>
+      <c r="G128" s="37"/>
+      <c r="H128" s="37"/>
+      <c r="I128" s="37"/>
+      <c r="J128" s="37"/>
+      <c r="K128" s="37"/>
+      <c r="L128" s="37"/>
+      <c r="M128" s="37"/>
+      <c r="N128" s="37"/>
     </row>
     <row r="129" spans="5:14" ht="15.75" customHeight="1">
-      <c r="E129" s="39"/>
-      <c r="F129" s="39"/>
-      <c r="G129" s="39"/>
-      <c r="H129" s="39"/>
-      <c r="I129" s="39"/>
-      <c r="J129" s="39"/>
-      <c r="K129" s="39"/>
-      <c r="L129" s="39"/>
-      <c r="M129" s="39"/>
-      <c r="N129" s="39"/>
+      <c r="E129" s="37"/>
+      <c r="F129" s="37"/>
+      <c r="G129" s="37"/>
+      <c r="H129" s="37"/>
+      <c r="I129" s="37"/>
+      <c r="J129" s="37"/>
+      <c r="K129" s="37"/>
+      <c r="L129" s="37"/>
+      <c r="M129" s="37"/>
+      <c r="N129" s="37"/>
     </row>
     <row r="130" spans="5:14" ht="15.75" customHeight="1">
-      <c r="E130" s="39"/>
-      <c r="F130" s="39"/>
-      <c r="G130" s="39"/>
-      <c r="H130" s="39"/>
-      <c r="I130" s="39"/>
-      <c r="J130" s="39"/>
-      <c r="K130" s="39"/>
-      <c r="L130" s="39"/>
-      <c r="M130" s="39"/>
-      <c r="N130" s="39"/>
+      <c r="E130" s="37"/>
+      <c r="F130" s="37"/>
+      <c r="G130" s="37"/>
+      <c r="H130" s="37"/>
+      <c r="I130" s="37"/>
+      <c r="J130" s="37"/>
+      <c r="K130" s="37"/>
+      <c r="L130" s="37"/>
+      <c r="M130" s="37"/>
+      <c r="N130" s="37"/>
     </row>
     <row r="131" spans="5:14" ht="15.75" customHeight="1">
-      <c r="E131" s="39"/>
-      <c r="F131" s="39"/>
-      <c r="G131" s="39"/>
-      <c r="H131" s="39"/>
-      <c r="I131" s="39"/>
-      <c r="J131" s="39"/>
-      <c r="K131" s="39"/>
-      <c r="L131" s="39"/>
-      <c r="M131" s="39"/>
-      <c r="N131" s="39"/>
+      <c r="E131" s="37"/>
+      <c r="F131" s="37"/>
+      <c r="G131" s="37"/>
+      <c r="H131" s="37"/>
+      <c r="I131" s="37"/>
+      <c r="J131" s="37"/>
+      <c r="K131" s="37"/>
+      <c r="L131" s="37"/>
+      <c r="M131" s="37"/>
+      <c r="N131" s="37"/>
     </row>
     <row r="132" spans="5:14" ht="15.75" customHeight="1">
-      <c r="E132" s="39"/>
-      <c r="F132" s="39"/>
-      <c r="G132" s="39"/>
-      <c r="H132" s="39"/>
-      <c r="I132" s="39"/>
-      <c r="J132" s="39"/>
-      <c r="K132" s="39"/>
-      <c r="L132" s="39"/>
-      <c r="M132" s="39"/>
-      <c r="N132" s="39"/>
+      <c r="E132" s="37"/>
+      <c r="F132" s="37"/>
+      <c r="G132" s="37"/>
+      <c r="H132" s="37"/>
+      <c r="I132" s="37"/>
+      <c r="J132" s="37"/>
+      <c r="K132" s="37"/>
+      <c r="L132" s="37"/>
+      <c r="M132" s="37"/>
+      <c r="N132" s="37"/>
     </row>
     <row r="133" spans="5:14" ht="15.75" customHeight="1">
-      <c r="E133" s="39"/>
-      <c r="F133" s="39"/>
-      <c r="G133" s="39"/>
-      <c r="H133" s="39"/>
-      <c r="I133" s="39"/>
-      <c r="J133" s="39"/>
-      <c r="K133" s="39"/>
-      <c r="L133" s="39"/>
-      <c r="M133" s="39"/>
-      <c r="N133" s="39"/>
+      <c r="E133" s="37"/>
+      <c r="F133" s="37"/>
+      <c r="G133" s="37"/>
+      <c r="H133" s="37"/>
+      <c r="I133" s="37"/>
+      <c r="J133" s="37"/>
+      <c r="K133" s="37"/>
+      <c r="L133" s="37"/>
+      <c r="M133" s="37"/>
+      <c r="N133" s="37"/>
     </row>
     <row r="134" spans="5:14" ht="15.75" customHeight="1">
-      <c r="E134" s="39"/>
-      <c r="F134" s="39"/>
-      <c r="G134" s="39"/>
-      <c r="H134" s="39"/>
-      <c r="I134" s="39"/>
-      <c r="J134" s="39"/>
-      <c r="K134" s="39"/>
-      <c r="L134" s="39"/>
-      <c r="M134" s="39"/>
-      <c r="N134" s="39"/>
+      <c r="E134" s="37"/>
+      <c r="F134" s="37"/>
+      <c r="G134" s="37"/>
+      <c r="H134" s="37"/>
+      <c r="I134" s="37"/>
+      <c r="J134" s="37"/>
+      <c r="K134" s="37"/>
+      <c r="L134" s="37"/>
+      <c r="M134" s="37"/>
+      <c r="N134" s="37"/>
     </row>
     <row r="135" spans="5:14" ht="15.75" customHeight="1">
-      <c r="E135" s="39"/>
-      <c r="F135" s="39"/>
-      <c r="G135" s="39"/>
-      <c r="H135" s="39"/>
-      <c r="I135" s="39"/>
-      <c r="J135" s="39"/>
-      <c r="K135" s="39"/>
-      <c r="L135" s="39"/>
-      <c r="M135" s="39"/>
-      <c r="N135" s="39"/>
+      <c r="E135" s="37"/>
+      <c r="F135" s="37"/>
+      <c r="G135" s="37"/>
+      <c r="H135" s="37"/>
+      <c r="I135" s="37"/>
+      <c r="J135" s="37"/>
+      <c r="K135" s="37"/>
+      <c r="L135" s="37"/>
+      <c r="M135" s="37"/>
+      <c r="N135" s="37"/>
     </row>
     <row r="136" spans="5:14" ht="15.75" customHeight="1">
-      <c r="E136" s="39"/>
-      <c r="F136" s="39"/>
-      <c r="G136" s="39"/>
-      <c r="H136" s="39"/>
-      <c r="I136" s="39"/>
-      <c r="J136" s="39"/>
-      <c r="K136" s="39"/>
-      <c r="L136" s="39"/>
-      <c r="M136" s="39"/>
-      <c r="N136" s="39"/>
+      <c r="E136" s="37"/>
+      <c r="F136" s="37"/>
+      <c r="G136" s="37"/>
+      <c r="H136" s="37"/>
+      <c r="I136" s="37"/>
+      <c r="J136" s="37"/>
+      <c r="K136" s="37"/>
+      <c r="L136" s="37"/>
+      <c r="M136" s="37"/>
+      <c r="N136" s="37"/>
     </row>
     <row r="137" spans="5:14" ht="15.75" customHeight="1">
-      <c r="E137" s="39"/>
-      <c r="F137" s="39"/>
-      <c r="G137" s="39"/>
-      <c r="H137" s="39"/>
-      <c r="I137" s="39"/>
-      <c r="J137" s="39"/>
-      <c r="K137" s="39"/>
-      <c r="L137" s="39"/>
-      <c r="M137" s="39"/>
-      <c r="N137" s="39"/>
+      <c r="E137" s="37"/>
+      <c r="F137" s="37"/>
+      <c r="G137" s="37"/>
+      <c r="H137" s="37"/>
+      <c r="I137" s="37"/>
+      <c r="J137" s="37"/>
+      <c r="K137" s="37"/>
+      <c r="L137" s="37"/>
+      <c r="M137" s="37"/>
+      <c r="N137" s="37"/>
     </row>
     <row r="138" spans="5:14" ht="15.75" customHeight="1">
-      <c r="E138" s="39"/>
-      <c r="F138" s="39"/>
-      <c r="G138" s="39"/>
-      <c r="H138" s="39"/>
-      <c r="I138" s="39"/>
-      <c r="J138" s="39"/>
-      <c r="K138" s="39"/>
-      <c r="L138" s="39"/>
-      <c r="M138" s="39"/>
-      <c r="N138" s="39"/>
+      <c r="E138" s="37"/>
+      <c r="F138" s="37"/>
+      <c r="G138" s="37"/>
+      <c r="H138" s="37"/>
+      <c r="I138" s="37"/>
+      <c r="J138" s="37"/>
+      <c r="K138" s="37"/>
+      <c r="L138" s="37"/>
+      <c r="M138" s="37"/>
+      <c r="N138" s="37"/>
     </row>
     <row r="139" spans="5:14" ht="15.75" customHeight="1">
-      <c r="E139" s="39"/>
-      <c r="F139" s="39"/>
-      <c r="G139" s="39"/>
-      <c r="H139" s="39"/>
-      <c r="I139" s="39"/>
-      <c r="J139" s="39"/>
-      <c r="K139" s="39"/>
-      <c r="L139" s="39"/>
-      <c r="M139" s="39"/>
-      <c r="N139" s="39"/>
+      <c r="E139" s="37"/>
+      <c r="F139" s="37"/>
+      <c r="G139" s="37"/>
+      <c r="H139" s="37"/>
+      <c r="I139" s="37"/>
+      <c r="J139" s="37"/>
+      <c r="K139" s="37"/>
+      <c r="L139" s="37"/>
+      <c r="M139" s="37"/>
+      <c r="N139" s="37"/>
     </row>
     <row r="140" spans="5:14" ht="15.75" customHeight="1">
-      <c r="E140" s="39"/>
-      <c r="F140" s="39"/>
-      <c r="G140" s="39"/>
-      <c r="H140" s="39"/>
-      <c r="I140" s="39"/>
-      <c r="J140" s="39"/>
-      <c r="K140" s="39"/>
-      <c r="L140" s="39"/>
-      <c r="M140" s="39"/>
-      <c r="N140" s="39"/>
+      <c r="E140" s="37"/>
+      <c r="F140" s="37"/>
+      <c r="G140" s="37"/>
+      <c r="H140" s="37"/>
+      <c r="I140" s="37"/>
+      <c r="J140" s="37"/>
+      <c r="K140" s="37"/>
+      <c r="L140" s="37"/>
+      <c r="M140" s="37"/>
+      <c r="N140" s="37"/>
     </row>
     <row r="141" spans="5:14" ht="15.75" customHeight="1">
-      <c r="E141" s="39"/>
-      <c r="F141" s="39"/>
-      <c r="G141" s="39"/>
-      <c r="H141" s="39"/>
-      <c r="I141" s="39"/>
-      <c r="J141" s="39"/>
-      <c r="K141" s="39"/>
-      <c r="L141" s="39"/>
-      <c r="M141" s="39"/>
-      <c r="N141" s="39"/>
+      <c r="E141" s="37"/>
+      <c r="F141" s="37"/>
+      <c r="G141" s="37"/>
+      <c r="H141" s="37"/>
+      <c r="I141" s="37"/>
+      <c r="J141" s="37"/>
+      <c r="K141" s="37"/>
+      <c r="L141" s="37"/>
+      <c r="M141" s="37"/>
+      <c r="N141" s="37"/>
     </row>
     <row r="142" spans="5:14" ht="15.75" customHeight="1">
-      <c r="E142" s="39"/>
-      <c r="F142" s="39"/>
-      <c r="G142" s="39"/>
-      <c r="H142" s="39"/>
-      <c r="I142" s="39"/>
-      <c r="J142" s="39"/>
-      <c r="K142" s="39"/>
-      <c r="L142" s="39"/>
-      <c r="M142" s="39"/>
-      <c r="N142" s="39"/>
+      <c r="E142" s="37"/>
+      <c r="F142" s="37"/>
+      <c r="G142" s="37"/>
+      <c r="H142" s="37"/>
+      <c r="I142" s="37"/>
+      <c r="J142" s="37"/>
+      <c r="K142" s="37"/>
+      <c r="L142" s="37"/>
+      <c r="M142" s="37"/>
+      <c r="N142" s="37"/>
     </row>
     <row r="143" spans="5:14" ht="15.75" customHeight="1">
-      <c r="E143" s="39"/>
-      <c r="F143" s="39"/>
-      <c r="G143" s="39"/>
-      <c r="H143" s="39"/>
-      <c r="I143" s="39"/>
-      <c r="J143" s="39"/>
-      <c r="K143" s="39"/>
-      <c r="L143" s="39"/>
-      <c r="M143" s="39"/>
-      <c r="N143" s="39"/>
+      <c r="E143" s="37"/>
+      <c r="F143" s="37"/>
+      <c r="G143" s="37"/>
+      <c r="H143" s="37"/>
+      <c r="I143" s="37"/>
+      <c r="J143" s="37"/>
+      <c r="K143" s="37"/>
+      <c r="L143" s="37"/>
+      <c r="M143" s="37"/>
+      <c r="N143" s="37"/>
     </row>
     <row r="144" spans="5:14" ht="15.75" customHeight="1">
-      <c r="E144" s="39"/>
-      <c r="F144" s="39"/>
-      <c r="G144" s="39"/>
-      <c r="H144" s="39"/>
-      <c r="I144" s="39"/>
-      <c r="J144" s="39"/>
-      <c r="K144" s="39"/>
-      <c r="L144" s="39"/>
-      <c r="M144" s="39"/>
-      <c r="N144" s="39"/>
+      <c r="E144" s="37"/>
+      <c r="F144" s="37"/>
+      <c r="G144" s="37"/>
+      <c r="H144" s="37"/>
+      <c r="I144" s="37"/>
+      <c r="J144" s="37"/>
+      <c r="K144" s="37"/>
+      <c r="L144" s="37"/>
+      <c r="M144" s="37"/>
+      <c r="N144" s="37"/>
     </row>
     <row r="145" spans="5:14" ht="15.75" customHeight="1">
-      <c r="E145" s="39"/>
-      <c r="F145" s="39"/>
-      <c r="G145" s="39"/>
-      <c r="H145" s="39"/>
-      <c r="I145" s="39"/>
-      <c r="J145" s="39"/>
-      <c r="K145" s="39"/>
-      <c r="L145" s="39"/>
-      <c r="M145" s="39"/>
-      <c r="N145" s="39"/>
+      <c r="E145" s="37"/>
+      <c r="F145" s="37"/>
+      <c r="G145" s="37"/>
+      <c r="H145" s="37"/>
+      <c r="I145" s="37"/>
+      <c r="J145" s="37"/>
+      <c r="K145" s="37"/>
+      <c r="L145" s="37"/>
+      <c r="M145" s="37"/>
+      <c r="N145" s="37"/>
     </row>
   </sheetData>
   <mergeCells count="5">
@@ -3884,50 +3917,50 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D8AC00B6-697C-45E4-9E65-51AD1E2696C6}">
   <dimension ref="A3:R43"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="190" zoomScaleNormal="190" workbookViewId="0">
+    <sheetView topLeftCell="A13" zoomScale="190" zoomScaleNormal="190" workbookViewId="0">
       <selection activeCell="B31" sqref="B31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
   <sheetData>
     <row r="3" spans="1:18">
-      <c r="A3" s="55" t="s">
+      <c r="A3" s="51" t="s">
         <v>153</v>
       </c>
     </row>
     <row r="4" spans="1:18">
-      <c r="A4" s="54" t="s">
+      <c r="A4" s="50" t="s">
         <v>154</v>
       </c>
     </row>
     <row r="5" spans="1:18">
-      <c r="B5" s="55" t="s">
+      <c r="B5" s="51" t="s">
         <v>132</v>
       </c>
-      <c r="C5" s="55" t="s">
+      <c r="C5" s="51" t="s">
         <v>127</v>
       </c>
       <c r="F5" t="s">
         <v>128</v>
       </c>
-      <c r="G5" s="57" t="s">
+      <c r="G5" s="53" t="s">
         <v>129</v>
       </c>
     </row>
     <row r="6" spans="1:18">
-      <c r="B6" s="55" t="s">
+      <c r="B6" s="51" t="s">
         <v>133</v>
       </c>
-      <c r="C6" s="55" t="s">
+      <c r="C6" s="51" t="s">
         <v>142</v>
       </c>
       <c r="F6" t="s">
         <v>128</v>
       </c>
-      <c r="G6" s="58" t="s">
+      <c r="G6" s="54" t="s">
         <v>130</v>
       </c>
-      <c r="L6" s="59" t="s">
+      <c r="L6" s="55" t="s">
         <v>131</v>
       </c>
       <c r="R6" t="s">
@@ -3935,35 +3968,35 @@
       </c>
     </row>
     <row r="7" spans="1:18">
-      <c r="B7" s="55" t="s">
+      <c r="B7" s="51" t="s">
         <v>137</v>
       </c>
-      <c r="C7" s="55" t="s">
+      <c r="C7" s="51" t="s">
         <v>138</v>
       </c>
-      <c r="G7" s="56" t="s">
+      <c r="G7" s="52" t="s">
         <v>140</v>
       </c>
-      <c r="L7" s="56" t="s">
+      <c r="L7" s="52" t="s">
         <v>141</v>
       </c>
     </row>
     <row r="8" spans="1:18">
-      <c r="C8" s="55" t="s">
+      <c r="C8" s="51" t="s">
         <v>139</v>
       </c>
     </row>
     <row r="9" spans="1:18">
-      <c r="A9" s="54" t="s">
+      <c r="A9" s="50" t="s">
         <v>162</v>
       </c>
-      <c r="C9" s="55"/>
+      <c r="C9" s="51"/>
     </row>
     <row r="10" spans="1:18">
-      <c r="B10" s="65" t="s">
+      <c r="B10" s="61" t="s">
         <v>163</v>
       </c>
-      <c r="C10" s="55"/>
+      <c r="C10" s="51"/>
     </row>
     <row r="11" spans="1:18">
       <c r="A11" t="s">
@@ -3971,7 +4004,7 @@
       </c>
     </row>
     <row r="12" spans="1:18">
-      <c r="A12" s="54" t="s">
+      <c r="A12" s="50" t="s">
         <v>143</v>
       </c>
     </row>
@@ -3981,63 +4014,63 @@
       </c>
     </row>
     <row r="16" spans="1:18">
-      <c r="A16" s="54" t="s">
+      <c r="A16" s="50" t="s">
         <v>150</v>
       </c>
-      <c r="B16" s="54" t="s">
+      <c r="B16" s="50" t="s">
         <v>151</v>
       </c>
     </row>
     <row r="17" spans="1:3">
-      <c r="A17" s="55" t="s">
+      <c r="A17" s="51" t="s">
         <v>144</v>
       </c>
-      <c r="B17" s="54" t="s">
+      <c r="B17" s="50" t="s">
         <v>152</v>
       </c>
     </row>
     <row r="18" spans="1:3">
-      <c r="A18" s="55"/>
-      <c r="B18" s="54"/>
-      <c r="C18" s="54" t="s">
+      <c r="A18" s="51"/>
+      <c r="B18" s="50"/>
+      <c r="C18" s="50" t="s">
         <v>147</v>
       </c>
     </row>
     <row r="19" spans="1:3">
-      <c r="A19" s="55"/>
-      <c r="B19" s="54"/>
-      <c r="C19" s="55" t="s">
+      <c r="A19" s="51"/>
+      <c r="B19" s="50"/>
+      <c r="C19" s="51" t="s">
         <v>169</v>
       </c>
     </row>
     <row r="20" spans="1:3">
-      <c r="A20" s="55" t="s">
+      <c r="A20" s="51" t="s">
         <v>148</v>
       </c>
-      <c r="B20" s="54" t="s">
+      <c r="B20" s="50" t="s">
         <v>149</v>
       </c>
     </row>
     <row r="21" spans="1:3">
-      <c r="A21" s="55"/>
-      <c r="B21" s="54" t="s">
+      <c r="A21" s="51"/>
+      <c r="B21" s="50" t="s">
         <v>166</v>
       </c>
     </row>
     <row r="22" spans="1:3">
-      <c r="A22" s="55" t="s">
+      <c r="A22" s="51" t="s">
         <v>155</v>
       </c>
-      <c r="B22" s="54"/>
+      <c r="B22" s="50"/>
     </row>
     <row r="23" spans="1:3">
-      <c r="A23" s="55"/>
-      <c r="B23" s="54" t="s">
+      <c r="A23" s="51"/>
+      <c r="B23" s="50" t="s">
         <v>175</v>
       </c>
     </row>
     <row r="24" spans="1:3">
-      <c r="A24" s="55" t="s">
+      <c r="A24" s="51" t="s">
         <v>145</v>
       </c>
       <c r="B24" t="s">
@@ -4045,46 +4078,46 @@
       </c>
     </row>
     <row r="25" spans="1:3">
-      <c r="A25" s="54"/>
-      <c r="B25" s="55" t="s">
+      <c r="A25" s="50"/>
+      <c r="B25" s="51" t="s">
         <v>156</v>
       </c>
     </row>
     <row r="26" spans="1:3">
-      <c r="A26" s="55" t="s">
+      <c r="A26" s="51" t="s">
         <v>157</v>
       </c>
-      <c r="B26" s="55" t="s">
+      <c r="B26" s="51" t="s">
         <v>164</v>
       </c>
     </row>
     <row r="27" spans="1:3">
-      <c r="A27" s="54"/>
-      <c r="B27" s="54" t="s">
+      <c r="A27" s="50"/>
+      <c r="B27" s="50" t="s">
         <v>158</v>
       </c>
     </row>
     <row r="28" spans="1:3">
-      <c r="A28" s="54"/>
-      <c r="B28" s="55" t="s">
+      <c r="A28" s="50"/>
+      <c r="B28" s="51" t="s">
         <v>159</v>
       </c>
     </row>
     <row r="29" spans="1:3">
-      <c r="B29" s="55" t="s">
+      <c r="B29" s="51" t="s">
         <v>165</v>
       </c>
     </row>
     <row r="30" spans="1:3">
-      <c r="C30" s="71" t="s">
+      <c r="C30" s="67" t="s">
         <v>167</v>
       </c>
     </row>
     <row r="31" spans="1:3">
-      <c r="A31" s="55" t="s">
+      <c r="A31" s="51" t="s">
         <v>177</v>
       </c>
-      <c r="B31" s="54" t="s">
+      <c r="B31" s="50" t="s">
         <v>178</v>
       </c>
     </row>
@@ -4099,7 +4132,7 @@
       </c>
       <c r="B35" s="11"/>
       <c r="C35" s="11"/>
-      <c r="K35" s="54" t="s">
+      <c r="K35" s="50" t="s">
         <v>160</v>
       </c>
     </row>
@@ -4111,7 +4144,7 @@
       <c r="C36" s="10" t="s">
         <v>57</v>
       </c>
-      <c r="L36" s="54" t="s">
+      <c r="L36" s="50" t="s">
         <v>161</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Chapter 1 Kelvin TR Edit done.
</commit_message>
<xml_diff>
--- a/Word/PlanAndDealines.xlsx
+++ b/Word/PlanAndDealines.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20376"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20377"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ksung\Desktop\GitHub\GTCS-GameEngine2\Word\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A4D214D7-0157-412B-A8D0-482D6694100A}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{24851925-21C0-4D0E-BE29-3C1267003319}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="33645" windowHeight="15855" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -833,7 +833,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="41">
+  <fonts count="42">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -1077,6 +1077,13 @@
       <name val="Arial"/>
       <family val="2"/>
     </font>
+    <font>
+      <strike/>
+      <sz val="10"/>
+      <color theme="0" tint="-0.499984740745262"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
   </fonts>
   <fills count="3">
     <fill>
@@ -1177,7 +1184,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="89">
+  <cellXfs count="90">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
@@ -1377,6 +1384,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="41" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1594,8 +1602,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D8AC00B6-697C-45E4-9E65-51AD1E2696C6}">
   <dimension ref="A3:R44"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" zoomScale="190" zoomScaleNormal="190" workbookViewId="0">
-      <selection activeCell="A32" sqref="A32"/>
+    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="190" zoomScaleNormal="190" workbookViewId="0">
+      <selection activeCell="K16" sqref="K16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
@@ -1694,7 +1702,7 @@
       <c r="A16" s="49" t="s">
         <v>150</v>
       </c>
-      <c r="B16" s="49" t="s">
+      <c r="B16" s="89" t="s">
         <v>151</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Chap 5, 7 10, after TR review
</commit_message>
<xml_diff>
--- a/Word/PlanAndDealines.xlsx
+++ b/Word/PlanAndDealines.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20376"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20377"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ksungAD\Desktop\GitHub\GTCS-GameEngine2\Word\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ksung\Desktop\GitHub\GTCS-GameEngine2\Word\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0F859D6B-ED83-4693-A0C5-34F3AE6B7F10}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4641C9C2-0B2E-4631-89D0-14E0352908B5}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="33648" windowHeight="15858" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="33645" windowHeight="15855" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Final Changes Must make" sheetId="8" r:id="rId1"/>
@@ -830,7 +830,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="45">
+  <fonts count="46">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -1102,6 +1102,12 @@
       <name val="Arial"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="10"/>
+      <color theme="0" tint="-0.14996795556505021"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
   </fonts>
   <fills count="4">
     <fill>
@@ -1208,7 +1214,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="98">
+  <cellXfs count="99">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
@@ -1423,6 +1429,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="45" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1640,11 +1647,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D8AC00B6-697C-45E4-9E65-51AD1E2696C6}">
   <dimension ref="A3:R47"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="B22" sqref="B22"/>
+    <sheetView tabSelected="1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
+      <selection activeCell="N25" sqref="N25"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.3"/>
+  <sheetFormatPr defaultRowHeight="12.75"/>
   <sheetData>
     <row r="3" spans="1:18">
       <c r="A3" s="50" t="s">
@@ -1656,7 +1663,7 @@
         <v>153</v>
       </c>
     </row>
-    <row r="5" spans="1:18" ht="12.6">
+    <row r="5" spans="1:18">
       <c r="B5" s="50" t="s">
         <v>132</v>
       </c>
@@ -1799,7 +1806,7 @@
       <c r="A24" s="50" t="s">
         <v>145</v>
       </c>
-      <c r="B24" t="s">
+      <c r="B24" s="98" t="s">
         <v>146</v>
       </c>
     </row>
@@ -1897,7 +1904,7 @@
         <v>159</v>
       </c>
     </row>
-    <row r="41" spans="1:12" ht="15">
+    <row r="41" spans="1:12" ht="15.75">
       <c r="A41" s="12" t="s">
         <v>58</v>
       </c>
@@ -1977,11 +1984,11 @@
       <selection activeCell="V16" sqref="V16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15.75" customHeight="1"/>
+  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1"/>
   <cols>
-    <col min="7" max="7" width="1.83203125" customWidth="1"/>
-    <col min="8" max="8" width="9.44140625" customWidth="1"/>
-    <col min="9" max="9" width="9.5546875" customWidth="1"/>
+    <col min="7" max="7" width="1.85546875" customWidth="1"/>
+    <col min="8" max="8" width="9.42578125" customWidth="1"/>
+    <col min="9" max="9" width="9.5703125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="2:12" ht="15.75" customHeight="1">
@@ -2000,7 +2007,7 @@
       <c r="I2" s="94"/>
       <c r="J2" s="94"/>
     </row>
-    <row r="3" spans="2:12" ht="12.3">
+    <row r="3" spans="2:12" ht="12.75">
       <c r="B3" s="3" t="s">
         <v>19</v>
       </c>
@@ -2029,7 +2036,7 @@
       <c r="K3" s="5"/>
       <c r="L3" s="5"/>
     </row>
-    <row r="4" spans="2:12" ht="12.3">
+    <row r="4" spans="2:12" ht="12.75">
       <c r="B4" s="6" t="s">
         <v>24</v>
       </c>
@@ -2055,7 +2062,7 @@
       <c r="K4" s="5"/>
       <c r="L4" s="5"/>
     </row>
-    <row r="5" spans="2:12" ht="12.3">
+    <row r="5" spans="2:12" ht="12.75">
       <c r="B5" s="6" t="s">
         <v>25</v>
       </c>
@@ -2083,7 +2090,7 @@
       <c r="K5" s="5"/>
       <c r="L5" s="5"/>
     </row>
-    <row r="6" spans="2:12" ht="12.3">
+    <row r="6" spans="2:12" ht="12.75">
       <c r="B6" s="6" t="s">
         <v>27</v>
       </c>
@@ -2141,7 +2148,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="8" spans="2:12" ht="12.3">
+    <row r="8" spans="2:12" ht="12.75">
       <c r="B8" s="6" t="s">
         <v>32</v>
       </c>
@@ -2171,7 +2178,7 @@
       </c>
       <c r="L8" s="5"/>
     </row>
-    <row r="9" spans="2:12" ht="12.3">
+    <row r="9" spans="2:12" ht="12.75">
       <c r="B9" s="6" t="s">
         <v>35</v>
       </c>
@@ -2197,7 +2204,7 @@
       <c r="K9" s="5"/>
       <c r="L9" s="5"/>
     </row>
-    <row r="10" spans="2:12" ht="12.3">
+    <row r="10" spans="2:12" ht="12.75">
       <c r="B10" s="6" t="s">
         <v>36</v>
       </c>
@@ -2225,7 +2232,7 @@
       <c r="K10" s="5"/>
       <c r="L10" s="5"/>
     </row>
-    <row r="11" spans="2:12" ht="12.3">
+    <row r="11" spans="2:12" ht="12.75">
       <c r="B11" s="6" t="s">
         <v>38</v>
       </c>
@@ -2339,7 +2346,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="15" spans="2:12" ht="12.3">
+    <row r="15" spans="2:12" ht="12.75">
       <c r="B15" s="6" t="s">
         <v>50</v>
       </c>
@@ -2367,7 +2374,7 @@
       <c r="K15" s="5"/>
       <c r="L15" s="5"/>
     </row>
-    <row r="16" spans="2:12" ht="12.3">
+    <row r="16" spans="2:12" ht="12.75">
       <c r="B16" s="6" t="s">
         <v>52</v>
       </c>
@@ -2395,7 +2402,7 @@
       <c r="K16" s="5"/>
       <c r="L16" s="5"/>
     </row>
-    <row r="17" spans="2:12" ht="12.3">
+    <row r="17" spans="2:12" ht="12.75">
       <c r="B17" s="5"/>
       <c r="C17" s="5"/>
       <c r="D17" s="5"/>
@@ -2410,7 +2417,7 @@
       <c r="K17" s="5"/>
       <c r="L17" s="5"/>
     </row>
-    <row r="18" spans="2:12" ht="12.3">
+    <row r="18" spans="2:12" ht="12.75">
       <c r="B18" s="5"/>
       <c r="C18" s="5"/>
       <c r="D18" s="5"/>
@@ -2423,19 +2430,19 @@
       <c r="K18" s="5"/>
       <c r="L18" s="5"/>
     </row>
-    <row r="23" spans="2:12" ht="12.3">
+    <row r="23" spans="2:12" ht="12.75">
       <c r="B23" s="2" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="24" spans="2:12" ht="12.3">
+    <row r="24" spans="2:12" ht="12.75">
       <c r="B24" s="10" t="s">
         <v>55</v>
       </c>
       <c r="C24" s="11"/>
       <c r="D24" s="11"/>
     </row>
-    <row r="25" spans="2:12" ht="12.3">
+    <row r="25" spans="2:12" ht="12.75">
       <c r="B25" s="12" t="s">
         <v>56</v>
       </c>
@@ -2444,7 +2451,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="26" spans="2:12" ht="15">
+    <row r="26" spans="2:12">
       <c r="B26" s="12" t="s">
         <v>58</v>
       </c>
@@ -2453,7 +2460,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="27" spans="2:12" ht="12.3">
+    <row r="27" spans="2:12" ht="12.75">
       <c r="B27" s="12" t="s">
         <v>60</v>
       </c>
@@ -2462,7 +2469,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="28" spans="2:12" ht="12.3">
+    <row r="28" spans="2:12" ht="12.75">
       <c r="B28" s="12" t="s">
         <v>62</v>
       </c>
@@ -2471,7 +2478,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="29" spans="2:12" ht="12.3">
+    <row r="29" spans="2:12" ht="12.75">
       <c r="B29" s="12" t="s">
         <v>63</v>
       </c>
@@ -2480,7 +2487,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="30" spans="2:12" ht="12.3">
+    <row r="30" spans="2:12" ht="12.75">
       <c r="B30" s="12" t="s">
         <v>65</v>
       </c>
@@ -2489,7 +2496,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="31" spans="2:12" ht="12.3">
+    <row r="31" spans="2:12" ht="12.75">
       <c r="B31" s="12" t="s">
         <v>67</v>
       </c>
@@ -2498,7 +2505,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="32" spans="2:12" ht="12.3">
+    <row r="32" spans="2:12" ht="12.75">
       <c r="B32" s="12" t="s">
         <v>40</v>
       </c>
@@ -2534,24 +2541,24 @@
       <selection activeCell="P18" sqref="P18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15.75" customHeight="1"/>
+  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1"/>
   <cols>
-    <col min="3" max="4" width="1.71875" customWidth="1"/>
-    <col min="5" max="5" width="7.44140625" style="31" customWidth="1"/>
-    <col min="6" max="6" width="7.44140625" style="30" customWidth="1"/>
-    <col min="7" max="7" width="7.44140625" style="31" customWidth="1"/>
+    <col min="3" max="4" width="1.7109375" customWidth="1"/>
+    <col min="5" max="5" width="7.42578125" style="31" customWidth="1"/>
+    <col min="6" max="6" width="7.42578125" style="30" customWidth="1"/>
+    <col min="7" max="7" width="7.42578125" style="31" customWidth="1"/>
     <col min="8" max="8" width="8" style="30" customWidth="1"/>
-    <col min="9" max="9" width="7.44140625" style="31" customWidth="1"/>
-    <col min="10" max="10" width="7.44140625" style="30" customWidth="1"/>
-    <col min="11" max="11" width="7.44140625" style="31" customWidth="1"/>
-    <col min="12" max="12" width="8.44140625" style="30" customWidth="1"/>
-    <col min="13" max="13" width="7.44140625" style="31" customWidth="1"/>
-    <col min="14" max="14" width="7.44140625" style="30" customWidth="1"/>
-    <col min="15" max="15" width="16.44140625" style="29" customWidth="1"/>
-    <col min="16" max="16" width="14.44140625" style="27"/>
+    <col min="9" max="9" width="7.42578125" style="31" customWidth="1"/>
+    <col min="10" max="10" width="7.42578125" style="30" customWidth="1"/>
+    <col min="11" max="11" width="7.42578125" style="31" customWidth="1"/>
+    <col min="12" max="12" width="8.42578125" style="30" customWidth="1"/>
+    <col min="13" max="13" width="7.42578125" style="31" customWidth="1"/>
+    <col min="14" max="14" width="7.42578125" style="30" customWidth="1"/>
+    <col min="15" max="15" width="16.42578125" style="29" customWidth="1"/>
+    <col min="16" max="16" width="14.42578125" style="27"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:19" ht="12.3">
+    <row r="1" spans="2:19" ht="12.75">
       <c r="C1" s="1"/>
       <c r="D1" s="1"/>
       <c r="E1" s="96" t="s">
@@ -2584,7 +2591,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="2" spans="2:19" ht="12.6" thickBot="1">
+    <row r="2" spans="2:19" ht="13.5" thickBot="1">
       <c r="C2" s="1"/>
       <c r="D2" s="1"/>
       <c r="E2" s="32" t="s">
@@ -4870,18 +4877,18 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15.75" customHeight="1"/>
+  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1"/>
   <cols>
-    <col min="2" max="2" width="33.1640625" customWidth="1"/>
-    <col min="3" max="3" width="27.71875" customWidth="1"/>
+    <col min="2" max="2" width="33.140625" customWidth="1"/>
+    <col min="3" max="3" width="27.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" ht="12.3">
+    <row r="1" spans="1:10" ht="12.75">
       <c r="A1" s="14" t="s">
         <v>70</v>
       </c>
     </row>
-    <row r="2" spans="1:10" ht="12.3">
+    <row r="2" spans="1:10" ht="12.75">
       <c r="B2" s="14" t="s">
         <v>19</v>
       </c>
@@ -4901,7 +4908,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="3" spans="1:10" ht="12.3">
+    <row r="3" spans="1:10" ht="12.75">
       <c r="B3" s="2" t="s">
         <v>76</v>
       </c>
@@ -4912,7 +4919,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="4" spans="1:10" ht="12.3">
+    <row r="4" spans="1:10" ht="12.75">
       <c r="C4" s="2" t="s">
         <v>79</v>
       </c>
@@ -4920,20 +4927,20 @@
         <v>80</v>
       </c>
     </row>
-    <row r="5" spans="1:10" ht="13.8">
+    <row r="5" spans="1:10" ht="14.25">
       <c r="C5" s="2" t="s">
         <v>81</v>
       </c>
       <c r="H5" s="15"/>
       <c r="J5" s="16"/>
     </row>
-    <row r="6" spans="1:10" ht="12.6">
+    <row r="6" spans="1:10" ht="12.75">
       <c r="C6" s="2" t="s">
         <v>82</v>
       </c>
       <c r="J6" s="17"/>
     </row>
-    <row r="7" spans="1:10" ht="12.3">
+    <row r="7" spans="1:10" ht="12.75">
       <c r="C7" s="2" t="s">
         <v>83</v>
       </c>
@@ -4942,7 +4949,7 @@
       <c r="H8" s="18"/>
       <c r="I8" s="18"/>
     </row>
-    <row r="9" spans="1:10" ht="13.8">
+    <row r="9" spans="1:10" ht="14.25">
       <c r="B9" s="19" t="s">
         <v>84</v>
       </c>
@@ -4970,7 +4977,7 @@
     <row r="13" spans="1:10" ht="15.75" customHeight="1">
       <c r="J13" s="21"/>
     </row>
-    <row r="15" spans="1:10" ht="12.3">
+    <row r="15" spans="1:10" ht="12.75">
       <c r="B15" s="2" t="s">
         <v>88</v>
       </c>
@@ -4981,12 +4988,12 @@
         <v>15</v>
       </c>
     </row>
-    <row r="16" spans="1:10" ht="12.3">
+    <row r="16" spans="1:10" ht="12.75">
       <c r="C16" s="2" t="s">
         <v>90</v>
       </c>
     </row>
-    <row r="17" spans="1:9" ht="12.3">
+    <row r="17" spans="1:9" ht="12.75">
       <c r="G17" s="14"/>
     </row>
     <row r="18" spans="1:9" ht="15.75" customHeight="1">
@@ -4995,17 +5002,17 @@
     <row r="19" spans="1:9" ht="15.75" customHeight="1">
       <c r="I19" s="21"/>
     </row>
-    <row r="20" spans="1:9" ht="12.3">
+    <row r="20" spans="1:9" ht="12.75">
       <c r="B20" s="2" t="s">
         <v>91</v>
       </c>
     </row>
-    <row r="29" spans="1:9" ht="12.3">
+    <row r="29" spans="1:9" ht="12.75">
       <c r="A29" s="14" t="s">
         <v>92</v>
       </c>
     </row>
-    <row r="30" spans="1:9" ht="13.8">
+    <row r="30" spans="1:9" ht="14.25">
       <c r="B30" s="15" t="s">
         <v>93</v>
       </c>
@@ -5013,7 +5020,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="31" spans="1:9" ht="12.6">
+    <row r="31" spans="1:9" ht="12.75">
       <c r="D31" s="22" t="s">
         <v>95</v>
       </c>
@@ -5026,7 +5033,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="34" spans="1:4" ht="13.8">
+    <row r="34" spans="1:4" ht="14.25">
       <c r="C34" s="24" t="s">
         <v>98</v>
       </c>
@@ -5052,7 +5059,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="42" spans="1:4" ht="12.3">
+    <row r="42" spans="1:4" ht="12.75">
       <c r="A42" s="14"/>
     </row>
     <row r="43" spans="1:4" ht="15.75" customHeight="1">
@@ -5083,10 +5090,10 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15.75" customHeight="1"/>
+  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1"/>
   <cols>
-    <col min="2" max="2" width="35.71875" customWidth="1"/>
-    <col min="3" max="3" width="36.44140625" customWidth="1"/>
+    <col min="2" max="2" width="35.7109375" customWidth="1"/>
+    <col min="3" max="3" width="36.42578125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" ht="15.75" customHeight="1">
@@ -5142,10 +5149,10 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15.75" customHeight="1"/>
+  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1"/>
   <cols>
-    <col min="2" max="2" width="35.71875" customWidth="1"/>
-    <col min="3" max="3" width="36.44140625" customWidth="1"/>
+    <col min="2" max="2" width="35.7109375" customWidth="1"/>
+    <col min="3" max="3" width="36.42578125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" ht="15.75" customHeight="1">
@@ -5199,10 +5206,10 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15.75" customHeight="1"/>
+  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1"/>
   <cols>
-    <col min="2" max="2" width="35.71875" customWidth="1"/>
-    <col min="3" max="3" width="36.44140625" customWidth="1"/>
+    <col min="2" max="2" width="35.7109375" customWidth="1"/>
+    <col min="3" max="3" width="36.42578125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" ht="15.75" customHeight="1">
@@ -5246,10 +5253,10 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15.75" customHeight="1"/>
+  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1"/>
   <cols>
-    <col min="2" max="2" width="35.71875" customWidth="1"/>
-    <col min="3" max="3" width="36.44140625" customWidth="1"/>
+    <col min="2" max="2" width="35.7109375" customWidth="1"/>
+    <col min="3" max="3" width="36.42578125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" ht="15.75" customHeight="1">

</xml_diff>

<commit_message>
Update file names to show not being worked on
</commit_message>
<xml_diff>
--- a/Word/PlanAndDealines.xlsx
+++ b/Word/PlanAndDealines.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ksung\Desktop\GitHub\GTCS-GameEngine2\Word\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4641C9C2-0B2E-4631-89D0-14E0352908B5}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3570CE91-0F6B-451A-A76C-8CA88D8216F4}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="33645" windowHeight="15855" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -550,20 +550,6 @@
         <family val="2"/>
       </rPr>
       <t>Need to review Chapters 1, 2, 3, 4, 5]</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">texture.js: </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FF000000"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t>unload must check if can actually delete</t>
     </r>
   </si>
   <si>
@@ -824,6 +810,20 @@
   </si>
   <si>
     <t>resource_map: now has reference count!</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">texture.js: </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="0" tint="-0.24994659260841701"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>unload must check if can actually delete</t>
+    </r>
   </si>
 </sst>
 </file>
@@ -1214,7 +1214,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="99">
+  <cellXfs count="100">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
@@ -1430,6 +1430,7 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="45" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="44" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1648,7 +1649,7 @@
   <dimension ref="A3:R47"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="N25" sqref="N25"/>
+      <selection activeCell="B25" sqref="B25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
@@ -1718,13 +1719,13 @@
     </row>
     <row r="9" spans="1:18">
       <c r="A9" s="49" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="C9" s="50"/>
     </row>
     <row r="10" spans="1:18">
       <c r="B10" s="60" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="C10" s="50"/>
     </row>
@@ -1771,7 +1772,7 @@
       <c r="A19" s="50"/>
       <c r="B19" s="49"/>
       <c r="C19" s="88" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
     </row>
     <row r="20" spans="1:3">
@@ -1779,27 +1780,27 @@
         <v>148</v>
       </c>
       <c r="B20" s="93" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
     </row>
     <row r="21" spans="1:3">
       <c r="A21" s="50"/>
       <c r="B21" s="76" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
     </row>
     <row r="22" spans="1:3">
       <c r="A22" s="50" t="s">
+        <v>183</v>
+      </c>
+      <c r="B22" s="93" t="s">
         <v>184</v>
-      </c>
-      <c r="B22" s="93" t="s">
-        <v>185</v>
       </c>
     </row>
     <row r="23" spans="1:3">
       <c r="A23" s="50"/>
       <c r="B23" s="93" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
     </row>
     <row r="24" spans="1:3">
@@ -1812,69 +1813,69 @@
     </row>
     <row r="25" spans="1:3">
       <c r="A25" s="49"/>
-      <c r="B25" s="50" t="s">
-        <v>154</v>
+      <c r="B25" s="99" t="s">
+        <v>185</v>
       </c>
     </row>
     <row r="26" spans="1:3">
       <c r="A26" s="50" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="B26" s="50"/>
     </row>
     <row r="27" spans="1:3">
       <c r="A27" s="50"/>
       <c r="B27" s="49" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
     </row>
     <row r="28" spans="1:3">
       <c r="A28" s="50" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="B28" s="50" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
     </row>
     <row r="29" spans="1:3">
       <c r="A29" s="49"/>
       <c r="B29" s="49" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
     </row>
     <row r="30" spans="1:3">
       <c r="A30" s="49"/>
       <c r="B30" s="50" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
     </row>
     <row r="31" spans="1:3">
       <c r="B31" s="50" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
     </row>
     <row r="32" spans="1:3">
       <c r="C32" s="65" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
     </row>
     <row r="33" spans="1:12">
       <c r="A33" s="50" t="s">
+        <v>173</v>
+      </c>
+      <c r="B33" s="49" t="s">
         <v>174</v>
-      </c>
-      <c r="B33" s="49" t="s">
-        <v>175</v>
       </c>
     </row>
     <row r="34" spans="1:12">
       <c r="A34" s="50"/>
       <c r="B34" s="49" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
     </row>
     <row r="35" spans="1:12">
       <c r="A35" s="50" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
     </row>
     <row r="38" spans="1:12">
@@ -1889,7 +1890,7 @@
       <c r="B39" s="11"/>
       <c r="C39" s="11"/>
       <c r="K39" s="49" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
     </row>
     <row r="40" spans="1:12">
@@ -1901,7 +1902,7 @@
         <v>57</v>
       </c>
       <c r="L40" s="49" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
     </row>
     <row r="41" spans="1:12" ht="15.75">
@@ -1996,13 +1997,13 @@
     </row>
     <row r="2" spans="2:12" ht="15.75" customHeight="1">
       <c r="D2" s="94" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="E2" s="95"/>
       <c r="F2" s="95"/>
       <c r="G2" s="90"/>
       <c r="H2" s="94" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="I2" s="94"/>
       <c r="J2" s="94"/>
@@ -2031,7 +2032,7 @@
         <v>22</v>
       </c>
       <c r="J3" s="50" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="K3" s="5"/>
       <c r="L3" s="5"/>
@@ -2999,7 +3000,7 @@
     </row>
     <row r="11" spans="2:19" ht="26.25" customHeight="1">
       <c r="B11" s="75" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="C11" s="76"/>
       <c r="D11" s="76"/>
@@ -3045,7 +3046,7 @@
     </row>
     <row r="12" spans="2:19" ht="26.25" customHeight="1">
       <c r="B12" s="75" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="C12" s="76"/>
       <c r="D12" s="76"/>
@@ -3062,7 +3063,7 @@
         <v>44375</v>
       </c>
       <c r="I12" s="77" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="J12" s="78">
         <v>44378</v>
@@ -3083,7 +3084,7 @@
     </row>
     <row r="13" spans="2:19" ht="26.25" customHeight="1">
       <c r="B13" s="75" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="C13" s="76"/>
       <c r="D13" s="76"/>
@@ -3225,7 +3226,7 @@
       <c r="C16" s="82"/>
       <c r="D16" s="82"/>
       <c r="E16" s="83" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="F16" s="84">
         <v>44346</v>
@@ -3234,7 +3235,7 @@
         <v>6</v>
       </c>
       <c r="H16" s="85" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="I16" s="83" t="s">
         <v>8</v>
@@ -3249,7 +3250,7 @@
         <v>44383</v>
       </c>
       <c r="M16" s="86" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="N16" s="85"/>
       <c r="O16" s="67">
@@ -3277,7 +3278,7 @@
       <c r="L17" s="36"/>
       <c r="M17" s="36"/>
       <c r="N17" s="68" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="P17" s="69">
         <v>44368</v>

</xml_diff>

<commit_message>
Progress on Chap 7
</commit_message>
<xml_diff>
--- a/Word/PlanAndDealines.xlsx
+++ b/Word/PlanAndDealines.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ksung\Desktop\GitHub\GTCS-GameEngine2\Word\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DDFDE18F-5070-45B5-80EE-CF3B8C3C88B2}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4A09DCDB-04EC-4479-9760-F8561B3D54E3}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="33645" windowHeight="15855" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="33645" windowHeight="15855" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Final Changes Must make" sheetId="8" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="313" uniqueCount="192">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="317" uniqueCount="196">
   <si>
     <t>First Pass</t>
   </si>
@@ -557,79 +557,6 @@
     <t>Chapter 7</t>
   </si>
   <si>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="10"/>
-        <color rgb="FF000000"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">Organize the Source Code: </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FF000000"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">compare this section to </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="10"/>
-        <color rgb="FF000000"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t>Chapter 6: Organize the source code</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FF000000"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve"> and refine. </t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">Remove: </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FF000000"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">the note on top of Page 6 (on </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="10"/>
-        <color rgb="FF000000"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t>aClass.prototype.method</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FF000000"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t>)</t>
-    </r>
-  </si>
-  <si>
     <t>Chapter 9 (Physics): should</t>
   </si>
   <si>
@@ -642,86 +569,7 @@
     <t>Lastly, remember to update the engine access file, index.js, to forward the newly defined functionality to the client.</t>
   </si>
   <si>
-    <r>
-      <t xml:space="preserve">Index.js: </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FF000000"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t>change into one sentence "Lastly, remember to update the engine access file, index.js, to forward the newly defined functionality to the client.</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="10"/>
-        <color rgb="FF000000"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t>"  (introduced in Chapter 6.1)</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">Need to: </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FF000000"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">Add in for CameraState (7.2) NOT exporting to the user … </t>
-    </r>
-  </si>
-  <si>
     <t>Example 3.1, when introduce the core folder, explain ALL modules within this folder are internal to the engine, NOT exported through index.js</t>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">Note that as the sophistication of the engine increases, so does the complexity of the supporting code. In this case, you have designed a internal utility class, </t>
-    </r>
-    <r>
-      <rPr>
-        <i/>
-        <sz val="9"/>
-        <rFont val="TheSansMonoConNormal"/>
-      </rPr>
-      <t xml:space="preserve">CameraState, </t>
-    </r>
-    <r>
-      <rPr>
-        <i/>
-        <sz val="9"/>
-        <color rgb="FF000000"/>
-        <rFont val="Utopia"/>
-      </rPr>
-      <t xml:space="preserve">for storing Camera internal state to support interpolation. This is an internal engine operation. There is no reason for the game programmer to access this class and thus the engine access file, </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <i/>
-        <sz val="9"/>
-        <color rgb="FF000000"/>
-        <rFont val="Utopia"/>
-      </rPr>
-      <t>index.js</t>
-    </r>
-    <r>
-      <rPr>
-        <i/>
-        <sz val="9"/>
-        <color rgb="FF000000"/>
-        <rFont val="Utopia"/>
-      </rPr>
-      <t>, should not be modified to forward the definition of this class.</t>
-    </r>
   </si>
   <si>
     <t>Jason</t>
@@ -843,6 +691,192 @@
   </si>
   <si>
     <t>Received on</t>
+  </si>
+  <si>
+    <t>Figure 8-3 (page 13), Shader &lt;-- should be replaced with SimpleShader</t>
+  </si>
+  <si>
+    <t>Figure 8-5 (page 26), Shader &lt;-- should be replaced with SimpleShader</t>
+  </si>
+  <si>
+    <t>Figure 8-19 (page 53), Shader &lt;-- should be replaced with SimpleShader</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Index.js: </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="0" tint="-0.249977111117893"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>change into one sentence "Lastly, remember to update the engine access file, index.js, to forward the newly defined functionality to the client.</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color theme="0" tint="-0.249977111117893"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>"  (introduced in Chapter 6.1)</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color theme="0" tint="-0.24994659260841701"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">Organize the Source Code: </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="0" tint="-0.24994659260841701"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">compare this section to </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color theme="0" tint="-0.24994659260841701"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>Chapter 6: Organize the source code</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="0" tint="-0.24994659260841701"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> and refine. </t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Copy this note (from 7.2 on </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color theme="0" tint="-0.249977111117893"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>aClass.prototype.method</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="0" tint="-0.249977111117893"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>) over to Page-40, righ before Implement Per-Pixel Collision section</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Remove: </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="0" tint="-0.249977111117893"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">the note on top of Page 6 (on </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color theme="0" tint="-0.249977111117893"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>aClass.prototype.method</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="0" tint="-0.249977111117893"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>)</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Need to: </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="0" tint="-0.249977111117893"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">Add in for CameraState (7.2) NOT exporting to the user … </t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Note that as the sophistication of the engine increases, so does the complexity of the supporting code. In this case, you have designed a internal utility class, </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="9"/>
+        <color theme="0" tint="-0.249977111117893"/>
+        <rFont val="TheSansMonoConNormal"/>
+      </rPr>
+      <t xml:space="preserve">CameraState, </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="9"/>
+        <color theme="0" tint="-0.249977111117893"/>
+        <rFont val="Utopia"/>
+      </rPr>
+      <t xml:space="preserve">for storing Camera internal state to support interpolation. This is an internal engine operation. There is no reason for the game programmer to access this class and thus the engine access file, </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <i/>
+        <sz val="9"/>
+        <color theme="0" tint="-0.249977111117893"/>
+        <rFont val="Utopia"/>
+      </rPr>
+      <t>index.js</t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="9"/>
+        <color theme="0" tint="-0.249977111117893"/>
+        <rFont val="Utopia"/>
+      </rPr>
+      <t>, should not be modified to forward the definition of this class.</t>
+    </r>
   </si>
 </sst>
 </file>
@@ -1044,24 +1078,6 @@
       <name val="Utopia"/>
     </font>
     <font>
-      <i/>
-      <sz val="9"/>
-      <color rgb="FF000000"/>
-      <name val="Utopia"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="9"/>
-      <name val="TheSansMonoConNormal"/>
-    </font>
-    <font>
-      <b/>
-      <i/>
-      <sz val="9"/>
-      <color rgb="FF000000"/>
-      <name val="Utopia"/>
-    </font>
-    <font>
       <sz val="10"/>
       <color theme="1"/>
       <name val="Arial"/>
@@ -1126,6 +1142,25 @@
       <color theme="0" tint="-0.14996795556505021"/>
       <name val="Arial"/>
       <family val="2"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="9"/>
+      <color theme="0" tint="-0.249977111117893"/>
+      <name val="Utopia"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="9"/>
+      <color theme="0" tint="-0.249977111117893"/>
+      <name val="TheSansMonoConNormal"/>
+    </font>
+    <font>
+      <b/>
+      <i/>
+      <sz val="9"/>
+      <color theme="0" tint="-0.249977111117893"/>
+      <name val="Utopia"/>
     </font>
   </fonts>
   <fills count="5">
@@ -1381,69 +1416,68 @@
     <xf numFmtId="0" fontId="30" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="33" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center"/>
+    <xf numFmtId="0" fontId="33" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="16" fontId="20" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="20" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="14" fontId="20" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="34" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="35" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="35" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="16" fontId="35" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="36" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="37" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="37" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="16" fontId="37" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="36" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="16" fontId="20" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="37" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="20" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="36" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="37" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="37" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="14" fontId="20" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="37" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="16" fontId="37" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="37" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="36" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
     <xf numFmtId="0" fontId="38" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="38" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="16" fontId="38" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf numFmtId="0" fontId="39" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="40" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="40" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="16" fontId="40" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="39" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="40" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="39" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="40" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="40" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="16" fontId="40" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="40" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="39" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="41" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="42" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="43" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="45" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="44" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="40" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="42" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="41" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="20" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1456,8 +1490,9 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="43" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1673,10 +1708,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D8AC00B6-697C-45E4-9E65-51AD1E2696C6}">
-  <dimension ref="A3:R47"/>
+  <dimension ref="A3:R51"/>
   <sheetViews>
-    <sheetView zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="B25" sqref="B25"/>
+    <sheetView tabSelected="1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
+      <selection activeCell="H25" sqref="H25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
@@ -1746,13 +1781,13 @@
     </row>
     <row r="9" spans="1:18">
       <c r="A9" s="49" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="C9" s="50"/>
     </row>
     <row r="10" spans="1:18">
       <c r="B10" s="60" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="C10" s="50"/>
     </row>
@@ -1775,7 +1810,7 @@
       <c r="A16" s="49" t="s">
         <v>149</v>
       </c>
-      <c r="B16" s="87" t="s">
+      <c r="B16" s="86" t="s">
         <v>150</v>
       </c>
     </row>
@@ -1783,215 +1818,241 @@
       <c r="A17" s="50" t="s">
         <v>144</v>
       </c>
-      <c r="B17" s="76" t="s">
+      <c r="B17" s="75" t="s">
         <v>151</v>
       </c>
-      <c r="C17" s="76"/>
+      <c r="C17" s="75"/>
     </row>
     <row r="18" spans="1:3">
       <c r="A18" s="50"/>
-      <c r="B18" s="76"/>
-      <c r="C18" s="76" t="s">
+      <c r="B18" s="75"/>
+      <c r="C18" s="75" t="s">
         <v>147</v>
       </c>
     </row>
     <row r="19" spans="1:3">
       <c r="A19" s="50"/>
       <c r="B19" s="49"/>
-      <c r="C19" s="88" t="s">
-        <v>166</v>
+      <c r="C19" s="87" t="s">
+        <v>161</v>
       </c>
     </row>
     <row r="20" spans="1:3">
       <c r="A20" s="50" t="s">
         <v>148</v>
       </c>
-      <c r="B20" s="93" t="s">
-        <v>180</v>
+      <c r="B20" s="92" t="s">
+        <v>175</v>
       </c>
     </row>
     <row r="21" spans="1:3">
       <c r="A21" s="50"/>
-      <c r="B21" s="76" t="s">
-        <v>163</v>
+      <c r="B21" s="75" t="s">
+        <v>159</v>
       </c>
     </row>
     <row r="22" spans="1:3">
       <c r="A22" s="50" t="s">
-        <v>183</v>
-      </c>
-      <c r="B22" s="93" t="s">
-        <v>184</v>
+        <v>178</v>
+      </c>
+      <c r="B22" s="92" t="s">
+        <v>179</v>
       </c>
     </row>
     <row r="23" spans="1:3">
       <c r="A23" s="50"/>
-      <c r="B23" s="93" t="s">
-        <v>181</v>
+      <c r="B23" s="92" t="s">
+        <v>176</v>
       </c>
     </row>
     <row r="24" spans="1:3">
       <c r="A24" s="50" t="s">
         <v>145</v>
       </c>
-      <c r="B24" s="94" t="s">
+      <c r="B24" s="93" t="s">
         <v>146</v>
       </c>
     </row>
     <row r="25" spans="1:3">
       <c r="A25" s="49"/>
-      <c r="B25" s="95" t="s">
-        <v>185</v>
+      <c r="B25" s="94" t="s">
+        <v>180</v>
       </c>
     </row>
     <row r="26" spans="1:3">
       <c r="A26" s="50" t="s">
-        <v>182</v>
+        <v>177</v>
       </c>
       <c r="B26" s="50"/>
     </row>
     <row r="27" spans="1:3">
       <c r="A27" s="50"/>
       <c r="B27" s="49" t="s">
-        <v>181</v>
+        <v>176</v>
       </c>
     </row>
     <row r="28" spans="1:3">
-      <c r="A28" s="50" t="s">
+      <c r="A28" s="50"/>
+      <c r="B28" s="75" t="s">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3">
+      <c r="A29" s="50" t="s">
         <v>154</v>
       </c>
-      <c r="B28" s="50" t="s">
-        <v>161</v>
-      </c>
-    </row>
-    <row r="29" spans="1:3">
-      <c r="A29" s="49"/>
-      <c r="B29" s="49" t="s">
-        <v>155</v>
+      <c r="B29" s="74" t="s">
+        <v>190</v>
       </c>
     </row>
     <row r="30" spans="1:3">
       <c r="A30" s="49"/>
-      <c r="B30" s="50" t="s">
-        <v>156</v>
+      <c r="B30" s="92" t="s">
+        <v>191</v>
       </c>
     </row>
     <row r="31" spans="1:3">
-      <c r="B31" s="50" t="s">
-        <v>162</v>
+      <c r="A31" s="49"/>
+      <c r="B31" s="74" t="s">
+        <v>193</v>
       </c>
     </row>
     <row r="32" spans="1:3">
-      <c r="C32" s="65" t="s">
-        <v>164</v>
-      </c>
+      <c r="B32" s="74" t="s">
+        <v>194</v>
+      </c>
+      <c r="C32" s="75"/>
     </row>
     <row r="33" spans="1:12">
-      <c r="A33" s="50" t="s">
-        <v>173</v>
-      </c>
-      <c r="B33" s="49" t="s">
+      <c r="B33" s="75"/>
+      <c r="C33" s="101" t="s">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="34" spans="1:12">
+      <c r="A34" s="50" t="s">
+        <v>168</v>
+      </c>
+      <c r="B34" s="49" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="35" spans="1:12">
+      <c r="A35" s="50"/>
+      <c r="B35" s="49" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="36" spans="1:12">
+      <c r="A36" s="50"/>
+      <c r="B36" s="49" t="s">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="37" spans="1:12">
+      <c r="A37" s="50"/>
+      <c r="B37" s="49" t="s">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="38" spans="1:12">
+      <c r="A38" s="50"/>
+      <c r="B38" s="49" t="s">
         <v>174</v>
       </c>
     </row>
-    <row r="34" spans="1:12">
-      <c r="A34" s="50"/>
-      <c r="B34" s="49" t="s">
-        <v>179</v>
-      </c>
-    </row>
-    <row r="35" spans="1:12">
-      <c r="A35" s="50" t="s">
-        <v>175</v>
-      </c>
-    </row>
-    <row r="38" spans="1:12">
-      <c r="A38" s="2" t="s">
+    <row r="39" spans="1:12">
+      <c r="A39" s="50" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="42" spans="1:12">
+      <c r="A42" s="2" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="39" spans="1:12">
-      <c r="A39" s="10" t="s">
+    <row r="43" spans="1:12">
+      <c r="A43" s="10" t="s">
         <v>55</v>
       </c>
-      <c r="B39" s="11"/>
-      <c r="C39" s="11"/>
-      <c r="K39" s="49" t="s">
-        <v>157</v>
-      </c>
-    </row>
-    <row r="40" spans="1:12">
-      <c r="A40" s="12" t="s">
-        <v>56</v>
-      </c>
-      <c r="B40" s="11"/>
-      <c r="C40" s="10" t="s">
-        <v>57</v>
-      </c>
-      <c r="L40" s="49" t="s">
-        <v>158</v>
-      </c>
-    </row>
-    <row r="41" spans="1:12" ht="15.75">
-      <c r="A41" s="12" t="s">
-        <v>58</v>
-      </c>
-      <c r="B41" s="11"/>
-      <c r="C41" s="13" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="42" spans="1:12">
-      <c r="A42" s="12" t="s">
-        <v>60</v>
-      </c>
-      <c r="B42" s="11"/>
-      <c r="C42" s="10" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="43" spans="1:12">
-      <c r="A43" s="12" t="s">
-        <v>62</v>
-      </c>
       <c r="B43" s="11"/>
-      <c r="C43" s="10" t="s">
-        <v>61</v>
+      <c r="C43" s="11"/>
+      <c r="K43" s="49" t="s">
+        <v>155</v>
       </c>
     </row>
     <row r="44" spans="1:12">
       <c r="A44" s="12" t="s">
-        <v>63</v>
+        <v>56</v>
       </c>
       <c r="B44" s="11"/>
       <c r="C44" s="10" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="45" spans="1:12">
+        <v>57</v>
+      </c>
+      <c r="L44" s="49" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="45" spans="1:12" ht="15.75">
       <c r="A45" s="12" t="s">
-        <v>65</v>
+        <v>58</v>
       </c>
       <c r="B45" s="11"/>
-      <c r="C45" s="10" t="s">
-        <v>66</v>
+      <c r="C45" s="13" t="s">
+        <v>59</v>
       </c>
     </row>
     <row r="46" spans="1:12">
       <c r="A46" s="12" t="s">
-        <v>67</v>
+        <v>60</v>
       </c>
       <c r="B46" s="11"/>
       <c r="C46" s="10" t="s">
-        <v>68</v>
+        <v>61</v>
       </c>
     </row>
     <row r="47" spans="1:12">
       <c r="A47" s="12" t="s">
-        <v>40</v>
+        <v>62</v>
       </c>
       <c r="B47" s="11"/>
       <c r="C47" s="10" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="48" spans="1:12">
+      <c r="A48" s="12" t="s">
+        <v>63</v>
+      </c>
+      <c r="B48" s="11"/>
+      <c r="C48" s="10" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="49" spans="1:3">
+      <c r="A49" s="12" t="s">
+        <v>65</v>
+      </c>
+      <c r="B49" s="11"/>
+      <c r="C49" s="10" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="50" spans="1:3">
+      <c r="A50" s="12" t="s">
+        <v>67</v>
+      </c>
+      <c r="B50" s="11"/>
+      <c r="C50" s="10" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="51" spans="1:3">
+      <c r="A51" s="12" t="s">
+        <v>40</v>
+      </c>
+      <c r="B51" s="11"/>
+      <c r="C51" s="10" t="s">
         <v>69</v>
       </c>
     </row>
@@ -2020,20 +2081,20 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:12" ht="15.75" customHeight="1">
-      <c r="G1" s="90"/>
+      <c r="G1" s="89"/>
     </row>
     <row r="2" spans="2:12" ht="15.75" customHeight="1">
-      <c r="D2" s="96" t="s">
-        <v>176</v>
-      </c>
-      <c r="E2" s="97"/>
-      <c r="F2" s="97"/>
-      <c r="G2" s="90"/>
-      <c r="H2" s="96" t="s">
-        <v>177</v>
-      </c>
-      <c r="I2" s="96"/>
-      <c r="J2" s="96"/>
+      <c r="D2" s="97" t="s">
+        <v>171</v>
+      </c>
+      <c r="E2" s="98"/>
+      <c r="F2" s="98"/>
+      <c r="G2" s="89"/>
+      <c r="H2" s="97" t="s">
+        <v>172</v>
+      </c>
+      <c r="I2" s="97"/>
+      <c r="J2" s="97"/>
     </row>
     <row r="3" spans="2:12" ht="12.75">
       <c r="B3" s="3" t="s">
@@ -2051,7 +2112,7 @@
       <c r="F3" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="G3" s="91"/>
+      <c r="G3" s="90"/>
       <c r="H3" s="50" t="s">
         <v>21</v>
       </c>
@@ -2059,7 +2120,7 @@
         <v>22</v>
       </c>
       <c r="J3" s="50" t="s">
-        <v>178</v>
+        <v>173</v>
       </c>
       <c r="K3" s="5"/>
       <c r="L3" s="5"/>
@@ -2078,8 +2139,8 @@
         <v>15</v>
       </c>
       <c r="F4" s="5"/>
-      <c r="G4" s="92"/>
-      <c r="H4" s="89">
+      <c r="G4" s="91"/>
+      <c r="H4" s="88">
         <v>16</v>
       </c>
       <c r="I4" s="6">
@@ -2106,8 +2167,8 @@
       <c r="F5" s="6" t="s">
         <v>26</v>
       </c>
-      <c r="G5" s="92"/>
-      <c r="H5" s="89">
+      <c r="G5" s="91"/>
+      <c r="H5" s="88">
         <v>40</v>
       </c>
       <c r="I5" s="6">
@@ -2132,8 +2193,8 @@
         <v>75</v>
       </c>
       <c r="F6" s="5"/>
-      <c r="G6" s="92"/>
-      <c r="H6" s="89">
+      <c r="G6" s="91"/>
+      <c r="H6" s="88">
         <v>36</v>
       </c>
       <c r="I6" s="6">
@@ -2160,8 +2221,8 @@
       <c r="F7" s="6" t="s">
         <v>29</v>
       </c>
-      <c r="G7" s="92"/>
-      <c r="H7" s="89">
+      <c r="G7" s="91"/>
+      <c r="H7" s="88">
         <v>62</v>
       </c>
       <c r="I7" s="6">
@@ -2192,8 +2253,8 @@
       <c r="F8" s="6" t="s">
         <v>33</v>
       </c>
-      <c r="G8" s="92"/>
-      <c r="H8" s="89">
+      <c r="G8" s="91"/>
+      <c r="H8" s="88">
         <v>72</v>
       </c>
       <c r="I8" s="6">
@@ -2220,8 +2281,8 @@
         <v>230</v>
       </c>
       <c r="F9" s="5"/>
-      <c r="G9" s="92"/>
-      <c r="H9" s="89">
+      <c r="G9" s="91"/>
+      <c r="H9" s="88">
         <v>62</v>
       </c>
       <c r="I9" s="6">
@@ -2248,8 +2309,8 @@
       <c r="F10" s="6" t="s">
         <v>37</v>
       </c>
-      <c r="G10" s="92"/>
-      <c r="H10" s="89">
+      <c r="G10" s="91"/>
+      <c r="H10" s="88">
         <v>57</v>
       </c>
       <c r="I10" s="6">
@@ -2276,8 +2337,8 @@
       <c r="F11" s="6" t="s">
         <v>39</v>
       </c>
-      <c r="G11" s="92"/>
-      <c r="H11" s="89">
+      <c r="G11" s="91"/>
+      <c r="H11" s="88">
         <v>112</v>
       </c>
       <c r="I11" s="6">
@@ -2304,8 +2365,8 @@
       <c r="F12" s="6" t="s">
         <v>41</v>
       </c>
-      <c r="G12" s="92"/>
-      <c r="H12" s="89">
+      <c r="G12" s="91"/>
+      <c r="H12" s="88">
         <v>101</v>
       </c>
       <c r="I12" s="6">
@@ -2336,8 +2397,8 @@
       <c r="F13" s="6" t="s">
         <v>45</v>
       </c>
-      <c r="G13" s="92"/>
-      <c r="H13" s="89">
+      <c r="G13" s="91"/>
+      <c r="H13" s="88">
         <v>27</v>
       </c>
       <c r="I13" s="6">
@@ -2360,7 +2421,7 @@
         <v>525</v>
       </c>
       <c r="F14" s="5"/>
-      <c r="G14" s="92"/>
+      <c r="G14" s="91"/>
       <c r="H14" s="6"/>
       <c r="I14" s="6">
         <f t="shared" si="0"/>
@@ -2390,8 +2451,8 @@
       <c r="F15" s="6" t="s">
         <v>51</v>
       </c>
-      <c r="G15" s="92"/>
-      <c r="H15" s="89">
+      <c r="G15" s="91"/>
+      <c r="H15" s="88">
         <v>27</v>
       </c>
       <c r="I15" s="6">
@@ -2418,8 +2479,8 @@
       <c r="F16" s="6" t="s">
         <v>53</v>
       </c>
-      <c r="G16" s="92"/>
-      <c r="H16" s="89">
+      <c r="G16" s="91"/>
+      <c r="H16" s="88">
         <v>18</v>
       </c>
       <c r="I16" s="50">
@@ -2438,7 +2499,7 @@
         <v>575</v>
       </c>
       <c r="F17" s="5"/>
-      <c r="G17" s="92"/>
+      <c r="G17" s="91"/>
       <c r="H17" s="6"/>
       <c r="I17" s="6"/>
       <c r="J17" s="6"/>
@@ -2562,7 +2623,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1E946A0D-49B4-48B1-99B4-6819045C52D0}">
   <dimension ref="B4:H16"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="190" zoomScaleNormal="190" workbookViewId="0">
+    <sheetView zoomScale="190" zoomScaleNormal="190" workbookViewId="0">
       <selection activeCell="H8" sqref="H8"/>
     </sheetView>
   </sheetViews>
@@ -2573,48 +2634,48 @@
   </cols>
   <sheetData>
     <row r="4" spans="2:8">
-      <c r="B4" s="100" t="s">
+      <c r="B4" s="95" t="s">
+        <v>181</v>
+      </c>
+      <c r="C4" s="95" t="s">
         <v>186</v>
       </c>
-      <c r="C4" s="100" t="s">
-        <v>191</v>
-      </c>
-      <c r="D4" s="100" t="s">
-        <v>187</v>
-      </c>
-      <c r="E4" s="100" t="s">
-        <v>188</v>
-      </c>
-      <c r="F4" s="100" t="s">
-        <v>189</v>
-      </c>
-      <c r="G4" s="100" t="s">
-        <v>187</v>
-      </c>
-      <c r="H4" s="100" t="s">
-        <v>190</v>
+      <c r="D4" s="95" t="s">
+        <v>182</v>
+      </c>
+      <c r="E4" s="95" t="s">
+        <v>183</v>
+      </c>
+      <c r="F4" s="95" t="s">
+        <v>184</v>
+      </c>
+      <c r="G4" s="95" t="s">
+        <v>182</v>
+      </c>
+      <c r="H4" s="95" t="s">
+        <v>185</v>
       </c>
     </row>
     <row r="5" spans="2:8">
       <c r="B5">
         <v>1</v>
       </c>
-      <c r="C5" s="101">
+      <c r="C5" s="96">
         <v>44424</v>
       </c>
-      <c r="D5" s="101">
+      <c r="D5" s="96">
         <v>44427</v>
       </c>
-      <c r="E5" s="101">
+      <c r="E5" s="96">
         <v>44430</v>
       </c>
-      <c r="F5" s="101">
+      <c r="F5" s="96">
         <v>44435</v>
       </c>
-      <c r="G5" s="101">
+      <c r="G5" s="96">
         <v>44435</v>
       </c>
-      <c r="H5" s="101">
+      <c r="H5" s="96">
         <v>44435</v>
       </c>
     </row>
@@ -2622,22 +2683,22 @@
       <c r="B6">
         <v>2</v>
       </c>
-      <c r="C6" s="101">
+      <c r="C6" s="96">
         <v>44424</v>
       </c>
-      <c r="D6" s="101">
+      <c r="D6" s="96">
         <v>44428</v>
       </c>
-      <c r="E6" s="101">
+      <c r="E6" s="96">
         <v>44433</v>
       </c>
-      <c r="F6" s="101">
+      <c r="F6" s="96">
         <v>44436</v>
       </c>
-      <c r="G6" s="101">
+      <c r="G6" s="96">
         <v>44437</v>
       </c>
-      <c r="H6" s="101">
+      <c r="H6" s="96">
         <v>44437</v>
       </c>
     </row>
@@ -2645,22 +2706,22 @@
       <c r="B7">
         <v>3</v>
       </c>
-      <c r="C7" s="101">
+      <c r="C7" s="96">
         <v>44431</v>
       </c>
-      <c r="D7" s="101">
+      <c r="D7" s="96">
         <v>44433</v>
       </c>
-      <c r="E7" s="101">
+      <c r="E7" s="96">
         <v>44434</v>
       </c>
-      <c r="F7" s="101">
+      <c r="F7" s="96">
         <v>44438</v>
       </c>
-      <c r="G7" s="101">
+      <c r="G7" s="96">
         <v>44439</v>
       </c>
-      <c r="H7" s="101">
+      <c r="H7" s="96">
         <v>44439</v>
       </c>
     </row>
@@ -2668,13 +2729,13 @@
       <c r="B8">
         <v>4</v>
       </c>
-      <c r="C8" s="101">
+      <c r="C8" s="96">
         <v>44431</v>
       </c>
-      <c r="D8" s="101">
+      <c r="D8" s="96">
         <v>44434</v>
       </c>
-      <c r="E8" s="101">
+      <c r="E8" s="96">
         <v>44438</v>
       </c>
     </row>
@@ -2682,10 +2743,10 @@
       <c r="B9">
         <v>5</v>
       </c>
-      <c r="C9" s="101">
+      <c r="C9" s="96">
         <v>44438</v>
       </c>
-      <c r="D9" s="101">
+      <c r="D9" s="96">
         <v>44438</v>
       </c>
     </row>
@@ -2698,7 +2759,7 @@
       <c r="B11">
         <v>7</v>
       </c>
-      <c r="C11" s="101">
+      <c r="C11" s="96">
         <v>44438</v>
       </c>
     </row>
@@ -2716,10 +2777,10 @@
       <c r="B14">
         <v>10</v>
       </c>
-      <c r="C14" s="101">
+      <c r="C14" s="96">
         <v>44438</v>
       </c>
-      <c r="D14" s="101">
+      <c r="D14" s="96">
         <v>44439</v>
       </c>
     </row>
@@ -2770,26 +2831,26 @@
     <row r="1" spans="2:19" ht="12.75">
       <c r="C1" s="1"/>
       <c r="D1" s="1"/>
-      <c r="E1" s="98" t="s">
+      <c r="E1" s="99" t="s">
         <v>0</v>
       </c>
-      <c r="F1" s="99"/>
-      <c r="G1" s="98" t="s">
+      <c r="F1" s="100"/>
+      <c r="G1" s="99" t="s">
         <v>1</v>
       </c>
-      <c r="H1" s="99"/>
-      <c r="I1" s="98" t="s">
+      <c r="H1" s="100"/>
+      <c r="I1" s="99" t="s">
         <v>2</v>
       </c>
-      <c r="J1" s="99"/>
-      <c r="K1" s="98" t="s">
+      <c r="J1" s="100"/>
+      <c r="K1" s="99" t="s">
         <v>1</v>
       </c>
-      <c r="L1" s="99"/>
-      <c r="M1" s="98" t="s">
+      <c r="L1" s="100"/>
+      <c r="M1" s="99" t="s">
         <v>3</v>
       </c>
-      <c r="N1" s="99"/>
+      <c r="N1" s="100"/>
       <c r="O1" s="28" t="s">
         <v>4</v>
       </c>
@@ -3159,40 +3220,40 @@
       </c>
     </row>
     <row r="10" spans="2:19" ht="26.25" customHeight="1">
-      <c r="B10" s="71" t="s">
+      <c r="B10" s="70" t="s">
         <v>14</v>
       </c>
-      <c r="C10" s="72"/>
-      <c r="D10" s="72"/>
-      <c r="E10" s="73" t="s">
+      <c r="C10" s="71"/>
+      <c r="D10" s="71"/>
+      <c r="E10" s="72" t="s">
         <v>8</v>
       </c>
-      <c r="F10" s="74">
+      <c r="F10" s="73">
         <v>44333</v>
       </c>
-      <c r="G10" s="73" t="s">
+      <c r="G10" s="72" t="s">
         <v>15</v>
       </c>
-      <c r="H10" s="74">
+      <c r="H10" s="73">
         <v>44346</v>
       </c>
-      <c r="I10" s="73" t="s">
+      <c r="I10" s="72" t="s">
         <v>8</v>
       </c>
-      <c r="J10" s="74">
+      <c r="J10" s="73">
         <v>44369</v>
       </c>
-      <c r="K10" s="73" t="s">
+      <c r="K10" s="72" t="s">
         <v>6</v>
       </c>
-      <c r="L10" s="74">
+      <c r="L10" s="73">
         <v>44380</v>
       </c>
-      <c r="M10" s="73" t="s">
+      <c r="M10" s="72" t="s">
         <v>15</v>
       </c>
       <c r="N10" s="40"/>
-      <c r="O10" s="67">
+      <c r="O10" s="66">
         <v>44382</v>
       </c>
       <c r="P10" s="43">
@@ -3207,38 +3268,38 @@
       </c>
     </row>
     <row r="11" spans="2:19" ht="26.25" customHeight="1">
-      <c r="B11" s="75" t="s">
-        <v>167</v>
-      </c>
-      <c r="C11" s="76"/>
-      <c r="D11" s="76"/>
-      <c r="E11" s="77" t="s">
+      <c r="B11" s="74" t="s">
+        <v>162</v>
+      </c>
+      <c r="C11" s="75"/>
+      <c r="D11" s="75"/>
+      <c r="E11" s="76" t="s">
         <v>15</v>
       </c>
-      <c r="F11" s="78">
+      <c r="F11" s="77">
         <v>44362</v>
       </c>
-      <c r="G11" s="77" t="s">
+      <c r="G11" s="76" t="s">
         <v>8</v>
       </c>
-      <c r="H11" s="78">
+      <c r="H11" s="77">
         <v>44369</v>
       </c>
-      <c r="I11" s="77" t="s">
+      <c r="I11" s="76" t="s">
         <v>15</v>
       </c>
-      <c r="J11" s="78">
+      <c r="J11" s="77">
         <v>44378</v>
       </c>
-      <c r="K11" s="79" t="s">
+      <c r="K11" s="78" t="s">
         <v>6</v>
       </c>
-      <c r="L11" s="78">
+      <c r="L11" s="77">
         <v>44386</v>
       </c>
-      <c r="M11" s="77"/>
-      <c r="N11" s="80"/>
-      <c r="O11" s="67">
+      <c r="M11" s="76"/>
+      <c r="N11" s="79"/>
+      <c r="O11" s="66">
         <v>44389</v>
       </c>
       <c r="P11" s="43">
@@ -3253,76 +3314,76 @@
       </c>
     </row>
     <row r="12" spans="2:19" ht="26.25" customHeight="1">
-      <c r="B12" s="75" t="s">
-        <v>171</v>
-      </c>
-      <c r="C12" s="76"/>
-      <c r="D12" s="76"/>
-      <c r="E12" s="77" t="s">
+      <c r="B12" s="74" t="s">
+        <v>166</v>
+      </c>
+      <c r="C12" s="75"/>
+      <c r="D12" s="75"/>
+      <c r="E12" s="76" t="s">
         <v>15</v>
       </c>
-      <c r="F12" s="78">
+      <c r="F12" s="77">
         <v>44362</v>
       </c>
-      <c r="G12" s="77" t="s">
+      <c r="G12" s="76" t="s">
         <v>8</v>
       </c>
-      <c r="H12" s="78">
+      <c r="H12" s="77">
         <v>44375</v>
       </c>
-      <c r="I12" s="77" t="s">
-        <v>169</v>
-      </c>
-      <c r="J12" s="78">
+      <c r="I12" s="76" t="s">
+        <v>164</v>
+      </c>
+      <c r="J12" s="77">
         <v>44378</v>
       </c>
-      <c r="K12" s="79" t="s">
+      <c r="K12" s="78" t="s">
         <v>6</v>
       </c>
-      <c r="L12" s="78">
+      <c r="L12" s="77">
         <v>44386</v>
       </c>
-      <c r="M12" s="77"/>
-      <c r="N12" s="80"/>
-      <c r="O12" s="67">
+      <c r="M12" s="76"/>
+      <c r="N12" s="79"/>
+      <c r="O12" s="66">
         <v>44389</v>
       </c>
       <c r="P12" s="43"/>
       <c r="Q12" s="42"/>
     </row>
     <row r="13" spans="2:19" ht="26.25" customHeight="1">
-      <c r="B13" s="75" t="s">
-        <v>170</v>
-      </c>
-      <c r="C13" s="76"/>
-      <c r="D13" s="76"/>
-      <c r="E13" s="77" t="s">
+      <c r="B13" s="74" t="s">
+        <v>165</v>
+      </c>
+      <c r="C13" s="75"/>
+      <c r="D13" s="75"/>
+      <c r="E13" s="76" t="s">
         <v>15</v>
       </c>
-      <c r="F13" s="78">
+      <c r="F13" s="77">
         <v>44376</v>
       </c>
-      <c r="G13" s="79" t="s">
+      <c r="G13" s="78" t="s">
         <v>8</v>
       </c>
-      <c r="H13" s="78">
+      <c r="H13" s="77">
         <v>44382</v>
       </c>
-      <c r="I13" s="77" t="s">
+      <c r="I13" s="76" t="s">
         <v>15</v>
       </c>
-      <c r="J13" s="78">
+      <c r="J13" s="77">
         <v>44383</v>
       </c>
-      <c r="K13" s="79" t="s">
+      <c r="K13" s="78" t="s">
         <v>6</v>
       </c>
-      <c r="L13" s="78">
+      <c r="L13" s="77">
         <v>44387</v>
       </c>
-      <c r="M13" s="77"/>
-      <c r="N13" s="80"/>
-      <c r="O13" s="67">
+      <c r="M13" s="76"/>
+      <c r="N13" s="79"/>
+      <c r="O13" s="66">
         <v>44389</v>
       </c>
       <c r="P13" s="43"/>
@@ -3333,7 +3394,7 @@
         <v>16</v>
       </c>
       <c r="D14" s="2"/>
-      <c r="E14" s="66" t="s">
+      <c r="E14" s="65" t="s">
         <v>8</v>
       </c>
       <c r="F14" s="38">
@@ -3363,7 +3424,7 @@
       <c r="N14" s="38">
         <v>44393</v>
       </c>
-      <c r="O14" s="67">
+      <c r="O14" s="66">
         <v>44394</v>
       </c>
       <c r="P14" s="43">
@@ -3378,42 +3439,42 @@
       </c>
     </row>
     <row r="15" spans="2:19" ht="26.25" customHeight="1">
-      <c r="B15" s="71" t="s">
+      <c r="B15" s="70" t="s">
         <v>17</v>
       </c>
-      <c r="C15" s="72"/>
-      <c r="D15" s="72"/>
-      <c r="E15" s="73" t="s">
+      <c r="C15" s="71"/>
+      <c r="D15" s="71"/>
+      <c r="E15" s="72" t="s">
         <v>6</v>
       </c>
-      <c r="F15" s="74">
+      <c r="F15" s="73">
         <v>44332</v>
       </c>
-      <c r="G15" s="73" t="s">
+      <c r="G15" s="72" t="s">
         <v>15</v>
       </c>
-      <c r="H15" s="74">
+      <c r="H15" s="73">
         <v>44333</v>
       </c>
-      <c r="I15" s="73" t="s">
+      <c r="I15" s="72" t="s">
         <v>6</v>
       </c>
-      <c r="J15" s="74">
+      <c r="J15" s="73">
         <v>44337</v>
       </c>
-      <c r="K15" s="73" t="s">
+      <c r="K15" s="72" t="s">
         <v>15</v>
       </c>
-      <c r="L15" s="74">
+      <c r="L15" s="73">
         <v>44339</v>
       </c>
-      <c r="M15" s="73" t="s">
+      <c r="M15" s="72" t="s">
         <v>8</v>
       </c>
-      <c r="N15" s="74">
+      <c r="N15" s="73">
         <v>44354</v>
       </c>
-      <c r="O15" s="67">
+      <c r="O15" s="66">
         <v>44381</v>
       </c>
       <c r="P15" s="43">
@@ -3428,40 +3489,40 @@
       </c>
     </row>
     <row r="16" spans="2:19" ht="26.25" customHeight="1" thickBot="1">
-      <c r="B16" s="81" t="s">
+      <c r="B16" s="80" t="s">
         <v>18</v>
       </c>
-      <c r="C16" s="82"/>
-      <c r="D16" s="82"/>
-      <c r="E16" s="83" t="s">
-        <v>165</v>
-      </c>
-      <c r="F16" s="84">
+      <c r="C16" s="81"/>
+      <c r="D16" s="81"/>
+      <c r="E16" s="82" t="s">
+        <v>160</v>
+      </c>
+      <c r="F16" s="83">
         <v>44346</v>
       </c>
-      <c r="G16" s="83" t="s">
+      <c r="G16" s="82" t="s">
         <v>6</v>
       </c>
-      <c r="H16" s="85" t="s">
-        <v>168</v>
-      </c>
-      <c r="I16" s="83" t="s">
+      <c r="H16" s="84" t="s">
+        <v>163</v>
+      </c>
+      <c r="I16" s="82" t="s">
         <v>8</v>
       </c>
-      <c r="J16" s="84">
+      <c r="J16" s="83">
         <v>44382</v>
       </c>
-      <c r="K16" s="83" t="s">
+      <c r="K16" s="82" t="s">
         <v>15</v>
       </c>
-      <c r="L16" s="84">
+      <c r="L16" s="83">
         <v>44383</v>
       </c>
-      <c r="M16" s="86" t="s">
-        <v>165</v>
-      </c>
-      <c r="N16" s="85"/>
-      <c r="O16" s="67">
+      <c r="M16" s="85" t="s">
+        <v>160</v>
+      </c>
+      <c r="N16" s="84"/>
+      <c r="O16" s="66">
         <v>44389</v>
       </c>
       <c r="P16" s="44">
@@ -3485,13 +3546,13 @@
       <c r="K17" s="36"/>
       <c r="L17" s="36"/>
       <c r="M17" s="36"/>
-      <c r="N17" s="68" t="s">
-        <v>172</v>
-      </c>
-      <c r="P17" s="69">
+      <c r="N17" s="67" t="s">
+        <v>167</v>
+      </c>
+      <c r="P17" s="68">
         <v>44368</v>
       </c>
-      <c r="Q17" s="70">
+      <c r="Q17" s="69">
         <v>44394</v>
       </c>
       <c r="R17" s="50">

</xml_diff>

<commit_message>
Updates for Chap 8
</commit_message>
<xml_diff>
--- a/Word/PlanAndDealines.xlsx
+++ b/Word/PlanAndDealines.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ksung\Desktop\GitHub\GTCS-GameEngine2\Word\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4A09DCDB-04EC-4479-9760-F8561B3D54E3}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2A3B868F-FE0C-4830-8CB2-F5ABA39F27C5}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="33645" windowHeight="15855" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1711,7 +1711,7 @@
   <dimension ref="A3:R51"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="H25" sqref="H25"/>
+      <selection activeCell="L25" sqref="L25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
@@ -1939,25 +1939,25 @@
     </row>
     <row r="35" spans="1:12">
       <c r="A35" s="50"/>
-      <c r="B35" s="49" t="s">
+      <c r="B35" s="75" t="s">
         <v>187</v>
       </c>
     </row>
     <row r="36" spans="1:12">
       <c r="A36" s="50"/>
-      <c r="B36" s="49" t="s">
+      <c r="B36" s="75" t="s">
         <v>188</v>
       </c>
     </row>
     <row r="37" spans="1:12">
       <c r="A37" s="50"/>
-      <c r="B37" s="49" t="s">
+      <c r="B37" s="75" t="s">
         <v>189</v>
       </c>
     </row>
     <row r="38" spans="1:12">
       <c r="A38" s="50"/>
-      <c r="B38" s="49" t="s">
+      <c r="B38" s="75" t="s">
         <v>174</v>
       </c>
     </row>
@@ -2624,7 +2624,7 @@
   <dimension ref="B4:H16"/>
   <sheetViews>
     <sheetView zoomScale="190" zoomScaleNormal="190" workbookViewId="0">
-      <selection activeCell="H8" sqref="H8"/>
+      <selection activeCell="D12" sqref="D12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
@@ -2762,10 +2762,16 @@
       <c r="C11" s="96">
         <v>44438</v>
       </c>
+      <c r="D11" s="96">
+        <v>44440</v>
+      </c>
     </row>
     <row r="12" spans="2:8">
       <c r="B12">
         <v>8</v>
+      </c>
+      <c r="C12" s="96">
+        <v>44439</v>
       </c>
     </row>
     <row r="13" spans="2:8">

</xml_diff>

<commit_message>
TR Final Chap 4 and 5
</commit_message>
<xml_diff>
--- a/Word/PlanAndDealines.xlsx
+++ b/Word/PlanAndDealines.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ksung\Desktop\GitHub\GTCS-GameEngine2\Word\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C5B2EF2D-4C0C-4065-B16D-8D8C1AFC90BC}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D82BC02D-32A8-4421-8F3F-D816C48525C9}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="33645" windowHeight="15855" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -2649,7 +2649,7 @@
   <dimension ref="B4:H16"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="190" zoomScaleNormal="190" workbookViewId="0">
-      <selection activeCell="F9" sqref="F9"/>
+      <selection activeCell="D14" sqref="D14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
@@ -2766,6 +2766,12 @@
       <c r="F8" s="96">
         <v>44443</v>
       </c>
+      <c r="G8" s="96">
+        <v>44444</v>
+      </c>
+      <c r="H8" s="96">
+        <v>44444</v>
+      </c>
     </row>
     <row r="9" spans="2:8">
       <c r="B9">
@@ -2817,6 +2823,9 @@
       </c>
       <c r="C13" s="96">
         <v>44440</v>
+      </c>
+      <c r="D13" s="96">
+        <v>44444</v>
       </c>
     </row>
     <row r="14" spans="2:8">

</xml_diff>

<commit_message>
Chap 8 TR Edit Done
</commit_message>
<xml_diff>
--- a/Word/PlanAndDealines.xlsx
+++ b/Word/PlanAndDealines.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ksung\Desktop\GitHub\GTCS-GameEngine2\Word\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0226B6E1-FC4E-422C-B689-5392D3E115C0}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6EBD0A93-DAC2-4F3E-B899-11F7EFAE2622}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="33645" windowHeight="15855" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1491,6 +1491,7 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1503,7 +1504,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1721,8 +1721,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D8AC00B6-697C-45E4-9E65-51AD1E2696C6}">
   <dimension ref="A3:R53"/>
   <sheetViews>
-    <sheetView topLeftCell="A4" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="B24" sqref="B24"/>
+    <sheetView topLeftCell="A7" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
+      <selection activeCell="B29" sqref="B29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
@@ -1910,7 +1910,7 @@
     </row>
     <row r="29" spans="1:3">
       <c r="A29" s="50"/>
-      <c r="B29" s="49" t="s">
+      <c r="B29" s="75" t="s">
         <v>176</v>
       </c>
     </row>
@@ -2110,17 +2110,17 @@
       <c r="G1" s="89"/>
     </row>
     <row r="2" spans="2:12" ht="15.75" customHeight="1">
-      <c r="D2" s="99" t="s">
+      <c r="D2" s="100" t="s">
         <v>171</v>
       </c>
-      <c r="E2" s="100"/>
-      <c r="F2" s="100"/>
+      <c r="E2" s="101"/>
+      <c r="F2" s="101"/>
       <c r="G2" s="89"/>
-      <c r="H2" s="99" t="s">
+      <c r="H2" s="100" t="s">
         <v>172</v>
       </c>
-      <c r="I2" s="99"/>
-      <c r="J2" s="99"/>
+      <c r="I2" s="100"/>
+      <c r="J2" s="100"/>
     </row>
     <row r="3" spans="2:12" ht="12.75">
       <c r="B3" s="3" t="s">
@@ -2650,7 +2650,7 @@
   <dimension ref="B4:H16"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="190" zoomScaleNormal="190" workbookViewId="0">
-      <selection activeCell="H11" sqref="H11"/>
+      <selection activeCell="H24" sqref="H24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
@@ -2801,7 +2801,10 @@
       <c r="B10">
         <v>6</v>
       </c>
-      <c r="F10" s="103"/>
+      <c r="D10" s="96">
+        <v>44445</v>
+      </c>
+      <c r="F10" s="99"/>
     </row>
     <row r="11" spans="2:8">
       <c r="B11">
@@ -2816,7 +2819,7 @@
       <c r="E11" s="96">
         <v>44445</v>
       </c>
-      <c r="F11" s="103"/>
+      <c r="F11" s="99"/>
       <c r="G11" s="96">
         <v>44445</v>
       </c>
@@ -2834,7 +2837,16 @@
       <c r="D12" s="96">
         <v>44442</v>
       </c>
-      <c r="F12" s="103"/>
+      <c r="E12" s="96">
+        <v>44445</v>
+      </c>
+      <c r="F12" s="99"/>
+      <c r="G12" s="96">
+        <v>44446</v>
+      </c>
+      <c r="H12" s="96">
+        <v>44446</v>
+      </c>
     </row>
     <row r="13" spans="2:8">
       <c r="B13">
@@ -2846,7 +2858,7 @@
       <c r="D13" s="96">
         <v>44444</v>
       </c>
-      <c r="F13" s="103"/>
+      <c r="F13" s="99"/>
     </row>
     <row r="14" spans="2:8">
       <c r="B14">
@@ -2918,26 +2930,26 @@
     <row r="1" spans="2:19" ht="12.75">
       <c r="C1" s="1"/>
       <c r="D1" s="1"/>
-      <c r="E1" s="101" t="s">
+      <c r="E1" s="102" t="s">
         <v>0</v>
       </c>
-      <c r="F1" s="102"/>
-      <c r="G1" s="101" t="s">
+      <c r="F1" s="103"/>
+      <c r="G1" s="102" t="s">
         <v>1</v>
       </c>
-      <c r="H1" s="102"/>
-      <c r="I1" s="101" t="s">
+      <c r="H1" s="103"/>
+      <c r="I1" s="102" t="s">
         <v>2</v>
       </c>
-      <c r="J1" s="102"/>
-      <c r="K1" s="101" t="s">
+      <c r="J1" s="103"/>
+      <c r="K1" s="102" t="s">
         <v>1</v>
       </c>
-      <c r="L1" s="102"/>
-      <c r="M1" s="101" t="s">
+      <c r="L1" s="103"/>
+      <c r="M1" s="102" t="s">
         <v>3</v>
       </c>
-      <c r="N1" s="102"/>
+      <c r="N1" s="103"/>
       <c r="O1" s="28" t="s">
         <v>4</v>
       </c>

</xml_diff>

<commit_message>
Macro to detect long code lines
</commit_message>
<xml_diff>
--- a/Word/PlanAndDealines.xlsx
+++ b/Word/PlanAndDealines.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ksung\Desktop\GitHub\GTCS-GameEngine2\Word\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ksungAD\Desktop\GitHub\GTCS-GameEngine2\Word\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6EBD0A93-DAC2-4F3E-B899-11F7EFAE2622}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5F3FF0A8-5DD5-4D55-9562-CE8EFE776F3B}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="33645" windowHeight="15855" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="33648" windowHeight="15858" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Final Changes Must make" sheetId="8" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="320" uniqueCount="199">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="328" uniqueCount="207">
   <si>
     <t>First Pass</t>
   </si>
@@ -886,6 +886,30 @@
   </si>
   <si>
     <t>// …    should be change to without the "//"</t>
+  </si>
+  <si>
+    <t>1. Must load images to g-drive</t>
+  </si>
+  <si>
+    <t>2. code check</t>
+  </si>
+  <si>
+    <t>73 characters</t>
+  </si>
+  <si>
+    <t>Search for "code format" with "Tab"</t>
+  </si>
+  <si>
+    <t>Search for code with 73 characters</t>
+  </si>
+  <si>
+    <t>Search for code bold with 73 characters</t>
+  </si>
+  <si>
+    <t>Search for "code bold" with "Tab"</t>
+  </si>
+  <si>
+    <t>https://wordmvp.com/FAQs/General/UsingWildcards.htm</t>
   </si>
 </sst>
 </file>
@@ -1719,13 +1743,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D8AC00B6-697C-45E4-9E65-51AD1E2696C6}">
-  <dimension ref="A3:R53"/>
+  <dimension ref="A3:R62"/>
   <sheetViews>
-    <sheetView topLeftCell="A7" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="B29" sqref="B29"/>
+    <sheetView tabSelected="1" topLeftCell="A46" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
+      <selection activeCell="C57" sqref="C57"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.75"/>
+  <sheetFormatPr defaultRowHeight="12.3"/>
   <sheetData>
     <row r="3" spans="1:18">
       <c r="A3" s="50" t="s">
@@ -1737,7 +1761,7 @@
         <v>153</v>
       </c>
     </row>
-    <row r="5" spans="1:18">
+    <row r="5" spans="1:18" ht="12.6">
       <c r="B5" s="50" t="s">
         <v>132</v>
       </c>
@@ -2019,7 +2043,7 @@
         <v>156</v>
       </c>
     </row>
-    <row r="47" spans="1:12" ht="15.75">
+    <row r="47" spans="1:12" ht="15">
       <c r="A47" s="12" t="s">
         <v>58</v>
       </c>
@@ -2080,6 +2104,44 @@
       <c r="B53" s="11"/>
       <c r="C53" s="10" t="s">
         <v>69</v>
+      </c>
+    </row>
+    <row r="56" spans="1:3">
+      <c r="A56" s="50" t="s">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="57" spans="1:3">
+      <c r="A57" s="49" t="s">
+        <v>200</v>
+      </c>
+      <c r="C57" t="s">
+        <v>206</v>
+      </c>
+    </row>
+    <row r="58" spans="1:3">
+      <c r="B58" s="49" t="s">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="59" spans="1:3">
+      <c r="B59" s="49" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="60" spans="1:3">
+      <c r="B60" s="49" t="s">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="61" spans="1:3">
+      <c r="B61" s="49" t="s">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="62" spans="1:3">
+      <c r="B62" s="49" t="s">
+        <v>204</v>
       </c>
     </row>
   </sheetData>
@@ -2099,11 +2161,11 @@
       <selection activeCell="V16" sqref="V16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1"/>
+  <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15.75" customHeight="1"/>
   <cols>
-    <col min="7" max="7" width="1.85546875" customWidth="1"/>
-    <col min="8" max="8" width="9.42578125" customWidth="1"/>
-    <col min="9" max="9" width="9.5703125" customWidth="1"/>
+    <col min="7" max="7" width="1.83203125" customWidth="1"/>
+    <col min="8" max="8" width="9.44140625" customWidth="1"/>
+    <col min="9" max="9" width="9.5546875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="2:12" ht="15.75" customHeight="1">
@@ -2122,7 +2184,7 @@
       <c r="I2" s="100"/>
       <c r="J2" s="100"/>
     </row>
-    <row r="3" spans="2:12" ht="12.75">
+    <row r="3" spans="2:12" ht="12.3">
       <c r="B3" s="3" t="s">
         <v>19</v>
       </c>
@@ -2151,7 +2213,7 @@
       <c r="K3" s="5"/>
       <c r="L3" s="5"/>
     </row>
-    <row r="4" spans="2:12" ht="12.75">
+    <row r="4" spans="2:12" ht="12.3">
       <c r="B4" s="6" t="s">
         <v>24</v>
       </c>
@@ -2177,7 +2239,7 @@
       <c r="K4" s="5"/>
       <c r="L4" s="5"/>
     </row>
-    <row r="5" spans="2:12" ht="12.75">
+    <row r="5" spans="2:12" ht="12.3">
       <c r="B5" s="6" t="s">
         <v>25</v>
       </c>
@@ -2205,7 +2267,7 @@
       <c r="K5" s="5"/>
       <c r="L5" s="5"/>
     </row>
-    <row r="6" spans="2:12" ht="12.75">
+    <row r="6" spans="2:12" ht="12.3">
       <c r="B6" s="6" t="s">
         <v>27</v>
       </c>
@@ -2263,7 +2325,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="8" spans="2:12" ht="12.75">
+    <row r="8" spans="2:12" ht="12.3">
       <c r="B8" s="6" t="s">
         <v>32</v>
       </c>
@@ -2293,7 +2355,7 @@
       </c>
       <c r="L8" s="5"/>
     </row>
-    <row r="9" spans="2:12" ht="12.75">
+    <row r="9" spans="2:12" ht="12.3">
       <c r="B9" s="6" t="s">
         <v>35</v>
       </c>
@@ -2319,7 +2381,7 @@
       <c r="K9" s="5"/>
       <c r="L9" s="5"/>
     </row>
-    <row r="10" spans="2:12" ht="12.75">
+    <row r="10" spans="2:12" ht="12.3">
       <c r="B10" s="6" t="s">
         <v>36</v>
       </c>
@@ -2347,7 +2409,7 @@
       <c r="K10" s="5"/>
       <c r="L10" s="5"/>
     </row>
-    <row r="11" spans="2:12" ht="12.75">
+    <row r="11" spans="2:12" ht="12.3">
       <c r="B11" s="6" t="s">
         <v>38</v>
       </c>
@@ -2461,7 +2523,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="15" spans="2:12" ht="12.75">
+    <row r="15" spans="2:12" ht="12.3">
       <c r="B15" s="6" t="s">
         <v>50</v>
       </c>
@@ -2489,7 +2551,7 @@
       <c r="K15" s="5"/>
       <c r="L15" s="5"/>
     </row>
-    <row r="16" spans="2:12" ht="12.75">
+    <row r="16" spans="2:12" ht="12.3">
       <c r="B16" s="6" t="s">
         <v>52</v>
       </c>
@@ -2517,7 +2579,7 @@
       <c r="K16" s="5"/>
       <c r="L16" s="5"/>
     </row>
-    <row r="17" spans="2:12" ht="12.75">
+    <row r="17" spans="2:12" ht="12.3">
       <c r="B17" s="5"/>
       <c r="C17" s="5"/>
       <c r="D17" s="5"/>
@@ -2532,7 +2594,7 @@
       <c r="K17" s="5"/>
       <c r="L17" s="5"/>
     </row>
-    <row r="18" spans="2:12" ht="12.75">
+    <row r="18" spans="2:12" ht="12.3">
       <c r="B18" s="5"/>
       <c r="C18" s="5"/>
       <c r="D18" s="5"/>
@@ -2545,19 +2607,19 @@
       <c r="K18" s="5"/>
       <c r="L18" s="5"/>
     </row>
-    <row r="23" spans="2:12" ht="12.75">
+    <row r="23" spans="2:12" ht="12.3">
       <c r="B23" s="2" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="24" spans="2:12" ht="12.75">
+    <row r="24" spans="2:12" ht="12.3">
       <c r="B24" s="10" t="s">
         <v>55</v>
       </c>
       <c r="C24" s="11"/>
       <c r="D24" s="11"/>
     </row>
-    <row r="25" spans="2:12" ht="12.75">
+    <row r="25" spans="2:12" ht="12.3">
       <c r="B25" s="12" t="s">
         <v>56</v>
       </c>
@@ -2566,7 +2628,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="26" spans="2:12">
+    <row r="26" spans="2:12" ht="15">
       <c r="B26" s="12" t="s">
         <v>58</v>
       </c>
@@ -2575,7 +2637,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="27" spans="2:12" ht="12.75">
+    <row r="27" spans="2:12" ht="12.3">
       <c r="B27" s="12" t="s">
         <v>60</v>
       </c>
@@ -2584,7 +2646,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="28" spans="2:12" ht="12.75">
+    <row r="28" spans="2:12" ht="12.3">
       <c r="B28" s="12" t="s">
         <v>62</v>
       </c>
@@ -2593,7 +2655,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="29" spans="2:12" ht="12.75">
+    <row r="29" spans="2:12" ht="12.3">
       <c r="B29" s="12" t="s">
         <v>63</v>
       </c>
@@ -2602,7 +2664,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="30" spans="2:12" ht="12.75">
+    <row r="30" spans="2:12" ht="12.3">
       <c r="B30" s="12" t="s">
         <v>65</v>
       </c>
@@ -2611,7 +2673,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="31" spans="2:12" ht="12.75">
+    <row r="31" spans="2:12" ht="12.3">
       <c r="B31" s="12" t="s">
         <v>67</v>
       </c>
@@ -2620,7 +2682,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="32" spans="2:12" ht="12.75">
+    <row r="32" spans="2:12" ht="12.3">
       <c r="B32" s="12" t="s">
         <v>40</v>
       </c>
@@ -2649,14 +2711,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1E946A0D-49B4-48B1-99B4-6819045C52D0}">
   <dimension ref="B4:H16"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="190" zoomScaleNormal="190" workbookViewId="0">
+    <sheetView zoomScale="190" zoomScaleNormal="190" workbookViewId="0">
       <selection activeCell="H24" sqref="H24"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.75"/>
+  <sheetFormatPr defaultRowHeight="12.3"/>
   <cols>
-    <col min="3" max="3" width="12.5703125" customWidth="1"/>
-    <col min="4" max="8" width="14.5703125" customWidth="1"/>
+    <col min="3" max="3" width="12.5546875" customWidth="1"/>
+    <col min="4" max="8" width="14.5546875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="4" spans="2:8">
@@ -2910,24 +2972,24 @@
       <selection activeCell="P18" sqref="P18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1"/>
+  <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15.75" customHeight="1"/>
   <cols>
-    <col min="3" max="4" width="1.7109375" customWidth="1"/>
-    <col min="5" max="5" width="7.42578125" style="31" customWidth="1"/>
-    <col min="6" max="6" width="7.42578125" style="30" customWidth="1"/>
-    <col min="7" max="7" width="7.42578125" style="31" customWidth="1"/>
+    <col min="3" max="4" width="1.71875" customWidth="1"/>
+    <col min="5" max="5" width="7.44140625" style="31" customWidth="1"/>
+    <col min="6" max="6" width="7.44140625" style="30" customWidth="1"/>
+    <col min="7" max="7" width="7.44140625" style="31" customWidth="1"/>
     <col min="8" max="8" width="8" style="30" customWidth="1"/>
-    <col min="9" max="9" width="7.42578125" style="31" customWidth="1"/>
-    <col min="10" max="10" width="7.42578125" style="30" customWidth="1"/>
-    <col min="11" max="11" width="7.42578125" style="31" customWidth="1"/>
-    <col min="12" max="12" width="8.42578125" style="30" customWidth="1"/>
-    <col min="13" max="13" width="7.42578125" style="31" customWidth="1"/>
-    <col min="14" max="14" width="7.42578125" style="30" customWidth="1"/>
-    <col min="15" max="15" width="16.42578125" style="29" customWidth="1"/>
-    <col min="16" max="16" width="14.42578125" style="27"/>
+    <col min="9" max="9" width="7.44140625" style="31" customWidth="1"/>
+    <col min="10" max="10" width="7.44140625" style="30" customWidth="1"/>
+    <col min="11" max="11" width="7.44140625" style="31" customWidth="1"/>
+    <col min="12" max="12" width="8.44140625" style="30" customWidth="1"/>
+    <col min="13" max="13" width="7.44140625" style="31" customWidth="1"/>
+    <col min="14" max="14" width="7.44140625" style="30" customWidth="1"/>
+    <col min="15" max="15" width="16.44140625" style="29" customWidth="1"/>
+    <col min="16" max="16" width="14.44140625" style="27"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:19" ht="12.75">
+    <row r="1" spans="2:19" ht="12.3">
       <c r="C1" s="1"/>
       <c r="D1" s="1"/>
       <c r="E1" s="102" t="s">
@@ -2960,7 +3022,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="2" spans="2:19" ht="13.5" thickBot="1">
+    <row r="2" spans="2:19" ht="12.6" thickBot="1">
       <c r="C2" s="1"/>
       <c r="D2" s="1"/>
       <c r="E2" s="32" t="s">
@@ -5246,18 +5308,18 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1"/>
+  <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15.75" customHeight="1"/>
   <cols>
-    <col min="2" max="2" width="33.140625" customWidth="1"/>
-    <col min="3" max="3" width="27.7109375" customWidth="1"/>
+    <col min="2" max="2" width="33.1640625" customWidth="1"/>
+    <col min="3" max="3" width="27.71875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" ht="12.75">
+    <row r="1" spans="1:10" ht="12.3">
       <c r="A1" s="14" t="s">
         <v>70</v>
       </c>
     </row>
-    <row r="2" spans="1:10" ht="12.75">
+    <row r="2" spans="1:10" ht="12.3">
       <c r="B2" s="14" t="s">
         <v>19</v>
       </c>
@@ -5277,7 +5339,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="3" spans="1:10" ht="12.75">
+    <row r="3" spans="1:10" ht="12.3">
       <c r="B3" s="2" t="s">
         <v>76</v>
       </c>
@@ -5288,7 +5350,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="4" spans="1:10" ht="12.75">
+    <row r="4" spans="1:10" ht="12.3">
       <c r="C4" s="2" t="s">
         <v>79</v>
       </c>
@@ -5296,20 +5358,20 @@
         <v>80</v>
       </c>
     </row>
-    <row r="5" spans="1:10" ht="14.25">
+    <row r="5" spans="1:10" ht="13.8">
       <c r="C5" s="2" t="s">
         <v>81</v>
       </c>
       <c r="H5" s="15"/>
       <c r="J5" s="16"/>
     </row>
-    <row r="6" spans="1:10" ht="12.75">
+    <row r="6" spans="1:10" ht="12.6">
       <c r="C6" s="2" t="s">
         <v>82</v>
       </c>
       <c r="J6" s="17"/>
     </row>
-    <row r="7" spans="1:10" ht="12.75">
+    <row r="7" spans="1:10" ht="12.3">
       <c r="C7" s="2" t="s">
         <v>83</v>
       </c>
@@ -5318,7 +5380,7 @@
       <c r="H8" s="18"/>
       <c r="I8" s="18"/>
     </row>
-    <row r="9" spans="1:10" ht="14.25">
+    <row r="9" spans="1:10" ht="13.8">
       <c r="B9" s="19" t="s">
         <v>84</v>
       </c>
@@ -5346,7 +5408,7 @@
     <row r="13" spans="1:10" ht="15.75" customHeight="1">
       <c r="J13" s="21"/>
     </row>
-    <row r="15" spans="1:10" ht="12.75">
+    <row r="15" spans="1:10" ht="12.3">
       <c r="B15" s="2" t="s">
         <v>88</v>
       </c>
@@ -5357,12 +5419,12 @@
         <v>15</v>
       </c>
     </row>
-    <row r="16" spans="1:10" ht="12.75">
+    <row r="16" spans="1:10" ht="12.3">
       <c r="C16" s="2" t="s">
         <v>90</v>
       </c>
     </row>
-    <row r="17" spans="1:9" ht="12.75">
+    <row r="17" spans="1:9" ht="12.3">
       <c r="G17" s="14"/>
     </row>
     <row r="18" spans="1:9" ht="15.75" customHeight="1">
@@ -5371,17 +5433,17 @@
     <row r="19" spans="1:9" ht="15.75" customHeight="1">
       <c r="I19" s="21"/>
     </row>
-    <row r="20" spans="1:9" ht="12.75">
+    <row r="20" spans="1:9" ht="12.3">
       <c r="B20" s="2" t="s">
         <v>91</v>
       </c>
     </row>
-    <row r="29" spans="1:9" ht="12.75">
+    <row r="29" spans="1:9" ht="12.3">
       <c r="A29" s="14" t="s">
         <v>92</v>
       </c>
     </row>
-    <row r="30" spans="1:9" ht="14.25">
+    <row r="30" spans="1:9" ht="13.8">
       <c r="B30" s="15" t="s">
         <v>93</v>
       </c>
@@ -5389,7 +5451,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="31" spans="1:9" ht="12.75">
+    <row r="31" spans="1:9" ht="12.6">
       <c r="D31" s="22" t="s">
         <v>95</v>
       </c>
@@ -5402,7 +5464,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="34" spans="1:4" ht="14.25">
+    <row r="34" spans="1:4" ht="13.8">
       <c r="C34" s="24" t="s">
         <v>98</v>
       </c>
@@ -5428,7 +5490,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="42" spans="1:4" ht="12.75">
+    <row r="42" spans="1:4" ht="12.3">
       <c r="A42" s="14"/>
     </row>
     <row r="43" spans="1:4" ht="15.75" customHeight="1">
@@ -5459,10 +5521,10 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1"/>
+  <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15.75" customHeight="1"/>
   <cols>
-    <col min="2" max="2" width="35.7109375" customWidth="1"/>
-    <col min="3" max="3" width="36.42578125" customWidth="1"/>
+    <col min="2" max="2" width="35.71875" customWidth="1"/>
+    <col min="3" max="3" width="36.44140625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" ht="15.75" customHeight="1">
@@ -5518,10 +5580,10 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1"/>
+  <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15.75" customHeight="1"/>
   <cols>
-    <col min="2" max="2" width="35.7109375" customWidth="1"/>
-    <col min="3" max="3" width="36.42578125" customWidth="1"/>
+    <col min="2" max="2" width="35.71875" customWidth="1"/>
+    <col min="3" max="3" width="36.44140625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" ht="15.75" customHeight="1">
@@ -5575,10 +5637,10 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1"/>
+  <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15.75" customHeight="1"/>
   <cols>
-    <col min="2" max="2" width="35.7109375" customWidth="1"/>
-    <col min="3" max="3" width="36.42578125" customWidth="1"/>
+    <col min="2" max="2" width="35.71875" customWidth="1"/>
+    <col min="3" max="3" width="36.44140625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" ht="15.75" customHeight="1">
@@ -5622,10 +5684,10 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1"/>
+  <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15.75" customHeight="1"/>
   <cols>
-    <col min="2" max="2" width="35.7109375" customWidth="1"/>
-    <col min="3" max="3" width="36.42578125" customWidth="1"/>
+    <col min="2" max="2" width="35.71875" customWidth="1"/>
+    <col min="3" max="3" width="36.44140625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" ht="15.75" customHeight="1">

</xml_diff>

<commit_message>
Updates for final code format check
</commit_message>
<xml_diff>
--- a/Word/PlanAndDealines.xlsx
+++ b/Word/PlanAndDealines.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ksungAD\Desktop\GitHub\GTCS-GameEngine2\Word\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ksung\Desktop\GitHub\GTCS-GameEngine2\Word\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F1EF0D38-9205-4254-8AC5-0E3DB9261E91}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2764A55D-9E22-4633-8D42-F1C295B513E9}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="33648" windowHeight="15858" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="33645" windowHeight="15855" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Final Changes Must make" sheetId="8" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="328" uniqueCount="207">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="340" uniqueCount="210">
   <si>
     <t>First Pass</t>
   </si>
@@ -894,22 +894,31 @@
     <t>2. code check</t>
   </si>
   <si>
-    <t>73 characters</t>
-  </si>
-  <si>
-    <t>Search for "code format" with "Tab"</t>
-  </si>
-  <si>
-    <t>Search for code with 73 characters</t>
-  </si>
-  <si>
-    <t>Search for code bold with 73 characters</t>
-  </si>
-  <si>
-    <t>Search for "code bold" with "Tab"</t>
-  </si>
-  <si>
     <t>https://wordmvp.com/FAQs/General/UsingWildcards.htm</t>
+  </si>
+  <si>
+    <t>Space/Tabs/Indent</t>
+  </si>
+  <si>
+    <t>Too Long</t>
+  </si>
+  <si>
+    <t>Body Text First</t>
+  </si>
+  <si>
+    <t>Figure- Check Jason's Figures</t>
+  </si>
+  <si>
+    <t>Final Compare</t>
+  </si>
+  <si>
+    <t>Not Run</t>
+  </si>
+  <si>
+    <t>Checked</t>
+  </si>
+  <si>
+    <t>0/3/18</t>
   </si>
 </sst>
 </file>
@@ -1202,7 +1211,7 @@
       <name val="Arial"/>
     </font>
   </fonts>
-  <fills count="5">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1224,6 +1233,18 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="8" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.59996337778862885"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1314,7 +1335,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="46" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="105">
+  <cellXfs count="110">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
@@ -1523,6 +1544,10 @@
     </xf>
     <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="46" fillId="0" borderId="0" xfId="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1535,7 +1560,18 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="46" fillId="0" borderId="0" xfId="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="20" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -1752,13 +1788,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D8AC00B6-697C-45E4-9E65-51AD1E2696C6}">
-  <dimension ref="A3:R62"/>
+  <dimension ref="A3:R66"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A54" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="C57" sqref="C57"/>
+      <selection activeCell="C63" sqref="C63"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.3"/>
+  <sheetFormatPr defaultRowHeight="12.75"/>
   <sheetData>
     <row r="3" spans="1:18">
       <c r="A3" s="50" t="s">
@@ -1770,7 +1806,7 @@
         <v>153</v>
       </c>
     </row>
-    <row r="5" spans="1:18" ht="12.6">
+    <row r="5" spans="1:18">
       <c r="B5" s="50" t="s">
         <v>132</v>
       </c>
@@ -2052,7 +2088,7 @@
         <v>156</v>
       </c>
     </row>
-    <row r="47" spans="1:12" ht="15">
+    <row r="47" spans="1:12" ht="15.75">
       <c r="A47" s="12" t="s">
         <v>58</v>
       </c>
@@ -2070,7 +2106,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="49" spans="1:3">
+    <row r="49" spans="1:13">
       <c r="A49" s="12" t="s">
         <v>62</v>
       </c>
@@ -2079,7 +2115,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="50" spans="1:3">
+    <row r="50" spans="1:13">
       <c r="A50" s="12" t="s">
         <v>63</v>
       </c>
@@ -2088,7 +2124,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="51" spans="1:3">
+    <row r="51" spans="1:13">
       <c r="A51" s="12" t="s">
         <v>65</v>
       </c>
@@ -2097,7 +2133,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="52" spans="1:3">
+    <row r="52" spans="1:13">
       <c r="A52" s="12" t="s">
         <v>67</v>
       </c>
@@ -2106,7 +2142,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="53" spans="1:3">
+    <row r="53" spans="1:13">
       <c r="A53" s="12" t="s">
         <v>40</v>
       </c>
@@ -2115,42 +2151,167 @@
         <v>69</v>
       </c>
     </row>
-    <row r="56" spans="1:3">
+    <row r="56" spans="1:13">
       <c r="A56" s="50" t="s">
         <v>199</v>
       </c>
     </row>
-    <row r="57" spans="1:3">
+    <row r="57" spans="1:13">
       <c r="A57" s="49" t="s">
         <v>200</v>
       </c>
-      <c r="C57" s="104" t="s">
+      <c r="C57" s="101" t="s">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="58" spans="1:13">
+      <c r="B58" s="49"/>
+    </row>
+    <row r="59" spans="1:13">
+      <c r="B59" s="49"/>
+    </row>
+    <row r="60" spans="1:13">
+      <c r="B60" s="49"/>
+    </row>
+    <row r="61" spans="1:13">
+      <c r="B61" s="107">
+        <v>1</v>
+      </c>
+      <c r="C61" s="108">
+        <v>2</v>
+      </c>
+      <c r="D61" s="108">
+        <v>3</v>
+      </c>
+      <c r="E61" s="108">
+        <v>4</v>
+      </c>
+      <c r="F61" s="108">
+        <v>5</v>
+      </c>
+      <c r="G61" s="108">
+        <v>6</v>
+      </c>
+      <c r="H61" s="108">
+        <v>7</v>
+      </c>
+      <c r="I61" s="108">
+        <v>8</v>
+      </c>
+      <c r="J61" s="108">
+        <v>9</v>
+      </c>
+      <c r="K61" s="108">
+        <v>10</v>
+      </c>
+      <c r="L61" s="108">
+        <v>11</v>
+      </c>
+      <c r="M61" s="108">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="62" spans="1:13" ht="25.5">
+      <c r="A62" s="106" t="s">
+        <v>203</v>
+      </c>
+      <c r="B62" s="109" t="s">
+        <v>207</v>
+      </c>
+      <c r="C62" s="100">
+        <v>39</v>
+      </c>
+      <c r="D62" s="100"/>
+      <c r="E62" s="100"/>
+      <c r="F62" s="100"/>
+      <c r="G62" s="100"/>
+      <c r="H62" s="100"/>
+      <c r="I62" s="100"/>
+      <c r="J62" s="109" t="s">
+        <v>115</v>
+      </c>
+      <c r="K62" s="100"/>
+      <c r="L62" s="100"/>
+      <c r="M62" s="100"/>
+    </row>
+    <row r="63" spans="1:13" ht="38.25">
+      <c r="A63" s="106" t="s">
+        <v>202</v>
+      </c>
+      <c r="B63" s="109" t="s">
+        <v>207</v>
+      </c>
+      <c r="C63" s="109" t="s">
+        <v>209</v>
+      </c>
+      <c r="D63" s="100"/>
+      <c r="E63" s="100"/>
+      <c r="F63" s="100"/>
+      <c r="G63" s="100"/>
+      <c r="H63" s="100"/>
+      <c r="I63" s="100"/>
+      <c r="J63" s="109" t="s">
+        <v>115</v>
+      </c>
+      <c r="K63" s="100"/>
+      <c r="L63" s="100"/>
+      <c r="M63" s="100"/>
+    </row>
+    <row r="64" spans="1:13" ht="38.25">
+      <c r="A64" s="106" t="s">
+        <v>204</v>
+      </c>
+      <c r="B64" s="109" t="s">
+        <v>207</v>
+      </c>
+      <c r="C64" s="100">
+        <v>74</v>
+      </c>
+      <c r="D64" s="100"/>
+      <c r="E64" s="100"/>
+      <c r="F64" s="100"/>
+      <c r="G64" s="100"/>
+      <c r="H64" s="100"/>
+      <c r="I64" s="100"/>
+      <c r="J64" s="109" t="s">
+        <v>115</v>
+      </c>
+      <c r="K64" s="100"/>
+      <c r="L64" s="100"/>
+      <c r="M64" s="100"/>
+    </row>
+    <row r="65" spans="1:13" ht="51">
+      <c r="A65" s="106" t="s">
+        <v>205</v>
+      </c>
+      <c r="B65" s="109" t="s">
+        <v>208</v>
+      </c>
+      <c r="C65" s="109" t="s">
+        <v>208</v>
+      </c>
+      <c r="D65" s="100"/>
+      <c r="E65" s="100"/>
+      <c r="F65" s="100"/>
+      <c r="G65" s="100"/>
+      <c r="H65" s="100"/>
+      <c r="I65" s="100"/>
+      <c r="J65" s="109" t="s">
+        <v>115</v>
+      </c>
+      <c r="K65" s="100"/>
+      <c r="L65" s="100"/>
+      <c r="M65" s="100"/>
+    </row>
+    <row r="66" spans="1:13" ht="38.25">
+      <c r="A66" s="106" t="s">
         <v>206</v>
       </c>
-    </row>
-    <row r="58" spans="1:3">
-      <c r="B58" s="49" t="s">
-        <v>201</v>
-      </c>
-    </row>
-    <row r="59" spans="1:3">
-      <c r="B59" s="49" t="s">
-        <v>202</v>
-      </c>
-    </row>
-    <row r="60" spans="1:3">
-      <c r="B60" s="49" t="s">
-        <v>205</v>
-      </c>
-    </row>
-    <row r="61" spans="1:3">
-      <c r="B61" s="49" t="s">
-        <v>203</v>
-      </c>
-    </row>
-    <row r="62" spans="1:3">
-      <c r="B62" s="49" t="s">
-        <v>204</v>
+      <c r="B66" s="109" t="s">
+        <v>207</v>
+      </c>
+      <c r="J66" s="109" t="s">
+        <v>115</v>
       </c>
     </row>
   </sheetData>
@@ -2173,30 +2334,30 @@
       <selection activeCell="V16" sqref="V16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15.75" customHeight="1"/>
+  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1"/>
   <cols>
-    <col min="7" max="7" width="1.83203125" customWidth="1"/>
-    <col min="8" max="8" width="9.44140625" customWidth="1"/>
-    <col min="9" max="9" width="9.5546875" customWidth="1"/>
+    <col min="7" max="7" width="1.85546875" customWidth="1"/>
+    <col min="8" max="8" width="9.42578125" customWidth="1"/>
+    <col min="9" max="9" width="9.5703125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="2:12" ht="15.75" customHeight="1">
       <c r="G1" s="89"/>
     </row>
     <row r="2" spans="2:12" ht="15.75" customHeight="1">
-      <c r="D2" s="100" t="s">
+      <c r="D2" s="102" t="s">
         <v>171</v>
       </c>
-      <c r="E2" s="101"/>
-      <c r="F2" s="101"/>
+      <c r="E2" s="103"/>
+      <c r="F2" s="103"/>
       <c r="G2" s="89"/>
-      <c r="H2" s="100" t="s">
+      <c r="H2" s="102" t="s">
         <v>172</v>
       </c>
-      <c r="I2" s="100"/>
-      <c r="J2" s="100"/>
-    </row>
-    <row r="3" spans="2:12" ht="12.3">
+      <c r="I2" s="102"/>
+      <c r="J2" s="102"/>
+    </row>
+    <row r="3" spans="2:12" ht="12.75">
       <c r="B3" s="3" t="s">
         <v>19</v>
       </c>
@@ -2225,7 +2386,7 @@
       <c r="K3" s="5"/>
       <c r="L3" s="5"/>
     </row>
-    <row r="4" spans="2:12" ht="12.3">
+    <row r="4" spans="2:12" ht="12.75">
       <c r="B4" s="6" t="s">
         <v>24</v>
       </c>
@@ -2251,7 +2412,7 @@
       <c r="K4" s="5"/>
       <c r="L4" s="5"/>
     </row>
-    <row r="5" spans="2:12" ht="12.3">
+    <row r="5" spans="2:12" ht="12.75">
       <c r="B5" s="6" t="s">
         <v>25</v>
       </c>
@@ -2279,7 +2440,7 @@
       <c r="K5" s="5"/>
       <c r="L5" s="5"/>
     </row>
-    <row r="6" spans="2:12" ht="12.3">
+    <row r="6" spans="2:12" ht="12.75">
       <c r="B6" s="6" t="s">
         <v>27</v>
       </c>
@@ -2337,7 +2498,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="8" spans="2:12" ht="12.3">
+    <row r="8" spans="2:12" ht="12.75">
       <c r="B8" s="6" t="s">
         <v>32</v>
       </c>
@@ -2367,7 +2528,7 @@
       </c>
       <c r="L8" s="5"/>
     </row>
-    <row r="9" spans="2:12" ht="12.3">
+    <row r="9" spans="2:12" ht="12.75">
       <c r="B9" s="6" t="s">
         <v>35</v>
       </c>
@@ -2393,7 +2554,7 @@
       <c r="K9" s="5"/>
       <c r="L9" s="5"/>
     </row>
-    <row r="10" spans="2:12" ht="12.3">
+    <row r="10" spans="2:12" ht="12.75">
       <c r="B10" s="6" t="s">
         <v>36</v>
       </c>
@@ -2421,7 +2582,7 @@
       <c r="K10" s="5"/>
       <c r="L10" s="5"/>
     </row>
-    <row r="11" spans="2:12" ht="12.3">
+    <row r="11" spans="2:12" ht="12.75">
       <c r="B11" s="6" t="s">
         <v>38</v>
       </c>
@@ -2535,7 +2696,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="15" spans="2:12" ht="12.3">
+    <row r="15" spans="2:12" ht="12.75">
       <c r="B15" s="6" t="s">
         <v>50</v>
       </c>
@@ -2563,7 +2724,7 @@
       <c r="K15" s="5"/>
       <c r="L15" s="5"/>
     </row>
-    <row r="16" spans="2:12" ht="12.3">
+    <row r="16" spans="2:12" ht="12.75">
       <c r="B16" s="6" t="s">
         <v>52</v>
       </c>
@@ -2591,7 +2752,7 @@
       <c r="K16" s="5"/>
       <c r="L16" s="5"/>
     </row>
-    <row r="17" spans="2:12" ht="12.3">
+    <row r="17" spans="2:12" ht="12.75">
       <c r="B17" s="5"/>
       <c r="C17" s="5"/>
       <c r="D17" s="5"/>
@@ -2606,7 +2767,7 @@
       <c r="K17" s="5"/>
       <c r="L17" s="5"/>
     </row>
-    <row r="18" spans="2:12" ht="12.3">
+    <row r="18" spans="2:12" ht="12.75">
       <c r="B18" s="5"/>
       <c r="C18" s="5"/>
       <c r="D18" s="5"/>
@@ -2619,19 +2780,19 @@
       <c r="K18" s="5"/>
       <c r="L18" s="5"/>
     </row>
-    <row r="23" spans="2:12" ht="12.3">
+    <row r="23" spans="2:12" ht="12.75">
       <c r="B23" s="2" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="24" spans="2:12" ht="12.3">
+    <row r="24" spans="2:12" ht="12.75">
       <c r="B24" s="10" t="s">
         <v>55</v>
       </c>
       <c r="C24" s="11"/>
       <c r="D24" s="11"/>
     </row>
-    <row r="25" spans="2:12" ht="12.3">
+    <row r="25" spans="2:12" ht="12.75">
       <c r="B25" s="12" t="s">
         <v>56</v>
       </c>
@@ -2640,7 +2801,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="26" spans="2:12" ht="15">
+    <row r="26" spans="2:12">
       <c r="B26" s="12" t="s">
         <v>58</v>
       </c>
@@ -2649,7 +2810,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="27" spans="2:12" ht="12.3">
+    <row r="27" spans="2:12" ht="12.75">
       <c r="B27" s="12" t="s">
         <v>60</v>
       </c>
@@ -2658,7 +2819,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="28" spans="2:12" ht="12.3">
+    <row r="28" spans="2:12" ht="12.75">
       <c r="B28" s="12" t="s">
         <v>62</v>
       </c>
@@ -2667,7 +2828,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="29" spans="2:12" ht="12.3">
+    <row r="29" spans="2:12" ht="12.75">
       <c r="B29" s="12" t="s">
         <v>63</v>
       </c>
@@ -2676,7 +2837,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="30" spans="2:12" ht="12.3">
+    <row r="30" spans="2:12" ht="12.75">
       <c r="B30" s="12" t="s">
         <v>65</v>
       </c>
@@ -2685,7 +2846,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="31" spans="2:12" ht="12.3">
+    <row r="31" spans="2:12" ht="12.75">
       <c r="B31" s="12" t="s">
         <v>67</v>
       </c>
@@ -2694,7 +2855,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="32" spans="2:12" ht="12.3">
+    <row r="32" spans="2:12" ht="12.75">
       <c r="B32" s="12" t="s">
         <v>40</v>
       </c>
@@ -2727,10 +2888,10 @@
       <selection activeCell="H24" sqref="H24"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.3"/>
+  <sheetFormatPr defaultRowHeight="12.75"/>
   <cols>
-    <col min="3" max="3" width="12.5546875" customWidth="1"/>
-    <col min="4" max="8" width="14.5546875" customWidth="1"/>
+    <col min="3" max="3" width="12.5703125" customWidth="1"/>
+    <col min="4" max="8" width="14.5703125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="4" spans="2:8">
@@ -2984,46 +3145,46 @@
       <selection activeCell="P18" sqref="P18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15.75" customHeight="1"/>
+  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1"/>
   <cols>
-    <col min="3" max="4" width="1.71875" customWidth="1"/>
-    <col min="5" max="5" width="7.44140625" style="31" customWidth="1"/>
-    <col min="6" max="6" width="7.44140625" style="30" customWidth="1"/>
-    <col min="7" max="7" width="7.44140625" style="31" customWidth="1"/>
+    <col min="3" max="4" width="1.7109375" customWidth="1"/>
+    <col min="5" max="5" width="7.42578125" style="31" customWidth="1"/>
+    <col min="6" max="6" width="7.42578125" style="30" customWidth="1"/>
+    <col min="7" max="7" width="7.42578125" style="31" customWidth="1"/>
     <col min="8" max="8" width="8" style="30" customWidth="1"/>
-    <col min="9" max="9" width="7.44140625" style="31" customWidth="1"/>
-    <col min="10" max="10" width="7.44140625" style="30" customWidth="1"/>
-    <col min="11" max="11" width="7.44140625" style="31" customWidth="1"/>
-    <col min="12" max="12" width="8.44140625" style="30" customWidth="1"/>
-    <col min="13" max="13" width="7.44140625" style="31" customWidth="1"/>
-    <col min="14" max="14" width="7.44140625" style="30" customWidth="1"/>
-    <col min="15" max="15" width="16.44140625" style="29" customWidth="1"/>
-    <col min="16" max="16" width="14.44140625" style="27"/>
+    <col min="9" max="9" width="7.42578125" style="31" customWidth="1"/>
+    <col min="10" max="10" width="7.42578125" style="30" customWidth="1"/>
+    <col min="11" max="11" width="7.42578125" style="31" customWidth="1"/>
+    <col min="12" max="12" width="8.42578125" style="30" customWidth="1"/>
+    <col min="13" max="13" width="7.42578125" style="31" customWidth="1"/>
+    <col min="14" max="14" width="7.42578125" style="30" customWidth="1"/>
+    <col min="15" max="15" width="16.42578125" style="29" customWidth="1"/>
+    <col min="16" max="16" width="14.42578125" style="27"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:19" ht="12.3">
+    <row r="1" spans="2:19" ht="12.75">
       <c r="C1" s="1"/>
       <c r="D1" s="1"/>
-      <c r="E1" s="102" t="s">
+      <c r="E1" s="104" t="s">
         <v>0</v>
       </c>
-      <c r="F1" s="103"/>
-      <c r="G1" s="102" t="s">
+      <c r="F1" s="105"/>
+      <c r="G1" s="104" t="s">
         <v>1</v>
       </c>
-      <c r="H1" s="103"/>
-      <c r="I1" s="102" t="s">
+      <c r="H1" s="105"/>
+      <c r="I1" s="104" t="s">
         <v>2</v>
       </c>
-      <c r="J1" s="103"/>
-      <c r="K1" s="102" t="s">
+      <c r="J1" s="105"/>
+      <c r="K1" s="104" t="s">
         <v>1</v>
       </c>
-      <c r="L1" s="103"/>
-      <c r="M1" s="102" t="s">
+      <c r="L1" s="105"/>
+      <c r="M1" s="104" t="s">
         <v>3</v>
       </c>
-      <c r="N1" s="103"/>
+      <c r="N1" s="105"/>
       <c r="O1" s="28" t="s">
         <v>4</v>
       </c>
@@ -3034,7 +3195,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="2" spans="2:19" ht="12.6" thickBot="1">
+    <row r="2" spans="2:19" ht="13.5" thickBot="1">
       <c r="C2" s="1"/>
       <c r="D2" s="1"/>
       <c r="E2" s="32" t="s">
@@ -5320,18 +5481,18 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15.75" customHeight="1"/>
+  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1"/>
   <cols>
-    <col min="2" max="2" width="33.1640625" customWidth="1"/>
-    <col min="3" max="3" width="27.71875" customWidth="1"/>
+    <col min="2" max="2" width="33.140625" customWidth="1"/>
+    <col min="3" max="3" width="27.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" ht="12.3">
+    <row r="1" spans="1:10" ht="12.75">
       <c r="A1" s="14" t="s">
         <v>70</v>
       </c>
     </row>
-    <row r="2" spans="1:10" ht="12.3">
+    <row r="2" spans="1:10" ht="12.75">
       <c r="B2" s="14" t="s">
         <v>19</v>
       </c>
@@ -5351,7 +5512,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="3" spans="1:10" ht="12.3">
+    <row r="3" spans="1:10" ht="12.75">
       <c r="B3" s="2" t="s">
         <v>76</v>
       </c>
@@ -5362,7 +5523,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="4" spans="1:10" ht="12.3">
+    <row r="4" spans="1:10" ht="12.75">
       <c r="C4" s="2" t="s">
         <v>79</v>
       </c>
@@ -5370,20 +5531,20 @@
         <v>80</v>
       </c>
     </row>
-    <row r="5" spans="1:10" ht="13.8">
+    <row r="5" spans="1:10" ht="14.25">
       <c r="C5" s="2" t="s">
         <v>81</v>
       </c>
       <c r="H5" s="15"/>
       <c r="J5" s="16"/>
     </row>
-    <row r="6" spans="1:10" ht="12.6">
+    <row r="6" spans="1:10" ht="12.75">
       <c r="C6" s="2" t="s">
         <v>82</v>
       </c>
       <c r="J6" s="17"/>
     </row>
-    <row r="7" spans="1:10" ht="12.3">
+    <row r="7" spans="1:10" ht="12.75">
       <c r="C7" s="2" t="s">
         <v>83</v>
       </c>
@@ -5392,7 +5553,7 @@
       <c r="H8" s="18"/>
       <c r="I8" s="18"/>
     </row>
-    <row r="9" spans="1:10" ht="13.8">
+    <row r="9" spans="1:10" ht="14.25">
       <c r="B9" s="19" t="s">
         <v>84</v>
       </c>
@@ -5420,7 +5581,7 @@
     <row r="13" spans="1:10" ht="15.75" customHeight="1">
       <c r="J13" s="21"/>
     </row>
-    <row r="15" spans="1:10" ht="12.3">
+    <row r="15" spans="1:10" ht="12.75">
       <c r="B15" s="2" t="s">
         <v>88</v>
       </c>
@@ -5431,12 +5592,12 @@
         <v>15</v>
       </c>
     </row>
-    <row r="16" spans="1:10" ht="12.3">
+    <row r="16" spans="1:10" ht="12.75">
       <c r="C16" s="2" t="s">
         <v>90</v>
       </c>
     </row>
-    <row r="17" spans="1:9" ht="12.3">
+    <row r="17" spans="1:9" ht="12.75">
       <c r="G17" s="14"/>
     </row>
     <row r="18" spans="1:9" ht="15.75" customHeight="1">
@@ -5445,17 +5606,17 @@
     <row r="19" spans="1:9" ht="15.75" customHeight="1">
       <c r="I19" s="21"/>
     </row>
-    <row r="20" spans="1:9" ht="12.3">
+    <row r="20" spans="1:9" ht="12.75">
       <c r="B20" s="2" t="s">
         <v>91</v>
       </c>
     </row>
-    <row r="29" spans="1:9" ht="12.3">
+    <row r="29" spans="1:9" ht="12.75">
       <c r="A29" s="14" t="s">
         <v>92</v>
       </c>
     </row>
-    <row r="30" spans="1:9" ht="13.8">
+    <row r="30" spans="1:9" ht="14.25">
       <c r="B30" s="15" t="s">
         <v>93</v>
       </c>
@@ -5463,7 +5624,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="31" spans="1:9" ht="12.6">
+    <row r="31" spans="1:9" ht="12.75">
       <c r="D31" s="22" t="s">
         <v>95</v>
       </c>
@@ -5476,7 +5637,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="34" spans="1:4" ht="13.8">
+    <row r="34" spans="1:4" ht="14.25">
       <c r="C34" s="24" t="s">
         <v>98</v>
       </c>
@@ -5502,7 +5663,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="42" spans="1:4" ht="12.3">
+    <row r="42" spans="1:4" ht="12.75">
       <c r="A42" s="14"/>
     </row>
     <row r="43" spans="1:4" ht="15.75" customHeight="1">
@@ -5533,10 +5694,10 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15.75" customHeight="1"/>
+  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1"/>
   <cols>
-    <col min="2" max="2" width="35.71875" customWidth="1"/>
-    <col min="3" max="3" width="36.44140625" customWidth="1"/>
+    <col min="2" max="2" width="35.7109375" customWidth="1"/>
+    <col min="3" max="3" width="36.42578125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" ht="15.75" customHeight="1">
@@ -5592,10 +5753,10 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15.75" customHeight="1"/>
+  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1"/>
   <cols>
-    <col min="2" max="2" width="35.71875" customWidth="1"/>
-    <col min="3" max="3" width="36.44140625" customWidth="1"/>
+    <col min="2" max="2" width="35.7109375" customWidth="1"/>
+    <col min="3" max="3" width="36.42578125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" ht="15.75" customHeight="1">
@@ -5649,10 +5810,10 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15.75" customHeight="1"/>
+  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1"/>
   <cols>
-    <col min="2" max="2" width="35.71875" customWidth="1"/>
-    <col min="3" max="3" width="36.44140625" customWidth="1"/>
+    <col min="2" max="2" width="35.7109375" customWidth="1"/>
+    <col min="3" max="3" width="36.42578125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" ht="15.75" customHeight="1">
@@ -5696,10 +5857,10 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15.75" customHeight="1"/>
+  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1"/>
   <cols>
-    <col min="2" max="2" width="35.71875" customWidth="1"/>
-    <col min="3" max="3" width="36.44140625" customWidth="1"/>
+    <col min="2" max="2" width="35.7109375" customWidth="1"/>
+    <col min="3" max="3" width="36.42578125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" ht="15.75" customHeight="1">

</xml_diff>

<commit_message>
Code format check macro
</commit_message>
<xml_diff>
--- a/Word/PlanAndDealines.xlsx
+++ b/Word/PlanAndDealines.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ksung\Desktop\GitHub\GTCS-GameEngine2\Word\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2764A55D-9E22-4633-8D42-F1C295B513E9}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4C016B5A-F929-42D0-BFE6-B92159B7C0D9}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="33645" windowHeight="15855" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="340" uniqueCount="210">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="342" uniqueCount="212">
   <si>
     <t>First Pass</t>
   </si>
@@ -919,6 +919,12 @@
   </si>
   <si>
     <t>0/3/18</t>
+  </si>
+  <si>
+    <t>Consular</t>
+  </si>
+  <si>
+    <t>NOT YET</t>
   </si>
 </sst>
 </file>
@@ -1788,10 +1794,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D8AC00B6-697C-45E4-9E65-51AD1E2696C6}">
-  <dimension ref="A3:R66"/>
+  <dimension ref="A3:R67"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A54" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="C63" sqref="C63"/>
+      <selection activeCell="J62" sqref="J62"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
@@ -2211,16 +2217,12 @@
         <v>12</v>
       </c>
     </row>
-    <row r="62" spans="1:13" ht="25.5">
+    <row r="62" spans="1:13">
       <c r="A62" s="106" t="s">
-        <v>203</v>
-      </c>
-      <c r="B62" s="109" t="s">
-        <v>207</v>
-      </c>
-      <c r="C62" s="100">
-        <v>39</v>
-      </c>
+        <v>210</v>
+      </c>
+      <c r="B62" s="109"/>
+      <c r="C62" s="100"/>
       <c r="D62" s="100"/>
       <c r="E62" s="100"/>
       <c r="F62" s="100"/>
@@ -2228,21 +2230,21 @@
       <c r="H62" s="100"/>
       <c r="I62" s="100"/>
       <c r="J62" s="109" t="s">
-        <v>115</v>
+        <v>211</v>
       </c>
       <c r="K62" s="100"/>
       <c r="L62" s="100"/>
       <c r="M62" s="100"/>
     </row>
-    <row r="63" spans="1:13" ht="38.25">
+    <row r="63" spans="1:13" ht="25.5">
       <c r="A63" s="106" t="s">
-        <v>202</v>
+        <v>203</v>
       </c>
       <c r="B63" s="109" t="s">
         <v>207</v>
       </c>
-      <c r="C63" s="109" t="s">
-        <v>209</v>
+      <c r="C63" s="100">
+        <v>39</v>
       </c>
       <c r="D63" s="100"/>
       <c r="E63" s="100"/>
@@ -2259,13 +2261,13 @@
     </row>
     <row r="64" spans="1:13" ht="38.25">
       <c r="A64" s="106" t="s">
-        <v>204</v>
+        <v>202</v>
       </c>
       <c r="B64" s="109" t="s">
         <v>207</v>
       </c>
-      <c r="C64" s="100">
-        <v>74</v>
+      <c r="C64" s="109" t="s">
+        <v>209</v>
       </c>
       <c r="D64" s="100"/>
       <c r="E64" s="100"/>
@@ -2280,15 +2282,15 @@
       <c r="L64" s="100"/>
       <c r="M64" s="100"/>
     </row>
-    <row r="65" spans="1:13" ht="51">
+    <row r="65" spans="1:13" ht="38.25">
       <c r="A65" s="106" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="B65" s="109" t="s">
-        <v>208</v>
-      </c>
-      <c r="C65" s="109" t="s">
-        <v>208</v>
+        <v>207</v>
+      </c>
+      <c r="C65" s="100">
+        <v>74</v>
       </c>
       <c r="D65" s="100"/>
       <c r="E65" s="100"/>
@@ -2303,14 +2305,37 @@
       <c r="L65" s="100"/>
       <c r="M65" s="100"/>
     </row>
-    <row r="66" spans="1:13" ht="38.25">
+    <row r="66" spans="1:13" ht="51">
       <c r="A66" s="106" t="s">
+        <v>205</v>
+      </c>
+      <c r="B66" s="109" t="s">
+        <v>208</v>
+      </c>
+      <c r="C66" s="109" t="s">
+        <v>208</v>
+      </c>
+      <c r="D66" s="100"/>
+      <c r="E66" s="100"/>
+      <c r="F66" s="100"/>
+      <c r="G66" s="100"/>
+      <c r="H66" s="100"/>
+      <c r="I66" s="100"/>
+      <c r="J66" s="109" t="s">
+        <v>115</v>
+      </c>
+      <c r="K66" s="100"/>
+      <c r="L66" s="100"/>
+      <c r="M66" s="100"/>
+    </row>
+    <row r="67" spans="1:13" ht="38.25">
+      <c r="A67" s="106" t="s">
         <v>206</v>
       </c>
-      <c r="B66" s="109" t="s">
+      <c r="B67" s="109" t="s">
         <v>207</v>
       </c>
-      <c r="J66" s="109" t="s">
+      <c r="J67" s="109" t="s">
         <v>115</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Chap 6 done. Figures all submitted
</commit_message>
<xml_diff>
--- a/Word/PlanAndDealines.xlsx
+++ b/Word/PlanAndDealines.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ksung\Desktop\GitHub\GTCS-GameEngine2\Word\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F47F558F-4F2D-4CA5-A611-98912E983E69}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{964EF8B1-C674-4919-966B-C35732A89BE3}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="33645" windowHeight="15855" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="33645" windowHeight="15855" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Final Changes Must make" sheetId="8" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="379" uniqueCount="223">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="397" uniqueCount="221">
   <si>
     <t>First Pass</t>
   </si>
@@ -886,12 +886,6 @@
   </si>
   <si>
     <t>// …    should be change to without the "//"</t>
-  </si>
-  <si>
-    <t>1. Must load images to g-drive</t>
-  </si>
-  <si>
-    <t>2. code check</t>
   </si>
   <si>
     <t>https://wordmvp.com/FAQs/General/UsingWildcards.htm</t>
@@ -1250,7 +1244,7 @@
       <name val="Arial"/>
     </font>
   </fonts>
-  <fills count="9">
+  <fills count="10">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1296,6 +1290,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="4" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.39994506668294322"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1386,7 +1386,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="46" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="114">
+  <cellXfs count="115">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
@@ -1635,6 +1635,7 @@
     <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -1851,10 +1852,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D8AC00B6-697C-45E4-9E65-51AD1E2696C6}">
-  <dimension ref="A3:R73"/>
+  <dimension ref="A3:R60"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A54" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="H68" sqref="H68"/>
+    <sheetView topLeftCell="A39" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
+      <selection activeCell="A61" sqref="A61:N74"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
@@ -2169,7 +2170,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="49" spans="1:13">
+    <row r="49" spans="1:3">
       <c r="A49" s="12" t="s">
         <v>62</v>
       </c>
@@ -2178,7 +2179,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="50" spans="1:13">
+    <row r="50" spans="1:3">
       <c r="A50" s="12" t="s">
         <v>63</v>
       </c>
@@ -2187,7 +2188,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="51" spans="1:13">
+    <row r="51" spans="1:3">
       <c r="A51" s="12" t="s">
         <v>65</v>
       </c>
@@ -2196,7 +2197,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="52" spans="1:13">
+    <row r="52" spans="1:3">
       <c r="A52" s="12" t="s">
         <v>67</v>
       </c>
@@ -2205,7 +2206,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="53" spans="1:13">
+    <row r="53" spans="1:3">
       <c r="A53" s="12" t="s">
         <v>40</v>
       </c>
@@ -2214,284 +2215,23 @@
         <v>69</v>
       </c>
     </row>
-    <row r="56" spans="1:13">
-      <c r="A56" s="50" t="s">
+    <row r="56" spans="1:3">
+      <c r="A56" s="50"/>
+    </row>
+    <row r="57" spans="1:3">
+      <c r="A57" s="49"/>
+      <c r="C57" s="101" t="s">
         <v>199</v>
       </c>
     </row>
-    <row r="57" spans="1:13">
-      <c r="A57" s="49" t="s">
-        <v>200</v>
-      </c>
-      <c r="C57" s="101" t="s">
-        <v>201</v>
-      </c>
-    </row>
-    <row r="58" spans="1:13">
+    <row r="58" spans="1:3">
       <c r="B58" s="49"/>
     </row>
-    <row r="59" spans="1:13">
+    <row r="59" spans="1:3">
       <c r="B59" s="49"/>
     </row>
-    <row r="60" spans="1:13">
+    <row r="60" spans="1:3">
       <c r="B60" s="49"/>
-    </row>
-    <row r="61" spans="1:13">
-      <c r="B61" s="103">
-        <v>1</v>
-      </c>
-      <c r="C61" s="104">
-        <v>2</v>
-      </c>
-      <c r="D61" s="104">
-        <v>3</v>
-      </c>
-      <c r="E61" s="104">
-        <v>4</v>
-      </c>
-      <c r="F61" s="104">
-        <v>5</v>
-      </c>
-      <c r="G61" s="107">
-        <v>6</v>
-      </c>
-      <c r="H61" s="107">
-        <v>7</v>
-      </c>
-      <c r="I61" s="107">
-        <v>8</v>
-      </c>
-      <c r="J61" s="104">
-        <v>9</v>
-      </c>
-      <c r="K61" s="107">
-        <v>10</v>
-      </c>
-      <c r="L61" s="107">
-        <v>11</v>
-      </c>
-      <c r="M61" s="107">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="62" spans="1:13" ht="25.5">
-      <c r="A62" s="102" t="s">
-        <v>209</v>
-      </c>
-      <c r="B62" s="105"/>
-      <c r="C62" s="105" t="s">
-        <v>115</v>
-      </c>
-      <c r="D62" s="105" t="s">
-        <v>115</v>
-      </c>
-      <c r="E62" s="105" t="s">
-        <v>115</v>
-      </c>
-      <c r="F62" s="105" t="s">
-        <v>115</v>
-      </c>
-      <c r="G62" s="100"/>
-      <c r="H62" s="105" t="s">
-        <v>115</v>
-      </c>
-      <c r="I62" s="100"/>
-      <c r="J62" s="113" t="s">
-        <v>115</v>
-      </c>
-      <c r="K62" s="100"/>
-      <c r="L62" s="100"/>
-      <c r="M62" s="100"/>
-    </row>
-    <row r="63" spans="1:13" ht="25.5">
-      <c r="A63" s="102" t="s">
-        <v>203</v>
-      </c>
-      <c r="B63" s="105" t="s">
-        <v>207</v>
-      </c>
-      <c r="C63" s="100">
-        <v>0</v>
-      </c>
-      <c r="D63" s="112" t="s">
-        <v>221</v>
-      </c>
-      <c r="E63" s="105" t="s">
-        <v>115</v>
-      </c>
-      <c r="F63" s="105" t="s">
-        <v>115</v>
-      </c>
-      <c r="G63" s="100"/>
-      <c r="H63" s="105" t="s">
-        <v>222</v>
-      </c>
-      <c r="I63" s="100"/>
-      <c r="J63" s="105" t="s">
-        <v>115</v>
-      </c>
-      <c r="K63" s="100"/>
-      <c r="L63" s="100"/>
-      <c r="M63" s="100"/>
-    </row>
-    <row r="64" spans="1:13" ht="38.25">
-      <c r="A64" s="102" t="s">
-        <v>202</v>
-      </c>
-      <c r="B64" s="105" t="s">
-        <v>207</v>
-      </c>
-      <c r="C64" s="105" t="s">
-        <v>210</v>
-      </c>
-      <c r="D64" s="105" t="s">
-        <v>210</v>
-      </c>
-      <c r="E64" s="105" t="s">
-        <v>115</v>
-      </c>
-      <c r="F64" s="105" t="s">
-        <v>115</v>
-      </c>
-      <c r="G64" s="100"/>
-      <c r="H64" s="105" t="s">
-        <v>115</v>
-      </c>
-      <c r="I64" s="100"/>
-      <c r="J64" s="105" t="s">
-        <v>115</v>
-      </c>
-      <c r="K64" s="100"/>
-      <c r="L64" s="100"/>
-      <c r="M64" s="100"/>
-    </row>
-    <row r="65" spans="1:13" ht="38.25">
-      <c r="A65" s="102" t="s">
-        <v>204</v>
-      </c>
-      <c r="B65" s="105" t="s">
-        <v>207</v>
-      </c>
-      <c r="C65" s="105" t="s">
-        <v>208</v>
-      </c>
-      <c r="D65" s="105" t="s">
-        <v>208</v>
-      </c>
-      <c r="E65" s="105" t="s">
-        <v>115</v>
-      </c>
-      <c r="F65" s="105" t="s">
-        <v>115</v>
-      </c>
-      <c r="G65" s="100"/>
-      <c r="H65" s="105" t="s">
-        <v>115</v>
-      </c>
-      <c r="I65" s="100"/>
-      <c r="J65" s="105" t="s">
-        <v>115</v>
-      </c>
-      <c r="K65" s="100"/>
-      <c r="L65" s="100"/>
-      <c r="M65" s="100"/>
-    </row>
-    <row r="66" spans="1:13" ht="51">
-      <c r="A66" s="102" t="s">
-        <v>205</v>
-      </c>
-      <c r="B66" s="105" t="s">
-        <v>208</v>
-      </c>
-      <c r="C66" s="105" t="s">
-        <v>208</v>
-      </c>
-      <c r="D66" s="105" t="s">
-        <v>208</v>
-      </c>
-      <c r="E66" s="105" t="s">
-        <v>115</v>
-      </c>
-      <c r="F66" s="105" t="s">
-        <v>115</v>
-      </c>
-      <c r="G66" s="100"/>
-      <c r="H66" s="105" t="s">
-        <v>115</v>
-      </c>
-      <c r="I66" s="100"/>
-      <c r="J66" s="105" t="s">
-        <v>115</v>
-      </c>
-      <c r="K66" s="100"/>
-      <c r="L66" s="100"/>
-      <c r="M66" s="100"/>
-    </row>
-    <row r="67" spans="1:13" ht="38.25">
-      <c r="A67" s="102" t="s">
-        <v>206</v>
-      </c>
-      <c r="B67" s="105" t="s">
-        <v>207</v>
-      </c>
-      <c r="C67" s="105" t="s">
-        <v>115</v>
-      </c>
-      <c r="D67" s="105" t="s">
-        <v>115</v>
-      </c>
-      <c r="E67" s="105" t="s">
-        <v>115</v>
-      </c>
-      <c r="F67" s="105" t="s">
-        <v>115</v>
-      </c>
-      <c r="H67" s="105" t="s">
-        <v>115</v>
-      </c>
-      <c r="J67" s="105" t="s">
-        <v>115</v>
-      </c>
-    </row>
-    <row r="69" spans="1:13">
-      <c r="B69" s="105" t="s">
-        <v>215</v>
-      </c>
-      <c r="C69" s="106" t="s">
-        <v>220</v>
-      </c>
-    </row>
-    <row r="70" spans="1:13">
-      <c r="B70" s="105" t="s">
-        <v>211</v>
-      </c>
-      <c r="C70" s="106" t="s">
-        <v>212</v>
-      </c>
-    </row>
-    <row r="71" spans="1:13">
-      <c r="B71" s="105" t="s">
-        <v>213</v>
-      </c>
-      <c r="C71" s="106" t="s">
-        <v>214</v>
-      </c>
-    </row>
-    <row r="72" spans="1:13">
-      <c r="B72" s="105" t="s">
-        <v>216</v>
-      </c>
-      <c r="C72" s="106" t="s">
-        <v>217</v>
-      </c>
-    </row>
-    <row r="73" spans="1:13">
-      <c r="B73" s="105" t="s">
-        <v>218</v>
-      </c>
-      <c r="C73" s="106" t="s">
-        <v>219</v>
-      </c>
     </row>
   </sheetData>
   <hyperlinks>
@@ -3061,14 +2801,15 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1E946A0D-49B4-48B1-99B4-6819045C52D0}">
-  <dimension ref="B4:H16"/>
+  <dimension ref="A4:M32"/>
   <sheetViews>
-    <sheetView zoomScale="190" zoomScaleNormal="190" workbookViewId="0">
-      <selection activeCell="H24" sqref="H24"/>
+    <sheetView tabSelected="1" topLeftCell="A7" zoomScale="190" zoomScaleNormal="190" workbookViewId="0">
+      <selection activeCell="F36" sqref="F36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
   <cols>
+    <col min="1" max="1" width="19.85546875" customWidth="1"/>
     <col min="3" max="3" width="12.5703125" customWidth="1"/>
     <col min="4" max="8" width="14.5703125" customWidth="1"/>
   </cols>
@@ -3215,10 +2956,22 @@
       <c r="B10">
         <v>6</v>
       </c>
+      <c r="C10" s="96">
+        <v>44447</v>
+      </c>
       <c r="D10" s="96">
-        <v>44445</v>
+        <v>44448</v>
+      </c>
+      <c r="E10" s="96">
+        <v>44451</v>
       </c>
       <c r="F10" s="99"/>
+      <c r="G10" s="96">
+        <v>44451</v>
+      </c>
+      <c r="H10" s="96">
+        <v>44451</v>
+      </c>
     </row>
     <row r="11" spans="2:8">
       <c r="B11">
@@ -3272,7 +3025,16 @@
       <c r="D13" s="96">
         <v>44444</v>
       </c>
+      <c r="E13" s="96">
+        <v>44448</v>
+      </c>
       <c r="F13" s="99"/>
+      <c r="G13" s="96">
+        <v>44451</v>
+      </c>
+      <c r="H13" s="96">
+        <v>44451</v>
+      </c>
     </row>
     <row r="14" spans="2:8">
       <c r="B14">
@@ -3301,10 +3063,324 @@
       <c r="B15">
         <v>11</v>
       </c>
+      <c r="C15" s="96">
+        <v>44447</v>
+      </c>
+      <c r="D15" s="96">
+        <v>44449</v>
+      </c>
+      <c r="F15" s="114"/>
     </row>
     <row r="16" spans="2:8">
       <c r="B16">
         <v>12</v>
+      </c>
+      <c r="C16" s="96">
+        <v>44447</v>
+      </c>
+      <c r="D16" s="96">
+        <v>44449</v>
+      </c>
+      <c r="F16" s="114"/>
+    </row>
+    <row r="20" spans="1:13">
+      <c r="B20" s="103">
+        <v>1</v>
+      </c>
+      <c r="C20" s="104">
+        <v>2</v>
+      </c>
+      <c r="D20" s="104">
+        <v>3</v>
+      </c>
+      <c r="E20" s="104">
+        <v>4</v>
+      </c>
+      <c r="F20" s="104">
+        <v>5</v>
+      </c>
+      <c r="G20" s="104">
+        <v>6</v>
+      </c>
+      <c r="H20" s="104">
+        <v>7</v>
+      </c>
+      <c r="I20" s="104">
+        <v>8</v>
+      </c>
+      <c r="J20" s="104">
+        <v>9</v>
+      </c>
+      <c r="K20" s="104">
+        <v>10</v>
+      </c>
+      <c r="L20" s="107">
+        <v>11</v>
+      </c>
+      <c r="M20" s="107">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="21" spans="1:13">
+      <c r="A21" s="102" t="s">
+        <v>207</v>
+      </c>
+      <c r="B21" s="105"/>
+      <c r="C21" s="105" t="s">
+        <v>115</v>
+      </c>
+      <c r="D21" s="105" t="s">
+        <v>115</v>
+      </c>
+      <c r="E21" s="105" t="s">
+        <v>115</v>
+      </c>
+      <c r="F21" s="105" t="s">
+        <v>115</v>
+      </c>
+      <c r="G21" s="105" t="s">
+        <v>115</v>
+      </c>
+      <c r="H21" s="105" t="s">
+        <v>115</v>
+      </c>
+      <c r="I21" s="105" t="s">
+        <v>115</v>
+      </c>
+      <c r="J21" s="113" t="s">
+        <v>115</v>
+      </c>
+      <c r="K21" s="105" t="s">
+        <v>115</v>
+      </c>
+      <c r="L21" s="100"/>
+      <c r="M21" s="100"/>
+    </row>
+    <row r="22" spans="1:13">
+      <c r="A22" s="102" t="s">
+        <v>201</v>
+      </c>
+      <c r="B22" s="105" t="s">
+        <v>205</v>
+      </c>
+      <c r="C22" s="100">
+        <v>0</v>
+      </c>
+      <c r="D22" s="112" t="s">
+        <v>219</v>
+      </c>
+      <c r="E22" s="105" t="s">
+        <v>115</v>
+      </c>
+      <c r="F22" s="105" t="s">
+        <v>115</v>
+      </c>
+      <c r="G22" s="105" t="s">
+        <v>115</v>
+      </c>
+      <c r="H22" s="105" t="s">
+        <v>220</v>
+      </c>
+      <c r="I22" s="105" t="s">
+        <v>115</v>
+      </c>
+      <c r="J22" s="105" t="s">
+        <v>115</v>
+      </c>
+      <c r="K22" s="105" t="s">
+        <v>115</v>
+      </c>
+      <c r="L22" s="100"/>
+      <c r="M22" s="100"/>
+    </row>
+    <row r="23" spans="1:13">
+      <c r="A23" s="102" t="s">
+        <v>200</v>
+      </c>
+      <c r="B23" s="105" t="s">
+        <v>205</v>
+      </c>
+      <c r="C23" s="105" t="s">
+        <v>208</v>
+      </c>
+      <c r="D23" s="105" t="s">
+        <v>208</v>
+      </c>
+      <c r="E23" s="105" t="s">
+        <v>115</v>
+      </c>
+      <c r="F23" s="105" t="s">
+        <v>115</v>
+      </c>
+      <c r="G23" s="105" t="s">
+        <v>115</v>
+      </c>
+      <c r="H23" s="105" t="s">
+        <v>115</v>
+      </c>
+      <c r="I23" s="105" t="s">
+        <v>115</v>
+      </c>
+      <c r="J23" s="105" t="s">
+        <v>115</v>
+      </c>
+      <c r="K23" s="105" t="s">
+        <v>115</v>
+      </c>
+      <c r="L23" s="100"/>
+      <c r="M23" s="100"/>
+    </row>
+    <row r="24" spans="1:13">
+      <c r="A24" s="102" t="s">
+        <v>202</v>
+      </c>
+      <c r="B24" s="105" t="s">
+        <v>205</v>
+      </c>
+      <c r="C24" s="105" t="s">
+        <v>206</v>
+      </c>
+      <c r="D24" s="105" t="s">
+        <v>206</v>
+      </c>
+      <c r="E24" s="105" t="s">
+        <v>115</v>
+      </c>
+      <c r="F24" s="105" t="s">
+        <v>115</v>
+      </c>
+      <c r="G24" s="105" t="s">
+        <v>115</v>
+      </c>
+      <c r="H24" s="105" t="s">
+        <v>115</v>
+      </c>
+      <c r="I24" s="105" t="s">
+        <v>115</v>
+      </c>
+      <c r="J24" s="105" t="s">
+        <v>115</v>
+      </c>
+      <c r="K24" s="105" t="s">
+        <v>115</v>
+      </c>
+      <c r="L24" s="100"/>
+      <c r="M24" s="100"/>
+    </row>
+    <row r="25" spans="1:13" ht="25.5">
+      <c r="A25" s="102" t="s">
+        <v>203</v>
+      </c>
+      <c r="B25" s="105" t="s">
+        <v>206</v>
+      </c>
+      <c r="C25" s="105" t="s">
+        <v>206</v>
+      </c>
+      <c r="D25" s="105" t="s">
+        <v>206</v>
+      </c>
+      <c r="E25" s="105" t="s">
+        <v>115</v>
+      </c>
+      <c r="F25" s="105" t="s">
+        <v>115</v>
+      </c>
+      <c r="G25" s="105" t="s">
+        <v>115</v>
+      </c>
+      <c r="H25" s="105" t="s">
+        <v>115</v>
+      </c>
+      <c r="I25" s="105" t="s">
+        <v>115</v>
+      </c>
+      <c r="J25" s="105" t="s">
+        <v>115</v>
+      </c>
+      <c r="K25" s="105" t="s">
+        <v>115</v>
+      </c>
+      <c r="L25" s="105" t="s">
+        <v>115</v>
+      </c>
+      <c r="M25" s="105" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="26" spans="1:13">
+      <c r="A26" s="102" t="s">
+        <v>204</v>
+      </c>
+      <c r="B26" s="105" t="s">
+        <v>205</v>
+      </c>
+      <c r="C26" s="105" t="s">
+        <v>115</v>
+      </c>
+      <c r="D26" s="105" t="s">
+        <v>115</v>
+      </c>
+      <c r="E26" s="105" t="s">
+        <v>115</v>
+      </c>
+      <c r="F26" s="105" t="s">
+        <v>115</v>
+      </c>
+      <c r="G26" s="105" t="s">
+        <v>115</v>
+      </c>
+      <c r="H26" s="105" t="s">
+        <v>115</v>
+      </c>
+      <c r="I26" s="105" t="s">
+        <v>115</v>
+      </c>
+      <c r="J26" s="105" t="s">
+        <v>115</v>
+      </c>
+      <c r="K26" s="105" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="28" spans="1:13">
+      <c r="B28" s="105" t="s">
+        <v>213</v>
+      </c>
+      <c r="C28" s="106" t="s">
+        <v>218</v>
+      </c>
+    </row>
+    <row r="29" spans="1:13">
+      <c r="B29" s="105" t="s">
+        <v>209</v>
+      </c>
+      <c r="C29" s="106" t="s">
+        <v>210</v>
+      </c>
+    </row>
+    <row r="30" spans="1:13">
+      <c r="B30" s="105" t="s">
+        <v>211</v>
+      </c>
+      <c r="C30" s="106" t="s">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="31" spans="1:13">
+      <c r="B31" s="105" t="s">
+        <v>214</v>
+      </c>
+      <c r="C31" s="106" t="s">
+        <v>215</v>
+      </c>
+    </row>
+    <row r="32" spans="1:13">
+      <c r="B32" s="105" t="s">
+        <v>216</v>
+      </c>
+      <c r="C32" s="106" t="s">
+        <v>217</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Chap 11 and 12 are done.
</commit_message>
<xml_diff>
--- a/Word/PlanAndDealines.xlsx
+++ b/Word/PlanAndDealines.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ksung\Desktop\GitHub\GTCS-GameEngine2\Word\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FB28DBBD-5AC6-4B2E-A139-93D636415309}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B69A590C-6952-4518-A939-65EF4C32C062}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="33645" windowHeight="15855" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="397" uniqueCount="221">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="402" uniqueCount="222">
   <si>
     <t>First Pass</t>
   </si>
@@ -952,6 +952,9 @@
   </si>
   <si>
     <t>one line wrap</t>
+  </si>
+  <si>
+    <t>Nothing to compare with</t>
   </si>
 </sst>
 </file>
@@ -1386,7 +1389,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="46" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="118">
+  <cellXfs count="119">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
@@ -1617,16 +1620,7 @@
     <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="22" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
@@ -1644,6 +1638,18 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -2273,17 +2279,17 @@
       <c r="G1" s="89"/>
     </row>
     <row r="2" spans="2:12" ht="15.75" customHeight="1">
-      <c r="D2" s="108" t="s">
+      <c r="D2" s="115" t="s">
         <v>171</v>
       </c>
-      <c r="E2" s="109"/>
-      <c r="F2" s="109"/>
+      <c r="E2" s="116"/>
+      <c r="F2" s="116"/>
       <c r="G2" s="89"/>
-      <c r="H2" s="108" t="s">
+      <c r="H2" s="115" t="s">
         <v>172</v>
       </c>
-      <c r="I2" s="108"/>
-      <c r="J2" s="108"/>
+      <c r="I2" s="115"/>
+      <c r="J2" s="115"/>
     </row>
     <row r="3" spans="2:12" ht="12.75">
       <c r="B3" s="3" t="s">
@@ -2813,7 +2819,7 @@
   <dimension ref="A4:M32"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="190" zoomScaleNormal="190" workbookViewId="0">
-      <selection activeCell="F31" sqref="F31"/>
+      <selection activeCell="L27" sqref="L27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
@@ -3078,7 +3084,7 @@
       <c r="D15" s="96">
         <v>44449</v>
       </c>
-      <c r="F15" s="114"/>
+      <c r="F15" s="111"/>
     </row>
     <row r="16" spans="2:8">
       <c r="B16">
@@ -3090,7 +3096,7 @@
       <c r="D16" s="96">
         <v>44449</v>
       </c>
-      <c r="F16" s="114"/>
+      <c r="F16" s="111"/>
     </row>
     <row r="20" spans="1:13">
       <c r="B20" s="103">
@@ -3156,13 +3162,15 @@
       <c r="I21" s="105" t="s">
         <v>115</v>
       </c>
-      <c r="J21" s="113" t="s">
+      <c r="J21" s="110" t="s">
         <v>115</v>
       </c>
       <c r="K21" s="105" t="s">
         <v>115</v>
       </c>
-      <c r="L21" s="100"/>
+      <c r="L21" s="100" t="s">
+        <v>115</v>
+      </c>
       <c r="M21" s="100"/>
     </row>
     <row r="22" spans="1:13">
@@ -3175,7 +3183,7 @@
       <c r="C22" s="100">
         <v>0</v>
       </c>
-      <c r="D22" s="112" t="s">
+      <c r="D22" s="109" t="s">
         <v>219</v>
       </c>
       <c r="E22" s="105" t="s">
@@ -3199,7 +3207,9 @@
       <c r="K22" s="105" t="s">
         <v>115</v>
       </c>
-      <c r="L22" s="100"/>
+      <c r="L22" s="100" t="s">
+        <v>115</v>
+      </c>
       <c r="M22" s="100"/>
     </row>
     <row r="23" spans="1:13">
@@ -3236,7 +3246,9 @@
       <c r="K23" s="105" t="s">
         <v>115</v>
       </c>
-      <c r="L23" s="100"/>
+      <c r="L23" s="100" t="s">
+        <v>115</v>
+      </c>
       <c r="M23" s="100"/>
     </row>
     <row r="24" spans="1:13">
@@ -3273,47 +3285,49 @@
       <c r="K24" s="105" t="s">
         <v>115</v>
       </c>
-      <c r="L24" s="100"/>
+      <c r="L24" s="100" t="s">
+        <v>115</v>
+      </c>
       <c r="M24" s="100"/>
     </row>
-    <row r="25" spans="1:13" s="117" customFormat="1" ht="25.5">
-      <c r="A25" s="115" t="s">
+    <row r="25" spans="1:13" s="114" customFormat="1" ht="25.5">
+      <c r="A25" s="112" t="s">
         <v>203</v>
       </c>
-      <c r="B25" s="116" t="s">
+      <c r="B25" s="113" t="s">
         <v>206</v>
       </c>
-      <c r="C25" s="116" t="s">
+      <c r="C25" s="113" t="s">
         <v>206</v>
       </c>
-      <c r="D25" s="116" t="s">
+      <c r="D25" s="113" t="s">
         <v>206</v>
       </c>
-      <c r="E25" s="116" t="s">
+      <c r="E25" s="113" t="s">
         <v>115</v>
       </c>
-      <c r="F25" s="116" t="s">
+      <c r="F25" s="113" t="s">
         <v>115</v>
       </c>
-      <c r="G25" s="116" t="s">
+      <c r="G25" s="113" t="s">
         <v>115</v>
       </c>
-      <c r="H25" s="116" t="s">
+      <c r="H25" s="113" t="s">
         <v>115</v>
       </c>
-      <c r="I25" s="116" t="s">
+      <c r="I25" s="113" t="s">
         <v>115</v>
       </c>
-      <c r="J25" s="116" t="s">
+      <c r="J25" s="113" t="s">
         <v>115</v>
       </c>
-      <c r="K25" s="116" t="s">
+      <c r="K25" s="113" t="s">
         <v>115</v>
       </c>
-      <c r="L25" s="116" t="s">
+      <c r="L25" s="113" t="s">
         <v>115</v>
       </c>
-      <c r="M25" s="116" t="s">
+      <c r="M25" s="113" t="s">
         <v>115</v>
       </c>
     </row>
@@ -3350,6 +3364,9 @@
       </c>
       <c r="K26" s="105" t="s">
         <v>115</v>
+      </c>
+      <c r="L26" s="108" t="s">
+        <v>221</v>
       </c>
     </row>
     <row r="28" spans="1:13">
@@ -3429,26 +3446,26 @@
     <row r="1" spans="2:19" ht="12.75">
       <c r="C1" s="1"/>
       <c r="D1" s="1"/>
-      <c r="E1" s="110" t="s">
+      <c r="E1" s="117" t="s">
         <v>0</v>
       </c>
-      <c r="F1" s="111"/>
-      <c r="G1" s="110" t="s">
+      <c r="F1" s="118"/>
+      <c r="G1" s="117" t="s">
         <v>1</v>
       </c>
-      <c r="H1" s="111"/>
-      <c r="I1" s="110" t="s">
+      <c r="H1" s="118"/>
+      <c r="I1" s="117" t="s">
         <v>2</v>
       </c>
-      <c r="J1" s="111"/>
-      <c r="K1" s="110" t="s">
+      <c r="J1" s="118"/>
+      <c r="K1" s="117" t="s">
         <v>1</v>
       </c>
-      <c r="L1" s="111"/>
-      <c r="M1" s="110" t="s">
+      <c r="L1" s="118"/>
+      <c r="M1" s="117" t="s">
         <v>3</v>
       </c>
-      <c r="N1" s="111"/>
+      <c r="N1" s="118"/>
       <c r="O1" s="28" t="s">
         <v>4</v>
       </c>

</xml_diff>